<commit_message>
2024.01.04 每日一题 Gosper's Hack
</commit_message>
<xml_diff>
--- a/2024LeetCode刷题记录.xlsx
+++ b/2024LeetCode刷题记录.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\develop\GithubRepo\LeetCode\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{11E77F0F-3432-4CEC-87D9-795E3B54CAFD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F8DF9A37-B8E8-4713-BEA9-D2F508F47871}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-103" yWindow="-103" windowWidth="22149" windowHeight="11829" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="44">
   <si>
     <t>题目</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -176,6 +176,25 @@
   </si>
   <si>
     <t xml:space="preserve"> Deque&lt;ListNode&gt; stack = new ArrayDeque&lt;ListNode&gt;();</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>2024.01.04</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>2397. 被列覆盖的最多行数</t>
+  </si>
+  <si>
+    <t>Integer.bitCount(mask)。Gosper's Hack： 找到二进制串里的最后一个“01”，把他变成“10”，就是当前组合的下一个组合。还不够完整，01变成10之后，需要把10右边所有的1都往右移动到底。例如0101110，01变10之后就是0110110，移动到底变成0110011。</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>位运算、Gosper's Hack</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>⭐⭐⭐</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -616,10 +635,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G8"/>
+  <dimension ref="A1:G9"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="F11" sqref="F11"/>
+      <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.15" x14ac:dyDescent="0.35"/>
@@ -676,9 +695,6 @@
       <c r="F2" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="G2" s="6">
-        <v>1</v>
-      </c>
     </row>
     <row r="3" spans="1:7" ht="17.149999999999999" x14ac:dyDescent="0.55000000000000004">
       <c r="A3" s="4" t="s">
@@ -699,9 +715,6 @@
       <c r="F3" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="G3" s="6">
-        <v>1</v>
-      </c>
     </row>
     <row r="4" spans="1:7" ht="17.149999999999999" x14ac:dyDescent="0.55000000000000004">
       <c r="A4" s="4" t="s">
@@ -722,9 +735,6 @@
       <c r="F4" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="G4" s="6">
-        <v>1</v>
-      </c>
     </row>
     <row r="5" spans="1:7" ht="17.149999999999999" x14ac:dyDescent="0.55000000000000004">
       <c r="A5" s="4" t="s">
@@ -745,9 +755,6 @@
       <c r="F5" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="G5" s="6">
-        <v>1</v>
-      </c>
     </row>
     <row r="6" spans="1:7" ht="17.149999999999999" x14ac:dyDescent="0.55000000000000004">
       <c r="A6" s="10" t="s">
@@ -765,9 +772,6 @@
       <c r="E6" s="9" t="s">
         <v>28</v>
       </c>
-      <c r="G6" s="6">
-        <v>1</v>
-      </c>
     </row>
     <row r="7" spans="1:7" ht="17.149999999999999" x14ac:dyDescent="0.55000000000000004">
       <c r="A7" s="10" t="s">
@@ -788,9 +792,6 @@
       <c r="F7" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="G7" s="6">
-        <v>1</v>
-      </c>
     </row>
     <row r="8" spans="1:7" ht="17.149999999999999" x14ac:dyDescent="0.55000000000000004">
       <c r="A8" s="10" t="s">
@@ -811,8 +812,25 @@
       <c r="F8" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="G8" s="6">
-        <v>1</v>
+    </row>
+    <row r="9" spans="1:7" ht="17.149999999999999" x14ac:dyDescent="0.55000000000000004">
+      <c r="A9" s="10" t="s">
+        <v>40</v>
+      </c>
+      <c r="B9" s="6" t="s">
+        <v>42</v>
+      </c>
+      <c r="C9" s="7" t="s">
+        <v>43</v>
+      </c>
+      <c r="D9" s="8" t="s">
+        <v>39</v>
+      </c>
+      <c r="E9" s="9" t="s">
+        <v>23</v>
+      </c>
+      <c r="F9" s="3" t="s">
+        <v>41</v>
       </c>
     </row>
   </sheetData>
@@ -832,10 +850,12 @@
     <hyperlink ref="E7" r:id="rId12" xr:uid="{C7FFAB8C-8294-407A-AF24-C9D1899CE796}"/>
     <hyperlink ref="A8" r:id="rId13" display="https://leetcode.cn/problems/remove-nodes-from-linked-list/" xr:uid="{7D6CA718-D46A-4E15-A1D5-734F68A5EE6A}"/>
     <hyperlink ref="E8" r:id="rId14" xr:uid="{1BB1D542-CE6A-4F15-BAD0-8E150E86DAEE}"/>
+    <hyperlink ref="A9" r:id="rId15" display="https://leetcode.cn/problems/maximum-rows-covered-by-columns/" xr:uid="{EED2AFE8-A6A7-4831-A7F5-3B09768F94A3}"/>
+    <hyperlink ref="E9" r:id="rId16" xr:uid="{37A4ECD3-6A85-4A80-BADD-45ACC7A4BDAC}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <tableParts count="1">
-    <tablePart r:id="rId15"/>
+    <tablePart r:id="rId17"/>
   </tableParts>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
2024.01.16 每日一题 hard cv
</commit_message>
<xml_diff>
--- a/2024LeetCode刷题记录.xlsx
+++ b/2024LeetCode刷题记录.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\develop\GithubRepo\LeetCode\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8E11874C-1921-4A05-BC72-F17CAA415BA2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1A7280DF-61D5-42E5-B9EB-B807B9E48086}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-17190" yWindow="2535" windowWidth="16455" windowHeight="10695" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-21990" yWindow="3885" windowWidth="16455" windowHeight="10695" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="168" uniqueCount="124">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="178" uniqueCount="130">
   <si>
     <t>题目</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -494,6 +494,28 @@
   </si>
   <si>
     <t>if(window.get(cur).equals(need.get(cur))) {</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>734. 句子相似性</t>
+  </si>
+  <si>
+    <t>哈希表</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>2024.01.16</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>力扣官方</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>2719. 统计整数数目</t>
+  </si>
+  <si>
+    <t>数学、动态规划</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -934,10 +956,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G30"/>
+  <dimension ref="A1:G32"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B18" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="F30" sqref="F30"/>
+    <sheetView tabSelected="1" topLeftCell="A23" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="E34" sqref="E34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.15" x14ac:dyDescent="0.35"/>
@@ -1514,6 +1536,40 @@
       </c>
       <c r="F30" s="3" t="s">
         <v>123</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" ht="17.149999999999999" x14ac:dyDescent="0.55000000000000004">
+      <c r="A31" s="10" t="s">
+        <v>124</v>
+      </c>
+      <c r="B31" s="6" t="s">
+        <v>125</v>
+      </c>
+      <c r="C31" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="D31" s="8" t="s">
+        <v>126</v>
+      </c>
+      <c r="E31" s="9" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" ht="17.149999999999999" x14ac:dyDescent="0.55000000000000004">
+      <c r="A32" s="10" t="s">
+        <v>128</v>
+      </c>
+      <c r="B32" s="6" t="s">
+        <v>129</v>
+      </c>
+      <c r="C32" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="D32" s="8" t="s">
+        <v>126</v>
+      </c>
+      <c r="E32" s="9" t="s">
+        <v>127</v>
       </c>
     </row>
   </sheetData>
@@ -1574,10 +1630,14 @@
     <hyperlink ref="E29" r:id="rId53" xr:uid="{710F1479-585D-4444-83C8-6D53E855AFE0}"/>
     <hyperlink ref="A30" r:id="rId54" display="https://leetcode.cn/problems/find-all-anagrams-in-a-string/" xr:uid="{36A9C6AE-A4CD-4F4E-90F8-8E5D5CB43CAB}"/>
     <hyperlink ref="E30" r:id="rId55" xr:uid="{4FDD3B32-5D43-4481-A2CA-C7F81DDF97FA}"/>
+    <hyperlink ref="A31" r:id="rId56" display="https://leetcode.cn/problems/sentence-similarity/" xr:uid="{771EA040-6E9F-427A-9C87-C5F54FA18B80}"/>
+    <hyperlink ref="E31" r:id="rId57" xr:uid="{70C2F0B7-B280-4BFB-BECF-378146CDDA35}"/>
+    <hyperlink ref="A32" r:id="rId58" display="https://leetcode.cn/problems/count-of-integers/" xr:uid="{0F898565-2E05-4648-B060-6053E5749B06}"/>
+    <hyperlink ref="E32" r:id="rId59" xr:uid="{9A949AF4-4EB7-44E4-BACF-B1D5B5248519}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <tableParts count="1">
-    <tablePart r:id="rId56"/>
+    <tablePart r:id="rId60"/>
   </tableParts>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
2024.09.05 刷题心得 equals() vs ==
</commit_message>
<xml_diff>
--- a/2024LeetCode刷题记录.xlsx
+++ b/2024LeetCode刷题记录.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\develop\GithubRepo\LeetCode\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F847FB76-53C8-42AC-B7D4-4EB078B91BB6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A67E1861-AF09-48CE-A385-E0B349980491}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-103" yWindow="-103" windowWidth="22149" windowHeight="11829" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="637" uniqueCount="346">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="637" uniqueCount="347">
   <si>
     <t>题目</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -448,10 +448,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>if(window.get(cur).equals(need.get(cur))) {</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>734. 句子相似性</t>
   </si>
   <si>
@@ -1276,6 +1272,13 @@
   <si>
     <t>代码随想录</t>
     <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>2024.09.05</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>validCount很重要</t>
   </si>
 </sst>
 </file>
@@ -1445,7 +1448,7 @@
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{E5AA65A4-B8FD-4A83-87AF-D7798D621280}" name="表1" displayName="表1" ref="A1:G1048575" totalsRowShown="0" headerRowDxfId="8" dataDxfId="7">
   <autoFilter ref="A1:G1048575" xr:uid="{E5AA65A4-B8FD-4A83-87AF-D7798D621280}"/>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:G141">
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:G142">
     <sortCondition ref="A1:A1048575"/>
   </sortState>
   <tableColumns count="7">
@@ -1726,8 +1729,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G139"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A88" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="G98" sqref="G98"/>
+    <sheetView tabSelected="1" topLeftCell="A100" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="F106" sqref="F106"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="14.15" x14ac:dyDescent="0.35"/>
@@ -1776,7 +1779,7 @@
         <v>80</v>
       </c>
       <c r="D2" s="8" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="F2" s="6">
         <v>2</v>
@@ -1787,35 +1790,35 @@
     </row>
     <row r="3" spans="1:7" ht="17.149999999999999" x14ac:dyDescent="0.55000000000000004">
       <c r="A3" s="10" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="C3" s="7" t="s">
         <v>13</v>
       </c>
       <c r="D3" s="8" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
     </row>
     <row r="4" spans="1:7" ht="17.149999999999999" x14ac:dyDescent="0.55000000000000004">
       <c r="A4" s="10" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="C4" s="7" t="s">
         <v>13</v>
       </c>
       <c r="D4" s="8" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
     </row>
     <row r="5" spans="1:7" ht="17.149999999999999" x14ac:dyDescent="0.55000000000000004">
       <c r="A5" s="10" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="C5" s="7" t="s">
         <v>13</v>
       </c>
       <c r="D5" s="8" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
     </row>
     <row r="6" spans="1:7" ht="17.149999999999999" x14ac:dyDescent="0.55000000000000004">
@@ -1840,24 +1843,24 @@
     </row>
     <row r="7" spans="1:7" ht="17.149999999999999" x14ac:dyDescent="0.55000000000000004">
       <c r="A7" s="10" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="C7" s="7" t="s">
         <v>80</v>
       </c>
       <c r="D7" s="8" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
     </row>
     <row r="8" spans="1:7" ht="17.149999999999999" x14ac:dyDescent="0.55000000000000004">
       <c r="A8" s="10" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="C8" s="7" t="s">
         <v>42</v>
       </c>
       <c r="D8" s="8" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
     </row>
     <row r="9" spans="1:7" ht="17.149999999999999" x14ac:dyDescent="0.55000000000000004">
@@ -1865,13 +1868,13 @@
         <v>91</v>
       </c>
       <c r="B9" s="6" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="C9" s="7" t="s">
         <v>42</v>
       </c>
       <c r="D9" s="8" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="E9" s="9" t="s">
         <v>93</v>
@@ -1880,38 +1883,38 @@
         <v>3</v>
       </c>
       <c r="G9" s="3" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
     </row>
     <row r="10" spans="1:7" ht="17.149999999999999" x14ac:dyDescent="0.55000000000000004">
       <c r="A10" s="10" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="C10" s="7" t="s">
         <v>6</v>
       </c>
       <c r="D10" s="8" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
     </row>
     <row r="11" spans="1:7" ht="17.149999999999999" x14ac:dyDescent="0.55000000000000004">
       <c r="A11" s="10" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="B11" s="6" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="C11" s="7" t="s">
         <v>80</v>
       </c>
       <c r="D11" s="8" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="E11" s="9" t="s">
         <v>14</v>
       </c>
       <c r="G11" s="3" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
     </row>
     <row r="12" spans="1:7" ht="17.149999999999999" x14ac:dyDescent="0.55000000000000004">
@@ -1936,16 +1939,16 @@
     </row>
     <row r="13" spans="1:7" ht="17.149999999999999" x14ac:dyDescent="0.55000000000000004">
       <c r="A13" s="10" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="B13" s="6" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="C13" s="7" t="s">
         <v>6</v>
       </c>
       <c r="D13" s="8" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
     </row>
     <row r="14" spans="1:7" ht="17.149999999999999" x14ac:dyDescent="0.55000000000000004">
@@ -1970,35 +1973,35 @@
     </row>
     <row r="15" spans="1:7" ht="17.149999999999999" x14ac:dyDescent="0.55000000000000004">
       <c r="A15" s="10" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="B15" s="6" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="C15" s="7" t="s">
         <v>42</v>
       </c>
       <c r="D15" s="8" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
     </row>
     <row r="16" spans="1:7" ht="17.149999999999999" x14ac:dyDescent="0.55000000000000004">
       <c r="A16" s="10" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="C16" s="7" t="s">
         <v>13</v>
       </c>
       <c r="D16" s="8" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="G16" s="3" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
     </row>
     <row r="17" spans="1:7" ht="17.149999999999999" x14ac:dyDescent="0.55000000000000004">
       <c r="A17" s="10" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="B17" s="6" t="s">
         <v>79</v>
@@ -2007,7 +2010,7 @@
         <v>80</v>
       </c>
       <c r="D17" s="8" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="F17" s="6">
         <v>2</v>
@@ -2015,35 +2018,35 @@
     </row>
     <row r="18" spans="1:7" ht="17.149999999999999" x14ac:dyDescent="0.55000000000000004">
       <c r="A18" s="10" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="B18" s="6" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="C18" s="7" t="s">
         <v>13</v>
       </c>
       <c r="D18" s="8" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
     </row>
     <row r="19" spans="1:7" ht="17.149999999999999" x14ac:dyDescent="0.55000000000000004">
       <c r="A19" s="10" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="B19" s="6" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="C19" s="7" t="s">
         <v>28</v>
       </c>
       <c r="D19" s="8" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
     </row>
     <row r="20" spans="1:7" ht="17.149999999999999" x14ac:dyDescent="0.55000000000000004">
       <c r="A20" s="10" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="B20" s="6" t="s">
         <v>49</v>
@@ -2052,7 +2055,7 @@
         <v>13</v>
       </c>
       <c r="D20" s="8" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="E20" s="9" t="s">
         <v>87</v>
@@ -2060,16 +2063,16 @@
     </row>
     <row r="21" spans="1:7" ht="17.149999999999999" x14ac:dyDescent="0.55000000000000004">
       <c r="A21" s="10" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="B21" s="6" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="C21" s="7" t="s">
         <v>13</v>
       </c>
       <c r="D21" s="8" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="E21" s="9" t="s">
         <v>22</v>
@@ -2077,44 +2080,44 @@
     </row>
     <row r="22" spans="1:7" ht="17.149999999999999" x14ac:dyDescent="0.55000000000000004">
       <c r="A22" s="10" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="C22" s="7" t="s">
         <v>6</v>
       </c>
       <c r="D22" s="8" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="G22" s="3" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
     </row>
     <row r="23" spans="1:7" ht="17.149999999999999" x14ac:dyDescent="0.55000000000000004">
       <c r="A23" s="10" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="C23" s="7" t="s">
         <v>13</v>
       </c>
       <c r="D23" s="8" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="G23" s="3" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
     </row>
     <row r="24" spans="1:7" ht="17.149999999999999" x14ac:dyDescent="0.55000000000000004">
       <c r="A24" s="10" t="s">
+        <v>330</v>
+      </c>
+      <c r="B24" s="6" t="s">
         <v>331</v>
-      </c>
-      <c r="B24" s="6" t="s">
-        <v>332</v>
       </c>
       <c r="C24" s="7" t="s">
         <v>42</v>
       </c>
       <c r="D24" s="8" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="F24" s="6">
         <v>2</v>
@@ -2122,30 +2125,30 @@
     </row>
     <row r="25" spans="1:7" ht="17.149999999999999" x14ac:dyDescent="0.55000000000000004">
       <c r="A25" s="10" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="C25" s="7" t="s">
         <v>80</v>
       </c>
       <c r="D25" s="8" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="G25" s="3" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
     </row>
     <row r="26" spans="1:7" ht="17.149999999999999" x14ac:dyDescent="0.55000000000000004">
       <c r="A26" s="10" t="s">
+        <v>213</v>
+      </c>
+      <c r="B26" s="6" t="s">
         <v>214</v>
-      </c>
-      <c r="B26" s="6" t="s">
-        <v>215</v>
       </c>
       <c r="C26" s="7" t="s">
         <v>80</v>
       </c>
       <c r="D26" s="8" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
     </row>
     <row r="27" spans="1:7" ht="17.149999999999999" x14ac:dyDescent="0.55000000000000004">
@@ -2159,7 +2162,7 @@
         <v>13</v>
       </c>
       <c r="D27" s="8" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="E27" s="9" t="s">
         <v>97</v>
@@ -2168,40 +2171,40 @@
         <v>2</v>
       </c>
       <c r="G27" s="3" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
     </row>
     <row r="28" spans="1:7" ht="17.149999999999999" x14ac:dyDescent="0.55000000000000004">
       <c r="A28" s="10" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="B28" s="6" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="C28" s="7" t="s">
         <v>6</v>
       </c>
       <c r="D28" s="8" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
     </row>
     <row r="29" spans="1:7" ht="17.149999999999999" x14ac:dyDescent="0.55000000000000004">
       <c r="A29" s="10" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="B29" s="6" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="C29" s="7" t="s">
         <v>13</v>
       </c>
       <c r="D29" s="8" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
     </row>
     <row r="30" spans="1:7" ht="17.149999999999999" x14ac:dyDescent="0.55000000000000004">
       <c r="A30" s="10" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="B30" s="6" t="s">
         <v>59</v>
@@ -2210,7 +2213,7 @@
         <v>13</v>
       </c>
       <c r="D30" s="8" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="E30" s="9" t="s">
         <v>103</v>
@@ -2252,44 +2255,44 @@
     </row>
     <row r="33" spans="1:7" ht="17.149999999999999" x14ac:dyDescent="0.55000000000000004">
       <c r="A33" s="10" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="C33" s="7" t="s">
         <v>6</v>
       </c>
       <c r="D33" s="8" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="G33" s="3" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
     </row>
     <row r="34" spans="1:7" ht="17.149999999999999" x14ac:dyDescent="0.55000000000000004">
       <c r="A34" s="10" t="s">
+        <v>290</v>
+      </c>
+      <c r="B34" s="6" t="s">
         <v>291</v>
-      </c>
-      <c r="B34" s="6" t="s">
-        <v>292</v>
       </c>
       <c r="C34" s="7" t="s">
         <v>6</v>
       </c>
       <c r="D34" s="8" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
     </row>
     <row r="35" spans="1:7" ht="17.149999999999999" x14ac:dyDescent="0.55000000000000004">
       <c r="A35" s="10" t="s">
+        <v>246</v>
+      </c>
+      <c r="B35" s="6" t="s">
         <v>247</v>
-      </c>
-      <c r="B35" s="6" t="s">
-        <v>248</v>
       </c>
       <c r="C35" s="7" t="s">
         <v>80</v>
       </c>
       <c r="D35" s="8" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="E35" s="9" t="s">
         <v>22</v>
@@ -2297,65 +2300,65 @@
     </row>
     <row r="36" spans="1:7" ht="17.149999999999999" x14ac:dyDescent="0.55000000000000004">
       <c r="A36" s="4" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="C36" s="7" t="s">
         <v>28</v>
       </c>
       <c r="D36" s="8" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
     </row>
     <row r="37" spans="1:7" ht="17.149999999999999" x14ac:dyDescent="0.55000000000000004">
       <c r="A37" s="10" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="C37" s="7" t="s">
         <v>13</v>
       </c>
       <c r="D37" s="8" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
     </row>
     <row r="38" spans="1:7" ht="17.149999999999999" x14ac:dyDescent="0.55000000000000004">
       <c r="A38" s="10" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="B38" s="6" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="C38" s="7" t="s">
         <v>13</v>
       </c>
       <c r="D38" s="8" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
     </row>
     <row r="39" spans="1:7" ht="17.149999999999999" x14ac:dyDescent="0.55000000000000004">
       <c r="A39" s="10" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="C39" s="7" t="s">
         <v>42</v>
       </c>
       <c r="D39" s="8" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
     </row>
     <row r="40" spans="1:7" ht="17.149999999999999" x14ac:dyDescent="0.55000000000000004">
       <c r="A40" s="10" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="C40" s="7" t="s">
         <v>6</v>
       </c>
       <c r="D40" s="8" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
     </row>
     <row r="41" spans="1:7" ht="17.149999999999999" x14ac:dyDescent="0.55000000000000004">
       <c r="A41" s="10" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="B41" s="6" t="s">
         <v>59</v>
@@ -2364,57 +2367,57 @@
         <v>80</v>
       </c>
       <c r="D41" s="8" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
     </row>
     <row r="42" spans="1:7" ht="17.149999999999999" x14ac:dyDescent="0.55000000000000004">
       <c r="A42" s="10" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="C42" s="7" t="s">
         <v>13</v>
       </c>
       <c r="D42" s="8" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="G42" s="3" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
     </row>
     <row r="43" spans="1:7" ht="17.149999999999999" x14ac:dyDescent="0.55000000000000004">
       <c r="A43" s="10" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="C43" s="7" t="s">
         <v>42</v>
       </c>
       <c r="D43" s="8" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="G43" s="3" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
     </row>
     <row r="44" spans="1:7" ht="17.149999999999999" x14ac:dyDescent="0.55000000000000004">
       <c r="A44" s="10" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="C44" s="7" t="s">
         <v>13</v>
       </c>
       <c r="D44" s="8" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
     </row>
     <row r="45" spans="1:7" ht="17.149999999999999" x14ac:dyDescent="0.55000000000000004">
       <c r="A45" s="10" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="C45" s="7" t="s">
         <v>13</v>
       </c>
       <c r="D45" s="8" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
     </row>
     <row r="46" spans="1:7" ht="17.149999999999999" x14ac:dyDescent="0.55000000000000004">
@@ -2439,44 +2442,44 @@
     </row>
     <row r="47" spans="1:7" ht="17.149999999999999" x14ac:dyDescent="0.55000000000000004">
       <c r="A47" s="11" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="C47" s="7" t="s">
         <v>6</v>
       </c>
       <c r="D47" s="8" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
     </row>
     <row r="48" spans="1:7" ht="17.149999999999999" x14ac:dyDescent="0.55000000000000004">
       <c r="A48" s="10" t="s">
+        <v>276</v>
+      </c>
+      <c r="B48" s="6" t="s">
         <v>277</v>
-      </c>
-      <c r="B48" s="6" t="s">
-        <v>278</v>
       </c>
       <c r="C48" s="7" t="s">
         <v>13</v>
       </c>
       <c r="D48" s="8" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
     </row>
     <row r="49" spans="1:7" ht="17.149999999999999" x14ac:dyDescent="0.55000000000000004">
       <c r="A49" s="10" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="B49" s="6" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="C49" s="7" t="s">
         <v>28</v>
       </c>
       <c r="D49" s="8" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="E49" s="9" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
     </row>
     <row r="50" spans="1:7" ht="17.149999999999999" x14ac:dyDescent="0.55000000000000004">
@@ -2501,114 +2504,114 @@
     </row>
     <row r="51" spans="1:7" ht="17.149999999999999" x14ac:dyDescent="0.55000000000000004">
       <c r="A51" s="10" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="B51" s="6" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="C51" s="7" t="s">
         <v>13</v>
       </c>
       <c r="D51" s="8" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
     </row>
     <row r="52" spans="1:7" ht="17.149999999999999" x14ac:dyDescent="0.55000000000000004">
       <c r="A52" s="10" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="C52" s="7" t="s">
         <v>13</v>
       </c>
       <c r="D52" s="8" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
     </row>
     <row r="53" spans="1:7" ht="17.149999999999999" x14ac:dyDescent="0.55000000000000004">
       <c r="A53" s="10" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="B53" s="6" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="C53" s="7" t="s">
         <v>13</v>
       </c>
       <c r="D53" s="8" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
     </row>
     <row r="54" spans="1:7" ht="17.149999999999999" x14ac:dyDescent="0.55000000000000004">
       <c r="A54" s="10" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="C54" s="7" t="s">
         <v>13</v>
       </c>
       <c r="D54" s="8" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
     </row>
     <row r="55" spans="1:7" ht="17.149999999999999" x14ac:dyDescent="0.55000000000000004">
       <c r="A55" s="10" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="C55" s="7" t="s">
         <v>13</v>
       </c>
       <c r="D55" s="8" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="G55" s="3" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
     </row>
     <row r="56" spans="1:7" ht="17.149999999999999" x14ac:dyDescent="0.55000000000000004">
       <c r="A56" s="10" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="C56" s="7" t="s">
         <v>42</v>
       </c>
       <c r="D56" s="8" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="E56" s="9" t="s">
         <v>93</v>
       </c>
       <c r="G56" s="3" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
     </row>
     <row r="57" spans="1:7" ht="17.149999999999999" x14ac:dyDescent="0.55000000000000004">
       <c r="A57" s="10" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="B57" s="6" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="C57" s="7" t="s">
         <v>6</v>
       </c>
       <c r="D57" s="8" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
     </row>
     <row r="58" spans="1:7" ht="17.149999999999999" x14ac:dyDescent="0.55000000000000004">
       <c r="A58" s="10" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="B58" s="6" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="C58" s="7" t="s">
         <v>95</v>
       </c>
       <c r="D58" s="8" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="E58" s="9" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="F58" s="6">
         <v>2</v>
@@ -2636,22 +2639,22 @@
     </row>
     <row r="60" spans="1:7" ht="17.149999999999999" x14ac:dyDescent="0.55000000000000004">
       <c r="A60" s="10" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="B60" s="6" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="C60" s="7" t="s">
         <v>6</v>
       </c>
       <c r="D60" s="8" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="E60" s="9" t="s">
         <v>93</v>
       </c>
       <c r="G60" s="3" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
     </row>
     <row r="61" spans="1:7" ht="17.149999999999999" x14ac:dyDescent="0.55000000000000004">
@@ -2676,16 +2679,16 @@
     </row>
     <row r="62" spans="1:7" ht="17.149999999999999" x14ac:dyDescent="0.55000000000000004">
       <c r="A62" s="10" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="B62" s="6" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="C62" s="7" t="s">
         <v>95</v>
       </c>
       <c r="D62" s="8" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="F62" s="6">
         <v>2</v>
@@ -2730,13 +2733,13 @@
     </row>
     <row r="65" spans="1:7" ht="17.149999999999999" x14ac:dyDescent="0.55000000000000004">
       <c r="A65" s="10" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
       <c r="C65" s="7" t="s">
         <v>42</v>
       </c>
       <c r="D65" s="8" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
     </row>
     <row r="66" spans="1:7" ht="17.149999999999999" x14ac:dyDescent="0.55000000000000004">
@@ -2758,50 +2761,50 @@
     </row>
     <row r="67" spans="1:7" ht="17.149999999999999" x14ac:dyDescent="0.55000000000000004">
       <c r="A67" s="10" t="s">
+        <v>115</v>
+      </c>
+      <c r="B67" s="6" t="s">
         <v>116</v>
-      </c>
-      <c r="B67" s="6" t="s">
-        <v>117</v>
       </c>
       <c r="C67" s="7" t="s">
         <v>6</v>
       </c>
       <c r="D67" s="8" t="s">
+        <v>113</v>
+      </c>
+      <c r="E67" s="9" t="s">
         <v>114</v>
-      </c>
-      <c r="E67" s="9" t="s">
-        <v>115</v>
       </c>
     </row>
     <row r="68" spans="1:7" ht="17.149999999999999" x14ac:dyDescent="0.55000000000000004">
       <c r="A68" s="10" t="s">
+        <v>125</v>
+      </c>
+      <c r="B68" s="6" t="s">
         <v>126</v>
-      </c>
-      <c r="B68" s="6" t="s">
-        <v>127</v>
       </c>
       <c r="C68" s="7" t="s">
         <v>28</v>
       </c>
       <c r="D68" s="8" t="s">
+        <v>127</v>
+      </c>
+      <c r="E68" s="9" t="s">
         <v>128</v>
-      </c>
-      <c r="E68" s="9" t="s">
-        <v>129</v>
       </c>
     </row>
     <row r="69" spans="1:7" ht="17.149999999999999" x14ac:dyDescent="0.55000000000000004">
       <c r="A69" s="10" t="s">
+        <v>154</v>
+      </c>
+      <c r="B69" s="6" t="s">
         <v>155</v>
-      </c>
-      <c r="B69" s="6" t="s">
-        <v>156</v>
       </c>
       <c r="C69" s="7" t="s">
         <v>6</v>
       </c>
       <c r="D69" s="8" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="E69" s="9" t="s">
         <v>47</v>
@@ -2809,42 +2812,42 @@
     </row>
     <row r="70" spans="1:7" ht="17.149999999999999" x14ac:dyDescent="0.55000000000000004">
       <c r="A70" s="10" t="s">
+        <v>143</v>
+      </c>
+      <c r="B70" s="6" t="s">
         <v>144</v>
-      </c>
-      <c r="B70" s="6" t="s">
-        <v>145</v>
       </c>
       <c r="C70" s="7" t="s">
         <v>6</v>
       </c>
       <c r="D70" s="8" t="s">
+        <v>145</v>
+      </c>
+      <c r="E70" s="9" t="s">
+        <v>147</v>
+      </c>
+      <c r="G70" s="3" t="s">
         <v>146</v>
-      </c>
-      <c r="E70" s="9" t="s">
-        <v>148</v>
-      </c>
-      <c r="G70" s="3" t="s">
-        <v>147</v>
       </c>
     </row>
     <row r="71" spans="1:7" ht="17.149999999999999" x14ac:dyDescent="0.55000000000000004">
       <c r="A71" s="10" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="B71" s="6" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="C71" s="7" t="s">
         <v>80</v>
       </c>
       <c r="D71" s="8" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="E71" s="12" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="G71" s="3" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
     </row>
     <row r="72" spans="1:7" ht="17.149999999999999" x14ac:dyDescent="0.55000000000000004">
@@ -2869,44 +2872,44 @@
     </row>
     <row r="73" spans="1:7" ht="17.149999999999999" x14ac:dyDescent="0.55000000000000004">
       <c r="A73" s="10" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="C73" s="7" t="s">
         <v>28</v>
       </c>
       <c r="D73" s="8" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
     </row>
     <row r="74" spans="1:7" ht="17.149999999999999" x14ac:dyDescent="0.55000000000000004">
       <c r="A74" s="10" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="B74" s="6" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="C74" s="7" t="s">
         <v>28</v>
       </c>
       <c r="D74" s="8" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="E74" s="9" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
     </row>
     <row r="75" spans="1:7" ht="17.149999999999999" x14ac:dyDescent="0.55000000000000004">
       <c r="A75" s="10" t="s">
+        <v>335</v>
+      </c>
+      <c r="B75" s="6" t="s">
         <v>336</v>
-      </c>
-      <c r="B75" s="6" t="s">
-        <v>337</v>
       </c>
       <c r="C75" s="7" t="s">
         <v>80</v>
       </c>
       <c r="D75" s="8" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="E75" s="9" t="s">
         <v>87</v>
@@ -2917,95 +2920,95 @@
     </row>
     <row r="76" spans="1:7" ht="17.149999999999999" x14ac:dyDescent="0.55000000000000004">
       <c r="A76" s="10" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="C76" s="7" t="s">
         <v>28</v>
       </c>
       <c r="D76" s="8" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
     </row>
     <row r="77" spans="1:7" ht="17.149999999999999" x14ac:dyDescent="0.55000000000000004">
       <c r="A77" s="10" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="B77" s="6" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="C77" s="7" t="s">
         <v>28</v>
       </c>
       <c r="D77" s="8" t="s">
+        <v>165</v>
+      </c>
+      <c r="G77" s="3" t="s">
         <v>166</v>
-      </c>
-      <c r="G77" s="3" t="s">
-        <v>167</v>
       </c>
     </row>
     <row r="78" spans="1:7" ht="17.149999999999999" x14ac:dyDescent="0.55000000000000004">
       <c r="A78" s="10" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="C78" s="7" t="s">
         <v>28</v>
       </c>
       <c r="D78" s="8" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
     </row>
     <row r="79" spans="1:7" ht="17.149999999999999" x14ac:dyDescent="0.55000000000000004">
       <c r="A79" s="10" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="B79" s="6" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="C79" s="7" t="s">
         <v>13</v>
       </c>
       <c r="D79" s="8" t="s">
+        <v>159</v>
+      </c>
+      <c r="E79" s="9" t="s">
         <v>160</v>
-      </c>
-      <c r="E79" s="9" t="s">
-        <v>161</v>
       </c>
     </row>
     <row r="80" spans="1:7" ht="17.149999999999999" x14ac:dyDescent="0.55000000000000004">
       <c r="A80" s="10" t="s">
+        <v>298</v>
+      </c>
+      <c r="B80" s="6" t="s">
         <v>299</v>
-      </c>
-      <c r="B80" s="6" t="s">
-        <v>300</v>
       </c>
       <c r="C80" s="7" t="s">
         <v>13</v>
       </c>
       <c r="D80" s="8" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="E80" s="9" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
     </row>
     <row r="81" spans="1:7" ht="17.149999999999999" x14ac:dyDescent="0.55000000000000004">
       <c r="A81" s="10" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="B81" s="6" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="C81" s="7" t="s">
         <v>80</v>
       </c>
       <c r="D81" s="8" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="E81" s="9" t="s">
         <v>8</v>
       </c>
       <c r="G81" s="3" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
     </row>
     <row r="82" spans="1:7" ht="17.149999999999999" x14ac:dyDescent="0.55000000000000004">
@@ -3019,7 +3022,7 @@
         <v>13</v>
       </c>
       <c r="D82" s="8" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
       <c r="E82" s="9" t="s">
         <v>109</v>
@@ -3028,114 +3031,114 @@
         <v>2</v>
       </c>
       <c r="G82" s="3" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
     </row>
     <row r="83" spans="1:7" ht="17.149999999999999" x14ac:dyDescent="0.55000000000000004">
       <c r="A83" s="10" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="B83" s="6" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="C83" s="7" t="s">
         <v>80</v>
       </c>
       <c r="D83" s="8" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="G83" s="3" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
     </row>
     <row r="84" spans="1:7" ht="17.149999999999999" x14ac:dyDescent="0.55000000000000004">
       <c r="A84" s="10" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="B84" s="6" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="C84" s="7" t="s">
         <v>42</v>
       </c>
       <c r="D84" s="8" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="E84" s="9" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
     </row>
     <row r="85" spans="1:7" ht="17.149999999999999" x14ac:dyDescent="0.55000000000000004">
       <c r="A85" s="10" t="s">
+        <v>327</v>
+      </c>
+      <c r="B85" s="6" t="s">
         <v>328</v>
-      </c>
-      <c r="B85" s="6" t="s">
-        <v>329</v>
       </c>
       <c r="C85" s="7" t="s">
         <v>28</v>
       </c>
       <c r="D85" s="8" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
     </row>
     <row r="86" spans="1:7" ht="17.149999999999999" x14ac:dyDescent="0.55000000000000004">
       <c r="A86" s="10" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="B86" s="6" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="C86" s="7" t="s">
         <v>13</v>
       </c>
       <c r="D86" s="8" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
     </row>
     <row r="87" spans="1:7" ht="17.149999999999999" x14ac:dyDescent="0.55000000000000004">
       <c r="A87" s="10" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="B87" s="6" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="C87" s="7" t="s">
         <v>13</v>
       </c>
       <c r="D87" s="8" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
     </row>
     <row r="88" spans="1:7" ht="17.149999999999999" x14ac:dyDescent="0.55000000000000004">
       <c r="A88" s="10" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="B88" s="6" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="C88" s="7" t="s">
         <v>80</v>
       </c>
       <c r="D88" s="8" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="E88" s="12" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
     </row>
     <row r="89" spans="1:7" ht="17.149999999999999" x14ac:dyDescent="0.55000000000000004">
       <c r="A89" s="10" t="s">
+        <v>255</v>
+      </c>
+      <c r="B89" s="6" t="s">
         <v>256</v>
-      </c>
-      <c r="B89" s="6" t="s">
-        <v>257</v>
       </c>
       <c r="C89" s="7" t="s">
         <v>80</v>
       </c>
       <c r="D89" s="8" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="E89" s="9" t="s">
         <v>22</v>
@@ -3143,44 +3146,44 @@
     </row>
     <row r="90" spans="1:7" ht="17.149999999999999" x14ac:dyDescent="0.55000000000000004">
       <c r="A90" s="10" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="B90" s="6" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="C90" s="7" t="s">
         <v>13</v>
       </c>
       <c r="D90" s="8" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
     </row>
     <row r="91" spans="1:7" ht="17.149999999999999" x14ac:dyDescent="0.55000000000000004">
       <c r="A91" s="10" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="B91" s="6" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="C91" s="7" t="s">
         <v>42</v>
       </c>
       <c r="D91" s="8" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
     </row>
     <row r="92" spans="1:7" ht="17.149999999999999" x14ac:dyDescent="0.55000000000000004">
       <c r="A92" s="10" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="B92" s="6" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="C92" s="7" t="s">
         <v>42</v>
       </c>
       <c r="D92" s="8" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
     </row>
     <row r="93" spans="1:7" ht="17.149999999999999" x14ac:dyDescent="0.55000000000000004">
@@ -3205,30 +3208,30 @@
     </row>
     <row r="94" spans="1:7" ht="17.149999999999999" x14ac:dyDescent="0.55000000000000004">
       <c r="A94" s="10" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="B94" s="6" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="C94" s="7" t="s">
         <v>80</v>
       </c>
       <c r="D94" s="8" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
     </row>
     <row r="95" spans="1:7" ht="17.149999999999999" x14ac:dyDescent="0.55000000000000004">
       <c r="A95" s="10" t="s">
+        <v>268</v>
+      </c>
+      <c r="B95" s="6" t="s">
         <v>269</v>
-      </c>
-      <c r="B95" s="6" t="s">
-        <v>270</v>
       </c>
       <c r="C95" s="7" t="s">
         <v>80</v>
       </c>
       <c r="D95" s="8" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="E95" s="9" t="s">
         <v>93</v>
@@ -3236,41 +3239,41 @@
     </row>
     <row r="96" spans="1:7" ht="17.149999999999999" x14ac:dyDescent="0.55000000000000004">
       <c r="A96" s="10" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="B96" s="6" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="C96" s="7" t="s">
         <v>80</v>
       </c>
       <c r="D96" s="8" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="E96" s="9" t="s">
         <v>98</v>
       </c>
       <c r="G96" s="3" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
     </row>
     <row r="97" spans="1:7" ht="17.149999999999999" x14ac:dyDescent="0.55000000000000004">
       <c r="A97" s="10" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="C97" s="7" t="s">
         <v>6</v>
       </c>
       <c r="D97" s="8" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="G97" s="3" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
     </row>
     <row r="98" spans="1:7" ht="17.149999999999999" x14ac:dyDescent="0.55000000000000004">
       <c r="A98" s="10" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="B98" s="6" t="s">
         <v>12</v>
@@ -3279,10 +3282,10 @@
         <v>80</v>
       </c>
       <c r="D98" s="8" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
       <c r="E98" s="9" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="F98" s="6">
         <v>3</v>
@@ -3302,7 +3305,7 @@
         <v>80</v>
       </c>
       <c r="D99" s="8" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
       <c r="E99" s="9" t="s">
         <v>98</v>
@@ -3316,18 +3319,18 @@
     </row>
     <row r="100" spans="1:7" ht="17.149999999999999" x14ac:dyDescent="0.55000000000000004">
       <c r="A100" s="10" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="C100" s="7" t="s">
         <v>42</v>
       </c>
       <c r="D100" s="8" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
     </row>
     <row r="101" spans="1:7" ht="17.149999999999999" x14ac:dyDescent="0.55000000000000004">
       <c r="A101" s="10" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="B101" s="6" t="s">
         <v>107</v>
@@ -3336,16 +3339,16 @@
         <v>95</v>
       </c>
       <c r="D101" s="8" t="s">
-        <v>157</v>
+        <v>345</v>
       </c>
       <c r="E101" s="9" t="s">
         <v>110</v>
       </c>
       <c r="F101" s="6">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="G101" s="3" t="s">
-        <v>111</v>
+        <v>346</v>
       </c>
     </row>
     <row r="102" spans="1:7" ht="17.149999999999999" x14ac:dyDescent="0.55000000000000004">
@@ -3370,36 +3373,36 @@
     </row>
     <row r="103" spans="1:7" ht="17.149999999999999" x14ac:dyDescent="0.55000000000000004">
       <c r="A103" s="10" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="B103" s="6" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="C103" s="7" t="s">
         <v>13</v>
       </c>
       <c r="D103" s="8" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
     </row>
     <row r="104" spans="1:7" ht="17.149999999999999" x14ac:dyDescent="0.55000000000000004">
       <c r="A104" s="10" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="B104" s="6" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="C104" s="7" t="s">
         <v>13</v>
       </c>
       <c r="D104" s="8" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="E104" s="9" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="G104" s="3" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
     </row>
     <row r="105" spans="1:7" ht="17.149999999999999" x14ac:dyDescent="0.55000000000000004">
@@ -3424,16 +3427,16 @@
     </row>
     <row r="106" spans="1:7" ht="17.149999999999999" x14ac:dyDescent="0.55000000000000004">
       <c r="A106" s="10" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="B106" s="6" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="C106" s="7" t="s">
         <v>6</v>
       </c>
       <c r="D106" s="8" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="E106" s="9" t="s">
         <v>93</v>
@@ -3450,27 +3453,27 @@
         <v>80</v>
       </c>
       <c r="D107" s="8" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="F107" s="6">
         <v>3</v>
       </c>
       <c r="G107" s="3" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
     </row>
     <row r="108" spans="1:7" ht="17.149999999999999" x14ac:dyDescent="0.55000000000000004">
       <c r="A108" s="10" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="B108" s="6" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="C108" s="7" t="s">
         <v>80</v>
       </c>
       <c r="D108" s="8" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="E108" s="9" t="s">
         <v>22</v>
@@ -3478,16 +3481,16 @@
     </row>
     <row r="109" spans="1:7" ht="17.149999999999999" x14ac:dyDescent="0.55000000000000004">
       <c r="A109" s="10" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="B109" s="6" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="C109" s="7" t="s">
         <v>80</v>
       </c>
       <c r="D109" s="8" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="E109" s="9" t="s">
         <v>14</v>
@@ -3495,121 +3498,121 @@
     </row>
     <row r="110" spans="1:7" ht="17.149999999999999" x14ac:dyDescent="0.55000000000000004">
       <c r="A110" s="10" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="B110" s="6" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="C110" s="7" t="s">
         <v>6</v>
       </c>
       <c r="D110" s="8" t="s">
+        <v>176</v>
+      </c>
+      <c r="E110" s="9" t="s">
         <v>177</v>
-      </c>
-      <c r="E110" s="9" t="s">
-        <v>178</v>
       </c>
     </row>
     <row r="111" spans="1:7" ht="17.149999999999999" x14ac:dyDescent="0.55000000000000004">
       <c r="A111" s="10" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="B111" s="6" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="C111" s="7" t="s">
         <v>80</v>
       </c>
       <c r="D111" s="8" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="E111" s="9" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="F111" s="6">
         <v>2</v>
       </c>
       <c r="G111" s="3" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
     </row>
     <row r="112" spans="1:7" ht="17.149999999999999" x14ac:dyDescent="0.55000000000000004">
       <c r="A112" s="10" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="C112" s="7" t="s">
         <v>6</v>
       </c>
       <c r="D112" s="8" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="E112" s="10" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
     </row>
     <row r="113" spans="1:7" ht="17.149999999999999" x14ac:dyDescent="0.55000000000000004">
       <c r="A113" s="10" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="C113" s="7" t="s">
         <v>13</v>
       </c>
       <c r="D113" s="8" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
     </row>
     <row r="114" spans="1:7" ht="17.149999999999999" x14ac:dyDescent="0.55000000000000004">
       <c r="A114" s="10" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="B114" s="6" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="C114" s="7" t="s">
         <v>42</v>
       </c>
       <c r="D114" s="8" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
     </row>
     <row r="115" spans="1:7" ht="17.149999999999999" x14ac:dyDescent="0.55000000000000004">
       <c r="A115" s="10" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="B115" s="6" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="C115" s="7" t="s">
         <v>80</v>
       </c>
       <c r="D115" s="8" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="E115" s="9" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="F115" s="6">
         <v>2</v>
       </c>
       <c r="G115" s="3" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
     </row>
     <row r="116" spans="1:7" ht="17.149999999999999" x14ac:dyDescent="0.55000000000000004">
       <c r="A116" s="10" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="B116" s="6" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="C116" s="7" t="s">
         <v>95</v>
       </c>
       <c r="D116" s="8" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="E116" s="9" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="F116" s="6">
         <v>3</v>
@@ -3617,16 +3620,16 @@
     </row>
     <row r="117" spans="1:7" ht="17.149999999999999" x14ac:dyDescent="0.55000000000000004">
       <c r="A117" s="10" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="B117" s="6" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="C117" s="7" t="s">
         <v>13</v>
       </c>
       <c r="D117" s="8" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="E117" s="9" t="s">
         <v>14</v>
@@ -3634,61 +3637,61 @@
     </row>
     <row r="118" spans="1:7" ht="17.149999999999999" x14ac:dyDescent="0.55000000000000004">
       <c r="A118" s="10" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="B118" s="6" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="C118" s="7" t="s">
         <v>13</v>
       </c>
       <c r="D118" s="8" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
     </row>
     <row r="119" spans="1:7" ht="17.149999999999999" x14ac:dyDescent="0.55000000000000004">
       <c r="A119" s="10" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="B119" s="6" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="C119" s="7" t="s">
         <v>6</v>
       </c>
       <c r="D119" s="8" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="E119" s="9" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="G119" s="3" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
     </row>
     <row r="120" spans="1:7" ht="17.149999999999999" x14ac:dyDescent="0.55000000000000004">
       <c r="A120" s="10" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="B120" s="6" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="C120" s="7" t="s">
         <v>42</v>
       </c>
       <c r="D120" s="8" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
     </row>
     <row r="121" spans="1:7" ht="17.149999999999999" x14ac:dyDescent="0.55000000000000004">
       <c r="A121" s="10" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="C121" s="7" t="s">
         <v>13</v>
       </c>
       <c r="D121" s="8" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
     </row>
     <row r="122" spans="1:7" ht="17.149999999999999" x14ac:dyDescent="0.55000000000000004">
@@ -3710,16 +3713,16 @@
     </row>
     <row r="123" spans="1:7" ht="17.149999999999999" x14ac:dyDescent="0.55000000000000004">
       <c r="A123" s="10" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="B123" s="6" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="C123" s="7" t="s">
         <v>80</v>
       </c>
       <c r="D123" s="8" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="E123" s="9" t="s">
         <v>14</v>
@@ -3727,92 +3730,92 @@
     </row>
     <row r="124" spans="1:7" ht="17.149999999999999" x14ac:dyDescent="0.55000000000000004">
       <c r="A124" s="10" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="C124" s="7" t="s">
         <v>42</v>
       </c>
       <c r="D124" s="8" t="s">
+        <v>189</v>
+      </c>
+      <c r="E124" s="9" t="s">
         <v>190</v>
       </c>
-      <c r="E124" s="9" t="s">
-        <v>191</v>
-      </c>
       <c r="G124" s="3" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
     </row>
     <row r="125" spans="1:7" ht="17.149999999999999" x14ac:dyDescent="0.55000000000000004">
       <c r="A125" s="10" t="s">
+        <v>111</v>
+      </c>
+      <c r="B125" s="6" t="s">
         <v>112</v>
-      </c>
-      <c r="B125" s="6" t="s">
-        <v>113</v>
       </c>
       <c r="C125" s="7" t="s">
         <v>6</v>
       </c>
       <c r="D125" s="8" t="s">
+        <v>113</v>
+      </c>
+      <c r="E125" s="9" t="s">
         <v>114</v>
-      </c>
-      <c r="E125" s="9" t="s">
-        <v>115</v>
       </c>
     </row>
     <row r="126" spans="1:7" ht="17.149999999999999" x14ac:dyDescent="0.55000000000000004">
       <c r="A126" s="10" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="B126" s="6" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="C126" s="7" t="s">
         <v>80</v>
       </c>
       <c r="D126" s="8" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="E126" s="9" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="G126" s="3" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
     </row>
     <row r="127" spans="1:7" ht="17.149999999999999" x14ac:dyDescent="0.55000000000000004">
       <c r="A127" s="10" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="B127" s="6" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="C127" s="7" t="s">
         <v>42</v>
       </c>
       <c r="D127" s="8" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
     </row>
     <row r="128" spans="1:7" ht="17.149999999999999" x14ac:dyDescent="0.55000000000000004">
       <c r="A128" s="10" t="s">
+        <v>292</v>
+      </c>
+      <c r="B128" s="6" t="s">
         <v>293</v>
-      </c>
-      <c r="B128" s="6" t="s">
-        <v>294</v>
       </c>
       <c r="C128" s="7" t="s">
         <v>6</v>
       </c>
       <c r="D128" s="8" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="G128" s="3" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
     </row>
     <row r="129" spans="1:7" ht="17.149999999999999" x14ac:dyDescent="0.55000000000000004">
       <c r="A129" s="10" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="B129" s="6" t="s">
         <v>107</v>
@@ -3821,27 +3824,27 @@
         <v>80</v>
       </c>
       <c r="D129" s="8" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="E129" s="9" t="s">
+        <v>123</v>
+      </c>
+      <c r="G129" s="3" t="s">
         <v>124</v>
-      </c>
-      <c r="G129" s="3" t="s">
-        <v>125</v>
       </c>
     </row>
     <row r="130" spans="1:7" ht="17.149999999999999" x14ac:dyDescent="0.55000000000000004">
       <c r="A130" s="10" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="B130" s="6" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="C130" s="7" t="s">
         <v>13</v>
       </c>
       <c r="D130" s="8" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="E130" s="9" t="s">
         <v>22</v>
@@ -3849,16 +3852,16 @@
     </row>
     <row r="131" spans="1:7" ht="17.149999999999999" x14ac:dyDescent="0.55000000000000004">
       <c r="A131" s="10" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="B131" s="6" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="C131" s="7" t="s">
         <v>13</v>
       </c>
       <c r="D131" s="8" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="E131" s="9" t="s">
         <v>47</v>
@@ -3866,16 +3869,16 @@
     </row>
     <row r="132" spans="1:7" ht="17.149999999999999" x14ac:dyDescent="0.55000000000000004">
       <c r="A132" s="10" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="B132" s="6" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="C132" s="7" t="s">
         <v>42</v>
       </c>
       <c r="D132" s="8" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="E132" s="9" t="s">
         <v>93</v>
@@ -3917,7 +3920,7 @@
     </row>
     <row r="135" spans="1:7" ht="17.149999999999999" x14ac:dyDescent="0.55000000000000004">
       <c r="A135" s="10" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="B135" s="6" t="s">
         <v>36</v>
@@ -3926,57 +3929,57 @@
         <v>80</v>
       </c>
       <c r="D135" s="8" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="E135" s="9" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="G135" s="3" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
     </row>
     <row r="136" spans="1:7" ht="17.149999999999999" x14ac:dyDescent="0.55000000000000004">
       <c r="A136" s="10" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="C136" s="7" t="s">
         <v>13</v>
       </c>
       <c r="D136" s="8" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
     </row>
     <row r="137" spans="1:7" ht="17.149999999999999" x14ac:dyDescent="0.55000000000000004">
       <c r="A137" s="10" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="C137" s="7" t="s">
         <v>42</v>
       </c>
       <c r="D137" s="8" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
     </row>
     <row r="138" spans="1:7" ht="17.149999999999999" x14ac:dyDescent="0.55000000000000004">
       <c r="A138" s="10" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="C138" s="7" t="s">
         <v>42</v>
       </c>
       <c r="D138" s="8" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
     </row>
     <row r="139" spans="1:7" ht="17.149999999999999" x14ac:dyDescent="0.55000000000000004">
       <c r="A139" s="10" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="C139" s="7" t="s">
         <v>42</v>
       </c>
       <c r="D139" s="8" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
2024.10.15 LeetCodeHot100 二刷 刷题心得更新
</commit_message>
<xml_diff>
--- a/2024LeetCode刷题记录.xlsx
+++ b/2024LeetCode刷题记录.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\develop\GithubRepo\LeetCode\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{178965B3-FCC8-4E20-9AC8-7FDAA5176C5E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E0521399-097A-4C1B-9524-69B8EC4D7590}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-103" yWindow="-103" windowWidth="22149" windowHeight="11829" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="684" uniqueCount="387">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="684" uniqueCount="389">
   <si>
     <t>题目</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -1424,6 +1424,14 @@
   </si>
   <si>
     <t>2024.10.08</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>2024.10.15</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>2024.10.14</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -1878,8 +1886,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G148"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A112" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="G123" sqref="G123"/>
+    <sheetView tabSelected="1" topLeftCell="A136" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="E147" sqref="E147"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="14.15" x14ac:dyDescent="0.35"/>
@@ -1959,7 +1967,10 @@
         <v>13</v>
       </c>
       <c r="D4" s="8" t="s">
-        <v>212</v>
+        <v>388</v>
+      </c>
+      <c r="F4" s="6">
+        <v>2</v>
       </c>
     </row>
     <row r="5" spans="1:7" ht="17.149999999999999" x14ac:dyDescent="0.55000000000000004">
@@ -2024,7 +2035,10 @@
         <v>42</v>
       </c>
       <c r="D8" s="8" t="s">
-        <v>212</v>
+        <v>387</v>
+      </c>
+      <c r="F8" s="6">
+        <v>2</v>
       </c>
     </row>
     <row r="9" spans="1:7" ht="17.149999999999999" x14ac:dyDescent="0.55000000000000004">
@@ -4375,7 +4389,10 @@
         <v>42</v>
       </c>
       <c r="D147" s="8" t="s">
-        <v>212</v>
+        <v>387</v>
+      </c>
+      <c r="F147" s="6">
+        <v>2</v>
       </c>
     </row>
     <row r="148" spans="1:6" ht="17.149999999999999" x14ac:dyDescent="0.55000000000000004">

</xml_diff>

<commit_message>
2024.11.06 LeetCodeHot100 二刷 Done!
</commit_message>
<xml_diff>
--- a/2024LeetCode刷题记录.xlsx
+++ b/2024LeetCode刷题记录.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\develop\GithubRepo\LeetCode\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{50AC259B-C39B-465C-9614-057052A4AFB7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9EF2DB1D-1F87-4CE2-9BBD-E150D3830F25}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-103" yWindow="-103" windowWidth="22149" windowHeight="11829" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="692" uniqueCount="403">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="694" uniqueCount="405">
   <si>
     <t>题目</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -1051,10 +1051,6 @@
     <t>152. 乘积最大子数组</t>
   </si>
   <si>
-    <t>2024.08.30</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>416. 分割等和子集</t>
   </si>
   <si>
@@ -1073,10 +1069,6 @@
     <t>1143. 最长公共子序列</t>
   </si>
   <si>
-    <t>m+1 n+1问题搞清楚</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>72. 编辑距离</t>
   </si>
   <si>
@@ -1488,6 +1480,22 @@
   </si>
   <si>
     <t>2024.11.05</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>2024.11.06</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Hard</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>m+1 n+1问题搞清楚；举例推导，看图理解；</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>相比1143.多一步初始化</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -1661,7 +1669,7 @@
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{E5AA65A4-B8FD-4A83-87AF-D7798D621280}" name="表1" displayName="表1" ref="A1:G1048574" totalsRowShown="0" headerRowDxfId="8" dataDxfId="7">
   <autoFilter ref="A1:G1048574" xr:uid="{E5AA65A4-B8FD-4A83-87AF-D7798D621280}"/>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:G149">
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:G150">
     <sortCondition ref="A1:A1048574"/>
   </sortState>
   <tableColumns count="7">
@@ -1942,8 +1950,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G148"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A85" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="F90" sqref="F90"/>
+    <sheetView tabSelected="1" topLeftCell="A124" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="G132" sqref="G132"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="14.15" x14ac:dyDescent="0.35"/>
@@ -1992,7 +2000,7 @@
         <v>80</v>
       </c>
       <c r="D2" s="8" t="s">
-        <v>305</v>
+        <v>303</v>
       </c>
       <c r="F2" s="6">
         <v>2</v>
@@ -2009,7 +2017,7 @@
         <v>13</v>
       </c>
       <c r="D3" s="8" t="s">
-        <v>371</v>
+        <v>369</v>
       </c>
       <c r="F3" s="6">
         <v>2</v>
@@ -2023,7 +2031,7 @@
         <v>13</v>
       </c>
       <c r="D4" s="8" t="s">
-        <v>373</v>
+        <v>371</v>
       </c>
       <c r="F4" s="6">
         <v>2</v>
@@ -2034,13 +2042,13 @@
         <v>208</v>
       </c>
       <c r="B5" s="6" t="s">
-        <v>370</v>
+        <v>368</v>
       </c>
       <c r="C5" s="7" t="s">
         <v>13</v>
       </c>
       <c r="D5" s="8" t="s">
-        <v>369</v>
+        <v>367</v>
       </c>
       <c r="F5" s="6">
         <v>2</v>
@@ -2057,7 +2065,7 @@
         <v>13</v>
       </c>
       <c r="D6" s="8" t="s">
-        <v>319</v>
+        <v>317</v>
       </c>
       <c r="E6" s="9" t="s">
         <v>14</v>
@@ -2077,7 +2085,7 @@
         <v>80</v>
       </c>
       <c r="D7" s="8" t="s">
-        <v>328</v>
+        <v>326</v>
       </c>
       <c r="F7" s="6">
         <v>2</v>
@@ -2091,7 +2099,7 @@
         <v>42</v>
       </c>
       <c r="D8" s="8" t="s">
-        <v>372</v>
+        <v>370</v>
       </c>
       <c r="F8" s="6">
         <v>2</v>
@@ -2108,7 +2116,7 @@
         <v>42</v>
       </c>
       <c r="D9" s="8" t="s">
-        <v>309</v>
+        <v>307</v>
       </c>
       <c r="E9" s="9" t="s">
         <v>93</v>
@@ -2117,7 +2125,7 @@
         <v>3</v>
       </c>
       <c r="G9" s="3" t="s">
-        <v>310</v>
+        <v>308</v>
       </c>
     </row>
     <row r="10" spans="1:7" ht="17.149999999999999" x14ac:dyDescent="0.55000000000000004">
@@ -2128,33 +2136,36 @@
         <v>42</v>
       </c>
       <c r="D10" s="8" t="s">
+        <v>373</v>
+      </c>
+      <c r="F10" s="6">
+        <v>2</v>
+      </c>
+      <c r="G10" s="3" t="s">
         <v>375</v>
-      </c>
-      <c r="F10" s="6">
-        <v>2</v>
-      </c>
-      <c r="G10" s="3" t="s">
-        <v>377</v>
       </c>
     </row>
     <row r="11" spans="1:7" ht="17.149999999999999" x14ac:dyDescent="0.55000000000000004">
       <c r="A11" s="10" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="B11" s="6" t="s">
         <v>130</v>
       </c>
       <c r="C11" s="7" t="s">
-        <v>80</v>
+        <v>95</v>
       </c>
       <c r="D11" s="8" t="s">
-        <v>286</v>
+        <v>401</v>
       </c>
       <c r="E11" s="9" t="s">
         <v>14</v>
       </c>
+      <c r="F11" s="6">
+        <v>2</v>
+      </c>
       <c r="G11" s="3" t="s">
-        <v>293</v>
+        <v>403</v>
       </c>
     </row>
     <row r="12" spans="1:7" ht="17.149999999999999" x14ac:dyDescent="0.55000000000000004">
@@ -2188,7 +2199,7 @@
         <v>6</v>
       </c>
       <c r="D13" s="8" t="s">
-        <v>402</v>
+        <v>400</v>
       </c>
       <c r="F13" s="6">
         <v>2</v>
@@ -2219,13 +2230,13 @@
         <v>260</v>
       </c>
       <c r="B15" s="6" t="s">
-        <v>334</v>
+        <v>332</v>
       </c>
       <c r="C15" s="7" t="s">
         <v>42</v>
       </c>
       <c r="D15" s="8" t="s">
-        <v>358</v>
+        <v>356</v>
       </c>
       <c r="E15" s="9" t="s">
         <v>14</v>
@@ -2236,16 +2247,16 @@
     </row>
     <row r="16" spans="1:7" ht="17.149999999999999" x14ac:dyDescent="0.55000000000000004">
       <c r="A16" s="10" t="s">
+        <v>361</v>
+      </c>
+      <c r="B16" s="6" t="s">
         <v>363</v>
-      </c>
-      <c r="B16" s="6" t="s">
-        <v>365</v>
       </c>
       <c r="C16" s="7" t="s">
         <v>13</v>
       </c>
       <c r="D16" s="8" t="s">
-        <v>364</v>
+        <v>362</v>
       </c>
       <c r="E16" s="9" t="s">
         <v>14</v>
@@ -2253,13 +2264,13 @@
     </row>
     <row r="17" spans="1:7" ht="17.149999999999999" x14ac:dyDescent="0.55000000000000004">
       <c r="A17" s="10" t="s">
-        <v>367</v>
+        <v>365</v>
       </c>
       <c r="C17" s="7" t="s">
         <v>42</v>
       </c>
       <c r="D17" s="8" t="s">
-        <v>368</v>
+        <v>366</v>
       </c>
       <c r="E17" s="9" t="s">
         <v>14</v>
@@ -2270,13 +2281,13 @@
         <v>221</v>
       </c>
       <c r="B18" s="6" t="s">
-        <v>383</v>
+        <v>381</v>
       </c>
       <c r="C18" s="7" t="s">
         <v>13</v>
       </c>
       <c r="D18" s="8" t="s">
-        <v>380</v>
+        <v>378</v>
       </c>
       <c r="F18" s="6">
         <v>2</v>
@@ -2287,7 +2298,7 @@
     </row>
     <row r="19" spans="1:7" ht="17.149999999999999" x14ac:dyDescent="0.55000000000000004">
       <c r="A19" s="10" t="s">
-        <v>306</v>
+        <v>304</v>
       </c>
       <c r="B19" s="6" t="s">
         <v>79</v>
@@ -2296,7 +2307,7 @@
         <v>80</v>
       </c>
       <c r="D19" s="8" t="s">
-        <v>305</v>
+        <v>303</v>
       </c>
       <c r="F19" s="6">
         <v>2</v>
@@ -2313,7 +2324,7 @@
         <v>13</v>
       </c>
       <c r="D20" s="8" t="s">
-        <v>390</v>
+        <v>388</v>
       </c>
       <c r="F20" s="6">
         <v>2</v>
@@ -2330,7 +2341,7 @@
         <v>28</v>
       </c>
       <c r="D21" s="8" t="s">
-        <v>400</v>
+        <v>398</v>
       </c>
       <c r="F21" s="6">
         <v>2</v>
@@ -2347,7 +2358,7 @@
         <v>13</v>
       </c>
       <c r="D22" s="8" t="s">
-        <v>362</v>
+        <v>360</v>
       </c>
       <c r="E22" s="9" t="s">
         <v>87</v>
@@ -2367,7 +2378,7 @@
         <v>13</v>
       </c>
       <c r="D23" s="8" t="s">
-        <v>339</v>
+        <v>337</v>
       </c>
       <c r="E23" s="9" t="s">
         <v>14</v>
@@ -2381,13 +2392,13 @@
         <v>195</v>
       </c>
       <c r="B24" s="6" t="s">
-        <v>354</v>
+        <v>352</v>
       </c>
       <c r="C24" s="7" t="s">
         <v>42</v>
       </c>
       <c r="D24" s="8" t="s">
-        <v>349</v>
+        <v>347</v>
       </c>
       <c r="F24" s="6">
         <v>2</v>
@@ -2401,30 +2412,30 @@
         <v>13</v>
       </c>
       <c r="D25" s="8" t="s">
-        <v>349</v>
+        <v>347</v>
       </c>
       <c r="E25" s="13" t="s">
-        <v>355</v>
+        <v>353</v>
       </c>
       <c r="F25" s="6">
         <v>2</v>
       </c>
       <c r="G25" s="3" t="s">
-        <v>356</v>
+        <v>354</v>
       </c>
     </row>
     <row r="26" spans="1:7" ht="17.149999999999999" x14ac:dyDescent="0.55000000000000004">
       <c r="A26" s="10" t="s">
-        <v>302</v>
+        <v>300</v>
       </c>
       <c r="B26" s="6" t="s">
-        <v>303</v>
+        <v>301</v>
       </c>
       <c r="C26" s="7" t="s">
         <v>42</v>
       </c>
       <c r="D26" s="8" t="s">
-        <v>304</v>
+        <v>302</v>
       </c>
       <c r="F26" s="6">
         <v>2</v>
@@ -2438,7 +2449,7 @@
         <v>80</v>
       </c>
       <c r="D27" s="8" t="s">
-        <v>366</v>
+        <v>364</v>
       </c>
       <c r="F27" s="6">
         <v>2</v>
@@ -2458,7 +2469,7 @@
         <v>80</v>
       </c>
       <c r="D28" s="8" t="s">
-        <v>366</v>
+        <v>364</v>
       </c>
       <c r="F28" s="6">
         <v>2</v>
@@ -2475,7 +2486,7 @@
         <v>13</v>
       </c>
       <c r="D29" s="8" t="s">
-        <v>309</v>
+        <v>307</v>
       </c>
       <c r="E29" s="9" t="s">
         <v>97</v>
@@ -2484,7 +2495,7 @@
         <v>2</v>
       </c>
       <c r="G29" s="3" t="s">
-        <v>311</v>
+        <v>309</v>
       </c>
     </row>
     <row r="30" spans="1:7" ht="17.149999999999999" x14ac:dyDescent="0.55000000000000004">
@@ -2498,7 +2509,7 @@
         <v>6</v>
       </c>
       <c r="D30" s="8" t="s">
-        <v>402</v>
+        <v>400</v>
       </c>
       <c r="F30" s="6">
         <v>2</v>
@@ -2515,13 +2526,13 @@
         <v>13</v>
       </c>
       <c r="D31" s="8" t="s">
+        <v>391</v>
+      </c>
+      <c r="F31" s="6">
+        <v>2</v>
+      </c>
+      <c r="G31" s="3" t="s">
         <v>393</v>
-      </c>
-      <c r="F31" s="6">
-        <v>2</v>
-      </c>
-      <c r="G31" s="3" t="s">
-        <v>395</v>
       </c>
     </row>
     <row r="32" spans="1:7" ht="17.149999999999999" x14ac:dyDescent="0.55000000000000004">
@@ -2535,7 +2546,7 @@
         <v>13</v>
       </c>
       <c r="D32" s="8" t="s">
-        <v>397</v>
+        <v>395</v>
       </c>
       <c r="E32" s="9" t="s">
         <v>103</v>
@@ -2586,16 +2597,16 @@
         <v>6</v>
       </c>
       <c r="D35" s="8" t="s">
+        <v>347</v>
+      </c>
+      <c r="E35" s="13" t="s">
         <v>349</v>
       </c>
-      <c r="E35" s="13" t="s">
-        <v>351</v>
-      </c>
       <c r="F35" s="6">
         <v>2</v>
       </c>
       <c r="G35" s="3" t="s">
-        <v>350</v>
+        <v>348</v>
       </c>
     </row>
     <row r="36" spans="1:7" ht="17.149999999999999" x14ac:dyDescent="0.55000000000000004">
@@ -2609,7 +2620,7 @@
         <v>13</v>
       </c>
       <c r="D36" s="8" t="s">
-        <v>400</v>
+        <v>398</v>
       </c>
       <c r="F36" s="6">
         <v>2</v>
@@ -2626,7 +2637,7 @@
         <v>80</v>
       </c>
       <c r="D37" s="8" t="s">
-        <v>388</v>
+        <v>386</v>
       </c>
       <c r="E37" s="9" t="s">
         <v>22</v>
@@ -2643,7 +2654,7 @@
         <v>28</v>
       </c>
       <c r="D38" s="8" t="s">
-        <v>333</v>
+        <v>331</v>
       </c>
       <c r="F38" s="6">
         <v>2</v>
@@ -2657,13 +2668,13 @@
         <v>13</v>
       </c>
       <c r="D39" s="8" t="s">
-        <v>358</v>
+        <v>356</v>
       </c>
       <c r="F39" s="6">
         <v>2</v>
       </c>
       <c r="G39" s="3" t="s">
-        <v>359</v>
+        <v>357</v>
       </c>
     </row>
     <row r="40" spans="1:7" ht="17.149999999999999" x14ac:dyDescent="0.55000000000000004">
@@ -2677,13 +2688,13 @@
         <v>80</v>
       </c>
       <c r="D40" s="8" t="s">
-        <v>344</v>
+        <v>342</v>
       </c>
       <c r="F40" s="6">
         <v>2</v>
       </c>
       <c r="G40" s="3" t="s">
-        <v>345</v>
+        <v>343</v>
       </c>
     </row>
     <row r="41" spans="1:7" ht="17.149999999999999" x14ac:dyDescent="0.55000000000000004">
@@ -2694,13 +2705,13 @@
         <v>13</v>
       </c>
       <c r="D41" s="8" t="s">
-        <v>375</v>
+        <v>373</v>
       </c>
       <c r="F41" s="6">
         <v>2</v>
       </c>
       <c r="G41" s="3" t="s">
-        <v>376</v>
+        <v>374</v>
       </c>
     </row>
     <row r="42" spans="1:7" ht="17.149999999999999" x14ac:dyDescent="0.55000000000000004">
@@ -2711,7 +2722,7 @@
         <v>6</v>
       </c>
       <c r="D42" s="8" t="s">
-        <v>358</v>
+        <v>356</v>
       </c>
       <c r="F42" s="6">
         <v>2</v>
@@ -2728,7 +2739,7 @@
         <v>80</v>
       </c>
       <c r="D43" s="8" t="s">
-        <v>397</v>
+        <v>395</v>
       </c>
       <c r="F43" s="6">
         <v>2</v>
@@ -2742,7 +2753,7 @@
         <v>13</v>
       </c>
       <c r="D44" s="8" t="s">
-        <v>384</v>
+        <v>382</v>
       </c>
       <c r="F44" s="6">
         <v>2</v>
@@ -2759,7 +2770,7 @@
         <v>80</v>
       </c>
       <c r="D45" s="8" t="s">
-        <v>349</v>
+        <v>347</v>
       </c>
       <c r="F45" s="6">
         <v>2</v>
@@ -2773,7 +2784,7 @@
         <v>80</v>
       </c>
       <c r="D46" s="8" t="s">
-        <v>385</v>
+        <v>383</v>
       </c>
       <c r="F46" s="6">
         <v>2</v>
@@ -2787,7 +2798,7 @@
         <v>13</v>
       </c>
       <c r="D47" s="8" t="s">
-        <v>385</v>
+        <v>383</v>
       </c>
       <c r="F47" s="6">
         <v>2</v>
@@ -2821,27 +2832,27 @@
         <v>42</v>
       </c>
       <c r="D49" s="8" t="s">
-        <v>358</v>
+        <v>356</v>
       </c>
       <c r="F49" s="6">
         <v>2</v>
       </c>
       <c r="G49" s="3" t="s">
-        <v>357</v>
+        <v>355</v>
       </c>
     </row>
     <row r="50" spans="1:7" ht="17.149999999999999" x14ac:dyDescent="0.55000000000000004">
       <c r="A50" s="10" t="s">
+        <v>344</v>
+      </c>
+      <c r="B50" s="6" t="s">
         <v>346</v>
-      </c>
-      <c r="B50" s="6" t="s">
-        <v>348</v>
       </c>
       <c r="C50" s="7" t="s">
         <v>13</v>
       </c>
       <c r="D50" s="8" t="s">
-        <v>347</v>
+        <v>345</v>
       </c>
       <c r="E50" s="9" t="s">
         <v>14</v>
@@ -2858,13 +2869,13 @@
         <v>13</v>
       </c>
       <c r="D51" s="8" t="s">
-        <v>400</v>
+        <v>398</v>
       </c>
       <c r="F51" s="6">
         <v>3</v>
       </c>
       <c r="G51" s="3" t="s">
-        <v>343</v>
+        <v>341</v>
       </c>
     </row>
     <row r="52" spans="1:7" ht="17.149999999999999" x14ac:dyDescent="0.55000000000000004">
@@ -2915,7 +2926,7 @@
         <v>13</v>
       </c>
       <c r="D54" s="8" t="s">
-        <v>389</v>
+        <v>387</v>
       </c>
       <c r="F54" s="6">
         <v>2</v>
@@ -2929,7 +2940,7 @@
         <v>13</v>
       </c>
       <c r="D55" s="8" t="s">
-        <v>369</v>
+        <v>367</v>
       </c>
       <c r="F55" s="6">
         <v>2</v>
@@ -2946,7 +2957,7 @@
         <v>13</v>
       </c>
       <c r="D56" s="8" t="s">
-        <v>366</v>
+        <v>364</v>
       </c>
       <c r="F56" s="6">
         <v>2</v>
@@ -2960,7 +2971,7 @@
         <v>13</v>
       </c>
       <c r="D57" s="8" t="s">
-        <v>374</v>
+        <v>372</v>
       </c>
       <c r="F57" s="6">
         <v>2</v>
@@ -2974,7 +2985,7 @@
         <v>95</v>
       </c>
       <c r="D58" s="8" t="s">
-        <v>349</v>
+        <v>347</v>
       </c>
       <c r="F58" s="6">
         <v>2</v>
@@ -2985,13 +2996,13 @@
         <v>220</v>
       </c>
       <c r="B59" s="6" t="s">
-        <v>381</v>
+        <v>379</v>
       </c>
       <c r="C59" s="7" t="s">
         <v>13</v>
       </c>
       <c r="D59" s="8" t="s">
-        <v>380</v>
+        <v>378</v>
       </c>
       <c r="E59" s="9" t="s">
         <v>93</v>
@@ -3000,7 +3011,7 @@
         <v>2</v>
       </c>
       <c r="G59" s="3" t="s">
-        <v>382</v>
+        <v>380</v>
       </c>
     </row>
     <row r="60" spans="1:7" ht="17.149999999999999" x14ac:dyDescent="0.55000000000000004">
@@ -3008,13 +3019,13 @@
         <v>178</v>
       </c>
       <c r="B60" s="6" t="s">
-        <v>336</v>
+        <v>334</v>
       </c>
       <c r="C60" s="7" t="s">
         <v>6</v>
       </c>
       <c r="D60" s="8" t="s">
-        <v>335</v>
+        <v>333</v>
       </c>
       <c r="F60" s="6">
         <v>2</v>
@@ -3031,7 +3042,7 @@
         <v>95</v>
       </c>
       <c r="D61" s="8" t="s">
-        <v>328</v>
+        <v>326</v>
       </c>
       <c r="E61" s="9" t="s">
         <v>118</v>
@@ -3062,13 +3073,13 @@
     </row>
     <row r="63" spans="1:7" ht="17.149999999999999" x14ac:dyDescent="0.55000000000000004">
       <c r="A63" s="10" t="s">
-        <v>360</v>
+        <v>358</v>
       </c>
       <c r="C63" s="7" t="s">
         <v>13</v>
       </c>
       <c r="D63" s="8" t="s">
-        <v>361</v>
+        <v>359</v>
       </c>
     </row>
     <row r="64" spans="1:7" ht="17.149999999999999" x14ac:dyDescent="0.55000000000000004">
@@ -3082,7 +3093,7 @@
         <v>42</v>
       </c>
       <c r="D64" s="8" t="s">
-        <v>344</v>
+        <v>342</v>
       </c>
       <c r="E64" s="9" t="s">
         <v>93</v>
@@ -3119,13 +3130,13 @@
         <v>200</v>
       </c>
       <c r="B66" s="6" t="s">
-        <v>301</v>
+        <v>299</v>
       </c>
       <c r="C66" s="7" t="s">
         <v>95</v>
       </c>
       <c r="D66" s="8" t="s">
-        <v>362</v>
+        <v>360</v>
       </c>
       <c r="F66" s="6">
         <v>3</v>
@@ -3170,13 +3181,13 @@
     </row>
     <row r="69" spans="1:7" ht="17.149999999999999" x14ac:dyDescent="0.55000000000000004">
       <c r="A69" s="10" t="s">
-        <v>297</v>
+        <v>295</v>
       </c>
       <c r="C69" s="7" t="s">
         <v>42</v>
       </c>
       <c r="D69" s="8" t="s">
-        <v>295</v>
+        <v>293</v>
       </c>
     </row>
     <row r="70" spans="1:7" ht="17.149999999999999" x14ac:dyDescent="0.55000000000000004">
@@ -3278,10 +3289,10 @@
         <v>80</v>
       </c>
       <c r="D75" s="8" t="s">
-        <v>335</v>
+        <v>333</v>
       </c>
       <c r="E75" s="13" t="s">
-        <v>338</v>
+        <v>336</v>
       </c>
       <c r="F75" s="6">
         <v>2</v>
@@ -3337,16 +3348,16 @@
     </row>
     <row r="79" spans="1:7" ht="17.149999999999999" x14ac:dyDescent="0.55000000000000004">
       <c r="A79" s="10" t="s">
-        <v>307</v>
+        <v>305</v>
       </c>
       <c r="B79" s="6" t="s">
-        <v>308</v>
+        <v>306</v>
       </c>
       <c r="C79" s="7" t="s">
         <v>80</v>
       </c>
       <c r="D79" s="8" t="s">
-        <v>305</v>
+        <v>303</v>
       </c>
       <c r="E79" s="9" t="s">
         <v>87</v>
@@ -3422,7 +3433,7 @@
         <v>13</v>
       </c>
       <c r="D84" s="8" t="s">
-        <v>400</v>
+        <v>398</v>
       </c>
       <c r="E84" s="9" t="s">
         <v>276</v>
@@ -3442,7 +3453,7 @@
         <v>80</v>
       </c>
       <c r="D85" s="8" t="s">
-        <v>400</v>
+        <v>398</v>
       </c>
       <c r="E85" s="9" t="s">
         <v>8</v>
@@ -3465,7 +3476,7 @@
         <v>13</v>
       </c>
       <c r="D86" s="8" t="s">
-        <v>314</v>
+        <v>312</v>
       </c>
       <c r="E86" s="9" t="s">
         <v>109</v>
@@ -3474,7 +3485,7 @@
         <v>2</v>
       </c>
       <c r="G86" s="3" t="s">
-        <v>315</v>
+        <v>313</v>
       </c>
     </row>
     <row r="87" spans="1:7" ht="17.149999999999999" x14ac:dyDescent="0.55000000000000004">
@@ -3488,7 +3499,7 @@
         <v>80</v>
       </c>
       <c r="D87" s="8" t="s">
-        <v>402</v>
+        <v>400</v>
       </c>
       <c r="F87" s="6">
         <v>2</v>
@@ -3508,7 +3519,7 @@
         <v>42</v>
       </c>
       <c r="D88" s="8" t="s">
-        <v>400</v>
+        <v>398</v>
       </c>
       <c r="E88" s="9" t="s">
         <v>272</v>
@@ -3519,18 +3530,18 @@
     </row>
     <row r="89" spans="1:7" ht="17.149999999999999" x14ac:dyDescent="0.55000000000000004">
       <c r="A89" s="10" t="s">
-        <v>300</v>
+        <v>298</v>
       </c>
       <c r="C89" s="7" t="s">
         <v>28</v>
       </c>
       <c r="D89" s="8" t="s">
-        <v>299</v>
+        <v>297</v>
       </c>
     </row>
     <row r="90" spans="1:7" ht="17.149999999999999" x14ac:dyDescent="0.55000000000000004">
       <c r="A90" s="10" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="B90" s="6" t="s">
         <v>130</v>
@@ -3539,7 +3550,7 @@
         <v>13</v>
       </c>
       <c r="D90" s="8" t="s">
-        <v>402</v>
+        <v>400</v>
       </c>
       <c r="F90" s="6">
         <v>2</v>
@@ -3550,13 +3561,13 @@
         <v>281</v>
       </c>
       <c r="B91" s="6" t="s">
-        <v>325</v>
+        <v>323</v>
       </c>
       <c r="C91" s="7" t="s">
         <v>13</v>
       </c>
       <c r="D91" s="8" t="s">
-        <v>326</v>
+        <v>324</v>
       </c>
       <c r="F91" s="6">
         <v>2</v>
@@ -3573,7 +3584,7 @@
         <v>95</v>
       </c>
       <c r="D92" s="8" t="s">
-        <v>393</v>
+        <v>391</v>
       </c>
       <c r="E92" s="12" t="s">
         <v>242</v>
@@ -3582,21 +3593,21 @@
         <v>2</v>
       </c>
       <c r="G92" s="3" t="s">
-        <v>394</v>
+        <v>392</v>
       </c>
     </row>
     <row r="93" spans="1:7" ht="17.149999999999999" x14ac:dyDescent="0.55000000000000004">
       <c r="A93" s="10" t="s">
-        <v>352</v>
+        <v>350</v>
       </c>
       <c r="B93" s="6" t="s">
-        <v>353</v>
+        <v>351</v>
       </c>
       <c r="C93" s="7" t="s">
         <v>13</v>
       </c>
       <c r="D93" s="8" t="s">
-        <v>349</v>
+        <v>347</v>
       </c>
       <c r="E93" s="9" t="s">
         <v>14</v>
@@ -3613,7 +3624,7 @@
         <v>80</v>
       </c>
       <c r="D94" s="8" t="s">
-        <v>392</v>
+        <v>390</v>
       </c>
       <c r="E94" s="9" t="s">
         <v>22</v>
@@ -3633,7 +3644,7 @@
         <v>13</v>
       </c>
       <c r="D95" s="8" t="s">
-        <v>400</v>
+        <v>398</v>
       </c>
       <c r="F95" s="6">
         <v>2</v>
@@ -3650,7 +3661,7 @@
         <v>42</v>
       </c>
       <c r="D96" s="8" t="s">
-        <v>392</v>
+        <v>390</v>
       </c>
       <c r="F96" s="6">
         <v>2</v>
@@ -3672,16 +3683,16 @@
     </row>
     <row r="98" spans="1:7" ht="17.149999999999999" x14ac:dyDescent="0.55000000000000004">
       <c r="A98" s="10" t="s">
+        <v>327</v>
+      </c>
+      <c r="B98" s="6" t="s">
         <v>329</v>
-      </c>
-      <c r="B98" s="6" t="s">
-        <v>331</v>
       </c>
       <c r="C98" s="7" t="s">
         <v>13</v>
       </c>
       <c r="D98" s="8" t="s">
-        <v>330</v>
+        <v>328</v>
       </c>
       <c r="E98" s="9" t="s">
         <v>14</v>
@@ -3718,7 +3729,7 @@
         <v>80</v>
       </c>
       <c r="D100" s="8" t="s">
-        <v>389</v>
+        <v>387</v>
       </c>
       <c r="F100" s="6">
         <v>2</v>
@@ -3735,7 +3746,7 @@
         <v>80</v>
       </c>
       <c r="D101" s="8" t="s">
-        <v>397</v>
+        <v>395</v>
       </c>
       <c r="E101" s="9" t="s">
         <v>93</v>
@@ -3755,13 +3766,13 @@
         <v>80</v>
       </c>
       <c r="D102" s="8" t="s">
-        <v>393</v>
+        <v>391</v>
       </c>
       <c r="E102" s="9" t="s">
         <v>98</v>
       </c>
       <c r="G102" s="3" t="s">
-        <v>396</v>
+        <v>394</v>
       </c>
     </row>
     <row r="103" spans="1:7" ht="17.149999999999999" x14ac:dyDescent="0.55000000000000004">
@@ -3775,18 +3786,18 @@
         <v>13</v>
       </c>
       <c r="D103" s="8" t="s">
+        <v>333</v>
+      </c>
+      <c r="F103" s="6">
+        <v>2</v>
+      </c>
+      <c r="G103" s="3" t="s">
         <v>335</v>
-      </c>
-      <c r="F103" s="6">
-        <v>2</v>
-      </c>
-      <c r="G103" s="3" t="s">
-        <v>337</v>
       </c>
     </row>
     <row r="104" spans="1:7" ht="17.149999999999999" x14ac:dyDescent="0.55000000000000004">
       <c r="A104" s="10" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="B104" s="6" t="s">
         <v>12</v>
@@ -3795,10 +3806,10 @@
         <v>80</v>
       </c>
       <c r="D104" s="8" t="s">
+        <v>312</v>
+      </c>
+      <c r="E104" s="9" t="s">
         <v>314</v>
-      </c>
-      <c r="E104" s="9" t="s">
-        <v>316</v>
       </c>
       <c r="F104" s="6">
         <v>3</v>
@@ -3818,7 +3829,7 @@
         <v>80</v>
       </c>
       <c r="D105" s="8" t="s">
-        <v>313</v>
+        <v>311</v>
       </c>
       <c r="E105" s="9" t="s">
         <v>98</v>
@@ -3835,19 +3846,19 @@
         <v>219</v>
       </c>
       <c r="B106" s="6" t="s">
-        <v>379</v>
+        <v>377</v>
       </c>
       <c r="C106" s="7" t="s">
         <v>13</v>
       </c>
       <c r="D106" s="8" t="s">
-        <v>375</v>
+        <v>373</v>
       </c>
       <c r="F106" s="6">
         <v>2</v>
       </c>
       <c r="G106" s="3" t="s">
-        <v>378</v>
+        <v>376</v>
       </c>
     </row>
     <row r="107" spans="1:7" ht="17.149999999999999" x14ac:dyDescent="0.55000000000000004">
@@ -3861,7 +3872,7 @@
         <v>95</v>
       </c>
       <c r="D107" s="8" t="s">
-        <v>317</v>
+        <v>315</v>
       </c>
       <c r="E107" s="9" t="s">
         <v>110</v>
@@ -3870,7 +3881,7 @@
         <v>3</v>
       </c>
       <c r="G107" s="3" t="s">
-        <v>318</v>
+        <v>316</v>
       </c>
     </row>
     <row r="108" spans="1:7" ht="17.149999999999999" x14ac:dyDescent="0.55000000000000004">
@@ -3904,7 +3915,7 @@
         <v>13</v>
       </c>
       <c r="D109" s="8" t="s">
-        <v>400</v>
+        <v>398</v>
       </c>
       <c r="F109" s="6">
         <v>2</v>
@@ -3921,7 +3932,7 @@
         <v>13</v>
       </c>
       <c r="D110" s="8" t="s">
-        <v>388</v>
+        <v>386</v>
       </c>
       <c r="E110" s="9" t="s">
         <v>128</v>
@@ -3955,16 +3966,16 @@
     </row>
     <row r="112" spans="1:7" ht="17.149999999999999" x14ac:dyDescent="0.55000000000000004">
       <c r="A112" s="10" t="s">
-        <v>323</v>
+        <v>321</v>
       </c>
       <c r="B112" s="6" t="s">
-        <v>324</v>
+        <v>322</v>
       </c>
       <c r="C112" s="7" t="s">
         <v>80</v>
       </c>
       <c r="D112" s="8" t="s">
-        <v>320</v>
+        <v>318</v>
       </c>
       <c r="E112" s="9" t="s">
         <v>14</v>
@@ -3998,27 +4009,27 @@
         <v>80</v>
       </c>
       <c r="D114" s="8" t="s">
-        <v>309</v>
+        <v>307</v>
       </c>
       <c r="F114" s="6">
         <v>3</v>
       </c>
       <c r="G114" s="3" t="s">
-        <v>312</v>
+        <v>310</v>
       </c>
     </row>
     <row r="115" spans="1:7" ht="17.149999999999999" x14ac:dyDescent="0.55000000000000004">
       <c r="A115" s="10" t="s">
-        <v>321</v>
+        <v>319</v>
       </c>
       <c r="B115" s="6" t="s">
-        <v>322</v>
+        <v>320</v>
       </c>
       <c r="C115" s="7" t="s">
         <v>80</v>
       </c>
       <c r="D115" s="8" t="s">
-        <v>320</v>
+        <v>318</v>
       </c>
       <c r="E115" s="9" t="s">
         <v>14</v>
@@ -4026,19 +4037,25 @@
     </row>
     <row r="116" spans="1:7" ht="17.149999999999999" x14ac:dyDescent="0.55000000000000004">
       <c r="A116" s="10" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="B116" s="6" t="s">
         <v>130</v>
       </c>
       <c r="C116" s="7" t="s">
-        <v>80</v>
+        <v>95</v>
       </c>
       <c r="D116" s="8" t="s">
-        <v>286</v>
+        <v>401</v>
       </c>
       <c r="E116" s="9" t="s">
         <v>22</v>
+      </c>
+      <c r="F116" s="6">
+        <v>2</v>
+      </c>
+      <c r="G116" s="3" t="s">
+        <v>402</v>
       </c>
     </row>
     <row r="117" spans="1:7" ht="17.149999999999999" x14ac:dyDescent="0.55000000000000004">
@@ -4052,7 +4069,7 @@
         <v>80</v>
       </c>
       <c r="D117" s="8" t="s">
-        <v>391</v>
+        <v>389</v>
       </c>
       <c r="E117" s="9" t="s">
         <v>14</v>
@@ -4080,16 +4097,16 @@
     </row>
     <row r="119" spans="1:7" ht="17.149999999999999" x14ac:dyDescent="0.55000000000000004">
       <c r="A119" s="10" t="s">
-        <v>327</v>
+        <v>325</v>
       </c>
       <c r="B119" s="6" t="s">
-        <v>325</v>
+        <v>323</v>
       </c>
       <c r="C119" s="7" t="s">
         <v>13</v>
       </c>
       <c r="D119" s="8" t="s">
-        <v>326</v>
+        <v>324</v>
       </c>
     </row>
     <row r="120" spans="1:7" ht="17.149999999999999" x14ac:dyDescent="0.55000000000000004">
@@ -4097,13 +4114,13 @@
         <v>127</v>
       </c>
       <c r="B120" s="6" t="s">
-        <v>334</v>
+        <v>332</v>
       </c>
       <c r="C120" s="7" t="s">
         <v>42</v>
       </c>
       <c r="D120" s="8" t="s">
-        <v>333</v>
+        <v>331</v>
       </c>
       <c r="E120" s="9" t="s">
         <v>128</v>
@@ -4117,13 +4134,13 @@
         <v>184</v>
       </c>
       <c r="B121" s="6" t="s">
-        <v>342</v>
+        <v>340</v>
       </c>
       <c r="C121" s="7" t="s">
         <v>42</v>
       </c>
       <c r="D121" s="8" t="s">
-        <v>339</v>
+        <v>337</v>
       </c>
       <c r="E121" s="10" t="s">
         <v>185</v>
@@ -4132,7 +4149,7 @@
         <v>2</v>
       </c>
       <c r="G121" s="3" t="s">
-        <v>341</v>
+        <v>339</v>
       </c>
     </row>
     <row r="122" spans="1:7" ht="17.149999999999999" x14ac:dyDescent="0.55000000000000004">
@@ -4143,7 +4160,7 @@
         <v>13</v>
       </c>
       <c r="D122" s="8" t="s">
-        <v>371</v>
+        <v>369</v>
       </c>
       <c r="F122" s="6">
         <v>2</v>
@@ -4160,7 +4177,7 @@
         <v>42</v>
       </c>
       <c r="D123" s="8" t="s">
-        <v>400</v>
+        <v>398</v>
       </c>
       <c r="F123" s="6">
         <v>2</v>
@@ -4177,7 +4194,7 @@
         <v>80</v>
       </c>
       <c r="D124" s="8" t="s">
-        <v>333</v>
+        <v>331</v>
       </c>
       <c r="E124" s="9" t="s">
         <v>131</v>
@@ -4197,7 +4214,7 @@
         <v>95</v>
       </c>
       <c r="D125" s="8" t="s">
-        <v>319</v>
+        <v>317</v>
       </c>
       <c r="E125" s="9" t="s">
         <v>118</v>
@@ -4208,7 +4225,7 @@
     </row>
     <row r="126" spans="1:7" ht="17.149999999999999" x14ac:dyDescent="0.55000000000000004">
       <c r="A126" s="10" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="B126" s="6" t="s">
         <v>130</v>
@@ -4217,15 +4234,18 @@
         <v>13</v>
       </c>
       <c r="D126" s="8" t="s">
-        <v>286</v>
+        <v>401</v>
       </c>
       <c r="E126" s="9" t="s">
         <v>14</v>
       </c>
+      <c r="F126" s="6">
+        <v>2</v>
+      </c>
     </row>
     <row r="127" spans="1:7" ht="17.149999999999999" x14ac:dyDescent="0.55000000000000004">
       <c r="A127" s="10" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="B127" s="6" t="s">
         <v>130</v>
@@ -4234,7 +4254,10 @@
         <v>13</v>
       </c>
       <c r="D127" s="8" t="s">
-        <v>286</v>
+        <v>401</v>
+      </c>
+      <c r="F127" s="6">
+        <v>2</v>
       </c>
     </row>
     <row r="128" spans="1:7" ht="17.149999999999999" x14ac:dyDescent="0.55000000000000004">
@@ -4268,7 +4291,7 @@
         <v>42</v>
       </c>
       <c r="D129" s="8" t="s">
-        <v>335</v>
+        <v>333</v>
       </c>
       <c r="F129" s="6">
         <v>2</v>
@@ -4276,13 +4299,13 @@
     </row>
     <row r="130" spans="1:7" ht="17.149999999999999" x14ac:dyDescent="0.55000000000000004">
       <c r="A130" s="10" t="s">
-        <v>296</v>
+        <v>294</v>
       </c>
       <c r="C130" s="7" t="s">
         <v>13</v>
       </c>
       <c r="D130" s="8" t="s">
-        <v>295</v>
+        <v>293</v>
       </c>
     </row>
     <row r="131" spans="1:7" ht="17.149999999999999" x14ac:dyDescent="0.55000000000000004">
@@ -4304,7 +4327,7 @@
     </row>
     <row r="132" spans="1:7" ht="17.149999999999999" x14ac:dyDescent="0.55000000000000004">
       <c r="A132" s="10" t="s">
-        <v>294</v>
+        <v>292</v>
       </c>
       <c r="B132" s="6" t="s">
         <v>130</v>
@@ -4313,10 +4336,16 @@
         <v>80</v>
       </c>
       <c r="D132" s="8" t="s">
-        <v>286</v>
+        <v>401</v>
       </c>
       <c r="E132" s="9" t="s">
         <v>14</v>
+      </c>
+      <c r="F132" s="6">
+        <v>2</v>
+      </c>
+      <c r="G132" s="3" t="s">
+        <v>404</v>
       </c>
     </row>
     <row r="133" spans="1:7" ht="17.149999999999999" x14ac:dyDescent="0.55000000000000004">
@@ -4324,13 +4353,13 @@
         <v>181</v>
       </c>
       <c r="B133" s="6" t="s">
-        <v>340</v>
+        <v>338</v>
       </c>
       <c r="C133" s="7" t="s">
         <v>42</v>
       </c>
       <c r="D133" s="8" t="s">
-        <v>339</v>
+        <v>337</v>
       </c>
       <c r="E133" s="9" t="s">
         <v>183</v>
@@ -4370,7 +4399,7 @@
         <v>80</v>
       </c>
       <c r="D135" s="8" t="s">
-        <v>398</v>
+        <v>396</v>
       </c>
       <c r="E135" s="9" t="s">
         <v>251</v>
@@ -4393,7 +4422,7 @@
         <v>42</v>
       </c>
       <c r="D136" s="8" t="s">
-        <v>392</v>
+        <v>390</v>
       </c>
       <c r="F136" s="6">
         <v>2</v>
@@ -4410,7 +4439,7 @@
         <v>6</v>
       </c>
       <c r="D137" s="8" t="s">
-        <v>400</v>
+        <v>398</v>
       </c>
       <c r="F137" s="6">
         <v>2</v>
@@ -4427,7 +4456,7 @@
         <v>80</v>
       </c>
       <c r="D138" s="8" t="s">
-        <v>332</v>
+        <v>330</v>
       </c>
       <c r="E138" s="9" t="s">
         <v>122</v>
@@ -4447,7 +4476,7 @@
         <v>13</v>
       </c>
       <c r="D139" s="8" t="s">
-        <v>401</v>
+        <v>399</v>
       </c>
       <c r="E139" s="9" t="s">
         <v>22</v>
@@ -4464,7 +4493,7 @@
         <v>13</v>
       </c>
       <c r="D140" s="8" t="s">
-        <v>400</v>
+        <v>398</v>
       </c>
       <c r="E140" s="9" t="s">
         <v>47</v>
@@ -4484,7 +4513,7 @@
         <v>42</v>
       </c>
       <c r="D141" s="8" t="s">
-        <v>389</v>
+        <v>387</v>
       </c>
       <c r="E141" s="9" t="s">
         <v>93</v>
@@ -4538,7 +4567,7 @@
         <v>80</v>
       </c>
       <c r="D144" s="8" t="s">
-        <v>398</v>
+        <v>396</v>
       </c>
       <c r="E144" s="9" t="s">
         <v>128</v>
@@ -4547,7 +4576,7 @@
         <v>2</v>
       </c>
       <c r="G144" s="3" t="s">
-        <v>399</v>
+        <v>397</v>
       </c>
     </row>
     <row r="145" spans="1:7" ht="17.149999999999999" x14ac:dyDescent="0.55000000000000004">
@@ -4558,7 +4587,7 @@
         <v>13</v>
       </c>
       <c r="D145" s="8" t="s">
-        <v>369</v>
+        <v>367</v>
       </c>
       <c r="F145" s="6">
         <v>2</v>
@@ -4566,13 +4595,13 @@
     </row>
     <row r="146" spans="1:7" ht="17.149999999999999" x14ac:dyDescent="0.55000000000000004">
       <c r="A146" s="10" t="s">
-        <v>298</v>
+        <v>296</v>
       </c>
       <c r="C146" s="7" t="s">
         <v>42</v>
       </c>
       <c r="D146" s="8" t="s">
-        <v>295</v>
+        <v>293</v>
       </c>
     </row>
     <row r="147" spans="1:7" ht="17.149999999999999" x14ac:dyDescent="0.55000000000000004">
@@ -4583,7 +4612,7 @@
         <v>42</v>
       </c>
       <c r="D147" s="8" t="s">
-        <v>372</v>
+        <v>370</v>
       </c>
       <c r="F147" s="6">
         <v>2</v>
@@ -4594,19 +4623,19 @@
         <v>224</v>
       </c>
       <c r="B148" s="6" t="s">
-        <v>386</v>
+        <v>384</v>
       </c>
       <c r="C148" s="7" t="s">
         <v>13</v>
       </c>
       <c r="D148" s="8" t="s">
+        <v>383</v>
+      </c>
+      <c r="F148" s="6">
+        <v>2</v>
+      </c>
+      <c r="G148" s="3" t="s">
         <v>385</v>
-      </c>
-      <c r="F148" s="6">
-        <v>2</v>
-      </c>
-      <c r="G148" s="3" t="s">
-        <v>387</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
2024.11.19 LeetCodeHot100 三刷 11.15.
</commit_message>
<xml_diff>
--- a/2024LeetCode刷题记录.xlsx
+++ b/2024LeetCode刷题记录.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\develop\GithubRepo\LeetCode\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A574A920-7018-4447-A82F-0CA402FB263B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7CC62C6A-02D5-4D23-9FB6-C52D08EC5ECD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-30828" yWindow="-108" windowWidth="30936" windowHeight="16776" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1119,10 +1119,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>2024.09.02</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>两边往中心收拢</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -1535,6 +1531,10 @@
   </si>
   <si>
     <t>2024.11.18</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>2024.11.19</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -1989,8 +1989,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G153"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A64" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="L86" sqref="L86"/>
+    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="F29" sqref="F29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="14.15" x14ac:dyDescent="0.35"/>
@@ -2039,7 +2039,7 @@
         <v>80</v>
       </c>
       <c r="D2" s="8" t="s">
-        <v>414</v>
+        <v>413</v>
       </c>
       <c r="F2" s="6">
         <v>3</v>
@@ -2056,7 +2056,7 @@
         <v>13</v>
       </c>
       <c r="D3" s="8" t="s">
-        <v>368</v>
+        <v>367</v>
       </c>
       <c r="F3" s="6">
         <v>2</v>
@@ -2070,7 +2070,7 @@
         <v>13</v>
       </c>
       <c r="D4" s="8" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
       <c r="F4" s="6">
         <v>2</v>
@@ -2081,13 +2081,13 @@
         <v>208</v>
       </c>
       <c r="B5" s="6" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
       <c r="C5" s="7" t="s">
         <v>13</v>
       </c>
       <c r="D5" s="8" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
       <c r="F5" s="6">
         <v>2</v>
@@ -2104,7 +2104,7 @@
         <v>13</v>
       </c>
       <c r="D6" s="8" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="E6" s="9" t="s">
         <v>14</v>
@@ -2124,7 +2124,7 @@
         <v>80</v>
       </c>
       <c r="D7" s="8" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
       <c r="F7" s="6">
         <v>2</v>
@@ -2138,7 +2138,7 @@
         <v>42</v>
       </c>
       <c r="D8" s="8" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
       <c r="F8" s="6">
         <v>2</v>
@@ -2155,16 +2155,16 @@
         <v>42</v>
       </c>
       <c r="D9" s="8" t="s">
-        <v>306</v>
+        <v>415</v>
       </c>
       <c r="E9" s="9" t="s">
         <v>93</v>
       </c>
       <c r="F9" s="6">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="G9" s="3" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
     </row>
     <row r="10" spans="1:7" ht="17.149999999999999" x14ac:dyDescent="0.55000000000000004">
@@ -2175,13 +2175,13 @@
         <v>42</v>
       </c>
       <c r="D10" s="8" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
       <c r="F10" s="6">
         <v>2</v>
       </c>
       <c r="G10" s="3" t="s">
-        <v>374</v>
+        <v>373</v>
       </c>
     </row>
     <row r="11" spans="1:7" ht="17.149999999999999" x14ac:dyDescent="0.55000000000000004">
@@ -2195,7 +2195,7 @@
         <v>95</v>
       </c>
       <c r="D11" s="8" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
       <c r="E11" s="9" t="s">
         <v>14</v>
@@ -2204,7 +2204,7 @@
         <v>2</v>
       </c>
       <c r="G11" s="3" t="s">
-        <v>402</v>
+        <v>401</v>
       </c>
     </row>
     <row r="12" spans="1:7" ht="17.149999999999999" x14ac:dyDescent="0.55000000000000004">
@@ -2238,7 +2238,7 @@
         <v>6</v>
       </c>
       <c r="D13" s="8" t="s">
-        <v>399</v>
+        <v>398</v>
       </c>
       <c r="F13" s="6">
         <v>2</v>
@@ -2269,13 +2269,13 @@
         <v>260</v>
       </c>
       <c r="B15" s="6" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
       <c r="C15" s="7" t="s">
         <v>42</v>
       </c>
       <c r="D15" s="8" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
       <c r="E15" s="9" t="s">
         <v>14</v>
@@ -2286,16 +2286,16 @@
     </row>
     <row r="16" spans="1:7" ht="17.149999999999999" x14ac:dyDescent="0.55000000000000004">
       <c r="A16" s="10" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
       <c r="B16" s="6" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
       <c r="C16" s="7" t="s">
         <v>13</v>
       </c>
       <c r="D16" s="8" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
       <c r="E16" s="9" t="s">
         <v>14</v>
@@ -2303,13 +2303,13 @@
     </row>
     <row r="17" spans="1:7" ht="17.149999999999999" x14ac:dyDescent="0.55000000000000004">
       <c r="A17" s="10" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
       <c r="C17" s="7" t="s">
         <v>42</v>
       </c>
       <c r="D17" s="8" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
       <c r="E17" s="9" t="s">
         <v>14</v>
@@ -2320,13 +2320,13 @@
         <v>221</v>
       </c>
       <c r="B18" s="6" t="s">
-        <v>380</v>
+        <v>379</v>
       </c>
       <c r="C18" s="7" t="s">
         <v>13</v>
       </c>
       <c r="D18" s="8" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
       <c r="F18" s="6">
         <v>2</v>
@@ -2346,7 +2346,7 @@
         <v>80</v>
       </c>
       <c r="D19" s="8" t="s">
-        <v>414</v>
+        <v>413</v>
       </c>
       <c r="F19" s="6">
         <v>3</v>
@@ -2363,7 +2363,7 @@
         <v>13</v>
       </c>
       <c r="D20" s="8" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
       <c r="F20" s="6">
         <v>2</v>
@@ -2380,7 +2380,7 @@
         <v>28</v>
       </c>
       <c r="D21" s="8" t="s">
-        <v>397</v>
+        <v>396</v>
       </c>
       <c r="F21" s="6">
         <v>2</v>
@@ -2397,7 +2397,7 @@
         <v>13</v>
       </c>
       <c r="D22" s="8" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
       <c r="E22" s="9" t="s">
         <v>87</v>
@@ -2417,7 +2417,7 @@
         <v>13</v>
       </c>
       <c r="D23" s="8" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="E23" s="9" t="s">
         <v>14</v>
@@ -2431,13 +2431,13 @@
         <v>195</v>
       </c>
       <c r="B24" s="6" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
       <c r="C24" s="7" t="s">
         <v>42</v>
       </c>
       <c r="D24" s="8" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
       <c r="F24" s="6">
         <v>2</v>
@@ -2451,16 +2451,16 @@
         <v>13</v>
       </c>
       <c r="D25" s="8" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
       <c r="E25" s="13" t="s">
+        <v>351</v>
+      </c>
+      <c r="F25" s="6">
+        <v>2</v>
+      </c>
+      <c r="G25" s="3" t="s">
         <v>352</v>
-      </c>
-      <c r="F25" s="6">
-        <v>2</v>
-      </c>
-      <c r="G25" s="3" t="s">
-        <v>353</v>
       </c>
     </row>
     <row r="26" spans="1:7" ht="17.149999999999999" x14ac:dyDescent="0.55000000000000004">
@@ -2488,7 +2488,7 @@
         <v>80</v>
       </c>
       <c r="D27" s="8" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
       <c r="F27" s="6">
         <v>2</v>
@@ -2508,7 +2508,7 @@
         <v>80</v>
       </c>
       <c r="D28" s="8" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
       <c r="F28" s="6">
         <v>2</v>
@@ -2525,16 +2525,16 @@
         <v>13</v>
       </c>
       <c r="D29" s="8" t="s">
-        <v>306</v>
+        <v>415</v>
       </c>
       <c r="E29" s="9" t="s">
         <v>97</v>
       </c>
       <c r="F29" s="6">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="G29" s="3" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
     </row>
     <row r="30" spans="1:7" ht="17.149999999999999" x14ac:dyDescent="0.55000000000000004">
@@ -2548,7 +2548,7 @@
         <v>6</v>
       </c>
       <c r="D30" s="8" t="s">
-        <v>399</v>
+        <v>398</v>
       </c>
       <c r="F30" s="6">
         <v>2</v>
@@ -2565,13 +2565,13 @@
         <v>13</v>
       </c>
       <c r="D31" s="8" t="s">
-        <v>390</v>
+        <v>389</v>
       </c>
       <c r="F31" s="6">
         <v>2</v>
       </c>
       <c r="G31" s="3" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
     </row>
     <row r="32" spans="1:7" ht="17.149999999999999" x14ac:dyDescent="0.55000000000000004">
@@ -2585,7 +2585,7 @@
         <v>13</v>
       </c>
       <c r="D32" s="8" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
       <c r="E32" s="9" t="s">
         <v>103</v>
@@ -2636,16 +2636,16 @@
         <v>6</v>
       </c>
       <c r="D35" s="8" t="s">
+        <v>345</v>
+      </c>
+      <c r="E35" s="13" t="s">
+        <v>347</v>
+      </c>
+      <c r="F35" s="6">
+        <v>2</v>
+      </c>
+      <c r="G35" s="3" t="s">
         <v>346</v>
-      </c>
-      <c r="E35" s="13" t="s">
-        <v>348</v>
-      </c>
-      <c r="F35" s="6">
-        <v>2</v>
-      </c>
-      <c r="G35" s="3" t="s">
-        <v>347</v>
       </c>
     </row>
     <row r="36" spans="1:7" ht="17.149999999999999" x14ac:dyDescent="0.55000000000000004">
@@ -2659,7 +2659,7 @@
         <v>13</v>
       </c>
       <c r="D36" s="8" t="s">
-        <v>397</v>
+        <v>396</v>
       </c>
       <c r="F36" s="6">
         <v>2</v>
@@ -2676,7 +2676,7 @@
         <v>80</v>
       </c>
       <c r="D37" s="8" t="s">
-        <v>385</v>
+        <v>384</v>
       </c>
       <c r="E37" s="9" t="s">
         <v>22</v>
@@ -2693,7 +2693,7 @@
         <v>28</v>
       </c>
       <c r="D38" s="8" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="F38" s="6">
         <v>2</v>
@@ -2707,13 +2707,13 @@
         <v>13</v>
       </c>
       <c r="D39" s="8" t="s">
+        <v>354</v>
+      </c>
+      <c r="F39" s="6">
+        <v>2</v>
+      </c>
+      <c r="G39" s="3" t="s">
         <v>355</v>
-      </c>
-      <c r="F39" s="6">
-        <v>2</v>
-      </c>
-      <c r="G39" s="3" t="s">
-        <v>356</v>
       </c>
     </row>
     <row r="40" spans="1:7" ht="17.149999999999999" x14ac:dyDescent="0.55000000000000004">
@@ -2727,13 +2727,13 @@
         <v>80</v>
       </c>
       <c r="D40" s="8" t="s">
+        <v>340</v>
+      </c>
+      <c r="F40" s="6">
+        <v>2</v>
+      </c>
+      <c r="G40" s="3" t="s">
         <v>341</v>
-      </c>
-      <c r="F40" s="6">
-        <v>2</v>
-      </c>
-      <c r="G40" s="3" t="s">
-        <v>342</v>
       </c>
     </row>
     <row r="41" spans="1:7" ht="17.149999999999999" x14ac:dyDescent="0.55000000000000004">
@@ -2744,13 +2744,13 @@
         <v>13</v>
       </c>
       <c r="D41" s="8" t="s">
+        <v>371</v>
+      </c>
+      <c r="F41" s="6">
+        <v>2</v>
+      </c>
+      <c r="G41" s="3" t="s">
         <v>372</v>
-      </c>
-      <c r="F41" s="6">
-        <v>2</v>
-      </c>
-      <c r="G41" s="3" t="s">
-        <v>373</v>
       </c>
     </row>
     <row r="42" spans="1:7" ht="17.149999999999999" x14ac:dyDescent="0.55000000000000004">
@@ -2761,7 +2761,7 @@
         <v>6</v>
       </c>
       <c r="D42" s="8" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
       <c r="F42" s="6">
         <v>2</v>
@@ -2778,7 +2778,7 @@
         <v>80</v>
       </c>
       <c r="D43" s="8" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
       <c r="F43" s="6">
         <v>2</v>
@@ -2792,7 +2792,7 @@
         <v>13</v>
       </c>
       <c r="D44" s="8" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
       <c r="F44" s="6">
         <v>2</v>
@@ -2809,7 +2809,7 @@
         <v>80</v>
       </c>
       <c r="D45" s="8" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
       <c r="F45" s="6">
         <v>2</v>
@@ -2823,7 +2823,7 @@
         <v>80</v>
       </c>
       <c r="D46" s="8" t="s">
-        <v>382</v>
+        <v>381</v>
       </c>
       <c r="F46" s="6">
         <v>2</v>
@@ -2837,7 +2837,7 @@
         <v>13</v>
       </c>
       <c r="D47" s="8" t="s">
-        <v>382</v>
+        <v>381</v>
       </c>
       <c r="F47" s="6">
         <v>2</v>
@@ -2871,27 +2871,27 @@
         <v>42</v>
       </c>
       <c r="D49" s="8" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
       <c r="F49" s="6">
         <v>2</v>
       </c>
       <c r="G49" s="3" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
     </row>
     <row r="50" spans="1:7" ht="17.149999999999999" x14ac:dyDescent="0.55000000000000004">
       <c r="A50" s="10" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
       <c r="B50" s="6" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="C50" s="7" t="s">
         <v>13</v>
       </c>
       <c r="D50" s="8" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
       <c r="E50" s="9" t="s">
         <v>14</v>
@@ -2908,13 +2908,13 @@
         <v>13</v>
       </c>
       <c r="D51" s="8" t="s">
-        <v>397</v>
+        <v>396</v>
       </c>
       <c r="F51" s="6">
         <v>3</v>
       </c>
       <c r="G51" s="3" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
     </row>
     <row r="52" spans="1:7" ht="17.149999999999999" x14ac:dyDescent="0.55000000000000004">
@@ -2965,7 +2965,7 @@
         <v>13</v>
       </c>
       <c r="D54" s="8" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
       <c r="F54" s="6">
         <v>2</v>
@@ -2979,7 +2979,7 @@
         <v>13</v>
       </c>
       <c r="D55" s="8" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
       <c r="F55" s="6">
         <v>2</v>
@@ -2996,7 +2996,7 @@
         <v>13</v>
       </c>
       <c r="D56" s="8" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
       <c r="F56" s="6">
         <v>2</v>
@@ -3010,7 +3010,7 @@
         <v>13</v>
       </c>
       <c r="D57" s="8" t="s">
-        <v>371</v>
+        <v>370</v>
       </c>
       <c r="F57" s="6">
         <v>2</v>
@@ -3024,7 +3024,7 @@
         <v>95</v>
       </c>
       <c r="D58" s="8" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
       <c r="F58" s="6">
         <v>2</v>
@@ -3035,13 +3035,13 @@
         <v>220</v>
       </c>
       <c r="B59" s="6" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="C59" s="7" t="s">
         <v>13</v>
       </c>
       <c r="D59" s="8" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
       <c r="E59" s="9" t="s">
         <v>93</v>
@@ -3050,7 +3050,7 @@
         <v>2</v>
       </c>
       <c r="G59" s="3" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
     </row>
     <row r="60" spans="1:7" ht="17.149999999999999" x14ac:dyDescent="0.55000000000000004">
@@ -3058,13 +3058,13 @@
         <v>178</v>
       </c>
       <c r="B60" s="6" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="C60" s="7" t="s">
         <v>6</v>
       </c>
       <c r="D60" s="8" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="F60" s="6">
         <v>2</v>
@@ -3081,7 +3081,7 @@
         <v>95</v>
       </c>
       <c r="D61" s="8" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
       <c r="E61" s="9" t="s">
         <v>118</v>
@@ -3112,13 +3112,13 @@
     </row>
     <row r="63" spans="1:7" ht="17.149999999999999" x14ac:dyDescent="0.55000000000000004">
       <c r="A63" s="10" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
       <c r="C63" s="7" t="s">
         <v>13</v>
       </c>
       <c r="D63" s="8" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
     </row>
     <row r="64" spans="1:7" ht="17.149999999999999" x14ac:dyDescent="0.55000000000000004">
@@ -3132,7 +3132,7 @@
         <v>42</v>
       </c>
       <c r="D64" s="8" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="E64" s="9" t="s">
         <v>93</v>
@@ -3175,7 +3175,7 @@
         <v>95</v>
       </c>
       <c r="D66" s="8" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
       <c r="F66" s="6">
         <v>3</v>
@@ -3328,10 +3328,10 @@
         <v>80</v>
       </c>
       <c r="D75" s="8" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="E75" s="13" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="F75" s="6">
         <v>2</v>
@@ -3396,7 +3396,7 @@
         <v>80</v>
       </c>
       <c r="D79" s="8" t="s">
-        <v>415</v>
+        <v>414</v>
       </c>
       <c r="E79" s="9" t="s">
         <v>87</v>
@@ -3472,7 +3472,7 @@
         <v>13</v>
       </c>
       <c r="D84" s="8" t="s">
-        <v>397</v>
+        <v>396</v>
       </c>
       <c r="E84" s="9" t="s">
         <v>276</v>
@@ -3492,7 +3492,7 @@
         <v>80</v>
       </c>
       <c r="D85" s="8" t="s">
-        <v>397</v>
+        <v>396</v>
       </c>
       <c r="E85" s="9" t="s">
         <v>8</v>
@@ -3515,7 +3515,7 @@
         <v>13</v>
       </c>
       <c r="D86" s="8" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="E86" s="9" t="s">
         <v>109</v>
@@ -3524,7 +3524,7 @@
         <v>2</v>
       </c>
       <c r="G86" s="3" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
     </row>
     <row r="87" spans="1:7" ht="17.149999999999999" x14ac:dyDescent="0.55000000000000004">
@@ -3538,7 +3538,7 @@
         <v>80</v>
       </c>
       <c r="D87" s="8" t="s">
-        <v>399</v>
+        <v>398</v>
       </c>
       <c r="F87" s="6">
         <v>2</v>
@@ -3558,7 +3558,7 @@
         <v>42</v>
       </c>
       <c r="D88" s="8" t="s">
-        <v>397</v>
+        <v>396</v>
       </c>
       <c r="E88" s="9" t="s">
         <v>272</v>
@@ -3589,7 +3589,7 @@
         <v>13</v>
       </c>
       <c r="D90" s="8" t="s">
-        <v>399</v>
+        <v>398</v>
       </c>
       <c r="F90" s="6">
         <v>2</v>
@@ -3600,13 +3600,13 @@
         <v>281</v>
       </c>
       <c r="B91" s="6" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="C91" s="7" t="s">
         <v>13</v>
       </c>
       <c r="D91" s="8" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="F91" s="6">
         <v>2</v>
@@ -3623,7 +3623,7 @@
         <v>95</v>
       </c>
       <c r="D92" s="8" t="s">
-        <v>390</v>
+        <v>389</v>
       </c>
       <c r="E92" s="12" t="s">
         <v>242</v>
@@ -3632,21 +3632,21 @@
         <v>2</v>
       </c>
       <c r="G92" s="3" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
     </row>
     <row r="93" spans="1:7" ht="17.149999999999999" x14ac:dyDescent="0.55000000000000004">
       <c r="A93" s="10" t="s">
+        <v>348</v>
+      </c>
+      <c r="B93" s="6" t="s">
         <v>349</v>
-      </c>
-      <c r="B93" s="6" t="s">
-        <v>350</v>
       </c>
       <c r="C93" s="7" t="s">
         <v>13</v>
       </c>
       <c r="D93" s="8" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
       <c r="E93" s="9" t="s">
         <v>14</v>
@@ -3663,7 +3663,7 @@
         <v>80</v>
       </c>
       <c r="D94" s="8" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
       <c r="E94" s="9" t="s">
         <v>22</v>
@@ -3683,7 +3683,7 @@
         <v>13</v>
       </c>
       <c r="D95" s="8" t="s">
-        <v>397</v>
+        <v>396</v>
       </c>
       <c r="F95" s="6">
         <v>2</v>
@@ -3700,7 +3700,7 @@
         <v>42</v>
       </c>
       <c r="D96" s="8" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
       <c r="F96" s="6">
         <v>2</v>
@@ -3722,16 +3722,16 @@
     </row>
     <row r="98" spans="1:7" ht="17.149999999999999" x14ac:dyDescent="0.55000000000000004">
       <c r="A98" s="10" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="B98" s="6" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
       <c r="C98" s="7" t="s">
         <v>13</v>
       </c>
       <c r="D98" s="8" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="E98" s="9" t="s">
         <v>14</v>
@@ -3768,7 +3768,7 @@
         <v>80</v>
       </c>
       <c r="D100" s="8" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
       <c r="F100" s="6">
         <v>2</v>
@@ -3785,7 +3785,7 @@
         <v>80</v>
       </c>
       <c r="D101" s="8" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
       <c r="E101" s="9" t="s">
         <v>93</v>
@@ -3805,13 +3805,13 @@
         <v>80</v>
       </c>
       <c r="D102" s="8" t="s">
-        <v>390</v>
+        <v>389</v>
       </c>
       <c r="E102" s="9" t="s">
         <v>98</v>
       </c>
       <c r="G102" s="3" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
     </row>
     <row r="103" spans="1:7" ht="17.149999999999999" x14ac:dyDescent="0.55000000000000004">
@@ -3825,13 +3825,13 @@
         <v>13</v>
       </c>
       <c r="D103" s="8" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="F103" s="6">
         <v>2</v>
       </c>
       <c r="G103" s="3" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
     </row>
     <row r="104" spans="1:7" ht="17.149999999999999" x14ac:dyDescent="0.55000000000000004">
@@ -3845,10 +3845,10 @@
         <v>80</v>
       </c>
       <c r="D104" s="8" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="E104" s="9" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="F104" s="6">
         <v>3</v>
@@ -3868,7 +3868,7 @@
         <v>80</v>
       </c>
       <c r="D105" s="8" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="E105" s="9" t="s">
         <v>98</v>
@@ -3885,19 +3885,19 @@
         <v>219</v>
       </c>
       <c r="B106" s="6" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
       <c r="C106" s="7" t="s">
         <v>13</v>
       </c>
       <c r="D106" s="8" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
       <c r="F106" s="6">
         <v>2</v>
       </c>
       <c r="G106" s="3" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
     </row>
     <row r="107" spans="1:7" ht="17.149999999999999" x14ac:dyDescent="0.55000000000000004">
@@ -3911,7 +3911,7 @@
         <v>95</v>
       </c>
       <c r="D107" s="8" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="E107" s="9" t="s">
         <v>110</v>
@@ -3920,7 +3920,7 @@
         <v>3</v>
       </c>
       <c r="G107" s="3" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
     </row>
     <row r="108" spans="1:7" ht="17.149999999999999" x14ac:dyDescent="0.55000000000000004">
@@ -3954,7 +3954,7 @@
         <v>13</v>
       </c>
       <c r="D109" s="8" t="s">
-        <v>397</v>
+        <v>396</v>
       </c>
       <c r="F109" s="6">
         <v>2</v>
@@ -3971,7 +3971,7 @@
         <v>13</v>
       </c>
       <c r="D110" s="8" t="s">
-        <v>385</v>
+        <v>384</v>
       </c>
       <c r="E110" s="9" t="s">
         <v>128</v>
@@ -4005,16 +4005,16 @@
     </row>
     <row r="112" spans="1:7" ht="17.149999999999999" x14ac:dyDescent="0.55000000000000004">
       <c r="A112" s="10" t="s">
+        <v>319</v>
+      </c>
+      <c r="B112" s="6" t="s">
         <v>320</v>
-      </c>
-      <c r="B112" s="6" t="s">
-        <v>321</v>
       </c>
       <c r="C112" s="7" t="s">
         <v>80</v>
       </c>
       <c r="D112" s="8" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="E112" s="9" t="s">
         <v>14</v>
@@ -4048,27 +4048,27 @@
         <v>80</v>
       </c>
       <c r="D114" s="8" t="s">
-        <v>414</v>
+        <v>413</v>
       </c>
       <c r="F114" s="6">
         <v>4</v>
       </c>
       <c r="G114" s="3" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
     </row>
     <row r="115" spans="1:7" ht="17.149999999999999" x14ac:dyDescent="0.55000000000000004">
       <c r="A115" s="10" t="s">
+        <v>317</v>
+      </c>
+      <c r="B115" s="6" t="s">
         <v>318</v>
-      </c>
-      <c r="B115" s="6" t="s">
-        <v>319</v>
       </c>
       <c r="C115" s="7" t="s">
         <v>80</v>
       </c>
       <c r="D115" s="8" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="E115" s="9" t="s">
         <v>14</v>
@@ -4085,7 +4085,7 @@
         <v>95</v>
       </c>
       <c r="D116" s="8" t="s">
-        <v>414</v>
+        <v>413</v>
       </c>
       <c r="E116" s="9" t="s">
         <v>22</v>
@@ -4094,7 +4094,7 @@
         <v>3</v>
       </c>
       <c r="G116" s="3" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
     </row>
     <row r="117" spans="1:7" ht="17.149999999999999" x14ac:dyDescent="0.55000000000000004">
@@ -4108,7 +4108,7 @@
         <v>80</v>
       </c>
       <c r="D117" s="8" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
       <c r="E117" s="9" t="s">
         <v>14</v>
@@ -4136,16 +4136,16 @@
     </row>
     <row r="119" spans="1:7" ht="17.149999999999999" x14ac:dyDescent="0.55000000000000004">
       <c r="A119" s="10" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="B119" s="6" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="C119" s="7" t="s">
         <v>13</v>
       </c>
       <c r="D119" s="8" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
     </row>
     <row r="120" spans="1:7" ht="17.149999999999999" x14ac:dyDescent="0.55000000000000004">
@@ -4153,13 +4153,13 @@
         <v>127</v>
       </c>
       <c r="B120" s="6" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
       <c r="C120" s="7" t="s">
         <v>42</v>
       </c>
       <c r="D120" s="8" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="E120" s="9" t="s">
         <v>128</v>
@@ -4173,13 +4173,13 @@
         <v>184</v>
       </c>
       <c r="B121" s="6" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
       <c r="C121" s="7" t="s">
         <v>42</v>
       </c>
       <c r="D121" s="8" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="E121" s="10" t="s">
         <v>185</v>
@@ -4188,7 +4188,7 @@
         <v>2</v>
       </c>
       <c r="G121" s="3" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
     </row>
     <row r="122" spans="1:7" ht="17.149999999999999" x14ac:dyDescent="0.55000000000000004">
@@ -4199,7 +4199,7 @@
         <v>13</v>
       </c>
       <c r="D122" s="8" t="s">
-        <v>368</v>
+        <v>367</v>
       </c>
       <c r="F122" s="6">
         <v>2</v>
@@ -4216,7 +4216,7 @@
         <v>42</v>
       </c>
       <c r="D123" s="8" t="s">
-        <v>397</v>
+        <v>396</v>
       </c>
       <c r="F123" s="6">
         <v>2</v>
@@ -4233,7 +4233,7 @@
         <v>80</v>
       </c>
       <c r="D124" s="8" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="E124" s="9" t="s">
         <v>131</v>
@@ -4253,7 +4253,7 @@
         <v>95</v>
       </c>
       <c r="D125" s="8" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="E125" s="9" t="s">
         <v>118</v>
@@ -4273,7 +4273,7 @@
         <v>13</v>
       </c>
       <c r="D126" s="8" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
       <c r="E126" s="9" t="s">
         <v>14</v>
@@ -4293,7 +4293,7 @@
         <v>13</v>
       </c>
       <c r="D127" s="8" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
       <c r="F127" s="6">
         <v>2</v>
@@ -4330,7 +4330,7 @@
         <v>42</v>
       </c>
       <c r="D129" s="8" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="F129" s="6">
         <v>2</v>
@@ -4375,7 +4375,7 @@
         <v>80</v>
       </c>
       <c r="D132" s="8" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
       <c r="E132" s="9" t="s">
         <v>14</v>
@@ -4384,7 +4384,7 @@
         <v>2</v>
       </c>
       <c r="G132" s="3" t="s">
-        <v>403</v>
+        <v>402</v>
       </c>
     </row>
     <row r="133" spans="1:7" ht="17.149999999999999" x14ac:dyDescent="0.55000000000000004">
@@ -4392,13 +4392,13 @@
         <v>181</v>
       </c>
       <c r="B133" s="6" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="C133" s="7" t="s">
         <v>42</v>
       </c>
       <c r="D133" s="8" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="E133" s="9" t="s">
         <v>183</v>
@@ -4438,7 +4438,7 @@
         <v>80</v>
       </c>
       <c r="D135" s="8" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
       <c r="E135" s="9" t="s">
         <v>251</v>
@@ -4461,7 +4461,7 @@
         <v>42</v>
       </c>
       <c r="D136" s="8" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
       <c r="F136" s="6">
         <v>2</v>
@@ -4478,7 +4478,7 @@
         <v>6</v>
       </c>
       <c r="D137" s="8" t="s">
-        <v>397</v>
+        <v>396</v>
       </c>
       <c r="F137" s="6">
         <v>2</v>
@@ -4495,7 +4495,7 @@
         <v>80</v>
       </c>
       <c r="D138" s="8" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
       <c r="E138" s="9" t="s">
         <v>122</v>
@@ -4515,7 +4515,7 @@
         <v>13</v>
       </c>
       <c r="D139" s="8" t="s">
-        <v>398</v>
+        <v>397</v>
       </c>
       <c r="E139" s="9" t="s">
         <v>22</v>
@@ -4532,7 +4532,7 @@
         <v>13</v>
       </c>
       <c r="D140" s="8" t="s">
-        <v>397</v>
+        <v>396</v>
       </c>
       <c r="E140" s="9" t="s">
         <v>47</v>
@@ -4552,7 +4552,7 @@
         <v>42</v>
       </c>
       <c r="D141" s="8" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
       <c r="E141" s="9" t="s">
         <v>93</v>
@@ -4606,7 +4606,7 @@
         <v>80</v>
       </c>
       <c r="D144" s="8" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
       <c r="E144" s="9" t="s">
         <v>128</v>
@@ -4615,7 +4615,7 @@
         <v>2</v>
       </c>
       <c r="G144" s="3" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
     </row>
     <row r="145" spans="1:7" ht="17.149999999999999" x14ac:dyDescent="0.55000000000000004">
@@ -4626,7 +4626,7 @@
         <v>13</v>
       </c>
       <c r="D145" s="8" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
       <c r="F145" s="6">
         <v>2</v>
@@ -4651,7 +4651,7 @@
         <v>42</v>
       </c>
       <c r="D147" s="8" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
       <c r="F147" s="6">
         <v>2</v>
@@ -4662,83 +4662,83 @@
         <v>224</v>
       </c>
       <c r="B148" s="6" t="s">
-        <v>383</v>
+        <v>382</v>
       </c>
       <c r="C148" s="7" t="s">
         <v>13</v>
       </c>
       <c r="D148" s="8" t="s">
-        <v>382</v>
+        <v>381</v>
       </c>
       <c r="F148" s="6">
         <v>2</v>
       </c>
       <c r="G148" s="3" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
     </row>
     <row r="149" spans="1:7" ht="17.149999999999999" x14ac:dyDescent="0.55000000000000004">
       <c r="A149" s="10" t="s">
-        <v>404</v>
+        <v>403</v>
       </c>
       <c r="C149" s="7" t="s">
         <v>42</v>
       </c>
       <c r="D149" s="8" t="s">
-        <v>405</v>
+        <v>404</v>
       </c>
     </row>
     <row r="150" spans="1:7" ht="17.149999999999999" x14ac:dyDescent="0.55000000000000004">
       <c r="A150" s="10" t="s">
-        <v>407</v>
+        <v>406</v>
       </c>
       <c r="C150" s="7" t="s">
         <v>13</v>
       </c>
       <c r="D150" s="8" t="s">
+        <v>404</v>
+      </c>
+      <c r="G150" s="3" t="s">
         <v>405</v>
-      </c>
-      <c r="G150" s="3" t="s">
-        <v>406</v>
       </c>
     </row>
     <row r="151" spans="1:7" ht="17.149999999999999" x14ac:dyDescent="0.55000000000000004">
       <c r="A151" s="10" t="s">
-        <v>408</v>
+        <v>407</v>
       </c>
       <c r="C151" s="7" t="s">
         <v>13</v>
       </c>
       <c r="D151" s="8" t="s">
-        <v>405</v>
+        <v>404</v>
       </c>
     </row>
     <row r="152" spans="1:7" ht="17.149999999999999" x14ac:dyDescent="0.55000000000000004">
       <c r="A152" s="10" t="s">
-        <v>409</v>
+        <v>408</v>
       </c>
       <c r="C152" s="7" t="s">
         <v>42</v>
       </c>
       <c r="D152" s="8" t="s">
-        <v>405</v>
+        <v>404</v>
       </c>
       <c r="E152" s="9" t="s">
+        <v>409</v>
+      </c>
+      <c r="G152" s="3" t="s">
         <v>410</v>
-      </c>
-      <c r="G152" s="3" t="s">
-        <v>411</v>
       </c>
     </row>
     <row r="153" spans="1:7" ht="17.149999999999999" x14ac:dyDescent="0.55000000000000004">
       <c r="A153" s="10" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
       <c r="C153" s="7" t="s">
         <v>42</v>
       </c>
       <c r="D153" s="8" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
2024.12.08 LeetCodeHot100 三刷 新增卡码笔记
</commit_message>
<xml_diff>
--- a/2024LeetCode刷题记录.xlsx
+++ b/2024LeetCode刷题记录.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28129"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28227"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\develop\GithubRepo\LeetCode\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8F31EB61-FF9D-4AD3-8037-B3977B626888}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A1E94D92-362C-4CB4-97A1-9021AC26D34C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-30828" yWindow="-108" windowWidth="30936" windowHeight="16776" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="715" uniqueCount="419">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="719" uniqueCount="420">
   <si>
     <t>题目</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -1303,18 +1303,10 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>2024.09.30</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>二叉树</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>2024.10.08</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>2024.10.15</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -1547,6 +1539,18 @@
   </si>
   <si>
     <t>2024.12.07</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>2024.12.08</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>递归</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>res全局变量</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -1724,7 +1728,7 @@
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{E5AA65A4-B8FD-4A83-87AF-D7798D621280}" name="表1" displayName="表1" ref="A1:G1048574" totalsRowShown="0" headerRowDxfId="8" dataDxfId="7">
   <autoFilter ref="A1:G1048574" xr:uid="{E5AA65A4-B8FD-4A83-87AF-D7798D621280}"/>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:G150">
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:G153">
     <sortCondition ref="A1:A1048574"/>
   </sortState>
   <tableColumns count="7">
@@ -2005,8 +2009,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G153"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="F27" sqref="F27"/>
+    <sheetView tabSelected="1" topLeftCell="A112" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="G126" sqref="G126"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="14.15" x14ac:dyDescent="0.35"/>
@@ -2055,7 +2059,7 @@
         <v>80</v>
       </c>
       <c r="D2" s="8" t="s">
-        <v>404</v>
+        <v>402</v>
       </c>
       <c r="F2" s="6">
         <v>3</v>
@@ -2069,13 +2073,16 @@
         <v>209</v>
       </c>
       <c r="C3" s="7" t="s">
-        <v>13</v>
+        <v>42</v>
       </c>
       <c r="D3" s="8" t="s">
-        <v>358</v>
+        <v>417</v>
       </c>
       <c r="F3" s="6">
-        <v>2</v>
+        <v>3</v>
+      </c>
+      <c r="G3" s="14" t="s">
+        <v>418</v>
       </c>
     </row>
     <row r="4" spans="1:7" ht="17.149999999999999" x14ac:dyDescent="0.55000000000000004">
@@ -2086,7 +2093,7 @@
         <v>13</v>
       </c>
       <c r="D4" s="8" t="s">
-        <v>360</v>
+        <v>358</v>
       </c>
       <c r="F4" s="6">
         <v>2</v>
@@ -2097,16 +2104,19 @@
         <v>207</v>
       </c>
       <c r="B5" s="6" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
       <c r="C5" s="7" t="s">
-        <v>13</v>
+        <v>42</v>
       </c>
       <c r="D5" s="8" t="s">
-        <v>356</v>
+        <v>417</v>
       </c>
       <c r="F5" s="6">
-        <v>2</v>
+        <v>3</v>
+      </c>
+      <c r="G5" s="14" t="s">
+        <v>418</v>
       </c>
     </row>
     <row r="6" spans="1:7" ht="17.149999999999999" x14ac:dyDescent="0.55000000000000004">
@@ -2148,184 +2158,181 @@
     </row>
     <row r="8" spans="1:7" ht="17.149999999999999" x14ac:dyDescent="0.55000000000000004">
       <c r="A8" s="10" t="s">
-        <v>212</v>
+        <v>396</v>
       </c>
       <c r="C8" s="7" t="s">
-        <v>42</v>
+        <v>13</v>
       </c>
       <c r="D8" s="8" t="s">
-        <v>359</v>
-      </c>
-      <c r="F8" s="6">
-        <v>2</v>
+        <v>393</v>
       </c>
     </row>
     <row r="9" spans="1:7" ht="17.149999999999999" x14ac:dyDescent="0.55000000000000004">
       <c r="A9" s="10" t="s">
-        <v>91</v>
-      </c>
-      <c r="B9" s="6" t="s">
-        <v>148</v>
+        <v>212</v>
       </c>
       <c r="C9" s="7" t="s">
         <v>42</v>
       </c>
       <c r="D9" s="8" t="s">
-        <v>406</v>
-      </c>
-      <c r="E9" s="9" t="s">
-        <v>93</v>
+        <v>357</v>
       </c>
       <c r="F9" s="6">
-        <v>4</v>
-      </c>
-      <c r="G9" s="14" t="s">
-        <v>305</v>
+        <v>2</v>
       </c>
     </row>
     <row r="10" spans="1:7" ht="17.149999999999999" x14ac:dyDescent="0.55000000000000004">
       <c r="A10" s="10" t="s">
-        <v>216</v>
+        <v>91</v>
+      </c>
+      <c r="B10" s="6" t="s">
+        <v>148</v>
       </c>
       <c r="C10" s="7" t="s">
         <v>42</v>
       </c>
       <c r="D10" s="8" t="s">
-        <v>362</v>
+        <v>404</v>
+      </c>
+      <c r="E10" s="9" t="s">
+        <v>93</v>
       </c>
       <c r="F10" s="6">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="G10" s="14" t="s">
-        <v>364</v>
+        <v>305</v>
       </c>
     </row>
     <row r="11" spans="1:7" ht="17.149999999999999" x14ac:dyDescent="0.55000000000000004">
       <c r="A11" s="10" t="s">
+        <v>216</v>
+      </c>
+      <c r="C11" s="7" t="s">
+        <v>42</v>
+      </c>
+      <c r="D11" s="8" t="s">
+        <v>360</v>
+      </c>
+      <c r="F11" s="6">
+        <v>2</v>
+      </c>
+      <c r="G11" s="14" t="s">
+        <v>362</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" ht="17.149999999999999" x14ac:dyDescent="0.55000000000000004">
+      <c r="A12" s="10" t="s">
         <v>290</v>
       </c>
-      <c r="B11" s="6" t="s">
+      <c r="B12" s="6" t="s">
         <v>130</v>
       </c>
-      <c r="C11" s="7" t="s">
+      <c r="C12" s="7" t="s">
         <v>95</v>
       </c>
-      <c r="D11" s="8" t="s">
+      <c r="D12" s="8" t="s">
+        <v>388</v>
+      </c>
+      <c r="E12" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="F12" s="6">
+        <v>2</v>
+      </c>
+      <c r="G12" s="14" t="s">
         <v>390</v>
       </c>
-      <c r="E11" s="9" t="s">
-        <v>14</v>
-      </c>
-      <c r="F11" s="6">
-        <v>2</v>
-      </c>
-      <c r="G11" s="14" t="s">
-        <v>392</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7" ht="17.149999999999999" x14ac:dyDescent="0.55000000000000004">
-      <c r="A12" s="4" t="s">
+    </row>
+    <row r="13" spans="1:7" ht="17.149999999999999" x14ac:dyDescent="0.55000000000000004">
+      <c r="A13" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="B12" s="6" t="s">
+      <c r="B13" s="6" t="s">
         <v>20</v>
-      </c>
-      <c r="C12" s="7" t="s">
-        <v>6</v>
-      </c>
-      <c r="D12" s="8" t="s">
-        <v>21</v>
-      </c>
-      <c r="E12" s="9" t="s">
-        <v>22</v>
-      </c>
-      <c r="G12" s="14" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7" ht="17.149999999999999" x14ac:dyDescent="0.55000000000000004">
-      <c r="A13" s="10" t="s">
-        <v>277</v>
-      </c>
-      <c r="B13" s="6" t="s">
-        <v>187</v>
       </c>
       <c r="C13" s="7" t="s">
         <v>6</v>
       </c>
       <c r="D13" s="8" t="s">
-        <v>389</v>
-      </c>
-      <c r="F13" s="6">
-        <v>2</v>
+        <v>21</v>
+      </c>
+      <c r="E13" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="G13" s="14" t="s">
+        <v>23</v>
       </c>
     </row>
     <row r="14" spans="1:7" ht="17.149999999999999" x14ac:dyDescent="0.55000000000000004">
-      <c r="A14" s="4" t="s">
-        <v>4</v>
+      <c r="A14" s="10" t="s">
+        <v>277</v>
       </c>
       <c r="B14" s="6" t="s">
-        <v>9</v>
+        <v>187</v>
       </c>
       <c r="C14" s="7" t="s">
         <v>6</v>
       </c>
       <c r="D14" s="8" t="s">
+        <v>387</v>
+      </c>
+      <c r="F14" s="6">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" ht="17.149999999999999" x14ac:dyDescent="0.55000000000000004">
+      <c r="A15" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="B15" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="C15" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="D15" s="8" t="s">
         <v>5</v>
       </c>
-      <c r="E14" s="9" t="s">
+      <c r="E15" s="9" t="s">
         <v>8</v>
       </c>
-      <c r="G14" s="14" t="s">
+      <c r="G15" s="14" t="s">
         <v>11</v>
-      </c>
-    </row>
-    <row r="15" spans="1:7" ht="17.149999999999999" x14ac:dyDescent="0.55000000000000004">
-      <c r="A15" s="10" t="s">
-        <v>259</v>
-      </c>
-      <c r="B15" s="6" t="s">
-        <v>325</v>
-      </c>
-      <c r="C15" s="7" t="s">
-        <v>42</v>
-      </c>
-      <c r="D15" s="8" t="s">
-        <v>348</v>
-      </c>
-      <c r="E15" s="9" t="s">
-        <v>14</v>
-      </c>
-      <c r="F15" s="6">
-        <v>2</v>
       </c>
     </row>
     <row r="16" spans="1:7" ht="17.149999999999999" x14ac:dyDescent="0.55000000000000004">
       <c r="A16" s="10" t="s">
-        <v>351</v>
+        <v>259</v>
       </c>
       <c r="B16" s="6" t="s">
-        <v>353</v>
+        <v>325</v>
       </c>
       <c r="C16" s="7" t="s">
-        <v>13</v>
+        <v>42</v>
       </c>
       <c r="D16" s="8" t="s">
-        <v>352</v>
+        <v>348</v>
       </c>
       <c r="E16" s="9" t="s">
         <v>14</v>
       </c>
+      <c r="F16" s="6">
+        <v>2</v>
+      </c>
     </row>
     <row r="17" spans="1:7" ht="17.149999999999999" x14ac:dyDescent="0.55000000000000004">
       <c r="A17" s="10" t="s">
-        <v>354</v>
+        <v>351</v>
+      </c>
+      <c r="B17" s="6" t="s">
+        <v>353</v>
       </c>
       <c r="C17" s="7" t="s">
-        <v>42</v>
+        <v>13</v>
       </c>
       <c r="D17" s="8" t="s">
-        <v>355</v>
+        <v>352</v>
       </c>
       <c r="E17" s="9" t="s">
         <v>14</v>
@@ -2333,70 +2340,67 @@
     </row>
     <row r="18" spans="1:7" ht="17.149999999999999" x14ac:dyDescent="0.55000000000000004">
       <c r="A18" s="10" t="s">
-        <v>220</v>
-      </c>
-      <c r="B18" s="6" t="s">
-        <v>370</v>
+        <v>354</v>
       </c>
       <c r="C18" s="7" t="s">
-        <v>13</v>
+        <v>42</v>
       </c>
       <c r="D18" s="8" t="s">
-        <v>367</v>
-      </c>
-      <c r="F18" s="6">
-        <v>2</v>
-      </c>
-      <c r="G18" s="14" t="s">
-        <v>221</v>
+        <v>355</v>
+      </c>
+      <c r="E18" s="9" t="s">
+        <v>14</v>
       </c>
     </row>
     <row r="19" spans="1:7" ht="17.149999999999999" x14ac:dyDescent="0.55000000000000004">
       <c r="A19" s="10" t="s">
-        <v>302</v>
+        <v>220</v>
       </c>
       <c r="B19" s="6" t="s">
-        <v>79</v>
+        <v>368</v>
       </c>
       <c r="C19" s="7" t="s">
-        <v>80</v>
+        <v>13</v>
       </c>
       <c r="D19" s="8" t="s">
-        <v>404</v>
+        <v>365</v>
       </c>
       <c r="F19" s="6">
-        <v>3</v>
+        <v>2</v>
+      </c>
+      <c r="G19" s="14" t="s">
+        <v>221</v>
       </c>
     </row>
     <row r="20" spans="1:7" ht="17.149999999999999" x14ac:dyDescent="0.55000000000000004">
       <c r="A20" s="10" t="s">
-        <v>235</v>
+        <v>302</v>
       </c>
       <c r="B20" s="6" t="s">
-        <v>230</v>
+        <v>79</v>
       </c>
       <c r="C20" s="7" t="s">
-        <v>13</v>
+        <v>80</v>
       </c>
       <c r="D20" s="8" t="s">
-        <v>377</v>
+        <v>402</v>
       </c>
       <c r="F20" s="6">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="21" spans="1:7" ht="17.149999999999999" x14ac:dyDescent="0.55000000000000004">
       <c r="A21" s="10" t="s">
-        <v>265</v>
+        <v>235</v>
       </c>
       <c r="B21" s="6" t="s">
-        <v>264</v>
+        <v>230</v>
       </c>
       <c r="C21" s="7" t="s">
-        <v>28</v>
+        <v>13</v>
       </c>
       <c r="D21" s="8" t="s">
-        <v>387</v>
+        <v>375</v>
       </c>
       <c r="F21" s="6">
         <v>2</v>
@@ -2404,210 +2408,204 @@
     </row>
     <row r="22" spans="1:7" ht="17.149999999999999" x14ac:dyDescent="0.55000000000000004">
       <c r="A22" s="10" t="s">
-        <v>200</v>
+        <v>265</v>
       </c>
       <c r="B22" s="6" t="s">
-        <v>49</v>
+        <v>264</v>
       </c>
       <c r="C22" s="7" t="s">
-        <v>13</v>
+        <v>28</v>
       </c>
       <c r="D22" s="8" t="s">
-        <v>414</v>
-      </c>
-      <c r="E22" s="9" t="s">
-        <v>87</v>
+        <v>385</v>
       </c>
       <c r="F22" s="6">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="23" spans="1:7" ht="17.149999999999999" x14ac:dyDescent="0.55000000000000004">
       <c r="A23" s="10" t="s">
-        <v>281</v>
+        <v>200</v>
       </c>
       <c r="B23" s="6" t="s">
-        <v>130</v>
+        <v>49</v>
       </c>
       <c r="C23" s="7" t="s">
         <v>13</v>
       </c>
       <c r="D23" s="8" t="s">
-        <v>330</v>
+        <v>412</v>
       </c>
       <c r="E23" s="9" t="s">
-        <v>14</v>
+        <v>87</v>
       </c>
       <c r="F23" s="6">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="24" spans="1:7" ht="17.149999999999999" x14ac:dyDescent="0.55000000000000004">
       <c r="A24" s="10" t="s">
-        <v>194</v>
+        <v>281</v>
       </c>
       <c r="B24" s="6" t="s">
-        <v>345</v>
+        <v>130</v>
       </c>
       <c r="C24" s="7" t="s">
-        <v>42</v>
+        <v>13</v>
       </c>
       <c r="D24" s="8" t="s">
-        <v>412</v>
+        <v>330</v>
+      </c>
+      <c r="E24" s="9" t="s">
+        <v>14</v>
       </c>
       <c r="F24" s="6">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="25" spans="1:7" ht="17.149999999999999" x14ac:dyDescent="0.55000000000000004">
       <c r="A25" s="10" t="s">
-        <v>195</v>
+        <v>194</v>
+      </c>
+      <c r="B25" s="6" t="s">
+        <v>345</v>
       </c>
       <c r="C25" s="7" t="s">
-        <v>13</v>
+        <v>42</v>
       </c>
       <c r="D25" s="8" t="s">
-        <v>412</v>
-      </c>
-      <c r="E25" s="13" t="s">
-        <v>346</v>
+        <v>410</v>
       </c>
       <c r="F25" s="6">
         <v>3</v>
       </c>
-      <c r="G25" s="14" t="s">
-        <v>413</v>
-      </c>
     </row>
     <row r="26" spans="1:7" ht="17.149999999999999" x14ac:dyDescent="0.55000000000000004">
       <c r="A26" s="10" t="s">
-        <v>299</v>
-      </c>
-      <c r="B26" s="6" t="s">
-        <v>300</v>
+        <v>195</v>
       </c>
       <c r="C26" s="7" t="s">
-        <v>42</v>
+        <v>13</v>
       </c>
       <c r="D26" s="8" t="s">
-        <v>301</v>
+        <v>410</v>
+      </c>
+      <c r="E26" s="13" t="s">
+        <v>346</v>
       </c>
       <c r="F26" s="6">
-        <v>2</v>
+        <v>3</v>
+      </c>
+      <c r="G26" s="14" t="s">
+        <v>411</v>
       </c>
     </row>
     <row r="27" spans="1:7" ht="17.149999999999999" x14ac:dyDescent="0.55000000000000004">
       <c r="A27" s="10" t="s">
-        <v>204</v>
+        <v>397</v>
       </c>
       <c r="C27" s="7" t="s">
-        <v>95</v>
+        <v>42</v>
       </c>
       <c r="D27" s="8" t="s">
-        <v>418</v>
-      </c>
-      <c r="F27" s="6">
-        <v>3</v>
+        <v>393</v>
+      </c>
+      <c r="E27" s="9" t="s">
+        <v>398</v>
       </c>
       <c r="G27" s="14" t="s">
-        <v>205</v>
+        <v>399</v>
       </c>
     </row>
     <row r="28" spans="1:7" ht="17.149999999999999" x14ac:dyDescent="0.55000000000000004">
       <c r="A28" s="10" t="s">
-        <v>201</v>
+        <v>299</v>
       </c>
       <c r="B28" s="6" t="s">
-        <v>202</v>
+        <v>300</v>
       </c>
       <c r="C28" s="7" t="s">
-        <v>80</v>
+        <v>42</v>
       </c>
       <c r="D28" s="8" t="s">
-        <v>414</v>
+        <v>301</v>
       </c>
       <c r="F28" s="6">
-        <v>3</v>
-      </c>
-      <c r="G28" s="14" t="s">
-        <v>417</v>
+        <v>2</v>
       </c>
     </row>
     <row r="29" spans="1:7" ht="17.149999999999999" x14ac:dyDescent="0.55000000000000004">
       <c r="A29" s="10" t="s">
-        <v>94</v>
-      </c>
-      <c r="B29" s="6" t="s">
-        <v>92</v>
+        <v>204</v>
       </c>
       <c r="C29" s="7" t="s">
-        <v>13</v>
+        <v>95</v>
       </c>
       <c r="D29" s="8" t="s">
-        <v>406</v>
-      </c>
-      <c r="E29" s="9" t="s">
-        <v>97</v>
+        <v>416</v>
       </c>
       <c r="F29" s="6">
         <v>3</v>
       </c>
       <c r="G29" s="14" t="s">
-        <v>306</v>
+        <v>205</v>
       </c>
     </row>
     <row r="30" spans="1:7" ht="17.149999999999999" x14ac:dyDescent="0.55000000000000004">
       <c r="A30" s="10" t="s">
-        <v>284</v>
+        <v>201</v>
       </c>
       <c r="B30" s="6" t="s">
-        <v>187</v>
+        <v>202</v>
       </c>
       <c r="C30" s="7" t="s">
-        <v>6</v>
+        <v>80</v>
       </c>
       <c r="D30" s="8" t="s">
-        <v>389</v>
+        <v>412</v>
       </c>
       <c r="F30" s="6">
-        <v>2</v>
+        <v>3</v>
+      </c>
+      <c r="G30" s="14" t="s">
+        <v>415</v>
       </c>
     </row>
     <row r="31" spans="1:7" ht="17.149999999999999" x14ac:dyDescent="0.55000000000000004">
       <c r="A31" s="10" t="s">
-        <v>243</v>
+        <v>94</v>
       </c>
       <c r="B31" s="6" t="s">
-        <v>238</v>
+        <v>92</v>
       </c>
       <c r="C31" s="7" t="s">
         <v>13</v>
       </c>
       <c r="D31" s="8" t="s">
-        <v>380</v>
+        <v>404</v>
+      </c>
+      <c r="E31" s="9" t="s">
+        <v>97</v>
       </c>
       <c r="F31" s="6">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="G31" s="14" t="s">
-        <v>382</v>
+        <v>306</v>
       </c>
     </row>
     <row r="32" spans="1:7" ht="17.149999999999999" x14ac:dyDescent="0.55000000000000004">
       <c r="A32" s="10" t="s">
-        <v>246</v>
+        <v>284</v>
       </c>
       <c r="B32" s="6" t="s">
-        <v>59</v>
+        <v>187</v>
       </c>
       <c r="C32" s="7" t="s">
-        <v>13</v>
+        <v>6</v>
       </c>
       <c r="D32" s="8" t="s">
-        <v>384</v>
-      </c>
-      <c r="E32" s="9" t="s">
-        <v>103</v>
+        <v>387</v>
       </c>
       <c r="F32" s="6">
         <v>2</v>
@@ -2615,217 +2613,220 @@
     </row>
     <row r="33" spans="1:7" ht="17.149999999999999" x14ac:dyDescent="0.55000000000000004">
       <c r="A33" s="10" t="s">
-        <v>104</v>
+        <v>243</v>
       </c>
       <c r="B33" s="6" t="s">
-        <v>106</v>
+        <v>238</v>
       </c>
       <c r="C33" s="7" t="s">
-        <v>28</v>
+        <v>13</v>
       </c>
       <c r="D33" s="8" t="s">
-        <v>101</v>
-      </c>
-      <c r="E33" s="9" t="s">
-        <v>105</v>
+        <v>378</v>
+      </c>
+      <c r="F33" s="6">
+        <v>2</v>
+      </c>
+      <c r="G33" s="14" t="s">
+        <v>380</v>
       </c>
     </row>
     <row r="34" spans="1:7" ht="17.149999999999999" x14ac:dyDescent="0.55000000000000004">
       <c r="A34" s="10" t="s">
-        <v>24</v>
+        <v>246</v>
       </c>
       <c r="B34" s="6" t="s">
-        <v>25</v>
+        <v>59</v>
       </c>
       <c r="C34" s="7" t="s">
-        <v>28</v>
+        <v>13</v>
       </c>
       <c r="D34" s="8" t="s">
-        <v>26</v>
+        <v>382</v>
       </c>
       <c r="E34" s="9" t="s">
-        <v>27</v>
+        <v>103</v>
+      </c>
+      <c r="F34" s="6">
+        <v>2</v>
       </c>
     </row>
     <row r="35" spans="1:7" ht="17.149999999999999" x14ac:dyDescent="0.55000000000000004">
       <c r="A35" s="10" t="s">
-        <v>191</v>
+        <v>104</v>
+      </c>
+      <c r="B35" s="6" t="s">
+        <v>106</v>
       </c>
       <c r="C35" s="7" t="s">
-        <v>6</v>
+        <v>28</v>
       </c>
       <c r="D35" s="8" t="s">
-        <v>412</v>
-      </c>
-      <c r="E35" s="13" t="s">
-        <v>342</v>
-      </c>
-      <c r="F35" s="6">
-        <v>3</v>
-      </c>
-      <c r="G35" s="14" t="s">
-        <v>341</v>
+        <v>101</v>
+      </c>
+      <c r="E35" s="9" t="s">
+        <v>105</v>
       </c>
     </row>
     <row r="36" spans="1:7" ht="17.149999999999999" x14ac:dyDescent="0.55000000000000004">
       <c r="A36" s="10" t="s">
-        <v>266</v>
+        <v>24</v>
       </c>
       <c r="B36" s="6" t="s">
-        <v>267</v>
+        <v>25</v>
       </c>
       <c r="C36" s="7" t="s">
-        <v>13</v>
+        <v>28</v>
       </c>
       <c r="D36" s="8" t="s">
-        <v>387</v>
-      </c>
-      <c r="F36" s="6">
-        <v>2</v>
+        <v>26</v>
+      </c>
+      <c r="E36" s="9" t="s">
+        <v>27</v>
       </c>
     </row>
     <row r="37" spans="1:7" ht="17.149999999999999" x14ac:dyDescent="0.55000000000000004">
       <c r="A37" s="10" t="s">
-        <v>229</v>
-      </c>
-      <c r="B37" s="6" t="s">
-        <v>230</v>
+        <v>191</v>
       </c>
       <c r="C37" s="7" t="s">
-        <v>80</v>
+        <v>6</v>
       </c>
       <c r="D37" s="8" t="s">
-        <v>375</v>
-      </c>
-      <c r="E37" s="9" t="s">
-        <v>22</v>
+        <v>410</v>
+      </c>
+      <c r="E37" s="13" t="s">
+        <v>342</v>
       </c>
       <c r="F37" s="6">
-        <v>2</v>
+        <v>3</v>
+      </c>
+      <c r="G37" s="14" t="s">
+        <v>341</v>
       </c>
     </row>
     <row r="38" spans="1:7" ht="17.149999999999999" x14ac:dyDescent="0.55000000000000004">
-      <c r="A38" s="4" t="s">
-        <v>177</v>
+      <c r="A38" s="10" t="s">
+        <v>400</v>
       </c>
       <c r="C38" s="7" t="s">
-        <v>28</v>
+        <v>42</v>
       </c>
       <c r="D38" s="8" t="s">
-        <v>410</v>
-      </c>
-      <c r="F38" s="6">
-        <v>3</v>
+        <v>401</v>
       </c>
     </row>
     <row r="39" spans="1:7" ht="17.149999999999999" x14ac:dyDescent="0.55000000000000004">
       <c r="A39" s="10" t="s">
-        <v>198</v>
+        <v>266</v>
+      </c>
+      <c r="B39" s="6" t="s">
+        <v>267</v>
       </c>
       <c r="C39" s="7" t="s">
         <v>13</v>
       </c>
       <c r="D39" s="8" t="s">
-        <v>414</v>
+        <v>385</v>
       </c>
       <c r="F39" s="6">
-        <v>3</v>
-      </c>
-      <c r="G39" s="14" t="s">
-        <v>349</v>
+        <v>2</v>
       </c>
     </row>
     <row r="40" spans="1:7" ht="17.149999999999999" x14ac:dyDescent="0.55000000000000004">
       <c r="A40" s="10" t="s">
-        <v>278</v>
+        <v>229</v>
       </c>
       <c r="B40" s="6" t="s">
-        <v>130</v>
+        <v>230</v>
       </c>
       <c r="C40" s="7" t="s">
         <v>80</v>
       </c>
       <c r="D40" s="8" t="s">
-        <v>335</v>
+        <v>373</v>
+      </c>
+      <c r="E40" s="9" t="s">
+        <v>22</v>
       </c>
       <c r="F40" s="6">
         <v>2</v>
       </c>
-      <c r="G40" s="14" t="s">
-        <v>336</v>
-      </c>
     </row>
     <row r="41" spans="1:7" ht="17.149999999999999" x14ac:dyDescent="0.55000000000000004">
-      <c r="A41" s="10" t="s">
-        <v>215</v>
+      <c r="A41" s="4" t="s">
+        <v>177</v>
       </c>
       <c r="C41" s="7" t="s">
-        <v>13</v>
+        <v>28</v>
       </c>
       <c r="D41" s="8" t="s">
-        <v>362</v>
+        <v>408</v>
       </c>
       <c r="F41" s="6">
-        <v>2</v>
-      </c>
-      <c r="G41" s="14" t="s">
-        <v>363</v>
+        <v>3</v>
       </c>
     </row>
     <row r="42" spans="1:7" ht="17.149999999999999" x14ac:dyDescent="0.55000000000000004">
       <c r="A42" s="10" t="s">
-        <v>197</v>
+        <v>198</v>
       </c>
       <c r="C42" s="7" t="s">
-        <v>6</v>
+        <v>13</v>
       </c>
       <c r="D42" s="8" t="s">
-        <v>414</v>
+        <v>412</v>
       </c>
       <c r="F42" s="6">
         <v>3</v>
       </c>
+      <c r="G42" s="14" t="s">
+        <v>349</v>
+      </c>
     </row>
     <row r="43" spans="1:7" ht="17.149999999999999" x14ac:dyDescent="0.55000000000000004">
       <c r="A43" s="10" t="s">
-        <v>245</v>
+        <v>278</v>
       </c>
       <c r="B43" s="6" t="s">
-        <v>59</v>
+        <v>130</v>
       </c>
       <c r="C43" s="7" t="s">
         <v>80</v>
       </c>
       <c r="D43" s="8" t="s">
-        <v>384</v>
+        <v>335</v>
       </c>
       <c r="F43" s="6">
         <v>2</v>
+      </c>
+      <c r="G43" s="14" t="s">
+        <v>336</v>
       </c>
     </row>
     <row r="44" spans="1:7" ht="17.149999999999999" x14ac:dyDescent="0.55000000000000004">
       <c r="A44" s="10" t="s">
-        <v>222</v>
+        <v>215</v>
       </c>
       <c r="C44" s="7" t="s">
         <v>13</v>
       </c>
       <c r="D44" s="8" t="s">
-        <v>371</v>
+        <v>360</v>
       </c>
       <c r="F44" s="6">
         <v>2</v>
       </c>
       <c r="G44" s="14" t="s">
-        <v>221</v>
+        <v>361</v>
       </c>
     </row>
     <row r="45" spans="1:7" ht="17.149999999999999" x14ac:dyDescent="0.55000000000000004">
       <c r="A45" s="10" t="s">
-        <v>192</v>
+        <v>197</v>
       </c>
       <c r="C45" s="7" t="s">
-        <v>80</v>
+        <v>6</v>
       </c>
       <c r="D45" s="8" t="s">
         <v>412</v>
@@ -2836,13 +2837,16 @@
     </row>
     <row r="46" spans="1:7" ht="17.149999999999999" x14ac:dyDescent="0.55000000000000004">
       <c r="A46" s="10" t="s">
-        <v>224</v>
+        <v>245</v>
+      </c>
+      <c r="B46" s="6" t="s">
+        <v>59</v>
       </c>
       <c r="C46" s="7" t="s">
         <v>80</v>
       </c>
       <c r="D46" s="8" t="s">
-        <v>372</v>
+        <v>382</v>
       </c>
       <c r="F46" s="6">
         <v>2</v>
@@ -2850,186 +2854,186 @@
     </row>
     <row r="47" spans="1:7" ht="17.149999999999999" x14ac:dyDescent="0.55000000000000004">
       <c r="A47" s="10" t="s">
-        <v>225</v>
+        <v>222</v>
       </c>
       <c r="C47" s="7" t="s">
         <v>13</v>
       </c>
       <c r="D47" s="8" t="s">
-        <v>372</v>
+        <v>369</v>
       </c>
       <c r="F47" s="6">
         <v>2</v>
+      </c>
+      <c r="G47" s="14" t="s">
+        <v>221</v>
       </c>
     </row>
     <row r="48" spans="1:7" ht="17.149999999999999" x14ac:dyDescent="0.55000000000000004">
       <c r="A48" s="10" t="s">
-        <v>67</v>
-      </c>
-      <c r="B48" s="6" t="s">
-        <v>68</v>
+        <v>192</v>
       </c>
       <c r="C48" s="7" t="s">
-        <v>28</v>
+        <v>80</v>
       </c>
       <c r="D48" s="8" t="s">
-        <v>69</v>
-      </c>
-      <c r="E48" s="9" t="s">
-        <v>70</v>
-      </c>
-      <c r="G48" s="14" t="s">
-        <v>71</v>
+        <v>410</v>
+      </c>
+      <c r="F48" s="6">
+        <v>3</v>
       </c>
     </row>
     <row r="49" spans="1:7" ht="17.149999999999999" x14ac:dyDescent="0.55000000000000004">
-      <c r="A49" s="11" t="s">
-        <v>196</v>
+      <c r="A49" s="10" t="s">
+        <v>224</v>
       </c>
       <c r="C49" s="7" t="s">
-        <v>42</v>
+        <v>80</v>
       </c>
       <c r="D49" s="8" t="s">
-        <v>414</v>
+        <v>370</v>
       </c>
       <c r="F49" s="6">
-        <v>3</v>
-      </c>
-      <c r="G49" s="14" t="s">
-        <v>347</v>
+        <v>2</v>
       </c>
     </row>
     <row r="50" spans="1:7" ht="17.149999999999999" x14ac:dyDescent="0.55000000000000004">
       <c r="A50" s="10" t="s">
-        <v>337</v>
-      </c>
-      <c r="B50" s="6" t="s">
-        <v>339</v>
+        <v>225</v>
       </c>
       <c r="C50" s="7" t="s">
         <v>13</v>
       </c>
       <c r="D50" s="8" t="s">
-        <v>338</v>
-      </c>
-      <c r="E50" s="9" t="s">
-        <v>14</v>
+        <v>370</v>
+      </c>
+      <c r="F50" s="6">
+        <v>2</v>
       </c>
     </row>
     <row r="51" spans="1:7" ht="17.149999999999999" x14ac:dyDescent="0.55000000000000004">
       <c r="A51" s="10" t="s">
-        <v>254</v>
+        <v>67</v>
       </c>
       <c r="B51" s="6" t="s">
-        <v>255</v>
+        <v>68</v>
       </c>
       <c r="C51" s="7" t="s">
-        <v>13</v>
+        <v>28</v>
       </c>
       <c r="D51" s="8" t="s">
-        <v>387</v>
-      </c>
-      <c r="F51" s="6">
+        <v>69</v>
+      </c>
+      <c r="E51" s="9" t="s">
+        <v>70</v>
+      </c>
+      <c r="G51" s="14" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="52" spans="1:7" ht="17.149999999999999" x14ac:dyDescent="0.55000000000000004">
+      <c r="A52" s="11" t="s">
+        <v>196</v>
+      </c>
+      <c r="C52" s="7" t="s">
+        <v>42</v>
+      </c>
+      <c r="D52" s="8" t="s">
+        <v>412</v>
+      </c>
+      <c r="F52" s="6">
         <v>3</v>
       </c>
-      <c r="G51" s="14" t="s">
-        <v>334</v>
-      </c>
-    </row>
-    <row r="52" spans="1:7" ht="17.149999999999999" x14ac:dyDescent="0.55000000000000004">
-      <c r="A52" s="10" t="s">
-        <v>133</v>
-      </c>
-      <c r="B52" s="6" t="s">
-        <v>135</v>
-      </c>
-      <c r="C52" s="7" t="s">
-        <v>28</v>
-      </c>
-      <c r="D52" s="8" t="s">
-        <v>136</v>
-      </c>
-      <c r="E52" s="9" t="s">
-        <v>134</v>
+      <c r="G52" s="14" t="s">
+        <v>347</v>
       </c>
     </row>
     <row r="53" spans="1:7" ht="17.149999999999999" x14ac:dyDescent="0.55000000000000004">
       <c r="A53" s="10" t="s">
-        <v>72</v>
+        <v>337</v>
       </c>
       <c r="B53" s="6" t="s">
-        <v>73</v>
+        <v>339</v>
       </c>
       <c r="C53" s="7" t="s">
-        <v>76</v>
+        <v>13</v>
       </c>
       <c r="D53" s="8" t="s">
-        <v>74</v>
+        <v>338</v>
       </c>
       <c r="E53" s="9" t="s">
-        <v>75</v>
-      </c>
-      <c r="G53" s="14" t="s">
-        <v>77</v>
+        <v>14</v>
       </c>
     </row>
     <row r="54" spans="1:7" ht="17.149999999999999" x14ac:dyDescent="0.55000000000000004">
       <c r="A54" s="10" t="s">
-        <v>234</v>
+        <v>254</v>
       </c>
       <c r="B54" s="6" t="s">
-        <v>230</v>
+        <v>255</v>
       </c>
       <c r="C54" s="7" t="s">
         <v>13</v>
       </c>
       <c r="D54" s="8" t="s">
-        <v>376</v>
+        <v>385</v>
       </c>
       <c r="F54" s="6">
-        <v>2</v>
+        <v>3</v>
+      </c>
+      <c r="G54" s="14" t="s">
+        <v>334</v>
       </c>
     </row>
     <row r="55" spans="1:7" ht="17.149999999999999" x14ac:dyDescent="0.55000000000000004">
       <c r="A55" s="10" t="s">
-        <v>208</v>
+        <v>133</v>
+      </c>
+      <c r="B55" s="6" t="s">
+        <v>135</v>
       </c>
       <c r="C55" s="7" t="s">
-        <v>13</v>
+        <v>28</v>
       </c>
       <c r="D55" s="8" t="s">
-        <v>356</v>
-      </c>
-      <c r="F55" s="6">
-        <v>2</v>
+        <v>136</v>
+      </c>
+      <c r="E55" s="9" t="s">
+        <v>134</v>
       </c>
     </row>
     <row r="56" spans="1:7" ht="17.149999999999999" x14ac:dyDescent="0.55000000000000004">
       <c r="A56" s="10" t="s">
-        <v>203</v>
+        <v>72</v>
       </c>
       <c r="B56" s="6" t="s">
-        <v>202</v>
+        <v>73</v>
       </c>
       <c r="C56" s="7" t="s">
-        <v>13</v>
+        <v>76</v>
       </c>
       <c r="D56" s="8" t="s">
-        <v>418</v>
-      </c>
-      <c r="F56" s="6">
-        <v>3</v>
+        <v>74</v>
+      </c>
+      <c r="E56" s="9" t="s">
+        <v>75</v>
+      </c>
+      <c r="G56" s="14" t="s">
+        <v>77</v>
       </c>
     </row>
     <row r="57" spans="1:7" ht="17.149999999999999" x14ac:dyDescent="0.55000000000000004">
       <c r="A57" s="10" t="s">
-        <v>214</v>
+        <v>234</v>
+      </c>
+      <c r="B57" s="6" t="s">
+        <v>230</v>
       </c>
       <c r="C57" s="7" t="s">
         <v>13</v>
       </c>
       <c r="D57" s="8" t="s">
-        <v>361</v>
+        <v>374</v>
       </c>
       <c r="F57" s="6">
         <v>2</v>
@@ -3037,559 +3041,535 @@
     </row>
     <row r="58" spans="1:7" ht="17.149999999999999" x14ac:dyDescent="0.55000000000000004">
       <c r="A58" s="10" t="s">
-        <v>193</v>
+        <v>208</v>
       </c>
       <c r="C58" s="7" t="s">
-        <v>95</v>
+        <v>13</v>
       </c>
       <c r="D58" s="8" t="s">
-        <v>412</v>
+        <v>417</v>
       </c>
       <c r="F58" s="6">
         <v>3</v>
       </c>
+      <c r="G58" s="14" t="s">
+        <v>418</v>
+      </c>
     </row>
     <row r="59" spans="1:7" ht="17.149999999999999" x14ac:dyDescent="0.55000000000000004">
       <c r="A59" s="10" t="s">
-        <v>219</v>
+        <v>203</v>
       </c>
       <c r="B59" s="6" t="s">
-        <v>368</v>
+        <v>202</v>
       </c>
       <c r="C59" s="7" t="s">
         <v>13</v>
       </c>
       <c r="D59" s="8" t="s">
-        <v>367</v>
-      </c>
-      <c r="E59" s="9" t="s">
-        <v>93</v>
+        <v>416</v>
       </c>
       <c r="F59" s="6">
-        <v>2</v>
-      </c>
-      <c r="G59" s="14" t="s">
-        <v>369</v>
+        <v>3</v>
       </c>
     </row>
     <row r="60" spans="1:7" ht="17.149999999999999" x14ac:dyDescent="0.55000000000000004">
       <c r="A60" s="10" t="s">
-        <v>178</v>
-      </c>
-      <c r="B60" s="6" t="s">
-        <v>327</v>
+        <v>214</v>
       </c>
       <c r="C60" s="7" t="s">
-        <v>6</v>
+        <v>13</v>
       </c>
       <c r="D60" s="8" t="s">
-        <v>410</v>
+        <v>359</v>
       </c>
       <c r="F60" s="6">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="61" spans="1:7" ht="17.149999999999999" x14ac:dyDescent="0.55000000000000004">
       <c r="A61" s="10" t="s">
-        <v>151</v>
-      </c>
-      <c r="B61" s="6" t="s">
-        <v>121</v>
+        <v>193</v>
       </c>
       <c r="C61" s="7" t="s">
         <v>95</v>
       </c>
       <c r="D61" s="8" t="s">
-        <v>409</v>
-      </c>
-      <c r="E61" s="9" t="s">
-        <v>118</v>
+        <v>410</v>
       </c>
       <c r="F61" s="6">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="62" spans="1:7" ht="17.149999999999999" x14ac:dyDescent="0.55000000000000004">
       <c r="A62" s="10" t="s">
-        <v>39</v>
+        <v>219</v>
       </c>
       <c r="B62" s="6" t="s">
-        <v>41</v>
+        <v>366</v>
       </c>
       <c r="C62" s="7" t="s">
-        <v>42</v>
+        <v>13</v>
       </c>
       <c r="D62" s="8" t="s">
-        <v>38</v>
+        <v>365</v>
       </c>
       <c r="E62" s="9" t="s">
-        <v>22</v>
+        <v>93</v>
+      </c>
+      <c r="F62" s="6">
+        <v>2</v>
       </c>
       <c r="G62" s="14" t="s">
-        <v>40</v>
+        <v>367</v>
       </c>
     </row>
     <row r="63" spans="1:7" ht="17.149999999999999" x14ac:dyDescent="0.55000000000000004">
       <c r="A63" s="10" t="s">
-        <v>350</v>
+        <v>178</v>
+      </c>
+      <c r="B63" s="6" t="s">
+        <v>327</v>
       </c>
       <c r="C63" s="7" t="s">
-        <v>95</v>
+        <v>6</v>
       </c>
       <c r="D63" s="8" t="s">
-        <v>414</v>
+        <v>408</v>
       </c>
       <c r="F63" s="6">
         <v>3</v>
       </c>
-      <c r="G63" s="14" t="s">
-        <v>416</v>
-      </c>
     </row>
     <row r="64" spans="1:7" ht="17.149999999999999" x14ac:dyDescent="0.55000000000000004">
       <c r="A64" s="10" t="s">
-        <v>188</v>
+        <v>151</v>
       </c>
       <c r="B64" s="6" t="s">
-        <v>190</v>
+        <v>121</v>
       </c>
       <c r="C64" s="7" t="s">
-        <v>42</v>
+        <v>95</v>
       </c>
       <c r="D64" s="8" t="s">
-        <v>411</v>
+        <v>407</v>
       </c>
       <c r="E64" s="9" t="s">
-        <v>93</v>
+        <v>118</v>
       </c>
       <c r="F64" s="6">
-        <v>3</v>
-      </c>
-      <c r="G64" s="14" t="s">
-        <v>189</v>
+        <v>4</v>
       </c>
     </row>
     <row r="65" spans="1:7" ht="17.149999999999999" x14ac:dyDescent="0.55000000000000004">
       <c r="A65" s="10" t="s">
-        <v>34</v>
+        <v>39</v>
       </c>
       <c r="B65" s="6" t="s">
-        <v>36</v>
+        <v>41</v>
       </c>
       <c r="C65" s="7" t="s">
-        <v>6</v>
+        <v>42</v>
       </c>
       <c r="D65" s="8" t="s">
-        <v>35</v>
+        <v>38</v>
       </c>
       <c r="E65" s="9" t="s">
         <v>22</v>
       </c>
       <c r="G65" s="14" t="s">
-        <v>37</v>
+        <v>40</v>
       </c>
     </row>
     <row r="66" spans="1:7" ht="17.149999999999999" x14ac:dyDescent="0.55000000000000004">
       <c r="A66" s="10" t="s">
-        <v>199</v>
-      </c>
-      <c r="B66" s="6" t="s">
-        <v>298</v>
+        <v>350</v>
       </c>
       <c r="C66" s="7" t="s">
         <v>95</v>
       </c>
       <c r="D66" s="8" t="s">
+        <v>412</v>
+      </c>
+      <c r="F66" s="6">
+        <v>3</v>
+      </c>
+      <c r="G66" s="14" t="s">
         <v>414</v>
-      </c>
-      <c r="F66" s="6">
-        <v>4</v>
-      </c>
-      <c r="G66" s="14" t="s">
-        <v>415</v>
       </c>
     </row>
     <row r="67" spans="1:7" ht="17.149999999999999" x14ac:dyDescent="0.55000000000000004">
       <c r="A67" s="10" t="s">
-        <v>62</v>
+        <v>188</v>
       </c>
       <c r="B67" s="6" t="s">
-        <v>63</v>
+        <v>190</v>
       </c>
       <c r="C67" s="7" t="s">
         <v>42</v>
       </c>
       <c r="D67" s="8" t="s">
-        <v>64</v>
+        <v>409</v>
       </c>
       <c r="E67" s="9" t="s">
-        <v>65</v>
+        <v>93</v>
+      </c>
+      <c r="F67" s="6">
+        <v>3</v>
       </c>
       <c r="G67" s="14" t="s">
-        <v>66</v>
+        <v>189</v>
       </c>
     </row>
     <row r="68" spans="1:7" ht="17.149999999999999" x14ac:dyDescent="0.55000000000000004">
       <c r="A68" s="10" t="s">
-        <v>58</v>
+        <v>34</v>
       </c>
       <c r="B68" s="6" t="s">
-        <v>59</v>
+        <v>36</v>
       </c>
       <c r="C68" s="7" t="s">
-        <v>42</v>
+        <v>6</v>
       </c>
       <c r="D68" s="8" t="s">
-        <v>60</v>
+        <v>35</v>
       </c>
       <c r="E68" s="9" t="s">
-        <v>61</v>
+        <v>22</v>
+      </c>
+      <c r="G68" s="14" t="s">
+        <v>37</v>
       </c>
     </row>
     <row r="69" spans="1:7" ht="17.149999999999999" x14ac:dyDescent="0.55000000000000004">
       <c r="A69" s="10" t="s">
-        <v>294</v>
+        <v>199</v>
+      </c>
+      <c r="B69" s="6" t="s">
+        <v>298</v>
       </c>
       <c r="C69" s="7" t="s">
-        <v>42</v>
+        <v>95</v>
       </c>
       <c r="D69" s="8" t="s">
-        <v>292</v>
+        <v>412</v>
+      </c>
+      <c r="F69" s="6">
+        <v>4</v>
+      </c>
+      <c r="G69" s="14" t="s">
+        <v>413</v>
       </c>
     </row>
     <row r="70" spans="1:7" ht="17.149999999999999" x14ac:dyDescent="0.55000000000000004">
       <c r="A70" s="10" t="s">
-        <v>55</v>
+        <v>62</v>
       </c>
       <c r="B70" s="6" t="s">
-        <v>57</v>
+        <v>63</v>
       </c>
       <c r="C70" s="7" t="s">
         <v>42</v>
       </c>
       <c r="D70" s="8" t="s">
-        <v>56</v>
+        <v>64</v>
       </c>
       <c r="E70" s="9" t="s">
-        <v>27</v>
+        <v>65</v>
+      </c>
+      <c r="G70" s="14" t="s">
+        <v>66</v>
       </c>
     </row>
     <row r="71" spans="1:7" ht="17.149999999999999" x14ac:dyDescent="0.55000000000000004">
       <c r="A71" s="10" t="s">
-        <v>115</v>
+        <v>58</v>
       </c>
       <c r="B71" s="6" t="s">
-        <v>116</v>
+        <v>59</v>
       </c>
       <c r="C71" s="7" t="s">
-        <v>6</v>
+        <v>42</v>
       </c>
       <c r="D71" s="8" t="s">
-        <v>113</v>
+        <v>60</v>
       </c>
       <c r="E71" s="9" t="s">
-        <v>114</v>
+        <v>61</v>
       </c>
     </row>
     <row r="72" spans="1:7" ht="17.149999999999999" x14ac:dyDescent="0.55000000000000004">
       <c r="A72" s="10" t="s">
-        <v>123</v>
-      </c>
-      <c r="B72" s="6" t="s">
-        <v>124</v>
+        <v>294</v>
       </c>
       <c r="C72" s="7" t="s">
-        <v>28</v>
+        <v>42</v>
       </c>
       <c r="D72" s="8" t="s">
-        <v>125</v>
-      </c>
-      <c r="E72" s="9" t="s">
-        <v>126</v>
+        <v>292</v>
       </c>
     </row>
     <row r="73" spans="1:7" ht="17.149999999999999" x14ac:dyDescent="0.55000000000000004">
       <c r="A73" s="10" t="s">
-        <v>152</v>
+        <v>55</v>
       </c>
       <c r="B73" s="6" t="s">
-        <v>153</v>
+        <v>57</v>
       </c>
       <c r="C73" s="7" t="s">
-        <v>6</v>
+        <v>42</v>
       </c>
       <c r="D73" s="8" t="s">
-        <v>154</v>
+        <v>56</v>
       </c>
       <c r="E73" s="9" t="s">
-        <v>47</v>
+        <v>27</v>
       </c>
     </row>
     <row r="74" spans="1:7" ht="17.149999999999999" x14ac:dyDescent="0.55000000000000004">
       <c r="A74" s="10" t="s">
-        <v>141</v>
+        <v>115</v>
       </c>
       <c r="B74" s="6" t="s">
-        <v>142</v>
+        <v>116</v>
       </c>
       <c r="C74" s="7" t="s">
         <v>6</v>
       </c>
       <c r="D74" s="8" t="s">
-        <v>143</v>
+        <v>113</v>
       </c>
       <c r="E74" s="9" t="s">
-        <v>145</v>
-      </c>
-      <c r="G74" s="14" t="s">
-        <v>144</v>
+        <v>114</v>
       </c>
     </row>
     <row r="75" spans="1:7" ht="17.149999999999999" x14ac:dyDescent="0.55000000000000004">
       <c r="A75" s="10" t="s">
-        <v>279</v>
+        <v>123</v>
       </c>
       <c r="B75" s="6" t="s">
-        <v>130</v>
+        <v>124</v>
       </c>
       <c r="C75" s="7" t="s">
-        <v>80</v>
+        <v>28</v>
       </c>
       <c r="D75" s="8" t="s">
-        <v>326</v>
-      </c>
-      <c r="E75" s="13" t="s">
-        <v>329</v>
-      </c>
-      <c r="F75" s="6">
-        <v>2</v>
+        <v>125</v>
+      </c>
+      <c r="E75" s="9" t="s">
+        <v>126</v>
       </c>
     </row>
     <row r="76" spans="1:7" ht="17.149999999999999" x14ac:dyDescent="0.55000000000000004">
       <c r="A76" s="10" t="s">
-        <v>43</v>
+        <v>152</v>
       </c>
       <c r="B76" s="6" t="s">
-        <v>45</v>
+        <v>153</v>
       </c>
       <c r="C76" s="7" t="s">
-        <v>42</v>
+        <v>6</v>
       </c>
       <c r="D76" s="8" t="s">
-        <v>44</v>
+        <v>154</v>
       </c>
       <c r="E76" s="9" t="s">
         <v>47</v>
       </c>
-      <c r="G76" s="14" t="s">
-        <v>46</v>
-      </c>
     </row>
     <row r="77" spans="1:7" ht="17.149999999999999" x14ac:dyDescent="0.55000000000000004">
       <c r="A77" s="10" t="s">
-        <v>175</v>
+        <v>141</v>
+      </c>
+      <c r="B77" s="6" t="s">
+        <v>142</v>
       </c>
       <c r="C77" s="7" t="s">
-        <v>28</v>
+        <v>6</v>
       </c>
       <c r="D77" s="8" t="s">
-        <v>176</v>
+        <v>143</v>
+      </c>
+      <c r="E77" s="9" t="s">
+        <v>145</v>
+      </c>
+      <c r="G77" s="14" t="s">
+        <v>144</v>
       </c>
     </row>
     <row r="78" spans="1:7" ht="17.149999999999999" x14ac:dyDescent="0.55000000000000004">
       <c r="A78" s="10" t="s">
-        <v>137</v>
+        <v>279</v>
       </c>
       <c r="B78" s="6" t="s">
-        <v>139</v>
+        <v>130</v>
       </c>
       <c r="C78" s="7" t="s">
-        <v>28</v>
+        <v>80</v>
       </c>
       <c r="D78" s="8" t="s">
-        <v>138</v>
-      </c>
-      <c r="E78" s="9" t="s">
-        <v>140</v>
+        <v>326</v>
+      </c>
+      <c r="E78" s="13" t="s">
+        <v>329</v>
+      </c>
+      <c r="F78" s="6">
+        <v>2</v>
       </c>
     </row>
     <row r="79" spans="1:7" ht="17.149999999999999" x14ac:dyDescent="0.55000000000000004">
       <c r="A79" s="10" t="s">
-        <v>303</v>
-      </c>
-      <c r="B79" s="6" t="s">
-        <v>304</v>
+        <v>395</v>
       </c>
       <c r="C79" s="7" t="s">
-        <v>80</v>
+        <v>13</v>
       </c>
       <c r="D79" s="8" t="s">
-        <v>405</v>
-      </c>
-      <c r="E79" s="9" t="s">
-        <v>87</v>
-      </c>
-      <c r="F79" s="6">
-        <v>3</v>
+        <v>393</v>
+      </c>
+      <c r="G79" s="14" t="s">
+        <v>394</v>
       </c>
     </row>
     <row r="80" spans="1:7" ht="17.149999999999999" x14ac:dyDescent="0.55000000000000004">
       <c r="A80" s="10" t="s">
-        <v>164</v>
+        <v>43</v>
+      </c>
+      <c r="B80" s="6" t="s">
+        <v>45</v>
       </c>
       <c r="C80" s="7" t="s">
-        <v>28</v>
+        <v>42</v>
       </c>
       <c r="D80" s="8" t="s">
-        <v>165</v>
+        <v>44</v>
+      </c>
+      <c r="E80" s="9" t="s">
+        <v>47</v>
+      </c>
+      <c r="G80" s="14" t="s">
+        <v>46</v>
       </c>
     </row>
     <row r="81" spans="1:7" ht="17.149999999999999" x14ac:dyDescent="0.55000000000000004">
       <c r="A81" s="10" t="s">
-        <v>160</v>
-      </c>
-      <c r="B81" s="6" t="s">
-        <v>163</v>
+        <v>175</v>
       </c>
       <c r="C81" s="7" t="s">
         <v>28</v>
       </c>
       <c r="D81" s="8" t="s">
-        <v>161</v>
-      </c>
-      <c r="G81" s="14" t="s">
-        <v>162</v>
+        <v>176</v>
       </c>
     </row>
     <row r="82" spans="1:7" ht="17.149999999999999" x14ac:dyDescent="0.55000000000000004">
       <c r="A82" s="10" t="s">
-        <v>166</v>
+        <v>137</v>
+      </c>
+      <c r="B82" s="6" t="s">
+        <v>139</v>
       </c>
       <c r="C82" s="7" t="s">
         <v>28</v>
       </c>
       <c r="D82" s="8" t="s">
-        <v>167</v>
+        <v>138</v>
+      </c>
+      <c r="E82" s="9" t="s">
+        <v>140</v>
       </c>
     </row>
     <row r="83" spans="1:7" ht="17.149999999999999" x14ac:dyDescent="0.55000000000000004">
       <c r="A83" s="10" t="s">
-        <v>156</v>
+        <v>303</v>
       </c>
       <c r="B83" s="6" t="s">
-        <v>159</v>
+        <v>304</v>
       </c>
       <c r="C83" s="7" t="s">
-        <v>13</v>
+        <v>80</v>
       </c>
       <c r="D83" s="8" t="s">
-        <v>157</v>
+        <v>403</v>
       </c>
       <c r="E83" s="9" t="s">
-        <v>158</v>
+        <v>87</v>
+      </c>
+      <c r="F83" s="6">
+        <v>3</v>
       </c>
     </row>
     <row r="84" spans="1:7" ht="17.149999999999999" x14ac:dyDescent="0.55000000000000004">
       <c r="A84" s="10" t="s">
-        <v>273</v>
-      </c>
-      <c r="B84" s="6" t="s">
-        <v>274</v>
+        <v>164</v>
       </c>
       <c r="C84" s="7" t="s">
-        <v>13</v>
+        <v>28</v>
       </c>
       <c r="D84" s="8" t="s">
-        <v>387</v>
-      </c>
-      <c r="E84" s="9" t="s">
-        <v>275</v>
-      </c>
-      <c r="F84" s="6">
-        <v>2</v>
+        <v>165</v>
       </c>
     </row>
     <row r="85" spans="1:7" ht="17.149999999999999" x14ac:dyDescent="0.55000000000000004">
       <c r="A85" s="10" t="s">
-        <v>257</v>
+        <v>160</v>
       </c>
       <c r="B85" s="6" t="s">
-        <v>256</v>
+        <v>163</v>
       </c>
       <c r="C85" s="7" t="s">
-        <v>80</v>
+        <v>28</v>
       </c>
       <c r="D85" s="8" t="s">
-        <v>387</v>
-      </c>
-      <c r="E85" s="9" t="s">
-        <v>8</v>
-      </c>
-      <c r="F85" s="6">
-        <v>2</v>
+        <v>161</v>
       </c>
       <c r="G85" s="14" t="s">
-        <v>260</v>
+        <v>162</v>
       </c>
     </row>
     <row r="86" spans="1:7" ht="17.149999999999999" x14ac:dyDescent="0.55000000000000004">
       <c r="A86" s="10" t="s">
-        <v>108</v>
-      </c>
-      <c r="B86" s="6" t="s">
-        <v>107</v>
+        <v>166</v>
       </c>
       <c r="C86" s="7" t="s">
-        <v>80</v>
+        <v>28</v>
       </c>
       <c r="D86" s="8" t="s">
-        <v>407</v>
-      </c>
-      <c r="E86" s="9" t="s">
-        <v>109</v>
-      </c>
-      <c r="F86" s="6">
-        <v>3</v>
-      </c>
-      <c r="G86" s="14" t="s">
-        <v>309</v>
+        <v>167</v>
       </c>
     </row>
     <row r="87" spans="1:7" ht="17.149999999999999" x14ac:dyDescent="0.55000000000000004">
       <c r="A87" s="10" t="s">
-        <v>282</v>
+        <v>156</v>
       </c>
       <c r="B87" s="6" t="s">
-        <v>130</v>
+        <v>159</v>
       </c>
       <c r="C87" s="7" t="s">
-        <v>80</v>
+        <v>13</v>
       </c>
       <c r="D87" s="8" t="s">
-        <v>389</v>
-      </c>
-      <c r="F87" s="6">
-        <v>2</v>
-      </c>
-      <c r="G87" s="14" t="s">
-        <v>283</v>
+        <v>157</v>
+      </c>
+      <c r="E87" s="9" t="s">
+        <v>158</v>
       </c>
     </row>
     <row r="88" spans="1:7" ht="17.149999999999999" x14ac:dyDescent="0.55000000000000004">
       <c r="A88" s="10" t="s">
-        <v>270</v>
+        <v>273</v>
       </c>
       <c r="B88" s="6" t="s">
-        <v>272</v>
+        <v>274</v>
       </c>
       <c r="C88" s="7" t="s">
-        <v>42</v>
+        <v>13</v>
       </c>
       <c r="D88" s="8" t="s">
-        <v>387</v>
+        <v>385</v>
       </c>
       <c r="E88" s="9" t="s">
-        <v>271</v>
+        <v>275</v>
       </c>
       <c r="F88" s="6">
         <v>2</v>
@@ -3597,104 +3577,113 @@
     </row>
     <row r="89" spans="1:7" ht="17.149999999999999" x14ac:dyDescent="0.55000000000000004">
       <c r="A89" s="10" t="s">
-        <v>297</v>
+        <v>257</v>
+      </c>
+      <c r="B89" s="6" t="s">
+        <v>256</v>
       </c>
       <c r="C89" s="7" t="s">
-        <v>28</v>
+        <v>80</v>
       </c>
       <c r="D89" s="8" t="s">
-        <v>296</v>
+        <v>385</v>
+      </c>
+      <c r="E89" s="9" t="s">
+        <v>8</v>
+      </c>
+      <c r="F89" s="6">
+        <v>2</v>
+      </c>
+      <c r="G89" s="14" t="s">
+        <v>260</v>
       </c>
     </row>
     <row r="90" spans="1:7" ht="17.149999999999999" x14ac:dyDescent="0.55000000000000004">
       <c r="A90" s="10" t="s">
-        <v>286</v>
+        <v>108</v>
       </c>
       <c r="B90" s="6" t="s">
-        <v>130</v>
+        <v>107</v>
       </c>
       <c r="C90" s="7" t="s">
-        <v>13</v>
+        <v>80</v>
       </c>
       <c r="D90" s="8" t="s">
-        <v>389</v>
+        <v>405</v>
+      </c>
+      <c r="E90" s="9" t="s">
+        <v>109</v>
       </c>
       <c r="F90" s="6">
-        <v>2</v>
+        <v>3</v>
+      </c>
+      <c r="G90" s="14" t="s">
+        <v>309</v>
       </c>
     </row>
     <row r="91" spans="1:7" ht="17.149999999999999" x14ac:dyDescent="0.55000000000000004">
       <c r="A91" s="10" t="s">
-        <v>280</v>
+        <v>282</v>
       </c>
       <c r="B91" s="6" t="s">
-        <v>318</v>
+        <v>130</v>
       </c>
       <c r="C91" s="7" t="s">
-        <v>13</v>
+        <v>80</v>
       </c>
       <c r="D91" s="8" t="s">
-        <v>319</v>
+        <v>387</v>
       </c>
       <c r="F91" s="6">
         <v>2</v>
+      </c>
+      <c r="G91" s="14" t="s">
+        <v>283</v>
       </c>
     </row>
     <row r="92" spans="1:7" ht="17.149999999999999" x14ac:dyDescent="0.55000000000000004">
       <c r="A92" s="10" t="s">
-        <v>242</v>
+        <v>270</v>
       </c>
       <c r="B92" s="6" t="s">
-        <v>238</v>
+        <v>272</v>
       </c>
       <c r="C92" s="7" t="s">
-        <v>95</v>
+        <v>42</v>
       </c>
       <c r="D92" s="8" t="s">
-        <v>380</v>
-      </c>
-      <c r="E92" s="12" t="s">
-        <v>241</v>
+        <v>385</v>
+      </c>
+      <c r="E92" s="9" t="s">
+        <v>271</v>
       </c>
       <c r="F92" s="6">
         <v>2</v>
-      </c>
-      <c r="G92" s="14" t="s">
-        <v>381</v>
       </c>
     </row>
     <row r="93" spans="1:7" ht="17.149999999999999" x14ac:dyDescent="0.55000000000000004">
       <c r="A93" s="10" t="s">
-        <v>343</v>
-      </c>
-      <c r="B93" s="6" t="s">
-        <v>344</v>
+        <v>297</v>
       </c>
       <c r="C93" s="7" t="s">
-        <v>13</v>
+        <v>28</v>
       </c>
       <c r="D93" s="8" t="s">
-        <v>340</v>
-      </c>
-      <c r="E93" s="9" t="s">
-        <v>14</v>
+        <v>296</v>
       </c>
     </row>
     <row r="94" spans="1:7" ht="17.149999999999999" x14ac:dyDescent="0.55000000000000004">
       <c r="A94" s="10" t="s">
-        <v>237</v>
+        <v>286</v>
       </c>
       <c r="B94" s="6" t="s">
-        <v>238</v>
+        <v>130</v>
       </c>
       <c r="C94" s="7" t="s">
-        <v>80</v>
+        <v>13</v>
       </c>
       <c r="D94" s="8" t="s">
-        <v>379</v>
-      </c>
-      <c r="E94" s="9" t="s">
-        <v>22</v>
+        <v>387</v>
       </c>
       <c r="F94" s="6">
         <v>2</v>
@@ -3702,16 +3691,16 @@
     </row>
     <row r="95" spans="1:7" ht="17.149999999999999" x14ac:dyDescent="0.55000000000000004">
       <c r="A95" s="10" t="s">
-        <v>258</v>
+        <v>280</v>
       </c>
       <c r="B95" s="6" t="s">
-        <v>256</v>
+        <v>318</v>
       </c>
       <c r="C95" s="7" t="s">
         <v>13</v>
       </c>
       <c r="D95" s="8" t="s">
-        <v>387</v>
+        <v>319</v>
       </c>
       <c r="F95" s="6">
         <v>2</v>
@@ -3719,84 +3708,93 @@
     </row>
     <row r="96" spans="1:7" ht="17.149999999999999" x14ac:dyDescent="0.55000000000000004">
       <c r="A96" s="10" t="s">
-        <v>239</v>
+        <v>242</v>
       </c>
       <c r="B96" s="6" t="s">
         <v>238</v>
       </c>
       <c r="C96" s="7" t="s">
-        <v>42</v>
+        <v>95</v>
       </c>
       <c r="D96" s="8" t="s">
+        <v>378</v>
+      </c>
+      <c r="E96" s="12" t="s">
+        <v>241</v>
+      </c>
+      <c r="F96" s="6">
+        <v>2</v>
+      </c>
+      <c r="G96" s="14" t="s">
         <v>379</v>
-      </c>
-      <c r="F96" s="6">
-        <v>2</v>
       </c>
     </row>
     <row r="97" spans="1:7" ht="17.149999999999999" x14ac:dyDescent="0.55000000000000004">
       <c r="A97" s="10" t="s">
-        <v>168</v>
+        <v>343</v>
       </c>
       <c r="B97" s="6" t="s">
-        <v>170</v>
+        <v>344</v>
       </c>
       <c r="C97" s="7" t="s">
-        <v>42</v>
+        <v>13</v>
       </c>
       <c r="D97" s="8" t="s">
-        <v>169</v>
+        <v>340</v>
+      </c>
+      <c r="E97" s="9" t="s">
+        <v>14</v>
       </c>
     </row>
     <row r="98" spans="1:7" ht="17.149999999999999" x14ac:dyDescent="0.55000000000000004">
       <c r="A98" s="10" t="s">
-        <v>322</v>
+        <v>237</v>
       </c>
       <c r="B98" s="6" t="s">
-        <v>324</v>
+        <v>238</v>
       </c>
       <c r="C98" s="7" t="s">
-        <v>13</v>
+        <v>80</v>
       </c>
       <c r="D98" s="8" t="s">
-        <v>323</v>
+        <v>377</v>
       </c>
       <c r="E98" s="9" t="s">
-        <v>14</v>
+        <v>22</v>
+      </c>
+      <c r="F98" s="6">
+        <v>2</v>
       </c>
     </row>
     <row r="99" spans="1:7" ht="17.149999999999999" x14ac:dyDescent="0.55000000000000004">
       <c r="A99" s="10" t="s">
-        <v>48</v>
+        <v>258</v>
       </c>
       <c r="B99" s="6" t="s">
-        <v>49</v>
+        <v>256</v>
       </c>
       <c r="C99" s="7" t="s">
-        <v>28</v>
+        <v>13</v>
       </c>
       <c r="D99" s="8" t="s">
-        <v>50</v>
-      </c>
-      <c r="E99" s="9" t="s">
-        <v>22</v>
-      </c>
-      <c r="G99" s="14" t="s">
-        <v>51</v>
+        <v>385</v>
+      </c>
+      <c r="F99" s="6">
+        <v>2</v>
       </c>
     </row>
     <row r="100" spans="1:7" ht="17.149999999999999" x14ac:dyDescent="0.55000000000000004">
       <c r="A100" s="10" t="s">
-        <v>232</v>
+        <v>239</v>
       </c>
       <c r="B100" s="6" t="s">
-        <v>230</v>
+        <v>238</v>
       </c>
       <c r="C100" s="7" t="s">
-        <v>80</v>
+        <v>42</v>
       </c>
       <c r="D100" s="8" t="s">
-        <v>376</v>
+        <v>377</v>
       </c>
       <c r="F100" s="6">
         <v>2</v>
@@ -3804,265 +3802,253 @@
     </row>
     <row r="101" spans="1:7" ht="17.149999999999999" x14ac:dyDescent="0.55000000000000004">
       <c r="A101" s="10" t="s">
-        <v>247</v>
+        <v>168</v>
       </c>
       <c r="B101" s="6" t="s">
-        <v>248</v>
+        <v>170</v>
       </c>
       <c r="C101" s="7" t="s">
-        <v>80</v>
+        <v>42</v>
       </c>
       <c r="D101" s="8" t="s">
-        <v>384</v>
-      </c>
-      <c r="E101" s="9" t="s">
-        <v>93</v>
-      </c>
-      <c r="F101" s="6">
-        <v>2</v>
+        <v>169</v>
       </c>
     </row>
     <row r="102" spans="1:7" ht="17.149999999999999" x14ac:dyDescent="0.55000000000000004">
       <c r="A102" s="10" t="s">
-        <v>244</v>
+        <v>322</v>
       </c>
       <c r="B102" s="6" t="s">
-        <v>238</v>
+        <v>324</v>
       </c>
       <c r="C102" s="7" t="s">
-        <v>80</v>
+        <v>13</v>
       </c>
       <c r="D102" s="8" t="s">
-        <v>380</v>
+        <v>323</v>
       </c>
       <c r="E102" s="9" t="s">
-        <v>98</v>
-      </c>
-      <c r="G102" s="14" t="s">
-        <v>383</v>
+        <v>14</v>
       </c>
     </row>
     <row r="103" spans="1:7" ht="17.149999999999999" x14ac:dyDescent="0.55000000000000004">
       <c r="A103" s="10" t="s">
-        <v>179</v>
+        <v>48</v>
       </c>
       <c r="B103" s="6" t="s">
-        <v>180</v>
+        <v>49</v>
       </c>
       <c r="C103" s="7" t="s">
-        <v>13</v>
+        <v>28</v>
       </c>
       <c r="D103" s="8" t="s">
-        <v>410</v>
-      </c>
-      <c r="F103" s="6">
-        <v>3</v>
+        <v>50</v>
+      </c>
+      <c r="E103" s="9" t="s">
+        <v>22</v>
       </c>
       <c r="G103" s="14" t="s">
-        <v>328</v>
+        <v>51</v>
       </c>
     </row>
     <row r="104" spans="1:7" ht="17.149999999999999" x14ac:dyDescent="0.55000000000000004">
       <c r="A104" s="10" t="s">
-        <v>285</v>
+        <v>232</v>
       </c>
       <c r="B104" s="6" t="s">
-        <v>12</v>
+        <v>230</v>
       </c>
       <c r="C104" s="7" t="s">
         <v>80</v>
       </c>
       <c r="D104" s="8" t="s">
-        <v>308</v>
-      </c>
-      <c r="E104" s="9" t="s">
-        <v>310</v>
+        <v>374</v>
       </c>
       <c r="F104" s="6">
-        <v>3</v>
-      </c>
-      <c r="G104" s="14" t="s">
-        <v>15</v>
+        <v>2</v>
       </c>
     </row>
     <row r="105" spans="1:7" ht="17.149999999999999" x14ac:dyDescent="0.55000000000000004">
       <c r="A105" s="10" t="s">
-        <v>96</v>
+        <v>247</v>
       </c>
       <c r="B105" s="6" t="s">
-        <v>92</v>
+        <v>248</v>
       </c>
       <c r="C105" s="7" t="s">
         <v>80</v>
       </c>
       <c r="D105" s="8" t="s">
-        <v>407</v>
+        <v>382</v>
       </c>
       <c r="E105" s="9" t="s">
-        <v>98</v>
+        <v>93</v>
       </c>
       <c r="F105" s="6">
-        <v>3</v>
-      </c>
-      <c r="G105" s="14" t="s">
-        <v>99</v>
+        <v>2</v>
       </c>
     </row>
     <row r="106" spans="1:7" ht="17.149999999999999" x14ac:dyDescent="0.55000000000000004">
       <c r="A106" s="10" t="s">
-        <v>218</v>
+        <v>244</v>
       </c>
       <c r="B106" s="6" t="s">
-        <v>366</v>
+        <v>238</v>
       </c>
       <c r="C106" s="7" t="s">
-        <v>13</v>
+        <v>80</v>
       </c>
       <c r="D106" s="8" t="s">
-        <v>362</v>
-      </c>
-      <c r="F106" s="6">
-        <v>2</v>
+        <v>378</v>
+      </c>
+      <c r="E106" s="9" t="s">
+        <v>98</v>
       </c>
       <c r="G106" s="14" t="s">
-        <v>365</v>
+        <v>381</v>
       </c>
     </row>
     <row r="107" spans="1:7" ht="17.149999999999999" x14ac:dyDescent="0.55000000000000004">
       <c r="A107" s="10" t="s">
-        <v>155</v>
+        <v>179</v>
       </c>
       <c r="B107" s="6" t="s">
-        <v>107</v>
+        <v>180</v>
       </c>
       <c r="C107" s="7" t="s">
-        <v>95</v>
+        <v>13</v>
       </c>
       <c r="D107" s="8" t="s">
-        <v>407</v>
-      </c>
-      <c r="E107" s="9" t="s">
-        <v>110</v>
+        <v>408</v>
       </c>
       <c r="F107" s="6">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="G107" s="14" t="s">
-        <v>311</v>
+        <v>328</v>
       </c>
     </row>
     <row r="108" spans="1:7" ht="17.149999999999999" x14ac:dyDescent="0.55000000000000004">
       <c r="A108" s="10" t="s">
-        <v>52</v>
+        <v>285</v>
       </c>
       <c r="B108" s="6" t="s">
-        <v>49</v>
+        <v>12</v>
       </c>
       <c r="C108" s="7" t="s">
-        <v>28</v>
+        <v>80</v>
       </c>
       <c r="D108" s="8" t="s">
-        <v>53</v>
+        <v>308</v>
       </c>
       <c r="E108" s="9" t="s">
-        <v>22</v>
+        <v>310</v>
+      </c>
+      <c r="F108" s="6">
+        <v>3</v>
       </c>
       <c r="G108" s="14" t="s">
-        <v>54</v>
+        <v>15</v>
       </c>
     </row>
     <row r="109" spans="1:7" ht="17.149999999999999" x14ac:dyDescent="0.55000000000000004">
       <c r="A109" s="10" t="s">
-        <v>262</v>
+        <v>96</v>
       </c>
       <c r="B109" s="6" t="s">
-        <v>148</v>
+        <v>92</v>
       </c>
       <c r="C109" s="7" t="s">
-        <v>13</v>
+        <v>80</v>
       </c>
       <c r="D109" s="8" t="s">
-        <v>387</v>
+        <v>405</v>
+      </c>
+      <c r="E109" s="9" t="s">
+        <v>98</v>
       </c>
       <c r="F109" s="6">
-        <v>2</v>
+        <v>3</v>
+      </c>
+      <c r="G109" s="14" t="s">
+        <v>99</v>
       </c>
     </row>
     <row r="110" spans="1:7" ht="17.149999999999999" x14ac:dyDescent="0.55000000000000004">
       <c r="A110" s="10" t="s">
-        <v>226</v>
+        <v>218</v>
       </c>
       <c r="B110" s="6" t="s">
-        <v>231</v>
+        <v>364</v>
       </c>
       <c r="C110" s="7" t="s">
         <v>13</v>
       </c>
       <c r="D110" s="8" t="s">
-        <v>375</v>
-      </c>
-      <c r="E110" s="9" t="s">
-        <v>128</v>
+        <v>360</v>
       </c>
       <c r="F110" s="6">
         <v>2</v>
       </c>
       <c r="G110" s="14" t="s">
-        <v>227</v>
+        <v>363</v>
       </c>
     </row>
     <row r="111" spans="1:7" ht="17.149999999999999" x14ac:dyDescent="0.55000000000000004">
       <c r="A111" s="10" t="s">
-        <v>29</v>
+        <v>155</v>
       </c>
       <c r="B111" s="6" t="s">
-        <v>33</v>
+        <v>107</v>
       </c>
       <c r="C111" s="7" t="s">
-        <v>28</v>
+        <v>95</v>
       </c>
       <c r="D111" s="8" t="s">
-        <v>30</v>
+        <v>405</v>
       </c>
       <c r="E111" s="9" t="s">
-        <v>31</v>
+        <v>110</v>
+      </c>
+      <c r="F111" s="6">
+        <v>4</v>
       </c>
       <c r="G111" s="14" t="s">
-        <v>32</v>
+        <v>311</v>
       </c>
     </row>
     <row r="112" spans="1:7" ht="17.149999999999999" x14ac:dyDescent="0.55000000000000004">
       <c r="A112" s="10" t="s">
-        <v>316</v>
+        <v>52</v>
       </c>
       <c r="B112" s="6" t="s">
-        <v>317</v>
+        <v>49</v>
       </c>
       <c r="C112" s="7" t="s">
-        <v>80</v>
+        <v>28</v>
       </c>
       <c r="D112" s="8" t="s">
-        <v>313</v>
+        <v>53</v>
       </c>
       <c r="E112" s="9" t="s">
-        <v>14</v>
+        <v>22</v>
+      </c>
+      <c r="G112" s="14" t="s">
+        <v>54</v>
       </c>
     </row>
     <row r="113" spans="1:7" ht="17.149999999999999" x14ac:dyDescent="0.55000000000000004">
       <c r="A113" s="10" t="s">
-        <v>186</v>
+        <v>262</v>
       </c>
       <c r="B113" s="6" t="s">
-        <v>187</v>
+        <v>148</v>
       </c>
       <c r="C113" s="7" t="s">
-        <v>6</v>
+        <v>13</v>
       </c>
       <c r="D113" s="8" t="s">
-        <v>411</v>
-      </c>
-      <c r="E113" s="9" t="s">
-        <v>93</v>
+        <v>385</v>
       </c>
       <c r="F113" s="6">
         <v>2</v>
@@ -4070,79 +4056,79 @@
     </row>
     <row r="114" spans="1:7" ht="17.149999999999999" x14ac:dyDescent="0.55000000000000004">
       <c r="A114" s="10" t="s">
-        <v>82</v>
+        <v>226</v>
       </c>
       <c r="B114" s="6" t="s">
-        <v>79</v>
+        <v>231</v>
       </c>
       <c r="C114" s="7" t="s">
-        <v>80</v>
+        <v>13</v>
       </c>
       <c r="D114" s="8" t="s">
-        <v>404</v>
+        <v>373</v>
+      </c>
+      <c r="E114" s="9" t="s">
+        <v>128</v>
       </c>
       <c r="F114" s="6">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="G114" s="14" t="s">
-        <v>307</v>
+        <v>227</v>
       </c>
     </row>
     <row r="115" spans="1:7" ht="17.149999999999999" x14ac:dyDescent="0.55000000000000004">
       <c r="A115" s="10" t="s">
-        <v>314</v>
+        <v>29</v>
       </c>
       <c r="B115" s="6" t="s">
-        <v>315</v>
+        <v>33</v>
       </c>
       <c r="C115" s="7" t="s">
-        <v>80</v>
+        <v>28</v>
       </c>
       <c r="D115" s="8" t="s">
-        <v>313</v>
+        <v>30</v>
       </c>
       <c r="E115" s="9" t="s">
-        <v>14</v>
+        <v>31</v>
+      </c>
+      <c r="G115" s="14" t="s">
+        <v>32</v>
       </c>
     </row>
     <row r="116" spans="1:7" ht="17.149999999999999" x14ac:dyDescent="0.55000000000000004">
       <c r="A116" s="10" t="s">
-        <v>289</v>
+        <v>316</v>
       </c>
       <c r="B116" s="6" t="s">
-        <v>130</v>
+        <v>317</v>
       </c>
       <c r="C116" s="7" t="s">
-        <v>95</v>
+        <v>80</v>
       </c>
       <c r="D116" s="8" t="s">
-        <v>404</v>
+        <v>313</v>
       </c>
       <c r="E116" s="9" t="s">
-        <v>22</v>
-      </c>
-      <c r="F116" s="6">
-        <v>3</v>
-      </c>
-      <c r="G116" s="14" t="s">
-        <v>391</v>
+        <v>14</v>
       </c>
     </row>
     <row r="117" spans="1:7" ht="17.149999999999999" x14ac:dyDescent="0.55000000000000004">
       <c r="A117" s="10" t="s">
-        <v>236</v>
+        <v>186</v>
       </c>
       <c r="B117" s="6" t="s">
-        <v>230</v>
+        <v>187</v>
       </c>
       <c r="C117" s="7" t="s">
-        <v>80</v>
+        <v>6</v>
       </c>
       <c r="D117" s="8" t="s">
-        <v>378</v>
+        <v>409</v>
       </c>
       <c r="E117" s="9" t="s">
-        <v>14</v>
+        <v>93</v>
       </c>
       <c r="F117" s="6">
         <v>2</v>
@@ -4150,124 +4136,130 @@
     </row>
     <row r="118" spans="1:7" ht="17.149999999999999" x14ac:dyDescent="0.55000000000000004">
       <c r="A118" s="10" t="s">
-        <v>171</v>
+        <v>82</v>
       </c>
       <c r="B118" s="6" t="s">
-        <v>174</v>
+        <v>79</v>
       </c>
       <c r="C118" s="7" t="s">
-        <v>6</v>
+        <v>80</v>
       </c>
       <c r="D118" s="8" t="s">
-        <v>172</v>
-      </c>
-      <c r="E118" s="9" t="s">
-        <v>173</v>
+        <v>402</v>
+      </c>
+      <c r="F118" s="6">
+        <v>4</v>
+      </c>
+      <c r="G118" s="14" t="s">
+        <v>307</v>
       </c>
     </row>
     <row r="119" spans="1:7" ht="17.149999999999999" x14ac:dyDescent="0.55000000000000004">
       <c r="A119" s="10" t="s">
-        <v>320</v>
+        <v>314</v>
       </c>
       <c r="B119" s="6" t="s">
-        <v>318</v>
+        <v>315</v>
       </c>
       <c r="C119" s="7" t="s">
-        <v>13</v>
+        <v>80</v>
       </c>
       <c r="D119" s="8" t="s">
-        <v>319</v>
+        <v>313</v>
+      </c>
+      <c r="E119" s="9" t="s">
+        <v>14</v>
       </c>
     </row>
     <row r="120" spans="1:7" ht="17.149999999999999" x14ac:dyDescent="0.55000000000000004">
       <c r="A120" s="10" t="s">
-        <v>127</v>
+        <v>289</v>
       </c>
       <c r="B120" s="6" t="s">
-        <v>325</v>
+        <v>130</v>
       </c>
       <c r="C120" s="7" t="s">
-        <v>42</v>
+        <v>95</v>
       </c>
       <c r="D120" s="8" t="s">
-        <v>410</v>
+        <v>402</v>
       </c>
       <c r="E120" s="9" t="s">
-        <v>128</v>
+        <v>22</v>
       </c>
       <c r="F120" s="6">
-        <v>4</v>
+        <v>3</v>
+      </c>
+      <c r="G120" s="14" t="s">
+        <v>389</v>
       </c>
     </row>
     <row r="121" spans="1:7" ht="17.149999999999999" x14ac:dyDescent="0.55000000000000004">
       <c r="A121" s="10" t="s">
-        <v>184</v>
+        <v>236</v>
       </c>
       <c r="B121" s="6" t="s">
-        <v>333</v>
+        <v>230</v>
       </c>
       <c r="C121" s="7" t="s">
-        <v>42</v>
+        <v>80</v>
       </c>
       <c r="D121" s="8" t="s">
-        <v>411</v>
-      </c>
-      <c r="E121" s="10" t="s">
-        <v>185</v>
+        <v>376</v>
+      </c>
+      <c r="E121" s="9" t="s">
+        <v>14</v>
       </c>
       <c r="F121" s="6">
-        <v>3</v>
-      </c>
-      <c r="G121" s="14" t="s">
-        <v>332</v>
+        <v>2</v>
       </c>
     </row>
     <row r="122" spans="1:7" ht="17.149999999999999" x14ac:dyDescent="0.55000000000000004">
       <c r="A122" s="10" t="s">
-        <v>210</v>
+        <v>171</v>
+      </c>
+      <c r="B122" s="6" t="s">
+        <v>174</v>
       </c>
       <c r="C122" s="7" t="s">
-        <v>13</v>
+        <v>6</v>
       </c>
       <c r="D122" s="8" t="s">
-        <v>358</v>
-      </c>
-      <c r="F122" s="6">
-        <v>2</v>
+        <v>172</v>
+      </c>
+      <c r="E122" s="9" t="s">
+        <v>173</v>
       </c>
     </row>
     <row r="123" spans="1:7" ht="17.149999999999999" x14ac:dyDescent="0.55000000000000004">
       <c r="A123" s="10" t="s">
-        <v>261</v>
+        <v>320</v>
       </c>
       <c r="B123" s="6" t="s">
-        <v>148</v>
+        <v>318</v>
       </c>
       <c r="C123" s="7" t="s">
-        <v>42</v>
+        <v>13</v>
       </c>
       <c r="D123" s="8" t="s">
-        <v>387</v>
-      </c>
-      <c r="F123" s="6">
-        <v>2</v>
+        <v>319</v>
       </c>
     </row>
     <row r="124" spans="1:7" ht="17.149999999999999" x14ac:dyDescent="0.55000000000000004">
       <c r="A124" s="10" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="B124" s="6" t="s">
-        <v>132</v>
+        <v>325</v>
       </c>
       <c r="C124" s="7" t="s">
-        <v>80</v>
+        <v>42</v>
       </c>
       <c r="D124" s="8" t="s">
-        <v>410</v>
+        <v>408</v>
       </c>
       <c r="E124" s="9" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
       <c r="F124" s="6">
         <v>4</v>
@@ -4275,56 +4267,56 @@
     </row>
     <row r="125" spans="1:7" ht="17.149999999999999" x14ac:dyDescent="0.55000000000000004">
       <c r="A125" s="10" t="s">
-        <v>117</v>
+        <v>184</v>
       </c>
       <c r="B125" s="6" t="s">
-        <v>120</v>
+        <v>333</v>
       </c>
       <c r="C125" s="7" t="s">
-        <v>95</v>
+        <v>42</v>
       </c>
       <c r="D125" s="8" t="s">
-        <v>408</v>
-      </c>
-      <c r="E125" s="9" t="s">
-        <v>118</v>
+        <v>409</v>
+      </c>
+      <c r="E125" s="10" t="s">
+        <v>185</v>
       </c>
       <c r="F125" s="6">
-        <v>5</v>
+        <v>3</v>
+      </c>
+      <c r="G125" s="14" t="s">
+        <v>332</v>
       </c>
     </row>
     <row r="126" spans="1:7" ht="17.149999999999999" x14ac:dyDescent="0.55000000000000004">
       <c r="A126" s="10" t="s">
-        <v>287</v>
-      </c>
-      <c r="B126" s="6" t="s">
-        <v>130</v>
+        <v>210</v>
       </c>
       <c r="C126" s="7" t="s">
         <v>13</v>
       </c>
       <c r="D126" s="8" t="s">
-        <v>390</v>
-      </c>
-      <c r="E126" s="9" t="s">
-        <v>14</v>
+        <v>417</v>
       </c>
       <c r="F126" s="6">
-        <v>2</v>
+        <v>3</v>
+      </c>
+      <c r="G126" s="14" t="s">
+        <v>419</v>
       </c>
     </row>
     <row r="127" spans="1:7" ht="17.149999999999999" x14ac:dyDescent="0.55000000000000004">
       <c r="A127" s="10" t="s">
-        <v>288</v>
+        <v>261</v>
       </c>
       <c r="B127" s="6" t="s">
-        <v>130</v>
+        <v>148</v>
       </c>
       <c r="C127" s="7" t="s">
-        <v>13</v>
+        <v>42</v>
       </c>
       <c r="D127" s="8" t="s">
-        <v>390</v>
+        <v>385</v>
       </c>
       <c r="F127" s="6">
         <v>2</v>
@@ -4332,261 +4324,255 @@
     </row>
     <row r="128" spans="1:7" ht="17.149999999999999" x14ac:dyDescent="0.55000000000000004">
       <c r="A128" s="10" t="s">
-        <v>149</v>
+        <v>129</v>
       </c>
       <c r="B128" s="6" t="s">
-        <v>148</v>
+        <v>132</v>
       </c>
       <c r="C128" s="7" t="s">
-        <v>6</v>
+        <v>80</v>
       </c>
       <c r="D128" s="8" t="s">
-        <v>147</v>
+        <v>408</v>
       </c>
       <c r="E128" s="9" t="s">
-        <v>146</v>
-      </c>
-      <c r="G128" s="14" t="s">
-        <v>150</v>
+        <v>131</v>
+      </c>
+      <c r="F128" s="6">
+        <v>4</v>
       </c>
     </row>
     <row r="129" spans="1:7" ht="17.149999999999999" x14ac:dyDescent="0.55000000000000004">
       <c r="A129" s="10" t="s">
-        <v>276</v>
+        <v>117</v>
       </c>
       <c r="B129" s="6" t="s">
-        <v>130</v>
+        <v>120</v>
       </c>
       <c r="C129" s="7" t="s">
-        <v>42</v>
+        <v>95</v>
       </c>
       <c r="D129" s="8" t="s">
-        <v>326</v>
+        <v>406</v>
+      </c>
+      <c r="E129" s="9" t="s">
+        <v>118</v>
       </c>
       <c r="F129" s="6">
-        <v>2</v>
+        <v>5</v>
       </c>
     </row>
     <row r="130" spans="1:7" ht="17.149999999999999" x14ac:dyDescent="0.55000000000000004">
       <c r="A130" s="10" t="s">
-        <v>293</v>
+        <v>287</v>
+      </c>
+      <c r="B130" s="6" t="s">
+        <v>130</v>
       </c>
       <c r="C130" s="7" t="s">
         <v>13</v>
       </c>
       <c r="D130" s="8" t="s">
-        <v>292</v>
+        <v>388</v>
+      </c>
+      <c r="E130" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="F130" s="6">
+        <v>2</v>
       </c>
     </row>
     <row r="131" spans="1:7" ht="17.149999999999999" x14ac:dyDescent="0.55000000000000004">
       <c r="A131" s="10" t="s">
-        <v>88</v>
-      </c>
-      <c r="B131" s="6" t="s">
-        <v>89</v>
+        <v>392</v>
       </c>
       <c r="C131" s="7" t="s">
         <v>42</v>
       </c>
       <c r="D131" s="8" t="s">
-        <v>85</v>
-      </c>
-      <c r="E131" s="9" t="s">
-        <v>90</v>
+        <v>393</v>
       </c>
     </row>
     <row r="132" spans="1:7" ht="17.149999999999999" x14ac:dyDescent="0.55000000000000004">
       <c r="A132" s="10" t="s">
-        <v>291</v>
+        <v>288</v>
       </c>
       <c r="B132" s="6" t="s">
         <v>130</v>
       </c>
       <c r="C132" s="7" t="s">
-        <v>80</v>
+        <v>13</v>
       </c>
       <c r="D132" s="8" t="s">
-        <v>390</v>
-      </c>
-      <c r="E132" s="9" t="s">
-        <v>14</v>
+        <v>388</v>
       </c>
       <c r="F132" s="6">
         <v>2</v>
-      </c>
-      <c r="G132" s="14" t="s">
-        <v>393</v>
       </c>
     </row>
     <row r="133" spans="1:7" ht="17.149999999999999" x14ac:dyDescent="0.55000000000000004">
       <c r="A133" s="10" t="s">
-        <v>181</v>
+        <v>149</v>
       </c>
       <c r="B133" s="6" t="s">
-        <v>331</v>
+        <v>148</v>
       </c>
       <c r="C133" s="7" t="s">
-        <v>42</v>
+        <v>6</v>
       </c>
       <c r="D133" s="8" t="s">
-        <v>411</v>
+        <v>147</v>
       </c>
       <c r="E133" s="9" t="s">
-        <v>183</v>
-      </c>
-      <c r="F133" s="6">
-        <v>3</v>
+        <v>146</v>
       </c>
       <c r="G133" s="14" t="s">
-        <v>182</v>
+        <v>150</v>
       </c>
     </row>
     <row r="134" spans="1:7" ht="17.149999999999999" x14ac:dyDescent="0.55000000000000004">
       <c r="A134" s="10" t="s">
-        <v>111</v>
+        <v>276</v>
       </c>
       <c r="B134" s="6" t="s">
-        <v>112</v>
+        <v>130</v>
       </c>
       <c r="C134" s="7" t="s">
-        <v>6</v>
+        <v>42</v>
       </c>
       <c r="D134" s="8" t="s">
-        <v>113</v>
-      </c>
-      <c r="E134" s="9" t="s">
-        <v>114</v>
+        <v>326</v>
+      </c>
+      <c r="F134" s="6">
+        <v>2</v>
       </c>
     </row>
     <row r="135" spans="1:7" ht="17.149999999999999" x14ac:dyDescent="0.55000000000000004">
       <c r="A135" s="10" t="s">
-        <v>249</v>
-      </c>
-      <c r="B135" s="6" t="s">
-        <v>252</v>
+        <v>293</v>
       </c>
       <c r="C135" s="7" t="s">
-        <v>80</v>
+        <v>13</v>
       </c>
       <c r="D135" s="8" t="s">
-        <v>385</v>
-      </c>
-      <c r="E135" s="9" t="s">
-        <v>250</v>
-      </c>
-      <c r="F135" s="6">
-        <v>2</v>
-      </c>
-      <c r="G135" s="14" t="s">
-        <v>253</v>
+        <v>292</v>
       </c>
     </row>
     <row r="136" spans="1:7" ht="17.149999999999999" x14ac:dyDescent="0.55000000000000004">
       <c r="A136" s="10" t="s">
-        <v>240</v>
+        <v>88</v>
       </c>
       <c r="B136" s="6" t="s">
-        <v>238</v>
+        <v>89</v>
       </c>
       <c r="C136" s="7" t="s">
         <v>42</v>
       </c>
       <c r="D136" s="8" t="s">
-        <v>379</v>
-      </c>
-      <c r="F136" s="6">
-        <v>2</v>
+        <v>85</v>
+      </c>
+      <c r="E136" s="9" t="s">
+        <v>90</v>
       </c>
     </row>
     <row r="137" spans="1:7" ht="17.149999999999999" x14ac:dyDescent="0.55000000000000004">
       <c r="A137" s="10" t="s">
-        <v>268</v>
+        <v>291</v>
       </c>
       <c r="B137" s="6" t="s">
-        <v>269</v>
+        <v>130</v>
       </c>
       <c r="C137" s="7" t="s">
-        <v>6</v>
+        <v>80</v>
       </c>
       <c r="D137" s="8" t="s">
-        <v>387</v>
+        <v>388</v>
+      </c>
+      <c r="E137" s="9" t="s">
+        <v>14</v>
       </c>
       <c r="F137" s="6">
         <v>2</v>
+      </c>
+      <c r="G137" s="14" t="s">
+        <v>391</v>
       </c>
     </row>
     <row r="138" spans="1:7" ht="17.149999999999999" x14ac:dyDescent="0.55000000000000004">
       <c r="A138" s="10" t="s">
-        <v>119</v>
+        <v>181</v>
       </c>
       <c r="B138" s="6" t="s">
-        <v>107</v>
+        <v>331</v>
       </c>
       <c r="C138" s="7" t="s">
-        <v>95</v>
+        <v>42</v>
       </c>
       <c r="D138" s="8" t="s">
         <v>409</v>
       </c>
       <c r="E138" s="9" t="s">
-        <v>122</v>
+        <v>183</v>
       </c>
       <c r="F138" s="6">
         <v>3</v>
       </c>
+      <c r="G138" s="14" t="s">
+        <v>182</v>
+      </c>
     </row>
     <row r="139" spans="1:7" ht="17.149999999999999" x14ac:dyDescent="0.55000000000000004">
       <c r="A139" s="10" t="s">
-        <v>263</v>
+        <v>111</v>
       </c>
       <c r="B139" s="6" t="s">
-        <v>148</v>
+        <v>112</v>
       </c>
       <c r="C139" s="7" t="s">
-        <v>13</v>
+        <v>6</v>
       </c>
       <c r="D139" s="8" t="s">
-        <v>388</v>
+        <v>113</v>
       </c>
       <c r="E139" s="9" t="s">
-        <v>22</v>
+        <v>114</v>
       </c>
     </row>
     <row r="140" spans="1:7" ht="17.149999999999999" x14ac:dyDescent="0.55000000000000004">
       <c r="A140" s="10" t="s">
-        <v>228</v>
+        <v>249</v>
       </c>
       <c r="B140" s="6" t="s">
-        <v>230</v>
+        <v>252</v>
       </c>
       <c r="C140" s="7" t="s">
-        <v>13</v>
+        <v>80</v>
       </c>
       <c r="D140" s="8" t="s">
-        <v>387</v>
+        <v>383</v>
       </c>
       <c r="E140" s="9" t="s">
-        <v>47</v>
+        <v>250</v>
       </c>
       <c r="F140" s="6">
-        <v>3</v>
+        <v>2</v>
+      </c>
+      <c r="G140" s="14" t="s">
+        <v>253</v>
       </c>
     </row>
     <row r="141" spans="1:7" ht="17.149999999999999" x14ac:dyDescent="0.55000000000000004">
       <c r="A141" s="10" t="s">
-        <v>233</v>
+        <v>240</v>
       </c>
       <c r="B141" s="6" t="s">
-        <v>230</v>
+        <v>238</v>
       </c>
       <c r="C141" s="7" t="s">
         <v>42</v>
       </c>
       <c r="D141" s="8" t="s">
-        <v>376</v>
-      </c>
-      <c r="E141" s="9" t="s">
-        <v>93</v>
+        <v>377</v>
       </c>
       <c r="F141" s="6">
         <v>2</v>
@@ -4594,419 +4580,449 @@
     </row>
     <row r="142" spans="1:7" ht="17.149999999999999" x14ac:dyDescent="0.55000000000000004">
       <c r="A142" s="10" t="s">
-        <v>100</v>
+        <v>268</v>
       </c>
       <c r="B142" s="6" t="s">
-        <v>102</v>
+        <v>269</v>
       </c>
       <c r="C142" s="7" t="s">
         <v>6</v>
       </c>
       <c r="D142" s="8" t="s">
-        <v>101</v>
-      </c>
-      <c r="E142" s="9" t="s">
-        <v>103</v>
+        <v>385</v>
+      </c>
+      <c r="F142" s="6">
+        <v>2</v>
       </c>
     </row>
     <row r="143" spans="1:7" ht="17.149999999999999" x14ac:dyDescent="0.55000000000000004">
       <c r="A143" s="10" t="s">
-        <v>83</v>
+        <v>119</v>
       </c>
       <c r="B143" s="6" t="s">
-        <v>86</v>
+        <v>107</v>
       </c>
       <c r="C143" s="7" t="s">
-        <v>28</v>
+        <v>95</v>
       </c>
       <c r="D143" s="8" t="s">
-        <v>85</v>
+        <v>407</v>
       </c>
       <c r="E143" s="9" t="s">
-        <v>84</v>
+        <v>122</v>
+      </c>
+      <c r="F143" s="6">
+        <v>3</v>
       </c>
     </row>
     <row r="144" spans="1:7" ht="17.149999999999999" x14ac:dyDescent="0.55000000000000004">
       <c r="A144" s="10" t="s">
-        <v>251</v>
+        <v>263</v>
       </c>
       <c r="B144" s="6" t="s">
-        <v>36</v>
+        <v>148</v>
       </c>
       <c r="C144" s="7" t="s">
-        <v>80</v>
+        <v>13</v>
       </c>
       <c r="D144" s="8" t="s">
-        <v>385</v>
+        <v>386</v>
       </c>
       <c r="E144" s="9" t="s">
-        <v>128</v>
-      </c>
-      <c r="F144" s="6">
-        <v>2</v>
-      </c>
-      <c r="G144" s="14" t="s">
-        <v>386</v>
+        <v>22</v>
       </c>
     </row>
     <row r="145" spans="1:7" ht="17.149999999999999" x14ac:dyDescent="0.55000000000000004">
       <c r="A145" s="10" t="s">
-        <v>206</v>
+        <v>228</v>
+      </c>
+      <c r="B145" s="6" t="s">
+        <v>230</v>
       </c>
       <c r="C145" s="7" t="s">
         <v>13</v>
       </c>
       <c r="D145" s="8" t="s">
-        <v>356</v>
+        <v>385</v>
+      </c>
+      <c r="E145" s="9" t="s">
+        <v>47</v>
       </c>
       <c r="F145" s="6">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="146" spans="1:7" ht="17.149999999999999" x14ac:dyDescent="0.55000000000000004">
       <c r="A146" s="10" t="s">
-        <v>295</v>
+        <v>233</v>
+      </c>
+      <c r="B146" s="6" t="s">
+        <v>230</v>
       </c>
       <c r="C146" s="7" t="s">
         <v>42</v>
       </c>
       <c r="D146" s="8" t="s">
-        <v>292</v>
+        <v>374</v>
+      </c>
+      <c r="E146" s="9" t="s">
+        <v>93</v>
+      </c>
+      <c r="F146" s="6">
+        <v>2</v>
       </c>
     </row>
     <row r="147" spans="1:7" ht="17.149999999999999" x14ac:dyDescent="0.55000000000000004">
       <c r="A147" s="10" t="s">
-        <v>213</v>
+        <v>100</v>
+      </c>
+      <c r="B147" s="6" t="s">
+        <v>102</v>
       </c>
       <c r="C147" s="7" t="s">
-        <v>42</v>
+        <v>6</v>
       </c>
       <c r="D147" s="8" t="s">
-        <v>359</v>
-      </c>
-      <c r="F147" s="6">
-        <v>2</v>
+        <v>101</v>
+      </c>
+      <c r="E147" s="9" t="s">
+        <v>103</v>
       </c>
     </row>
     <row r="148" spans="1:7" ht="17.149999999999999" x14ac:dyDescent="0.55000000000000004">
       <c r="A148" s="10" t="s">
-        <v>223</v>
+        <v>83</v>
       </c>
       <c r="B148" s="6" t="s">
-        <v>373</v>
+        <v>86</v>
       </c>
       <c r="C148" s="7" t="s">
-        <v>13</v>
+        <v>28</v>
       </c>
       <c r="D148" s="8" t="s">
-        <v>372</v>
-      </c>
-      <c r="F148" s="6">
-        <v>2</v>
-      </c>
-      <c r="G148" s="14" t="s">
-        <v>374</v>
+        <v>85</v>
+      </c>
+      <c r="E148" s="9" t="s">
+        <v>84</v>
       </c>
     </row>
     <row r="149" spans="1:7" ht="17.149999999999999" x14ac:dyDescent="0.55000000000000004">
       <c r="A149" s="10" t="s">
-        <v>394</v>
+        <v>251</v>
+      </c>
+      <c r="B149" s="6" t="s">
+        <v>36</v>
       </c>
       <c r="C149" s="7" t="s">
-        <v>42</v>
+        <v>80</v>
       </c>
       <c r="D149" s="8" t="s">
-        <v>395</v>
+        <v>383</v>
+      </c>
+      <c r="E149" s="9" t="s">
+        <v>128</v>
+      </c>
+      <c r="F149" s="6">
+        <v>2</v>
+      </c>
+      <c r="G149" s="14" t="s">
+        <v>384</v>
       </c>
     </row>
     <row r="150" spans="1:7" ht="17.149999999999999" x14ac:dyDescent="0.55000000000000004">
       <c r="A150" s="10" t="s">
-        <v>397</v>
+        <v>206</v>
       </c>
       <c r="C150" s="7" t="s">
         <v>13</v>
       </c>
       <c r="D150" s="8" t="s">
-        <v>395</v>
-      </c>
-      <c r="G150" s="14" t="s">
-        <v>396</v>
+        <v>417</v>
+      </c>
+      <c r="F150" s="6">
+        <v>3</v>
       </c>
     </row>
     <row r="151" spans="1:7" ht="17.149999999999999" x14ac:dyDescent="0.55000000000000004">
       <c r="A151" s="10" t="s">
-        <v>398</v>
+        <v>295</v>
       </c>
       <c r="C151" s="7" t="s">
-        <v>13</v>
+        <v>42</v>
       </c>
       <c r="D151" s="8" t="s">
-        <v>395</v>
+        <v>292</v>
       </c>
     </row>
     <row r="152" spans="1:7" ht="17.149999999999999" x14ac:dyDescent="0.55000000000000004">
       <c r="A152" s="10" t="s">
-        <v>399</v>
+        <v>213</v>
       </c>
       <c r="C152" s="7" t="s">
         <v>42</v>
       </c>
       <c r="D152" s="8" t="s">
-        <v>395</v>
-      </c>
-      <c r="E152" s="9" t="s">
-        <v>400</v>
-      </c>
-      <c r="G152" s="14" t="s">
-        <v>401</v>
+        <v>357</v>
+      </c>
+      <c r="F152" s="6">
+        <v>2</v>
       </c>
     </row>
     <row r="153" spans="1:7" ht="17.149999999999999" x14ac:dyDescent="0.55000000000000004">
       <c r="A153" s="10" t="s">
-        <v>402</v>
+        <v>223</v>
+      </c>
+      <c r="B153" s="6" t="s">
+        <v>371</v>
       </c>
       <c r="C153" s="7" t="s">
-        <v>42</v>
+        <v>13</v>
       </c>
       <c r="D153" s="8" t="s">
-        <v>403</v>
+        <v>370</v>
+      </c>
+      <c r="F153" s="6">
+        <v>2</v>
+      </c>
+      <c r="G153" s="14" t="s">
+        <v>372</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <hyperlinks>
-    <hyperlink ref="A14" r:id="rId1" xr:uid="{7EC56A7A-8F87-41C9-98CC-02AAAEBAB926}"/>
+    <hyperlink ref="A15" r:id="rId1" xr:uid="{7EC56A7A-8F87-41C9-98CC-02AAAEBAB926}"/>
     <hyperlink ref="A6" r:id="rId2" xr:uid="{F961E7A6-1882-4065-8755-4DFD95604133}"/>
-    <hyperlink ref="A12" r:id="rId3" xr:uid="{8C3CDFDC-25C9-4FAF-8F7E-2274E4D633B4}"/>
-    <hyperlink ref="A34" r:id="rId4" display="https://leetcode.cn/problems/maximum-profit-of-operating-a-centennial-wheel/" xr:uid="{8AD5B24F-C946-4CD2-A7ED-CBF4D294FFAC}"/>
-    <hyperlink ref="A111" r:id="rId5" display="https://leetcode.cn/problems/count-the-repetitions/" xr:uid="{2DEBCDEE-8626-4B8A-9670-020E98C7275E}"/>
-    <hyperlink ref="A65" r:id="rId6" display="https://leetcode.cn/problems/remove-nodes-from-linked-list/" xr:uid="{7D6CA718-D46A-4E15-A1D5-734F68A5EE6A}"/>
-    <hyperlink ref="A62" r:id="rId7" display="https://leetcode.cn/problems/maximum-rows-covered-by-columns/" xr:uid="{EED2AFE8-A6A7-4831-A7F5-3B09768F94A3}"/>
-    <hyperlink ref="A76" r:id="rId8" display="https://leetcode.cn/problems/insert-greatest-common-divisors-in-linked-list/" xr:uid="{410009FF-742C-4E80-BAA2-A97802718358}"/>
-    <hyperlink ref="A99" r:id="rId9" display="https://leetcode.cn/problems/ransom-note/" xr:uid="{C28C0659-D2BF-4FB5-BF7C-6C914E7BE129}"/>
-    <hyperlink ref="A108" r:id="rId10" display="https://leetcode.cn/problems/number-of-boomerangs/" xr:uid="{C9A2CFEA-3781-4A9D-A66D-C91B26C162F6}"/>
-    <hyperlink ref="A70" r:id="rId11" display="https://leetcode.cn/problems/extra-characters-in-a-string/" xr:uid="{0769EC96-3D92-4ADC-9FC1-59F0F89565CF}"/>
-    <hyperlink ref="A68" r:id="rId12" display="https://leetcode.cn/problems/minimum-string-length-after-removing-substrings/" xr:uid="{3ACDCC8B-C58D-4497-B33A-691E866EAA92}"/>
-    <hyperlink ref="A67" r:id="rId13" display="https://leetcode.cn/problems/minimum-additions-to-make-valid-string/" xr:uid="{ACAA46A8-EF23-4C78-847F-71BCFE4ACB27}"/>
-    <hyperlink ref="A48" r:id="rId14" display="https://leetcode.cn/problems/count-common-words-with-one-occurrence/" xr:uid="{BA928EDA-4915-4B02-BDA8-BDA4292CC77D}"/>
-    <hyperlink ref="A53" r:id="rId15" display="https://leetcode.cn/problems/construct-string-with-repeat-limit/" xr:uid="{DC040670-E1CD-48C5-9F39-7E50C4D4D598}"/>
+    <hyperlink ref="A13" r:id="rId3" xr:uid="{8C3CDFDC-25C9-4FAF-8F7E-2274E4D633B4}"/>
+    <hyperlink ref="A36" r:id="rId4" display="https://leetcode.cn/problems/maximum-profit-of-operating-a-centennial-wheel/" xr:uid="{8AD5B24F-C946-4CD2-A7ED-CBF4D294FFAC}"/>
+    <hyperlink ref="A115" r:id="rId5" display="https://leetcode.cn/problems/count-the-repetitions/" xr:uid="{2DEBCDEE-8626-4B8A-9670-020E98C7275E}"/>
+    <hyperlink ref="A68" r:id="rId6" display="https://leetcode.cn/problems/remove-nodes-from-linked-list/" xr:uid="{7D6CA718-D46A-4E15-A1D5-734F68A5EE6A}"/>
+    <hyperlink ref="A65" r:id="rId7" display="https://leetcode.cn/problems/maximum-rows-covered-by-columns/" xr:uid="{EED2AFE8-A6A7-4831-A7F5-3B09768F94A3}"/>
+    <hyperlink ref="A80" r:id="rId8" display="https://leetcode.cn/problems/insert-greatest-common-divisors-in-linked-list/" xr:uid="{410009FF-742C-4E80-BAA2-A97802718358}"/>
+    <hyperlink ref="A103" r:id="rId9" display="https://leetcode.cn/problems/ransom-note/" xr:uid="{C28C0659-D2BF-4FB5-BF7C-6C914E7BE129}"/>
+    <hyperlink ref="A112" r:id="rId10" display="https://leetcode.cn/problems/number-of-boomerangs/" xr:uid="{C9A2CFEA-3781-4A9D-A66D-C91B26C162F6}"/>
+    <hyperlink ref="A73" r:id="rId11" display="https://leetcode.cn/problems/extra-characters-in-a-string/" xr:uid="{0769EC96-3D92-4ADC-9FC1-59F0F89565CF}"/>
+    <hyperlink ref="A71" r:id="rId12" display="https://leetcode.cn/problems/minimum-string-length-after-removing-substrings/" xr:uid="{3ACDCC8B-C58D-4497-B33A-691E866EAA92}"/>
+    <hyperlink ref="A70" r:id="rId13" display="https://leetcode.cn/problems/minimum-additions-to-make-valid-string/" xr:uid="{ACAA46A8-EF23-4C78-847F-71BCFE4ACB27}"/>
+    <hyperlink ref="A51" r:id="rId14" display="https://leetcode.cn/problems/count-common-words-with-one-occurrence/" xr:uid="{BA928EDA-4915-4B02-BDA8-BDA4292CC77D}"/>
+    <hyperlink ref="A56" r:id="rId15" display="https://leetcode.cn/problems/construct-string-with-repeat-limit/" xr:uid="{DC040670-E1CD-48C5-9F39-7E50C4D4D598}"/>
     <hyperlink ref="A2" r:id="rId16" display="https://leetcode.cn/problems/two-sum/" xr:uid="{DCC2FC31-A6D8-4A22-B418-13AC2E7FF237}"/>
-    <hyperlink ref="A114" r:id="rId17" display="https://leetcode.cn/problems/group-anagrams/" xr:uid="{8499950A-1DCD-4E4A-9D9A-5A7F78C5486B}"/>
-    <hyperlink ref="A19" r:id="rId18" display="https://leetcode.cn/problems/longest-consecutive-sequence/" xr:uid="{AC05C0D0-F6E1-4797-A42E-1235E7280CF6}"/>
-    <hyperlink ref="A143" r:id="rId19" display="https://leetcode.cn/problems/remove-duplicates-from-sorted-list/" xr:uid="{BC1100E9-A72F-40CD-9106-5C6D7E369605}"/>
-    <hyperlink ref="A79" r:id="rId20" display="https://leetcode.cn/problems/move-zeroes/" xr:uid="{3D57A5B2-C773-46BB-AAC1-384F5B1330AC}"/>
-    <hyperlink ref="A131" r:id="rId21" display="https://leetcode.cn/problems/insert-into-a-sorted-circular-linked-list/" xr:uid="{ABF9182A-9A32-45E2-840F-96A729F2801D}"/>
-    <hyperlink ref="A9" r:id="rId22" display="https://leetcode.cn/problems/container-with-most-water/" xr:uid="{4ED7D754-A6D7-4998-BB92-60F7FE4E11B9}"/>
-    <hyperlink ref="A29" r:id="rId23" display="https://leetcode.cn/problems/3sum/" xr:uid="{0DBAA8D9-3DE9-4828-BFF8-655B84431AA9}"/>
-    <hyperlink ref="A105" r:id="rId24" display="https://leetcode.cn/problems/trapping-rain-water/" xr:uid="{9CEE3039-70C6-486C-95F2-1E34859BC2B5}"/>
-    <hyperlink ref="A142" r:id="rId25" display="https://leetcode.cn/problems/remove-duplicates-from-sorted-list-ii/" xr:uid="{95C218B7-1B8A-4890-A292-F56103A4F9BD}"/>
-    <hyperlink ref="A33" r:id="rId26" display="https://leetcode.cn/problems/binary-tree-upside-down/" xr:uid="{7BE5D44B-F504-4178-853A-BECE3A0D6D9A}"/>
-    <hyperlink ref="A86" r:id="rId27" display="https://leetcode.cn/problems/longest-substring-without-repeating-characters/" xr:uid="{3FB010E6-0492-4655-9911-820A190155C4}"/>
-    <hyperlink ref="A107" r:id="rId28" display="https://leetcode.cn/problems/find-all-anagrams-in-a-string/" xr:uid="{36A9C6AE-A4CD-4F4E-90F8-8E5D5CB43CAB}"/>
-    <hyperlink ref="A134" r:id="rId29" display="https://leetcode.cn/problems/sentence-similarity/" xr:uid="{771EA040-6E9F-427A-9C87-C5F54FA18B80}"/>
-    <hyperlink ref="A71" r:id="rId30" display="https://leetcode.cn/problems/count-of-integers/" xr:uid="{0F898565-2E05-4648-B060-6053E5749B06}"/>
-    <hyperlink ref="A125" r:id="rId31" display="https://leetcode.cn/problems/subarray-sum-equals-k/" xr:uid="{2C0B7B2D-05D9-44D3-94B3-5D2FA3D976DF}"/>
-    <hyperlink ref="A61" r:id="rId32" display="https://leetcode.cn/problems/sliding-window-maximum/" xr:uid="{0260B44B-AA2D-4584-91E2-1E8B8C0ED199}"/>
-    <hyperlink ref="A138" r:id="rId33" display="https://leetcode.cn/problems/minimum-window-substring/" xr:uid="{185B34CF-C6F2-486E-90A5-D7E59F55DC96}"/>
-    <hyperlink ref="A72" r:id="rId34" display="https://leetcode.cn/problems/find-maximum-number-of-string-pairs/" xr:uid="{70FF04F5-EBD7-4063-8275-F8933C1B9F4E}"/>
-    <hyperlink ref="A120" r:id="rId35" display="https://leetcode.cn/problems/maximum-subarray/" xr:uid="{8CC0531C-8284-4F55-81E2-94DB6B274D9B}"/>
-    <hyperlink ref="A124" r:id="rId36" display="https://leetcode.cn/problems/merge-intervals/" xr:uid="{A402C0BD-BF9F-430B-842D-C42671ADDBF0}"/>
-    <hyperlink ref="A52" r:id="rId37" display="https://leetcode.cn/problems/removing-minimum-number-of-magic-beans/" xr:uid="{E1638EC4-5083-49D4-8A0A-0D939842E19A}"/>
-    <hyperlink ref="A78" r:id="rId38" display="https://leetcode.cn/problems/minimum-time-to-make-array-sum-at-most-x/" xr:uid="{BE73385E-7540-4A08-A19F-5C1A292B516F}"/>
-    <hyperlink ref="A74" r:id="rId39" display="https://leetcode.cn/problems/split-strings-by-separator/" xr:uid="{8B634E5D-9C33-4C10-BAD7-AE6EBB649868}"/>
-    <hyperlink ref="A128" r:id="rId40" display="https://leetcode.cn/problems/maximum-swap/" xr:uid="{F5DE5192-A9D2-425F-9BB1-C2457DA674E4}"/>
-    <hyperlink ref="E128" r:id="rId41" xr:uid="{FA1BFA2A-460D-459E-8F61-B097678D8B32}"/>
-    <hyperlink ref="E74" r:id="rId42" xr:uid="{29C300A3-266F-408E-8AE8-11EC2B639857}"/>
-    <hyperlink ref="E78" r:id="rId43" xr:uid="{A2D78C4F-0CF7-4025-9816-818BF49AB72E}"/>
-    <hyperlink ref="E52" r:id="rId44" xr:uid="{28B1021B-6E63-4976-9056-8BE378A05916}"/>
-    <hyperlink ref="E124" r:id="rId45" xr:uid="{6B77CBE0-0575-4283-A5EA-AACEB5B33C59}"/>
-    <hyperlink ref="E120" r:id="rId46" xr:uid="{3229D6F6-BBF7-4C3B-B191-8DEB682A8FD3}"/>
-    <hyperlink ref="E72" r:id="rId47" xr:uid="{59B4691E-76E8-4849-BF65-B7D31AC7A96D}"/>
-    <hyperlink ref="E138" r:id="rId48" xr:uid="{4A2B3D38-4B96-4BF0-94E8-EF4F01DADA60}"/>
-    <hyperlink ref="E61" r:id="rId49" xr:uid="{AB333045-700E-4C04-88E4-D32E0F6DB718}"/>
-    <hyperlink ref="E125" r:id="rId50" xr:uid="{582C87DD-55DC-4B35-9852-0734F202A602}"/>
-    <hyperlink ref="E71" r:id="rId51" xr:uid="{9A949AF4-4EB7-44E4-BACF-B1D5B5248519}"/>
-    <hyperlink ref="E134" r:id="rId52" xr:uid="{70C2F0B7-B280-4BFB-BECF-378146CDDA35}"/>
-    <hyperlink ref="E107" r:id="rId53" xr:uid="{4FDD3B32-5D43-4481-A2CA-C7F81DDF97FA}"/>
-    <hyperlink ref="E86" r:id="rId54" xr:uid="{710F1479-585D-4444-83C8-6D53E855AFE0}"/>
-    <hyperlink ref="E33" r:id="rId55" xr:uid="{7B7DB3A6-D345-447E-9F9A-467C29F36D49}"/>
-    <hyperlink ref="E142" r:id="rId56" xr:uid="{48A15251-608D-4C90-AD44-6D4945946072}"/>
-    <hyperlink ref="E105" r:id="rId57" xr:uid="{BD52CDA8-8190-48A9-BD92-085140195F73}"/>
-    <hyperlink ref="E29" r:id="rId58" xr:uid="{06E19791-8255-436E-9548-022FA2F67FC7}"/>
-    <hyperlink ref="E9" r:id="rId59" xr:uid="{B4600BAD-5CAA-424F-AC24-FBBB647DADA7}"/>
-    <hyperlink ref="E131" r:id="rId60" xr:uid="{5A80CC00-AD3B-4F26-9D70-5D113E212D77}"/>
-    <hyperlink ref="E79" r:id="rId61" xr:uid="{F62B22C6-0054-4391-8F93-7DCA4A04B6C2}"/>
-    <hyperlink ref="E143" r:id="rId62" xr:uid="{E7AB61B6-DBA5-4869-B79F-21DEA0A21A2A}"/>
-    <hyperlink ref="E53" r:id="rId63" xr:uid="{6C0CBDDC-15AB-41BC-8AD8-3A7678612FFE}"/>
-    <hyperlink ref="E48" r:id="rId64" xr:uid="{C082DBA3-BF6F-4354-A2B9-4DFDBCA41E3F}"/>
-    <hyperlink ref="E67" r:id="rId65" xr:uid="{4AD655D4-539F-43D1-AF21-FD652B3B7D1A}"/>
-    <hyperlink ref="E68" r:id="rId66" xr:uid="{6654DC65-6E3C-44E1-BADC-DCD564B4B33E}"/>
-    <hyperlink ref="E70" r:id="rId67" xr:uid="{F9C5079A-479B-4956-BAE5-1257C7FF1A4A}"/>
-    <hyperlink ref="E108" r:id="rId68" xr:uid="{F4ADA86A-0680-4EA9-B429-CCBEA806CBA2}"/>
-    <hyperlink ref="E99" r:id="rId69" xr:uid="{FA483143-C671-4E08-BA2A-668803FBAF30}"/>
-    <hyperlink ref="E76" r:id="rId70" xr:uid="{687D1EF4-BE40-4253-9888-F0EFA784DFFE}"/>
-    <hyperlink ref="E62" r:id="rId71" xr:uid="{37A4ECD3-6A85-4A80-BADD-45ACC7A4BDAC}"/>
-    <hyperlink ref="E65" r:id="rId72" xr:uid="{1BB1D542-CE6A-4F15-BAD0-8E150E86DAEE}"/>
-    <hyperlink ref="E111" r:id="rId73" xr:uid="{C7FFAB8C-8294-407A-AF24-C9D1899CE796}"/>
-    <hyperlink ref="E34" r:id="rId74" xr:uid="{617A546E-9511-4EBF-8D70-85AF693926F3}"/>
-    <hyperlink ref="E12" r:id="rId75" xr:uid="{CD6D90A1-D877-434B-81B9-16DC26D192AD}"/>
+    <hyperlink ref="A118" r:id="rId17" display="https://leetcode.cn/problems/group-anagrams/" xr:uid="{8499950A-1DCD-4E4A-9D9A-5A7F78C5486B}"/>
+    <hyperlink ref="A20" r:id="rId18" display="https://leetcode.cn/problems/longest-consecutive-sequence/" xr:uid="{AC05C0D0-F6E1-4797-A42E-1235E7280CF6}"/>
+    <hyperlink ref="A148" r:id="rId19" display="https://leetcode.cn/problems/remove-duplicates-from-sorted-list/" xr:uid="{BC1100E9-A72F-40CD-9106-5C6D7E369605}"/>
+    <hyperlink ref="A83" r:id="rId20" display="https://leetcode.cn/problems/move-zeroes/" xr:uid="{3D57A5B2-C773-46BB-AAC1-384F5B1330AC}"/>
+    <hyperlink ref="A136" r:id="rId21" display="https://leetcode.cn/problems/insert-into-a-sorted-circular-linked-list/" xr:uid="{ABF9182A-9A32-45E2-840F-96A729F2801D}"/>
+    <hyperlink ref="A10" r:id="rId22" display="https://leetcode.cn/problems/container-with-most-water/" xr:uid="{4ED7D754-A6D7-4998-BB92-60F7FE4E11B9}"/>
+    <hyperlink ref="A31" r:id="rId23" display="https://leetcode.cn/problems/3sum/" xr:uid="{0DBAA8D9-3DE9-4828-BFF8-655B84431AA9}"/>
+    <hyperlink ref="A109" r:id="rId24" display="https://leetcode.cn/problems/trapping-rain-water/" xr:uid="{9CEE3039-70C6-486C-95F2-1E34859BC2B5}"/>
+    <hyperlink ref="A147" r:id="rId25" display="https://leetcode.cn/problems/remove-duplicates-from-sorted-list-ii/" xr:uid="{95C218B7-1B8A-4890-A292-F56103A4F9BD}"/>
+    <hyperlink ref="A35" r:id="rId26" display="https://leetcode.cn/problems/binary-tree-upside-down/" xr:uid="{7BE5D44B-F504-4178-853A-BECE3A0D6D9A}"/>
+    <hyperlink ref="A90" r:id="rId27" display="https://leetcode.cn/problems/longest-substring-without-repeating-characters/" xr:uid="{3FB010E6-0492-4655-9911-820A190155C4}"/>
+    <hyperlink ref="A111" r:id="rId28" display="https://leetcode.cn/problems/find-all-anagrams-in-a-string/" xr:uid="{36A9C6AE-A4CD-4F4E-90F8-8E5D5CB43CAB}"/>
+    <hyperlink ref="A139" r:id="rId29" display="https://leetcode.cn/problems/sentence-similarity/" xr:uid="{771EA040-6E9F-427A-9C87-C5F54FA18B80}"/>
+    <hyperlink ref="A74" r:id="rId30" display="https://leetcode.cn/problems/count-of-integers/" xr:uid="{0F898565-2E05-4648-B060-6053E5749B06}"/>
+    <hyperlink ref="A129" r:id="rId31" display="https://leetcode.cn/problems/subarray-sum-equals-k/" xr:uid="{2C0B7B2D-05D9-44D3-94B3-5D2FA3D976DF}"/>
+    <hyperlink ref="A64" r:id="rId32" display="https://leetcode.cn/problems/sliding-window-maximum/" xr:uid="{0260B44B-AA2D-4584-91E2-1E8B8C0ED199}"/>
+    <hyperlink ref="A143" r:id="rId33" display="https://leetcode.cn/problems/minimum-window-substring/" xr:uid="{185B34CF-C6F2-486E-90A5-D7E59F55DC96}"/>
+    <hyperlink ref="A75" r:id="rId34" display="https://leetcode.cn/problems/find-maximum-number-of-string-pairs/" xr:uid="{70FF04F5-EBD7-4063-8275-F8933C1B9F4E}"/>
+    <hyperlink ref="A124" r:id="rId35" display="https://leetcode.cn/problems/maximum-subarray/" xr:uid="{8CC0531C-8284-4F55-81E2-94DB6B274D9B}"/>
+    <hyperlink ref="A128" r:id="rId36" display="https://leetcode.cn/problems/merge-intervals/" xr:uid="{A402C0BD-BF9F-430B-842D-C42671ADDBF0}"/>
+    <hyperlink ref="A55" r:id="rId37" display="https://leetcode.cn/problems/removing-minimum-number-of-magic-beans/" xr:uid="{E1638EC4-5083-49D4-8A0A-0D939842E19A}"/>
+    <hyperlink ref="A82" r:id="rId38" display="https://leetcode.cn/problems/minimum-time-to-make-array-sum-at-most-x/" xr:uid="{BE73385E-7540-4A08-A19F-5C1A292B516F}"/>
+    <hyperlink ref="A77" r:id="rId39" display="https://leetcode.cn/problems/split-strings-by-separator/" xr:uid="{8B634E5D-9C33-4C10-BAD7-AE6EBB649868}"/>
+    <hyperlink ref="A133" r:id="rId40" display="https://leetcode.cn/problems/maximum-swap/" xr:uid="{F5DE5192-A9D2-425F-9BB1-C2457DA674E4}"/>
+    <hyperlink ref="E133" r:id="rId41" xr:uid="{FA1BFA2A-460D-459E-8F61-B097678D8B32}"/>
+    <hyperlink ref="E77" r:id="rId42" xr:uid="{29C300A3-266F-408E-8AE8-11EC2B639857}"/>
+    <hyperlink ref="E82" r:id="rId43" xr:uid="{A2D78C4F-0CF7-4025-9816-818BF49AB72E}"/>
+    <hyperlink ref="E55" r:id="rId44" xr:uid="{28B1021B-6E63-4976-9056-8BE378A05916}"/>
+    <hyperlink ref="E128" r:id="rId45" xr:uid="{6B77CBE0-0575-4283-A5EA-AACEB5B33C59}"/>
+    <hyperlink ref="E124" r:id="rId46" xr:uid="{3229D6F6-BBF7-4C3B-B191-8DEB682A8FD3}"/>
+    <hyperlink ref="E75" r:id="rId47" xr:uid="{59B4691E-76E8-4849-BF65-B7D31AC7A96D}"/>
+    <hyperlink ref="E143" r:id="rId48" xr:uid="{4A2B3D38-4B96-4BF0-94E8-EF4F01DADA60}"/>
+    <hyperlink ref="E64" r:id="rId49" xr:uid="{AB333045-700E-4C04-88E4-D32E0F6DB718}"/>
+    <hyperlink ref="E129" r:id="rId50" xr:uid="{582C87DD-55DC-4B35-9852-0734F202A602}"/>
+    <hyperlink ref="E74" r:id="rId51" xr:uid="{9A949AF4-4EB7-44E4-BACF-B1D5B5248519}"/>
+    <hyperlink ref="E139" r:id="rId52" xr:uid="{70C2F0B7-B280-4BFB-BECF-378146CDDA35}"/>
+    <hyperlink ref="E111" r:id="rId53" xr:uid="{4FDD3B32-5D43-4481-A2CA-C7F81DDF97FA}"/>
+    <hyperlink ref="E90" r:id="rId54" xr:uid="{710F1479-585D-4444-83C8-6D53E855AFE0}"/>
+    <hyperlink ref="E35" r:id="rId55" xr:uid="{7B7DB3A6-D345-447E-9F9A-467C29F36D49}"/>
+    <hyperlink ref="E147" r:id="rId56" xr:uid="{48A15251-608D-4C90-AD44-6D4945946072}"/>
+    <hyperlink ref="E109" r:id="rId57" xr:uid="{BD52CDA8-8190-48A9-BD92-085140195F73}"/>
+    <hyperlink ref="E31" r:id="rId58" xr:uid="{06E19791-8255-436E-9548-022FA2F67FC7}"/>
+    <hyperlink ref="E10" r:id="rId59" xr:uid="{B4600BAD-5CAA-424F-AC24-FBBB647DADA7}"/>
+    <hyperlink ref="E136" r:id="rId60" xr:uid="{5A80CC00-AD3B-4F26-9D70-5D113E212D77}"/>
+    <hyperlink ref="E83" r:id="rId61" xr:uid="{F62B22C6-0054-4391-8F93-7DCA4A04B6C2}"/>
+    <hyperlink ref="E148" r:id="rId62" xr:uid="{E7AB61B6-DBA5-4869-B79F-21DEA0A21A2A}"/>
+    <hyperlink ref="E56" r:id="rId63" xr:uid="{6C0CBDDC-15AB-41BC-8AD8-3A7678612FFE}"/>
+    <hyperlink ref="E51" r:id="rId64" xr:uid="{C082DBA3-BF6F-4354-A2B9-4DFDBCA41E3F}"/>
+    <hyperlink ref="E70" r:id="rId65" xr:uid="{4AD655D4-539F-43D1-AF21-FD652B3B7D1A}"/>
+    <hyperlink ref="E71" r:id="rId66" xr:uid="{6654DC65-6E3C-44E1-BADC-DCD564B4B33E}"/>
+    <hyperlink ref="E73" r:id="rId67" xr:uid="{F9C5079A-479B-4956-BAE5-1257C7FF1A4A}"/>
+    <hyperlink ref="E112" r:id="rId68" xr:uid="{F4ADA86A-0680-4EA9-B429-CCBEA806CBA2}"/>
+    <hyperlink ref="E103" r:id="rId69" xr:uid="{FA483143-C671-4E08-BA2A-668803FBAF30}"/>
+    <hyperlink ref="E80" r:id="rId70" xr:uid="{687D1EF4-BE40-4253-9888-F0EFA784DFFE}"/>
+    <hyperlink ref="E65" r:id="rId71" xr:uid="{37A4ECD3-6A85-4A80-BADD-45ACC7A4BDAC}"/>
+    <hyperlink ref="E68" r:id="rId72" xr:uid="{1BB1D542-CE6A-4F15-BAD0-8E150E86DAEE}"/>
+    <hyperlink ref="E115" r:id="rId73" xr:uid="{C7FFAB8C-8294-407A-AF24-C9D1899CE796}"/>
+    <hyperlink ref="E36" r:id="rId74" xr:uid="{617A546E-9511-4EBF-8D70-85AF693926F3}"/>
+    <hyperlink ref="E13" r:id="rId75" xr:uid="{CD6D90A1-D877-434B-81B9-16DC26D192AD}"/>
     <hyperlink ref="E6" r:id="rId76" xr:uid="{87493A55-61B0-4662-A5B3-056967B0FE81}"/>
-    <hyperlink ref="E14" r:id="rId77" xr:uid="{2A03A969-6173-48EC-895A-2E4A35DA8F61}"/>
-    <hyperlink ref="A73" r:id="rId78" display="https://leetcode.cn/problems/longest-alternating-subarray/" xr:uid="{CE31139F-E3AD-47E7-A3DA-C247DEA5E681}"/>
-    <hyperlink ref="E73" r:id="rId79" xr:uid="{6C7253B6-9882-48B6-9A61-350BC52E34FE}"/>
-    <hyperlink ref="A83" r:id="rId80" display="https://leetcode.cn/problems/beautiful-towers-i/" xr:uid="{422E3E39-04D0-4C02-B237-FCAE1C661020}"/>
-    <hyperlink ref="E83" r:id="rId81" xr:uid="{88E2BA58-53D9-47A6-8186-881DD7B82E77}"/>
-    <hyperlink ref="A81" r:id="rId82" display="https://leetcode.cn/problems/sum-of-values-at-indices-with-k-set-bits/" xr:uid="{72686F91-2315-43ED-89E4-333E7C31926A}"/>
-    <hyperlink ref="A80" r:id="rId83" display="https://leetcode.cn/problems/minimum-edge-weight-equilibrium-queries-in-a-tree/" xr:uid="{715DDDC7-F3F9-4482-87DF-B8F707D5596F}"/>
-    <hyperlink ref="A82" r:id="rId84" display="https://leetcode.cn/problems/maximum-number-of-alloys/" xr:uid="{0ED65D93-5F0A-4C8F-8661-5D174085FFCE}"/>
-    <hyperlink ref="A97" r:id="rId85" display="https://leetcode.cn/problems/water-and-jug-problem/" xr:uid="{E5E9E3F5-D048-46DB-B377-9A61CA8A8946}"/>
-    <hyperlink ref="A118" r:id="rId86" display="https://leetcode.cn/problems/freedom-trail/" xr:uid="{A2C0B38F-65D7-44C4-9DF1-646C455842FC}"/>
-    <hyperlink ref="E118" r:id="rId87" xr:uid="{8699ADAE-95F0-4472-B227-9AA2813AA692}"/>
-    <hyperlink ref="A77" r:id="rId88" display="https://leetcode.cn/problems/minimum-seconds-to-equalize-a-circular-array/" xr:uid="{5C9C077F-45A3-452D-AC9D-D25D1D690EA2}"/>
-    <hyperlink ref="A38" r:id="rId89" xr:uid="{66EB66A9-8D6B-4BF6-A6C3-8A5954733BBF}"/>
-    <hyperlink ref="A60" r:id="rId90" display="https://leetcode.cn/problems/product-of-array-except-self/" xr:uid="{A190E6D7-6DC0-41FF-B880-4504E51AD0A8}"/>
-    <hyperlink ref="A103" r:id="rId91" display="https://leetcode.cn/problems/first-missing-positive/" xr:uid="{D6CDA410-39D8-4983-9BDC-15727DEDFCB0}"/>
-    <hyperlink ref="A133" r:id="rId92" display="https://leetcode.cn/problems/set-matrix-zeroes/" xr:uid="{C6A1E3B1-09D2-47A0-860B-48FEEBC1056B}"/>
-    <hyperlink ref="E133" r:id="rId93" xr:uid="{078E7176-F40A-4347-A445-D7A9552A387A}"/>
-    <hyperlink ref="A121" r:id="rId94" display="https://leetcode.cn/problems/spiral-matrix/" xr:uid="{F8766E35-A34B-4EFF-BDF3-0B4AC5DB8C10}"/>
-    <hyperlink ref="E121" r:id="rId95" xr:uid="{2D32183A-312F-4B64-A30F-0AB4B3726872}"/>
-    <hyperlink ref="A113" r:id="rId96" display="https://leetcode.cn/problems/rotate-image/" xr:uid="{5CD1B5B0-1C26-42C3-A789-7C54A1599DD5}"/>
-    <hyperlink ref="E113" r:id="rId97" xr:uid="{66D6968F-8499-47FC-9ABF-2814B77BDCB5}"/>
-    <hyperlink ref="A64" r:id="rId98" display="https://leetcode.cn/problems/search-a-2d-matrix-ii/" xr:uid="{ED4084D7-2655-4CA6-935F-AF9C27B5F84E}"/>
-    <hyperlink ref="E64" r:id="rId99" xr:uid="{371CE243-99B4-4416-810C-2B026B3F2BD8}"/>
-    <hyperlink ref="A35" r:id="rId100" display="https://leetcode.cn/problems/intersection-of-two-linked-lists/" xr:uid="{292AE10F-3B80-4BCE-B10F-041CC4AE4405}"/>
-    <hyperlink ref="A45" r:id="rId101" display="https://leetcode.cn/problems/reverse-linked-list/" xr:uid="{42B5B9DD-E787-4DDD-B00C-AC502AC14EBE}"/>
-    <hyperlink ref="A58" r:id="rId102" display="https://leetcode.cn/problems/palindrome-linked-list/" xr:uid="{3D9FB9AA-16D7-4F6F-AC03-B6BC2A3216BD}"/>
-    <hyperlink ref="A24" r:id="rId103" display="https://leetcode.cn/problems/linked-list-cycle/" xr:uid="{45893E70-1C1D-4F5A-80D5-B9498F0463D8}"/>
-    <hyperlink ref="A25" r:id="rId104" display="https://leetcode.cn/problems/linked-list-cycle-ii/" xr:uid="{AA6FE3C6-2E73-4EFD-A132-9E337F8D1562}"/>
-    <hyperlink ref="A49" r:id="rId105" display="https://leetcode.cn/problems/merge-two-sorted-lists/" xr:uid="{39409391-1893-4957-B20F-06437CA45923}"/>
-    <hyperlink ref="A42" r:id="rId106" display="https://leetcode.cn/problems/add-two-numbers/" xr:uid="{616C0CC1-D70D-4E3F-ABB5-494680939B0D}"/>
-    <hyperlink ref="A39" r:id="rId107" display="https://leetcode.cn/problems/remove-nth-node-from-end-of-list/" xr:uid="{6D487B38-6448-49A2-AF76-FF75034F6EDB}"/>
-    <hyperlink ref="A66" r:id="rId108" display="https://leetcode.cn/problems/reverse-nodes-in-k-group/" xr:uid="{FA1E34C3-C166-4D72-A30B-915F3F50CFF9}"/>
-    <hyperlink ref="A22" r:id="rId109" display="https://leetcode.cn/problems/copy-list-with-random-pointer/" xr:uid="{8D07E3E8-2095-44A3-A434-D33E7A1B9CB1}"/>
-    <hyperlink ref="E22" r:id="rId110" xr:uid="{15B76AA8-DD34-4170-8429-D661393E432B}"/>
-    <hyperlink ref="A28" r:id="rId111" display="https://leetcode.cn/problems/sort-list/" xr:uid="{C5653710-89D2-47AD-A92A-5BF876E756D0}"/>
-    <hyperlink ref="A56" r:id="rId112" display="https://leetcode.cn/problems/merge-k-sorted-lists/" xr:uid="{24641442-A295-4EC8-88E5-B0C09E4F3CAC}"/>
-    <hyperlink ref="A27" r:id="rId113" display="https://leetcode.cn/problems/lru-cache/" xr:uid="{B795428B-A2E2-46EA-A417-AF8114C9EF23}"/>
-    <hyperlink ref="A145" r:id="rId114" display="https://leetcode.cn/problems/binary-tree-inorder-traversal/" xr:uid="{BA958F34-070C-4276-8418-94164694D26B}"/>
+    <hyperlink ref="E15" r:id="rId77" xr:uid="{2A03A969-6173-48EC-895A-2E4A35DA8F61}"/>
+    <hyperlink ref="A76" r:id="rId78" display="https://leetcode.cn/problems/longest-alternating-subarray/" xr:uid="{CE31139F-E3AD-47E7-A3DA-C247DEA5E681}"/>
+    <hyperlink ref="E76" r:id="rId79" xr:uid="{6C7253B6-9882-48B6-9A61-350BC52E34FE}"/>
+    <hyperlink ref="A87" r:id="rId80" display="https://leetcode.cn/problems/beautiful-towers-i/" xr:uid="{422E3E39-04D0-4C02-B237-FCAE1C661020}"/>
+    <hyperlink ref="E87" r:id="rId81" xr:uid="{88E2BA58-53D9-47A6-8186-881DD7B82E77}"/>
+    <hyperlink ref="A85" r:id="rId82" display="https://leetcode.cn/problems/sum-of-values-at-indices-with-k-set-bits/" xr:uid="{72686F91-2315-43ED-89E4-333E7C31926A}"/>
+    <hyperlink ref="A84" r:id="rId83" display="https://leetcode.cn/problems/minimum-edge-weight-equilibrium-queries-in-a-tree/" xr:uid="{715DDDC7-F3F9-4482-87DF-B8F707D5596F}"/>
+    <hyperlink ref="A86" r:id="rId84" display="https://leetcode.cn/problems/maximum-number-of-alloys/" xr:uid="{0ED65D93-5F0A-4C8F-8661-5D174085FFCE}"/>
+    <hyperlink ref="A101" r:id="rId85" display="https://leetcode.cn/problems/water-and-jug-problem/" xr:uid="{E5E9E3F5-D048-46DB-B377-9A61CA8A8946}"/>
+    <hyperlink ref="A122" r:id="rId86" display="https://leetcode.cn/problems/freedom-trail/" xr:uid="{A2C0B38F-65D7-44C4-9DF1-646C455842FC}"/>
+    <hyperlink ref="E122" r:id="rId87" xr:uid="{8699ADAE-95F0-4472-B227-9AA2813AA692}"/>
+    <hyperlink ref="A81" r:id="rId88" display="https://leetcode.cn/problems/minimum-seconds-to-equalize-a-circular-array/" xr:uid="{5C9C077F-45A3-452D-AC9D-D25D1D690EA2}"/>
+    <hyperlink ref="A41" r:id="rId89" xr:uid="{66EB66A9-8D6B-4BF6-A6C3-8A5954733BBF}"/>
+    <hyperlink ref="A63" r:id="rId90" display="https://leetcode.cn/problems/product-of-array-except-self/" xr:uid="{A190E6D7-6DC0-41FF-B880-4504E51AD0A8}"/>
+    <hyperlink ref="A107" r:id="rId91" display="https://leetcode.cn/problems/first-missing-positive/" xr:uid="{D6CDA410-39D8-4983-9BDC-15727DEDFCB0}"/>
+    <hyperlink ref="A138" r:id="rId92" display="https://leetcode.cn/problems/set-matrix-zeroes/" xr:uid="{C6A1E3B1-09D2-47A0-860B-48FEEBC1056B}"/>
+    <hyperlink ref="E138" r:id="rId93" xr:uid="{078E7176-F40A-4347-A445-D7A9552A387A}"/>
+    <hyperlink ref="A125" r:id="rId94" display="https://leetcode.cn/problems/spiral-matrix/" xr:uid="{F8766E35-A34B-4EFF-BDF3-0B4AC5DB8C10}"/>
+    <hyperlink ref="E125" r:id="rId95" xr:uid="{2D32183A-312F-4B64-A30F-0AB4B3726872}"/>
+    <hyperlink ref="A117" r:id="rId96" display="https://leetcode.cn/problems/rotate-image/" xr:uid="{5CD1B5B0-1C26-42C3-A789-7C54A1599DD5}"/>
+    <hyperlink ref="E117" r:id="rId97" xr:uid="{66D6968F-8499-47FC-9ABF-2814B77BDCB5}"/>
+    <hyperlink ref="A67" r:id="rId98" display="https://leetcode.cn/problems/search-a-2d-matrix-ii/" xr:uid="{ED4084D7-2655-4CA6-935F-AF9C27B5F84E}"/>
+    <hyperlink ref="E67" r:id="rId99" xr:uid="{371CE243-99B4-4416-810C-2B026B3F2BD8}"/>
+    <hyperlink ref="A37" r:id="rId100" display="https://leetcode.cn/problems/intersection-of-two-linked-lists/" xr:uid="{292AE10F-3B80-4BCE-B10F-041CC4AE4405}"/>
+    <hyperlink ref="A48" r:id="rId101" display="https://leetcode.cn/problems/reverse-linked-list/" xr:uid="{42B5B9DD-E787-4DDD-B00C-AC502AC14EBE}"/>
+    <hyperlink ref="A61" r:id="rId102" display="https://leetcode.cn/problems/palindrome-linked-list/" xr:uid="{3D9FB9AA-16D7-4F6F-AC03-B6BC2A3216BD}"/>
+    <hyperlink ref="A25" r:id="rId103" display="https://leetcode.cn/problems/linked-list-cycle/" xr:uid="{45893E70-1C1D-4F5A-80D5-B9498F0463D8}"/>
+    <hyperlink ref="A26" r:id="rId104" display="https://leetcode.cn/problems/linked-list-cycle-ii/" xr:uid="{AA6FE3C6-2E73-4EFD-A132-9E337F8D1562}"/>
+    <hyperlink ref="A52" r:id="rId105" display="https://leetcode.cn/problems/merge-two-sorted-lists/" xr:uid="{39409391-1893-4957-B20F-06437CA45923}"/>
+    <hyperlink ref="A45" r:id="rId106" display="https://leetcode.cn/problems/add-two-numbers/" xr:uid="{616C0CC1-D70D-4E3F-ABB5-494680939B0D}"/>
+    <hyperlink ref="A42" r:id="rId107" display="https://leetcode.cn/problems/remove-nth-node-from-end-of-list/" xr:uid="{6D487B38-6448-49A2-AF76-FF75034F6EDB}"/>
+    <hyperlink ref="A69" r:id="rId108" display="https://leetcode.cn/problems/reverse-nodes-in-k-group/" xr:uid="{FA1E34C3-C166-4D72-A30B-915F3F50CFF9}"/>
+    <hyperlink ref="A23" r:id="rId109" display="https://leetcode.cn/problems/copy-list-with-random-pointer/" xr:uid="{8D07E3E8-2095-44A3-A434-D33E7A1B9CB1}"/>
+    <hyperlink ref="E23" r:id="rId110" xr:uid="{15B76AA8-DD34-4170-8429-D661393E432B}"/>
+    <hyperlink ref="A30" r:id="rId111" display="https://leetcode.cn/problems/sort-list/" xr:uid="{C5653710-89D2-47AD-A92A-5BF876E756D0}"/>
+    <hyperlink ref="A59" r:id="rId112" display="https://leetcode.cn/problems/merge-k-sorted-lists/" xr:uid="{24641442-A295-4EC8-88E5-B0C09E4F3CAC}"/>
+    <hyperlink ref="A29" r:id="rId113" display="https://leetcode.cn/problems/lru-cache/" xr:uid="{B795428B-A2E2-46EA-A417-AF8114C9EF23}"/>
+    <hyperlink ref="A150" r:id="rId114" display="https://leetcode.cn/problems/binary-tree-inorder-traversal/" xr:uid="{BA958F34-070C-4276-8418-94164694D26B}"/>
     <hyperlink ref="A5" r:id="rId115" display="https://leetcode.cn/problems/maximum-depth-of-binary-tree/" xr:uid="{E2779ECC-F6F2-4721-B2AF-013E62B4A44D}"/>
-    <hyperlink ref="A55" r:id="rId116" display="https://leetcode.cn/problems/invert-binary-tree/" xr:uid="{82BC3859-2166-43DC-BCBF-3CB1A966F7A6}"/>
+    <hyperlink ref="A58" r:id="rId116" display="https://leetcode.cn/problems/invert-binary-tree/" xr:uid="{82BC3859-2166-43DC-BCBF-3CB1A966F7A6}"/>
     <hyperlink ref="A3" r:id="rId117" display="https://leetcode.cn/problems/symmetric-tree/" xr:uid="{B28785EA-ECDF-44CC-8B01-1E8171DD13CE}"/>
-    <hyperlink ref="A122" r:id="rId118" display="https://leetcode.cn/problems/diameter-of-binary-tree/" xr:uid="{2359DD9C-2BD5-4AEC-B348-6813975B7912}"/>
+    <hyperlink ref="A126" r:id="rId118" display="https://leetcode.cn/problems/diameter-of-binary-tree/" xr:uid="{2359DD9C-2BD5-4AEC-B348-6813975B7912}"/>
     <hyperlink ref="A4" r:id="rId119" display="https://leetcode.cn/problems/binary-tree-level-order-traversal/" xr:uid="{1D68961A-6E60-46DE-B611-D7B5D25133FB}"/>
-    <hyperlink ref="A8" r:id="rId120" display="https://leetcode.cn/problems/convert-sorted-array-to-binary-search-tree/" xr:uid="{328BE4BD-3DD5-4615-826F-93546C63D4B0}"/>
-    <hyperlink ref="A147" r:id="rId121" display="https://leetcode.cn/problems/validate-binary-search-tree/" xr:uid="{743EA17A-87FE-4F4B-B0BF-739F3BEC24BD}"/>
-    <hyperlink ref="A57" r:id="rId122" display="https://leetcode.cn/problems/kth-smallest-element-in-a-bst/" xr:uid="{E8952E47-A552-42F7-872B-3FB6F8ABE394}"/>
-    <hyperlink ref="A41" r:id="rId123" display="https://leetcode.cn/problems/binary-tree-right-side-view/" xr:uid="{742E0E19-C628-4E6A-A389-82FC923F760C}"/>
-    <hyperlink ref="A10" r:id="rId124" display="https://leetcode.cn/problems/flatten-binary-tree-to-linked-list/" xr:uid="{11440A7B-C0FC-418F-8923-563E96F7E5C0}"/>
+    <hyperlink ref="A9" r:id="rId120" display="https://leetcode.cn/problems/convert-sorted-array-to-binary-search-tree/" xr:uid="{328BE4BD-3DD5-4615-826F-93546C63D4B0}"/>
+    <hyperlink ref="A152" r:id="rId121" display="https://leetcode.cn/problems/validate-binary-search-tree/" xr:uid="{743EA17A-87FE-4F4B-B0BF-739F3BEC24BD}"/>
+    <hyperlink ref="A60" r:id="rId122" display="https://leetcode.cn/problems/kth-smallest-element-in-a-bst/" xr:uid="{E8952E47-A552-42F7-872B-3FB6F8ABE394}"/>
+    <hyperlink ref="A44" r:id="rId123" display="https://leetcode.cn/problems/binary-tree-right-side-view/" xr:uid="{742E0E19-C628-4E6A-A389-82FC923F760C}"/>
+    <hyperlink ref="A11" r:id="rId124" display="https://leetcode.cn/problems/flatten-binary-tree-to-linked-list/" xr:uid="{11440A7B-C0FC-418F-8923-563E96F7E5C0}"/>
     <hyperlink ref="A7" r:id="rId125" display="https://leetcode.cn/problems/construct-binary-tree-from-preorder-and-inorder-traversal/" xr:uid="{3A9D1B28-E972-4D8B-82BE-26C4566DAF4F}"/>
-    <hyperlink ref="A106" r:id="rId126" display="https://leetcode.cn/problems/path-sum-iii/" xr:uid="{05551963-434C-40D6-A149-D640646C016A}"/>
-    <hyperlink ref="A59" r:id="rId127" display="https://leetcode.cn/problems/lowest-common-ancestor-of-a-binary-tree/" xr:uid="{C283A30B-A9D0-4642-834C-77EE1E2A81E8}"/>
-    <hyperlink ref="E59" r:id="rId128" xr:uid="{A9C856D9-9F85-4925-88CC-FF911C4EFD32}"/>
-    <hyperlink ref="A18" r:id="rId129" display="https://leetcode.cn/problems/binary-tree-maximum-path-sum/" xr:uid="{3678B77A-8804-4A64-AE6C-41376D22B9BC}"/>
-    <hyperlink ref="A44" r:id="rId130" display="https://leetcode.cn/problems/number-of-islands/" xr:uid="{A328C414-4CF6-4425-A56A-201C9BC6AD15}"/>
-    <hyperlink ref="A148" r:id="rId131" display="https://leetcode.cn/problems/rotting-oranges/" xr:uid="{C47F4890-A65B-4EA6-BE20-E06AFE42305B}"/>
-    <hyperlink ref="A46" r:id="rId132" display="https://leetcode.cn/problems/course-schedule/" xr:uid="{E474195F-F1D8-4B40-A072-95AA82E77F7B}"/>
-    <hyperlink ref="A47" r:id="rId133" display="https://leetcode.cn/problems/implement-trie-prefix-tree/" xr:uid="{ACDFE2DE-83AA-4BAD-8166-E20BAC48A7C3}"/>
-    <hyperlink ref="E110" r:id="rId134" xr:uid="{2E898F41-BA84-45AF-A705-0973EB8DB8EE}"/>
-    <hyperlink ref="A110" r:id="rId135" display="https://leetcode.cn/problems/permutations/" xr:uid="{8E4E13D8-2A7F-4DC6-A48B-A54ED93B27C0}"/>
-    <hyperlink ref="A140" r:id="rId136" display="https://leetcode.cn/problems/subsets/" xr:uid="{5C409365-541F-4E98-97A1-A1E29CC4F14F}"/>
-    <hyperlink ref="E140" r:id="rId137" xr:uid="{93490963-1363-4F0C-8181-651E214E0B18}"/>
-    <hyperlink ref="A37" r:id="rId138" display="https://leetcode.cn/problems/letter-combinations-of-a-phone-number/" xr:uid="{A72E7149-0969-4B87-A7FC-139F18FFD8BB}"/>
-    <hyperlink ref="E37" r:id="rId139" xr:uid="{31CD6DD9-B828-43FC-B338-7CAE71F2DFDF}"/>
-    <hyperlink ref="A100" r:id="rId140" display="https://leetcode.cn/problems/combination-sum/" xr:uid="{EFF7251F-6EB1-4CC3-B4A9-227B600CFFA1}"/>
-    <hyperlink ref="E141" r:id="rId141" xr:uid="{D009558D-60D6-4366-8677-9423BF894976}"/>
-    <hyperlink ref="A141" r:id="rId142" display="https://leetcode.cn/problems/word-search/" xr:uid="{6E176417-751F-4EED-B7EB-3128CCF61581}"/>
-    <hyperlink ref="A54" r:id="rId143" display="https://leetcode.cn/problems/generate-parentheses/" xr:uid="{30406B0C-B20F-496A-A2C4-D948173189C3}"/>
-    <hyperlink ref="A20" r:id="rId144" display="https://leetcode.cn/problems/palindrome-partitioning/" xr:uid="{C1C42340-3C82-4BD1-8608-8DFFF96FC75B}"/>
-    <hyperlink ref="A117" r:id="rId145" display="https://leetcode.cn/problems/n-queens/" xr:uid="{A0187B26-61AC-4C97-9A36-85A591E506B7}"/>
-    <hyperlink ref="E117" r:id="rId146" location="%E5%85%B6%E4%BB%96%E8%AF%AD%E8%A8%80%E8%A1%A5%E5%85%85" xr:uid="{7968323D-D06A-46E1-9DFB-D49E602D499C}"/>
-    <hyperlink ref="E94" r:id="rId147" xr:uid="{DDCFD87D-CD38-43E5-ADAF-24E527C68F8E}"/>
-    <hyperlink ref="A94" r:id="rId148" display="https://leetcode.cn/problems/find-first-and-last-position-of-element-in-sorted-array/" xr:uid="{BF08E923-B4D9-4EEF-8E92-E28C605CCE32}"/>
-    <hyperlink ref="A96" r:id="rId149" display="https://leetcode.cn/problems/search-insert-position/" xr:uid="{54241F2B-5AB4-4177-BC7C-5360532D265E}"/>
-    <hyperlink ref="A136" r:id="rId150" display="https://leetcode.cn/problems/search-a-2d-matrix/" xr:uid="{B827C295-310F-4C1E-8C97-04E52B4E0D8F}"/>
-    <hyperlink ref="E92" r:id="rId151" xr:uid="{66A0E0DB-2AE8-4C0D-B11E-7E0DDADB9B41}"/>
-    <hyperlink ref="A92" r:id="rId152" display="https://leetcode.cn/problems/search-in-rotated-sorted-array/" xr:uid="{B22B927E-2356-4B4E-BF35-F484D36559D4}"/>
-    <hyperlink ref="A31" r:id="rId153" display="https://leetcode.cn/problems/find-minimum-in-rotated-sorted-array/" xr:uid="{397D2DAE-9BE0-4951-B83D-824D7FBCE07E}"/>
-    <hyperlink ref="E102" r:id="rId154" xr:uid="{90EC8E40-2D47-4398-939E-3F09E808796E}"/>
-    <hyperlink ref="A43" r:id="rId155" display="https://leetcode.cn/problems/valid-parentheses/" xr:uid="{4BE72628-010D-4D86-BD85-8830898F69F1}"/>
-    <hyperlink ref="A102" r:id="rId156" display="https://leetcode.cn/problems/median-of-two-sorted-arrays/" xr:uid="{47FFFE22-7443-4E70-84C1-E1352C5D0139}"/>
-    <hyperlink ref="E32" r:id="rId157" xr:uid="{BC8DED09-4E1C-410D-A7D9-76EF7EA14100}"/>
-    <hyperlink ref="A32" r:id="rId158" display="https://leetcode.cn/problems/min-stack/" xr:uid="{BD6D5A5D-9717-4253-A2F5-A43EC62D1A5D}"/>
-    <hyperlink ref="A101" r:id="rId159" display="https://leetcode.cn/problems/decode-string/" xr:uid="{0B4CACA8-1935-41CF-967A-CAEFF5AECB53}"/>
-    <hyperlink ref="E101" r:id="rId160" xr:uid="{819C9DBC-04AA-4864-81C9-0C3EFC02339D}"/>
-    <hyperlink ref="A135" r:id="rId161" display="https://leetcode.cn/problems/daily-temperatures/" xr:uid="{B26C3125-EB8A-4499-B55F-A0327D4C49FD}"/>
-    <hyperlink ref="E135" r:id="rId162" xr:uid="{71B5751F-3CF1-4DC3-931E-B157AACD6558}"/>
-    <hyperlink ref="A144" r:id="rId163" display="https://leetcode.cn/problems/largest-rectangle-in-histogram/" xr:uid="{43247403-6670-4DAE-A4A7-F82A98DB1B18}"/>
-    <hyperlink ref="E144" r:id="rId164" xr:uid="{B99C6DBE-1E6B-4A91-B8BB-C628FC8F5E39}"/>
-    <hyperlink ref="A51" r:id="rId165" display="https://leetcode.cn/problems/kth-largest-element-in-an-array/" xr:uid="{6895E2EE-164A-44EC-87C0-E0780657C4D5}"/>
-    <hyperlink ref="E85" r:id="rId166" xr:uid="{9D276BED-6F9B-4561-A6CF-0DEE42145361}"/>
-    <hyperlink ref="A85" r:id="rId167" display="https://leetcode.cn/problems/find-median-from-data-stream/" xr:uid="{4DBDEEFB-711A-4C7C-B2FA-E0812141E933}"/>
-    <hyperlink ref="A95" r:id="rId168" display="https://leetcode.cn/problems/top-k-frequent-elements/" xr:uid="{8F33DAD7-780E-493E-95D1-8DAAF6F9CE55}"/>
-    <hyperlink ref="A15" r:id="rId169" display="https://leetcode.cn/problems/best-time-to-buy-and-sell-stock/" xr:uid="{725CC9CC-B5C3-4BC9-9C17-C040E5E57AA9}"/>
-    <hyperlink ref="A123" r:id="rId170" display="https://leetcode.cn/problems/jump-game/" xr:uid="{073E6AFF-55B0-4CBA-9CBA-8E80417E47AD}"/>
-    <hyperlink ref="A109" r:id="rId171" display="https://leetcode.cn/problems/jump-game-ii/" xr:uid="{06A56225-774B-41E5-A4C2-DA953CBB2320}"/>
-    <hyperlink ref="A139" r:id="rId172" display="https://leetcode.cn/problems/partition-labels/" xr:uid="{12848DB0-0318-4BDF-BE64-C3F92DACAB58}"/>
-    <hyperlink ref="E139" r:id="rId173" xr:uid="{47AA8A23-9E0A-418A-8B69-FBEB825EFBA9}"/>
-    <hyperlink ref="A21" r:id="rId174" display="https://leetcode.cn/problems/single-number/" xr:uid="{9BD4A482-0471-4E20-BFC3-734B1CA35641}"/>
-    <hyperlink ref="A36" r:id="rId175" display="https://leetcode.cn/problems/majority-element/" xr:uid="{37CD3B5F-77FD-4FD4-9183-F3C2613312F5}"/>
-    <hyperlink ref="A137" r:id="rId176" display="https://leetcode.cn/problems/sort-colors/" xr:uid="{0933A8C1-E6CB-4D8B-B587-B3AE5E152C60}"/>
-    <hyperlink ref="A88" r:id="rId177" display="https://leetcode.cn/problems/next-permutation/" xr:uid="{00924165-81E0-40E5-9B50-126714BD9EC1}"/>
-    <hyperlink ref="E88" r:id="rId178" xr:uid="{FA68184D-DC6E-4B73-905E-7367F174DAB4}"/>
-    <hyperlink ref="A84" r:id="rId179" display="https://leetcode.cn/problems/find-the-duplicate-number/" xr:uid="{71AD2502-07F8-491F-B447-E038CFD2DE0A}"/>
-    <hyperlink ref="E84" r:id="rId180" xr:uid="{4623A77E-B815-4BB6-8889-1925129DCFC0}"/>
-    <hyperlink ref="A129" r:id="rId181" display="https://leetcode.cn/problems/climbing-stairs/" xr:uid="{6474300B-1FFA-41B9-826D-DD197EEBF5D1}"/>
-    <hyperlink ref="A13" r:id="rId182" display="https://leetcode.cn/problems/pascals-triangle/" xr:uid="{96D3509F-CF38-44FE-AE13-4A7146A5957A}"/>
-    <hyperlink ref="A40" r:id="rId183" display="https://leetcode.cn/problems/house-robber/" xr:uid="{079C2458-4871-4F22-AB06-1D1A62CFE367}"/>
-    <hyperlink ref="A75" r:id="rId184" display="https://leetcode.cn/problems/perfect-squares/" xr:uid="{343AEFED-CE19-4897-8C8D-4475B2A1407B}"/>
-    <hyperlink ref="A23" r:id="rId185" display="https://leetcode.cn/problems/word-break/" xr:uid="{BF6D8200-0760-4091-BC5C-21AE6E881E31}"/>
-    <hyperlink ref="E23" r:id="rId186" location="%E5%85%B6%E4%BB%96%E8%AF%AD%E8%A8%80%E7%89%88%E6%9C%AC" xr:uid="{DD5556A3-46F8-41D5-98A7-E73337A29D00}"/>
-    <hyperlink ref="A87" r:id="rId187" display="https://leetcode.cn/problems/longest-increasing-subsequence/" xr:uid="{C613CD93-B015-40DE-B77D-98CD9C62426B}"/>
-    <hyperlink ref="A30" r:id="rId188" display="https://leetcode.cn/problems/maximum-product-subarray/" xr:uid="{56D5B9C8-5C69-4FE3-B1A6-87301E237F68}"/>
-    <hyperlink ref="A104" r:id="rId189" display="https://leetcode.cn/problems/partition-equal-subset-sum/" xr:uid="{2B3E4BC5-E239-44BE-99B2-1BB3C1D0824B}"/>
-    <hyperlink ref="A90" r:id="rId190" display="https://leetcode.cn/problems/longest-valid-parentheses/" xr:uid="{7BDAAF5F-4261-4559-B687-E752386ED066}"/>
-    <hyperlink ref="A126" r:id="rId191" display="https://leetcode.cn/problems/unique-paths/" xr:uid="{6A5EC3F6-9773-41E4-8A78-CBF6839C8CBC}"/>
-    <hyperlink ref="E126" r:id="rId192" location="%E7%AE%97%E6%B3%95%E5%85%AC%E5%BC%80%E8%AF%BE" xr:uid="{07032E5B-FFB4-4546-BDBF-6435EE8CB009}"/>
-    <hyperlink ref="A127" r:id="rId193" display="https://leetcode.cn/problems/minimum-path-sum/" xr:uid="{7CE3AEDD-230D-451A-B612-10ACA7BFEBAF}"/>
-    <hyperlink ref="A116" r:id="rId194" display="https://leetcode.cn/problems/longest-palindromic-substring/" xr:uid="{7CB78970-BA37-46EB-A639-685EFA3C19B4}"/>
-    <hyperlink ref="E116" r:id="rId195" xr:uid="{5CB9B51C-4ADC-465D-985F-47361FC2BE8A}"/>
-    <hyperlink ref="A11" r:id="rId196" display="https://leetcode.cn/problems/longest-common-subsequence/" xr:uid="{708E0024-B68F-45A5-941B-550E630409AF}"/>
-    <hyperlink ref="E11" r:id="rId197" xr:uid="{F6D25B62-12B1-4A86-A3DB-7CC7ACA6C9BC}"/>
-    <hyperlink ref="A132" r:id="rId198" display="https://leetcode.cn/problems/edit-distance/" xr:uid="{F38D478C-0D97-4DB6-852E-47E16D7FF6B2}"/>
-    <hyperlink ref="E132" r:id="rId199" location="%E7%AE%97%E6%B3%95%E5%85%AC%E5%BC%80%E8%AF%BE" xr:uid="{CD3FC349-C931-44B5-AB44-6E548F888619}"/>
-    <hyperlink ref="A130" r:id="rId200" display="https://leetcode.cn/problems/binary-search/" xr:uid="{85DCB780-B636-4DA3-8E98-BDD6E2AB99B6}"/>
-    <hyperlink ref="A69" r:id="rId201" display="https://leetcode.cn/problems/remove-element/" xr:uid="{74E7E043-E9D5-4F13-8753-25FD9681EED1}"/>
-    <hyperlink ref="A146" r:id="rId202" display="https://leetcode.cn/problems/squares-of-a-sorted-array/" xr:uid="{950D9E34-B826-4CA9-A2F0-6441BEDFF66B}"/>
-    <hyperlink ref="A89" r:id="rId203" display="https://leetcode.cn/problems/make-a-square-with-the-same-color/" xr:uid="{B400DA20-AE2E-4324-AC47-87BA46F421DE}"/>
-    <hyperlink ref="A26" r:id="rId204" display="https://leetcode.cn/problems/number-of-students-doing-homework-at-a-given-time/" xr:uid="{AA720C4C-25A2-4B25-89B7-BBECE40C40BB}"/>
-    <hyperlink ref="E104" r:id="rId205" location="%E7%AE%97%E6%B3%95%E5%85%AC%E5%BC%80%E8%AF%BE" xr:uid="{B37EB81F-EF1F-4396-86C4-07A4B6B4BD23}"/>
-    <hyperlink ref="E115" r:id="rId206" xr:uid="{E640F872-25EF-4BA1-9E59-499DF5F68C1F}"/>
-    <hyperlink ref="A115" r:id="rId207" display="https://leetcode.cn/problems/target-sum/" xr:uid="{20D963BF-935B-4ED4-929E-E539372B3AF7}"/>
-    <hyperlink ref="A112" r:id="rId208" display="https://leetcode.cn/problems/ones-and-zeroes/" xr:uid="{A745CEB2-6003-4380-A991-14868087F07F}"/>
-    <hyperlink ref="E112" r:id="rId209" location="%E7%AE%97%E6%B3%95%E5%85%AC%E5%BC%80%E8%AF%BE" xr:uid="{F5FEC363-C626-4269-AB6D-BB8E81A1A7FB}"/>
-    <hyperlink ref="A91" r:id="rId210" display="https://leetcode.cn/problems/coin-change/" xr:uid="{64F5B128-1E04-4732-AF12-90689477DA6D}"/>
-    <hyperlink ref="A119" r:id="rId211" display="https://leetcode.cn/problems/coin-change-ii/" xr:uid="{12DF8DE7-8ED9-41CC-B542-0942C84A3816}"/>
-    <hyperlink ref="A98" r:id="rId212" display="https://leetcode.cn/problems/combination-sum-iv/" xr:uid="{298B5B43-888B-4FE3-9586-FC5002886A6C}"/>
-    <hyperlink ref="E98" r:id="rId213" location="%E7%AE%97%E6%B3%95%E5%85%AC%E5%BC%80%E8%AF%BE" xr:uid="{DC60A958-2764-44A8-8EE2-77C17D2FDEA3}"/>
-    <hyperlink ref="E75" r:id="rId214" location="%E5%85%B6%E4%BB%96%E8%AF%AD%E8%A8%80%E7%89%88%E6%9C%AC" xr:uid="{D43FC4F4-2E6E-4131-A45D-CA8A1DFB898B}"/>
-    <hyperlink ref="A50" r:id="rId215" display="https://leetcode.cn/problems/house-robber-ii/" xr:uid="{011EF902-1A7F-4B2A-A6C4-9CC4170652F9}"/>
-    <hyperlink ref="E50" r:id="rId216" location="%E7%AE%97%E6%B3%95%E5%85%AC%E5%BC%80%E8%AF%BE" xr:uid="{1C2F2F2E-B768-4CB1-A423-461180A08345}"/>
-    <hyperlink ref="E35" r:id="rId217" xr:uid="{F6F61F5C-44EF-4160-8F04-C1B4D9954358}"/>
-    <hyperlink ref="A93" r:id="rId218" display="https://leetcode.cn/problems/house-robber-iii/" xr:uid="{F03A8C84-0846-4378-B0E5-7128A3F7648D}"/>
-    <hyperlink ref="E93" r:id="rId219" location="%E7%AE%97%E6%B3%95%E5%85%AC%E5%BC%80%E8%AF%BE" xr:uid="{7EFB6569-3C24-4DDB-85C3-2D694092BF07}"/>
-    <hyperlink ref="E25" r:id="rId220" xr:uid="{83508AB9-CE84-406E-A595-09E513D366DE}"/>
-    <hyperlink ref="E15" r:id="rId221" location="%E7%AE%97%E6%B3%95%E5%85%AC%E5%BC%80%E8%AF%BE" xr:uid="{D638CE32-5CF3-45F8-AB28-5C02249D688E}"/>
-    <hyperlink ref="A63" r:id="rId222" display="https://leetcode.cn/problems/swap-nodes-in-pairs/" xr:uid="{06FC87A8-9576-4A88-8A22-8C4507E31EAD}"/>
-    <hyperlink ref="A16" r:id="rId223" display="https://leetcode.cn/problems/best-time-to-buy-and-sell-stock-ii/" xr:uid="{44B4BF0B-837D-4651-B2FB-1620DC83FFE7}"/>
-    <hyperlink ref="E16" r:id="rId224" xr:uid="{6A854C66-D16C-43C1-9F99-F65ED77BCA5D}"/>
-    <hyperlink ref="A17" r:id="rId225" display="https://leetcode.cn/problems/best-time-to-buy-and-sell-stock-iii/" xr:uid="{FEA62B0B-FF2D-40F4-9CD9-468AC519A968}"/>
-    <hyperlink ref="E17" r:id="rId226" location="%E7%AE%97%E6%B3%95%E5%85%AC%E5%BC%80%E8%AF%BE" xr:uid="{D16F13D5-2313-46E7-856B-7CD15473073D}"/>
-    <hyperlink ref="A149" r:id="rId227" display="https://leetcode.cn/problems/maximum-distance-in-arrays/" xr:uid="{02D73743-9253-4929-B7CF-906C335822E4}"/>
-    <hyperlink ref="A150" r:id="rId228" display="https://leetcode.cn/problems/wiggle-sort/" xr:uid="{4C7841DB-76AF-4350-8D79-81752C4DE963}"/>
-    <hyperlink ref="A151" r:id="rId229" display="https://leetcode.cn/problems/confusing-number/" xr:uid="{3787BBD4-87CE-4CFB-95F0-72BF1983D4E0}"/>
-    <hyperlink ref="A152" r:id="rId230" display="https://leetcode.cn/problems/perform-string-shifts/" xr:uid="{DD8B1630-888D-4505-8B4B-A337C652FCDC}"/>
-    <hyperlink ref="E152" r:id="rId231" xr:uid="{9F832EE2-74ED-4675-BC97-4E11BC46C2C0}"/>
-    <hyperlink ref="A153" r:id="rId232" display="https://leetcode.cn/problems/one-edit-distance/" xr:uid="{E5267046-4F48-4788-8D8B-CE1C5168CCE8}"/>
+    <hyperlink ref="A110" r:id="rId126" display="https://leetcode.cn/problems/path-sum-iii/" xr:uid="{05551963-434C-40D6-A149-D640646C016A}"/>
+    <hyperlink ref="A62" r:id="rId127" display="https://leetcode.cn/problems/lowest-common-ancestor-of-a-binary-tree/" xr:uid="{C283A30B-A9D0-4642-834C-77EE1E2A81E8}"/>
+    <hyperlink ref="E62" r:id="rId128" xr:uid="{A9C856D9-9F85-4925-88CC-FF911C4EFD32}"/>
+    <hyperlink ref="A19" r:id="rId129" display="https://leetcode.cn/problems/binary-tree-maximum-path-sum/" xr:uid="{3678B77A-8804-4A64-AE6C-41376D22B9BC}"/>
+    <hyperlink ref="A47" r:id="rId130" display="https://leetcode.cn/problems/number-of-islands/" xr:uid="{A328C414-4CF6-4425-A56A-201C9BC6AD15}"/>
+    <hyperlink ref="A153" r:id="rId131" display="https://leetcode.cn/problems/rotting-oranges/" xr:uid="{C47F4890-A65B-4EA6-BE20-E06AFE42305B}"/>
+    <hyperlink ref="A49" r:id="rId132" display="https://leetcode.cn/problems/course-schedule/" xr:uid="{E474195F-F1D8-4B40-A072-95AA82E77F7B}"/>
+    <hyperlink ref="A50" r:id="rId133" display="https://leetcode.cn/problems/implement-trie-prefix-tree/" xr:uid="{ACDFE2DE-83AA-4BAD-8166-E20BAC48A7C3}"/>
+    <hyperlink ref="E114" r:id="rId134" xr:uid="{2E898F41-BA84-45AF-A705-0973EB8DB8EE}"/>
+    <hyperlink ref="A114" r:id="rId135" display="https://leetcode.cn/problems/permutations/" xr:uid="{8E4E13D8-2A7F-4DC6-A48B-A54ED93B27C0}"/>
+    <hyperlink ref="A145" r:id="rId136" display="https://leetcode.cn/problems/subsets/" xr:uid="{5C409365-541F-4E98-97A1-A1E29CC4F14F}"/>
+    <hyperlink ref="E145" r:id="rId137" xr:uid="{93490963-1363-4F0C-8181-651E214E0B18}"/>
+    <hyperlink ref="A40" r:id="rId138" display="https://leetcode.cn/problems/letter-combinations-of-a-phone-number/" xr:uid="{A72E7149-0969-4B87-A7FC-139F18FFD8BB}"/>
+    <hyperlink ref="E40" r:id="rId139" xr:uid="{31CD6DD9-B828-43FC-B338-7CAE71F2DFDF}"/>
+    <hyperlink ref="A104" r:id="rId140" display="https://leetcode.cn/problems/combination-sum/" xr:uid="{EFF7251F-6EB1-4CC3-B4A9-227B600CFFA1}"/>
+    <hyperlink ref="E146" r:id="rId141" xr:uid="{D009558D-60D6-4366-8677-9423BF894976}"/>
+    <hyperlink ref="A146" r:id="rId142" display="https://leetcode.cn/problems/word-search/" xr:uid="{6E176417-751F-4EED-B7EB-3128CCF61581}"/>
+    <hyperlink ref="A57" r:id="rId143" display="https://leetcode.cn/problems/generate-parentheses/" xr:uid="{30406B0C-B20F-496A-A2C4-D948173189C3}"/>
+    <hyperlink ref="A21" r:id="rId144" display="https://leetcode.cn/problems/palindrome-partitioning/" xr:uid="{C1C42340-3C82-4BD1-8608-8DFFF96FC75B}"/>
+    <hyperlink ref="A121" r:id="rId145" display="https://leetcode.cn/problems/n-queens/" xr:uid="{A0187B26-61AC-4C97-9A36-85A591E506B7}"/>
+    <hyperlink ref="E121" r:id="rId146" location="%E5%85%B6%E4%BB%96%E8%AF%AD%E8%A8%80%E8%A1%A5%E5%85%85" xr:uid="{7968323D-D06A-46E1-9DFB-D49E602D499C}"/>
+    <hyperlink ref="E98" r:id="rId147" xr:uid="{DDCFD87D-CD38-43E5-ADAF-24E527C68F8E}"/>
+    <hyperlink ref="A98" r:id="rId148" display="https://leetcode.cn/problems/find-first-and-last-position-of-element-in-sorted-array/" xr:uid="{BF08E923-B4D9-4EEF-8E92-E28C605CCE32}"/>
+    <hyperlink ref="A100" r:id="rId149" display="https://leetcode.cn/problems/search-insert-position/" xr:uid="{54241F2B-5AB4-4177-BC7C-5360532D265E}"/>
+    <hyperlink ref="A141" r:id="rId150" display="https://leetcode.cn/problems/search-a-2d-matrix/" xr:uid="{B827C295-310F-4C1E-8C97-04E52B4E0D8F}"/>
+    <hyperlink ref="E96" r:id="rId151" xr:uid="{66A0E0DB-2AE8-4C0D-B11E-7E0DDADB9B41}"/>
+    <hyperlink ref="A96" r:id="rId152" display="https://leetcode.cn/problems/search-in-rotated-sorted-array/" xr:uid="{B22B927E-2356-4B4E-BF35-F484D36559D4}"/>
+    <hyperlink ref="A33" r:id="rId153" display="https://leetcode.cn/problems/find-minimum-in-rotated-sorted-array/" xr:uid="{397D2DAE-9BE0-4951-B83D-824D7FBCE07E}"/>
+    <hyperlink ref="E106" r:id="rId154" xr:uid="{90EC8E40-2D47-4398-939E-3F09E808796E}"/>
+    <hyperlink ref="A46" r:id="rId155" display="https://leetcode.cn/problems/valid-parentheses/" xr:uid="{4BE72628-010D-4D86-BD85-8830898F69F1}"/>
+    <hyperlink ref="A106" r:id="rId156" display="https://leetcode.cn/problems/median-of-two-sorted-arrays/" xr:uid="{47FFFE22-7443-4E70-84C1-E1352C5D0139}"/>
+    <hyperlink ref="E34" r:id="rId157" xr:uid="{BC8DED09-4E1C-410D-A7D9-76EF7EA14100}"/>
+    <hyperlink ref="A34" r:id="rId158" display="https://leetcode.cn/problems/min-stack/" xr:uid="{BD6D5A5D-9717-4253-A2F5-A43EC62D1A5D}"/>
+    <hyperlink ref="A105" r:id="rId159" display="https://leetcode.cn/problems/decode-string/" xr:uid="{0B4CACA8-1935-41CF-967A-CAEFF5AECB53}"/>
+    <hyperlink ref="E105" r:id="rId160" xr:uid="{819C9DBC-04AA-4864-81C9-0C3EFC02339D}"/>
+    <hyperlink ref="A140" r:id="rId161" display="https://leetcode.cn/problems/daily-temperatures/" xr:uid="{B26C3125-EB8A-4499-B55F-A0327D4C49FD}"/>
+    <hyperlink ref="E140" r:id="rId162" xr:uid="{71B5751F-3CF1-4DC3-931E-B157AACD6558}"/>
+    <hyperlink ref="A149" r:id="rId163" display="https://leetcode.cn/problems/largest-rectangle-in-histogram/" xr:uid="{43247403-6670-4DAE-A4A7-F82A98DB1B18}"/>
+    <hyperlink ref="E149" r:id="rId164" xr:uid="{B99C6DBE-1E6B-4A91-B8BB-C628FC8F5E39}"/>
+    <hyperlink ref="A54" r:id="rId165" display="https://leetcode.cn/problems/kth-largest-element-in-an-array/" xr:uid="{6895E2EE-164A-44EC-87C0-E0780657C4D5}"/>
+    <hyperlink ref="E89" r:id="rId166" xr:uid="{9D276BED-6F9B-4561-A6CF-0DEE42145361}"/>
+    <hyperlink ref="A89" r:id="rId167" display="https://leetcode.cn/problems/find-median-from-data-stream/" xr:uid="{4DBDEEFB-711A-4C7C-B2FA-E0812141E933}"/>
+    <hyperlink ref="A99" r:id="rId168" display="https://leetcode.cn/problems/top-k-frequent-elements/" xr:uid="{8F33DAD7-780E-493E-95D1-8DAAF6F9CE55}"/>
+    <hyperlink ref="A16" r:id="rId169" display="https://leetcode.cn/problems/best-time-to-buy-and-sell-stock/" xr:uid="{725CC9CC-B5C3-4BC9-9C17-C040E5E57AA9}"/>
+    <hyperlink ref="A127" r:id="rId170" display="https://leetcode.cn/problems/jump-game/" xr:uid="{073E6AFF-55B0-4CBA-9CBA-8E80417E47AD}"/>
+    <hyperlink ref="A113" r:id="rId171" display="https://leetcode.cn/problems/jump-game-ii/" xr:uid="{06A56225-774B-41E5-A4C2-DA953CBB2320}"/>
+    <hyperlink ref="A144" r:id="rId172" display="https://leetcode.cn/problems/partition-labels/" xr:uid="{12848DB0-0318-4BDF-BE64-C3F92DACAB58}"/>
+    <hyperlink ref="E144" r:id="rId173" xr:uid="{47AA8A23-9E0A-418A-8B69-FBEB825EFBA9}"/>
+    <hyperlink ref="A22" r:id="rId174" display="https://leetcode.cn/problems/single-number/" xr:uid="{9BD4A482-0471-4E20-BFC3-734B1CA35641}"/>
+    <hyperlink ref="A39" r:id="rId175" display="https://leetcode.cn/problems/majority-element/" xr:uid="{37CD3B5F-77FD-4FD4-9183-F3C2613312F5}"/>
+    <hyperlink ref="A142" r:id="rId176" display="https://leetcode.cn/problems/sort-colors/" xr:uid="{0933A8C1-E6CB-4D8B-B587-B3AE5E152C60}"/>
+    <hyperlink ref="A92" r:id="rId177" display="https://leetcode.cn/problems/next-permutation/" xr:uid="{00924165-81E0-40E5-9B50-126714BD9EC1}"/>
+    <hyperlink ref="E92" r:id="rId178" xr:uid="{FA68184D-DC6E-4B73-905E-7367F174DAB4}"/>
+    <hyperlink ref="A88" r:id="rId179" display="https://leetcode.cn/problems/find-the-duplicate-number/" xr:uid="{71AD2502-07F8-491F-B447-E038CFD2DE0A}"/>
+    <hyperlink ref="E88" r:id="rId180" xr:uid="{4623A77E-B815-4BB6-8889-1925129DCFC0}"/>
+    <hyperlink ref="A134" r:id="rId181" display="https://leetcode.cn/problems/climbing-stairs/" xr:uid="{6474300B-1FFA-41B9-826D-DD197EEBF5D1}"/>
+    <hyperlink ref="A14" r:id="rId182" display="https://leetcode.cn/problems/pascals-triangle/" xr:uid="{96D3509F-CF38-44FE-AE13-4A7146A5957A}"/>
+    <hyperlink ref="A43" r:id="rId183" display="https://leetcode.cn/problems/house-robber/" xr:uid="{079C2458-4871-4F22-AB06-1D1A62CFE367}"/>
+    <hyperlink ref="A78" r:id="rId184" display="https://leetcode.cn/problems/perfect-squares/" xr:uid="{343AEFED-CE19-4897-8C8D-4475B2A1407B}"/>
+    <hyperlink ref="A24" r:id="rId185" display="https://leetcode.cn/problems/word-break/" xr:uid="{BF6D8200-0760-4091-BC5C-21AE6E881E31}"/>
+    <hyperlink ref="E24" r:id="rId186" location="%E5%85%B6%E4%BB%96%E8%AF%AD%E8%A8%80%E7%89%88%E6%9C%AC" xr:uid="{DD5556A3-46F8-41D5-98A7-E73337A29D00}"/>
+    <hyperlink ref="A91" r:id="rId187" display="https://leetcode.cn/problems/longest-increasing-subsequence/" xr:uid="{C613CD93-B015-40DE-B77D-98CD9C62426B}"/>
+    <hyperlink ref="A32" r:id="rId188" display="https://leetcode.cn/problems/maximum-product-subarray/" xr:uid="{56D5B9C8-5C69-4FE3-B1A6-87301E237F68}"/>
+    <hyperlink ref="A108" r:id="rId189" display="https://leetcode.cn/problems/partition-equal-subset-sum/" xr:uid="{2B3E4BC5-E239-44BE-99B2-1BB3C1D0824B}"/>
+    <hyperlink ref="A94" r:id="rId190" display="https://leetcode.cn/problems/longest-valid-parentheses/" xr:uid="{7BDAAF5F-4261-4559-B687-E752386ED066}"/>
+    <hyperlink ref="A130" r:id="rId191" display="https://leetcode.cn/problems/unique-paths/" xr:uid="{6A5EC3F6-9773-41E4-8A78-CBF6839C8CBC}"/>
+    <hyperlink ref="E130" r:id="rId192" location="%E7%AE%97%E6%B3%95%E5%85%AC%E5%BC%80%E8%AF%BE" xr:uid="{07032E5B-FFB4-4546-BDBF-6435EE8CB009}"/>
+    <hyperlink ref="A132" r:id="rId193" display="https://leetcode.cn/problems/minimum-path-sum/" xr:uid="{7CE3AEDD-230D-451A-B612-10ACA7BFEBAF}"/>
+    <hyperlink ref="A120" r:id="rId194" display="https://leetcode.cn/problems/longest-palindromic-substring/" xr:uid="{7CB78970-BA37-46EB-A639-685EFA3C19B4}"/>
+    <hyperlink ref="E120" r:id="rId195" xr:uid="{5CB9B51C-4ADC-465D-985F-47361FC2BE8A}"/>
+    <hyperlink ref="A12" r:id="rId196" display="https://leetcode.cn/problems/longest-common-subsequence/" xr:uid="{708E0024-B68F-45A5-941B-550E630409AF}"/>
+    <hyperlink ref="E12" r:id="rId197" xr:uid="{F6D25B62-12B1-4A86-A3DB-7CC7ACA6C9BC}"/>
+    <hyperlink ref="A137" r:id="rId198" display="https://leetcode.cn/problems/edit-distance/" xr:uid="{F38D478C-0D97-4DB6-852E-47E16D7FF6B2}"/>
+    <hyperlink ref="E137" r:id="rId199" location="%E7%AE%97%E6%B3%95%E5%85%AC%E5%BC%80%E8%AF%BE" xr:uid="{CD3FC349-C931-44B5-AB44-6E548F888619}"/>
+    <hyperlink ref="A135" r:id="rId200" display="https://leetcode.cn/problems/binary-search/" xr:uid="{85DCB780-B636-4DA3-8E98-BDD6E2AB99B6}"/>
+    <hyperlink ref="A72" r:id="rId201" display="https://leetcode.cn/problems/remove-element/" xr:uid="{74E7E043-E9D5-4F13-8753-25FD9681EED1}"/>
+    <hyperlink ref="A151" r:id="rId202" display="https://leetcode.cn/problems/squares-of-a-sorted-array/" xr:uid="{950D9E34-B826-4CA9-A2F0-6441BEDFF66B}"/>
+    <hyperlink ref="A93" r:id="rId203" display="https://leetcode.cn/problems/make-a-square-with-the-same-color/" xr:uid="{B400DA20-AE2E-4324-AC47-87BA46F421DE}"/>
+    <hyperlink ref="A28" r:id="rId204" display="https://leetcode.cn/problems/number-of-students-doing-homework-at-a-given-time/" xr:uid="{AA720C4C-25A2-4B25-89B7-BBECE40C40BB}"/>
+    <hyperlink ref="E108" r:id="rId205" location="%E7%AE%97%E6%B3%95%E5%85%AC%E5%BC%80%E8%AF%BE" xr:uid="{B37EB81F-EF1F-4396-86C4-07A4B6B4BD23}"/>
+    <hyperlink ref="E119" r:id="rId206" xr:uid="{E640F872-25EF-4BA1-9E59-499DF5F68C1F}"/>
+    <hyperlink ref="A119" r:id="rId207" display="https://leetcode.cn/problems/target-sum/" xr:uid="{20D963BF-935B-4ED4-929E-E539372B3AF7}"/>
+    <hyperlink ref="A116" r:id="rId208" display="https://leetcode.cn/problems/ones-and-zeroes/" xr:uid="{A745CEB2-6003-4380-A991-14868087F07F}"/>
+    <hyperlink ref="E116" r:id="rId209" location="%E7%AE%97%E6%B3%95%E5%85%AC%E5%BC%80%E8%AF%BE" xr:uid="{F5FEC363-C626-4269-AB6D-BB8E81A1A7FB}"/>
+    <hyperlink ref="A95" r:id="rId210" display="https://leetcode.cn/problems/coin-change/" xr:uid="{64F5B128-1E04-4732-AF12-90689477DA6D}"/>
+    <hyperlink ref="A123" r:id="rId211" display="https://leetcode.cn/problems/coin-change-ii/" xr:uid="{12DF8DE7-8ED9-41CC-B542-0942C84A3816}"/>
+    <hyperlink ref="A102" r:id="rId212" display="https://leetcode.cn/problems/combination-sum-iv/" xr:uid="{298B5B43-888B-4FE3-9586-FC5002886A6C}"/>
+    <hyperlink ref="E102" r:id="rId213" location="%E7%AE%97%E6%B3%95%E5%85%AC%E5%BC%80%E8%AF%BE" xr:uid="{DC60A958-2764-44A8-8EE2-77C17D2FDEA3}"/>
+    <hyperlink ref="E78" r:id="rId214" location="%E5%85%B6%E4%BB%96%E8%AF%AD%E8%A8%80%E7%89%88%E6%9C%AC" xr:uid="{D43FC4F4-2E6E-4131-A45D-CA8A1DFB898B}"/>
+    <hyperlink ref="A53" r:id="rId215" display="https://leetcode.cn/problems/house-robber-ii/" xr:uid="{011EF902-1A7F-4B2A-A6C4-9CC4170652F9}"/>
+    <hyperlink ref="E53" r:id="rId216" location="%E7%AE%97%E6%B3%95%E5%85%AC%E5%BC%80%E8%AF%BE" xr:uid="{1C2F2F2E-B768-4CB1-A423-461180A08345}"/>
+    <hyperlink ref="E37" r:id="rId217" xr:uid="{F6F61F5C-44EF-4160-8F04-C1B4D9954358}"/>
+    <hyperlink ref="A97" r:id="rId218" display="https://leetcode.cn/problems/house-robber-iii/" xr:uid="{F03A8C84-0846-4378-B0E5-7128A3F7648D}"/>
+    <hyperlink ref="E97" r:id="rId219" location="%E7%AE%97%E6%B3%95%E5%85%AC%E5%BC%80%E8%AF%BE" xr:uid="{7EFB6569-3C24-4DDB-85C3-2D694092BF07}"/>
+    <hyperlink ref="E26" r:id="rId220" xr:uid="{83508AB9-CE84-406E-A595-09E513D366DE}"/>
+    <hyperlink ref="E16" r:id="rId221" location="%E7%AE%97%E6%B3%95%E5%85%AC%E5%BC%80%E8%AF%BE" xr:uid="{D638CE32-5CF3-45F8-AB28-5C02249D688E}"/>
+    <hyperlink ref="A66" r:id="rId222" display="https://leetcode.cn/problems/swap-nodes-in-pairs/" xr:uid="{06FC87A8-9576-4A88-8A22-8C4507E31EAD}"/>
+    <hyperlink ref="A17" r:id="rId223" display="https://leetcode.cn/problems/best-time-to-buy-and-sell-stock-ii/" xr:uid="{44B4BF0B-837D-4651-B2FB-1620DC83FFE7}"/>
+    <hyperlink ref="E17" r:id="rId224" xr:uid="{6A854C66-D16C-43C1-9F99-F65ED77BCA5D}"/>
+    <hyperlink ref="A18" r:id="rId225" display="https://leetcode.cn/problems/best-time-to-buy-and-sell-stock-iii/" xr:uid="{FEA62B0B-FF2D-40F4-9CD9-468AC519A968}"/>
+    <hyperlink ref="E18" r:id="rId226" location="%E7%AE%97%E6%B3%95%E5%85%AC%E5%BC%80%E8%AF%BE" xr:uid="{D16F13D5-2313-46E7-856B-7CD15473073D}"/>
+    <hyperlink ref="A131" r:id="rId227" display="https://leetcode.cn/problems/maximum-distance-in-arrays/" xr:uid="{02D73743-9253-4929-B7CF-906C335822E4}"/>
+    <hyperlink ref="A79" r:id="rId228" display="https://leetcode.cn/problems/wiggle-sort/" xr:uid="{4C7841DB-76AF-4350-8D79-81752C4DE963}"/>
+    <hyperlink ref="A8" r:id="rId229" display="https://leetcode.cn/problems/confusing-number/" xr:uid="{3787BBD4-87CE-4CFB-95F0-72BF1983D4E0}"/>
+    <hyperlink ref="A27" r:id="rId230" display="https://leetcode.cn/problems/perform-string-shifts/" xr:uid="{DD8B1630-888D-4505-8B4B-A337C652FCDC}"/>
+    <hyperlink ref="E27" r:id="rId231" xr:uid="{9F832EE2-74ED-4675-BC97-4E11BC46C2C0}"/>
+    <hyperlink ref="A38" r:id="rId232" display="https://leetcode.cn/problems/one-edit-distance/" xr:uid="{E5267046-4F48-4788-8D8B-CE1C5168CCE8}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <tableParts count="1">

</xml_diff>

<commit_message>
2024.12.17 LeetCodeHot100 三刷 二分查找Done
</commit_message>
<xml_diff>
--- a/2024LeetCode刷题记录.xlsx
+++ b/2024LeetCode刷题记录.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\develop\GithubRepo\LeetCode\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1174D8A9-98F2-4348-B34B-EE5F3EB7E267}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BEE9E607-69DF-44A6-9734-2EBB20B25864}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-30828" yWindow="-108" windowWidth="30936" windowHeight="16776" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-20916" yWindow="2952" windowWidth="19356" windowHeight="11928" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -1339,18 +1339,10 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>2024.10.29</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>33题的子集</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>方法四；Hardddd</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>2024.10.30</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -1563,6 +1555,14 @@
   </si>
   <si>
     <t>nums[mid%n]为了避免(-1)%7，联系34，先找中轴点</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>2024.12.17</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>解法四Hardddd；还是解法三更人性化一点；</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -2021,8 +2021,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G153"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A82" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="G96" sqref="G96"/>
+    <sheetView tabSelected="1" topLeftCell="A98" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="G108" sqref="G108"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="14.15" x14ac:dyDescent="0.35"/>
@@ -2071,7 +2071,7 @@
         <v>80</v>
       </c>
       <c r="D2" s="8" t="s">
-        <v>388</v>
+        <v>386</v>
       </c>
       <c r="F2" s="6">
         <v>3</v>
@@ -2088,13 +2088,13 @@
         <v>42</v>
       </c>
       <c r="D3" s="8" t="s">
-        <v>403</v>
+        <v>401</v>
       </c>
       <c r="F3" s="6">
         <v>3</v>
       </c>
       <c r="G3" s="14" t="s">
-        <v>404</v>
+        <v>402</v>
       </c>
     </row>
     <row r="4" spans="1:7" ht="17.149999999999999" x14ac:dyDescent="0.55000000000000004">
@@ -2105,7 +2105,7 @@
         <v>13</v>
       </c>
       <c r="D4" s="8" t="s">
-        <v>406</v>
+        <v>404</v>
       </c>
       <c r="F4" s="6">
         <v>3</v>
@@ -2122,13 +2122,13 @@
         <v>42</v>
       </c>
       <c r="D5" s="8" t="s">
-        <v>403</v>
+        <v>401</v>
       </c>
       <c r="F5" s="6">
         <v>3</v>
       </c>
       <c r="G5" s="14" t="s">
-        <v>404</v>
+        <v>402</v>
       </c>
     </row>
     <row r="6" spans="1:7" ht="17.149999999999999" x14ac:dyDescent="0.55000000000000004">
@@ -2162,7 +2162,7 @@
         <v>80</v>
       </c>
       <c r="D7" s="8" t="s">
-        <v>408</v>
+        <v>406</v>
       </c>
       <c r="F7" s="6">
         <v>3</v>
@@ -2170,13 +2170,13 @@
     </row>
     <row r="8" spans="1:7" ht="17.149999999999999" x14ac:dyDescent="0.55000000000000004">
       <c r="A8" s="10" t="s">
-        <v>382</v>
+        <v>380</v>
       </c>
       <c r="C8" s="7" t="s">
         <v>13</v>
       </c>
       <c r="D8" s="8" t="s">
-        <v>379</v>
+        <v>377</v>
       </c>
     </row>
     <row r="9" spans="1:7" ht="17.149999999999999" x14ac:dyDescent="0.55000000000000004">
@@ -2187,7 +2187,7 @@
         <v>13</v>
       </c>
       <c r="D9" s="8" t="s">
-        <v>406</v>
+        <v>404</v>
       </c>
       <c r="F9" s="6">
         <v>3</v>
@@ -2204,7 +2204,7 @@
         <v>42</v>
       </c>
       <c r="D10" s="8" t="s">
-        <v>390</v>
+        <v>388</v>
       </c>
       <c r="E10" s="9" t="s">
         <v>93</v>
@@ -2224,7 +2224,7 @@
         <v>13</v>
       </c>
       <c r="D11" s="8" t="s">
-        <v>406</v>
+        <v>404</v>
       </c>
       <c r="F11" s="6">
         <v>3</v>
@@ -2244,7 +2244,7 @@
         <v>95</v>
       </c>
       <c r="D12" s="8" t="s">
-        <v>374</v>
+        <v>372</v>
       </c>
       <c r="E12" s="9" t="s">
         <v>14</v>
@@ -2253,7 +2253,7 @@
         <v>2</v>
       </c>
       <c r="G12" s="14" t="s">
-        <v>376</v>
+        <v>374</v>
       </c>
     </row>
     <row r="13" spans="1:7" ht="17.149999999999999" x14ac:dyDescent="0.55000000000000004">
@@ -2287,7 +2287,7 @@
         <v>6</v>
       </c>
       <c r="D14" s="8" t="s">
-        <v>373</v>
+        <v>371</v>
       </c>
       <c r="F14" s="6">
         <v>2</v>
@@ -2375,7 +2375,7 @@
         <v>13</v>
       </c>
       <c r="D19" s="8" t="s">
-        <v>410</v>
+        <v>408</v>
       </c>
       <c r="F19" s="6">
         <v>3</v>
@@ -2395,7 +2395,7 @@
         <v>80</v>
       </c>
       <c r="D20" s="8" t="s">
-        <v>388</v>
+        <v>386</v>
       </c>
       <c r="F20" s="6">
         <v>3</v>
@@ -2412,7 +2412,7 @@
         <v>95</v>
       </c>
       <c r="D21" s="8" t="s">
-        <v>414</v>
+        <v>412</v>
       </c>
       <c r="E21" s="9" t="s">
         <v>128</v>
@@ -2421,7 +2421,7 @@
         <v>3</v>
       </c>
       <c r="G21" s="14" t="s">
-        <v>416</v>
+        <v>414</v>
       </c>
     </row>
     <row r="22" spans="1:7" ht="17.149999999999999" x14ac:dyDescent="0.55000000000000004">
@@ -2435,7 +2435,7 @@
         <v>28</v>
       </c>
       <c r="D22" s="8" t="s">
-        <v>371</v>
+        <v>369</v>
       </c>
       <c r="F22" s="6">
         <v>2</v>
@@ -2452,7 +2452,7 @@
         <v>13</v>
       </c>
       <c r="D23" s="8" t="s">
-        <v>398</v>
+        <v>396</v>
       </c>
       <c r="E23" s="9" t="s">
         <v>87</v>
@@ -2492,7 +2492,7 @@
         <v>42</v>
       </c>
       <c r="D25" s="8" t="s">
-        <v>396</v>
+        <v>394</v>
       </c>
       <c r="F25" s="6">
         <v>3</v>
@@ -2506,7 +2506,7 @@
         <v>13</v>
       </c>
       <c r="D26" s="8" t="s">
-        <v>396</v>
+        <v>394</v>
       </c>
       <c r="E26" s="13" t="s">
         <v>345</v>
@@ -2515,24 +2515,24 @@
         <v>3</v>
       </c>
       <c r="G26" s="14" t="s">
-        <v>397</v>
+        <v>395</v>
       </c>
     </row>
     <row r="27" spans="1:7" ht="17.149999999999999" x14ac:dyDescent="0.55000000000000004">
       <c r="A27" s="10" t="s">
-        <v>383</v>
+        <v>381</v>
       </c>
       <c r="C27" s="7" t="s">
         <v>42</v>
       </c>
       <c r="D27" s="8" t="s">
-        <v>379</v>
+        <v>377</v>
       </c>
       <c r="E27" s="9" t="s">
-        <v>384</v>
+        <v>382</v>
       </c>
       <c r="G27" s="14" t="s">
-        <v>385</v>
+        <v>383</v>
       </c>
     </row>
     <row r="28" spans="1:7" ht="17.149999999999999" x14ac:dyDescent="0.55000000000000004">
@@ -2560,7 +2560,7 @@
         <v>95</v>
       </c>
       <c r="D29" s="8" t="s">
-        <v>402</v>
+        <v>400</v>
       </c>
       <c r="F29" s="6">
         <v>3</v>
@@ -2580,13 +2580,13 @@
         <v>80</v>
       </c>
       <c r="D30" s="8" t="s">
-        <v>398</v>
+        <v>396</v>
       </c>
       <c r="F30" s="6">
         <v>3</v>
       </c>
       <c r="G30" s="14" t="s">
-        <v>401</v>
+        <v>399</v>
       </c>
     </row>
     <row r="31" spans="1:7" ht="17.149999999999999" x14ac:dyDescent="0.55000000000000004">
@@ -2600,7 +2600,7 @@
         <v>13</v>
       </c>
       <c r="D31" s="8" t="s">
-        <v>390</v>
+        <v>388</v>
       </c>
       <c r="E31" s="9" t="s">
         <v>97</v>
@@ -2623,7 +2623,7 @@
         <v>6</v>
       </c>
       <c r="D32" s="8" t="s">
-        <v>373</v>
+        <v>371</v>
       </c>
       <c r="F32" s="6">
         <v>2</v>
@@ -2640,13 +2640,13 @@
         <v>13</v>
       </c>
       <c r="D33" s="8" t="s">
+        <v>421</v>
+      </c>
+      <c r="F33" s="6">
+        <v>3</v>
+      </c>
+      <c r="G33" s="14" t="s">
         <v>365</v>
-      </c>
-      <c r="F33" s="6">
-        <v>2</v>
-      </c>
-      <c r="G33" s="14" t="s">
-        <v>366</v>
       </c>
     </row>
     <row r="34" spans="1:7" ht="17.149999999999999" x14ac:dyDescent="0.55000000000000004">
@@ -2660,7 +2660,7 @@
         <v>13</v>
       </c>
       <c r="D34" s="8" t="s">
-        <v>368</v>
+        <v>366</v>
       </c>
       <c r="E34" s="9" t="s">
         <v>103</v>
@@ -2711,7 +2711,7 @@
         <v>6</v>
       </c>
       <c r="D37" s="8" t="s">
-        <v>396</v>
+        <v>394</v>
       </c>
       <c r="E37" s="13" t="s">
         <v>341</v>
@@ -2725,13 +2725,13 @@
     </row>
     <row r="38" spans="1:7" ht="17.149999999999999" x14ac:dyDescent="0.55000000000000004">
       <c r="A38" s="10" t="s">
-        <v>386</v>
+        <v>384</v>
       </c>
       <c r="C38" s="7" t="s">
         <v>42</v>
       </c>
       <c r="D38" s="8" t="s">
-        <v>387</v>
+        <v>385</v>
       </c>
     </row>
     <row r="39" spans="1:7" ht="17.149999999999999" x14ac:dyDescent="0.55000000000000004">
@@ -2745,7 +2745,7 @@
         <v>13</v>
       </c>
       <c r="D39" s="8" t="s">
-        <v>371</v>
+        <v>369</v>
       </c>
       <c r="F39" s="6">
         <v>2</v>
@@ -2762,7 +2762,7 @@
         <v>80</v>
       </c>
       <c r="D40" s="8" t="s">
-        <v>411</v>
+        <v>409</v>
       </c>
       <c r="E40" s="9" t="s">
         <v>22</v>
@@ -2779,7 +2779,7 @@
         <v>28</v>
       </c>
       <c r="D41" s="8" t="s">
-        <v>394</v>
+        <v>392</v>
       </c>
       <c r="F41" s="6">
         <v>3</v>
@@ -2793,7 +2793,7 @@
         <v>13</v>
       </c>
       <c r="D42" s="8" t="s">
-        <v>398</v>
+        <v>396</v>
       </c>
       <c r="F42" s="6">
         <v>3</v>
@@ -2830,7 +2830,7 @@
         <v>13</v>
       </c>
       <c r="D44" s="8" t="s">
-        <v>406</v>
+        <v>404</v>
       </c>
       <c r="F44" s="6">
         <v>3</v>
@@ -2847,7 +2847,7 @@
         <v>6</v>
       </c>
       <c r="D45" s="8" t="s">
-        <v>398</v>
+        <v>396</v>
       </c>
       <c r="F45" s="6">
         <v>3</v>
@@ -2864,7 +2864,7 @@
         <v>80</v>
       </c>
       <c r="D46" s="8" t="s">
-        <v>368</v>
+        <v>366</v>
       </c>
       <c r="F46" s="6">
         <v>2</v>
@@ -2878,7 +2878,7 @@
         <v>13</v>
       </c>
       <c r="D47" s="8" t="s">
-        <v>410</v>
+        <v>408</v>
       </c>
       <c r="F47" s="6">
         <v>3</v>
@@ -2895,7 +2895,7 @@
         <v>80</v>
       </c>
       <c r="D48" s="8" t="s">
-        <v>396</v>
+        <v>394</v>
       </c>
       <c r="F48" s="6">
         <v>3</v>
@@ -2909,7 +2909,7 @@
         <v>80</v>
       </c>
       <c r="D49" s="8" t="s">
-        <v>411</v>
+        <v>409</v>
       </c>
       <c r="F49" s="6">
         <v>3</v>
@@ -2923,7 +2923,7 @@
         <v>13</v>
       </c>
       <c r="D50" s="8" t="s">
-        <v>411</v>
+        <v>409</v>
       </c>
       <c r="F50" s="6">
         <v>3</v>
@@ -2957,7 +2957,7 @@
         <v>42</v>
       </c>
       <c r="D52" s="8" t="s">
-        <v>398</v>
+        <v>396</v>
       </c>
       <c r="F52" s="6">
         <v>3</v>
@@ -2994,7 +2994,7 @@
         <v>13</v>
       </c>
       <c r="D54" s="8" t="s">
-        <v>371</v>
+        <v>369</v>
       </c>
       <c r="F54" s="6">
         <v>3</v>
@@ -3051,10 +3051,10 @@
         <v>13</v>
       </c>
       <c r="D57" s="8" t="s">
-        <v>414</v>
+        <v>412</v>
       </c>
       <c r="E57" s="9" t="s">
-        <v>415</v>
+        <v>413</v>
       </c>
       <c r="F57" s="6">
         <v>3</v>
@@ -3068,13 +3068,13 @@
         <v>13</v>
       </c>
       <c r="D58" s="8" t="s">
-        <v>403</v>
+        <v>401</v>
       </c>
       <c r="F58" s="6">
         <v>3</v>
       </c>
       <c r="G58" s="14" t="s">
-        <v>404</v>
+        <v>402</v>
       </c>
     </row>
     <row r="59" spans="1:7" ht="17.149999999999999" x14ac:dyDescent="0.55000000000000004">
@@ -3088,7 +3088,7 @@
         <v>13</v>
       </c>
       <c r="D59" s="8" t="s">
-        <v>402</v>
+        <v>400</v>
       </c>
       <c r="F59" s="6">
         <v>3</v>
@@ -3102,13 +3102,13 @@
         <v>13</v>
       </c>
       <c r="D60" s="8" t="s">
-        <v>406</v>
+        <v>404</v>
       </c>
       <c r="F60" s="6">
         <v>3</v>
       </c>
       <c r="G60" s="14" t="s">
-        <v>407</v>
+        <v>405</v>
       </c>
     </row>
     <row r="61" spans="1:7" ht="17.149999999999999" x14ac:dyDescent="0.55000000000000004">
@@ -3119,7 +3119,7 @@
         <v>95</v>
       </c>
       <c r="D61" s="8" t="s">
-        <v>396</v>
+        <v>394</v>
       </c>
       <c r="F61" s="6">
         <v>3</v>
@@ -3136,7 +3136,7 @@
         <v>80</v>
       </c>
       <c r="D62" s="8" t="s">
-        <v>409</v>
+        <v>407</v>
       </c>
       <c r="E62" s="9" t="s">
         <v>93</v>
@@ -3159,7 +3159,7 @@
         <v>6</v>
       </c>
       <c r="D63" s="8" t="s">
-        <v>394</v>
+        <v>392</v>
       </c>
       <c r="F63" s="6">
         <v>3</v>
@@ -3176,7 +3176,7 @@
         <v>95</v>
       </c>
       <c r="D64" s="8" t="s">
-        <v>393</v>
+        <v>391</v>
       </c>
       <c r="E64" s="9" t="s">
         <v>118</v>
@@ -3213,13 +3213,13 @@
         <v>95</v>
       </c>
       <c r="D66" s="8" t="s">
+        <v>396</v>
+      </c>
+      <c r="F66" s="6">
+        <v>3</v>
+      </c>
+      <c r="G66" s="14" t="s">
         <v>398</v>
-      </c>
-      <c r="F66" s="6">
-        <v>3</v>
-      </c>
-      <c r="G66" s="14" t="s">
-        <v>400</v>
       </c>
     </row>
     <row r="67" spans="1:7" ht="17.149999999999999" x14ac:dyDescent="0.55000000000000004">
@@ -3233,7 +3233,7 @@
         <v>42</v>
       </c>
       <c r="D67" s="8" t="s">
-        <v>395</v>
+        <v>393</v>
       </c>
       <c r="E67" s="9" t="s">
         <v>93</v>
@@ -3276,13 +3276,13 @@
         <v>95</v>
       </c>
       <c r="D69" s="8" t="s">
-        <v>398</v>
+        <v>396</v>
       </c>
       <c r="F69" s="6">
         <v>4</v>
       </c>
       <c r="G69" s="14" t="s">
-        <v>399</v>
+        <v>397</v>
       </c>
     </row>
     <row r="70" spans="1:7" ht="17.149999999999999" x14ac:dyDescent="0.55000000000000004">
@@ -3443,16 +3443,16 @@
     </row>
     <row r="79" spans="1:7" ht="17.149999999999999" x14ac:dyDescent="0.55000000000000004">
       <c r="A79" s="10" t="s">
-        <v>381</v>
+        <v>379</v>
       </c>
       <c r="C79" s="7" t="s">
         <v>13</v>
       </c>
       <c r="D79" s="8" t="s">
-        <v>379</v>
+        <v>377</v>
       </c>
       <c r="G79" s="14" t="s">
-        <v>380</v>
+        <v>378</v>
       </c>
     </row>
     <row r="80" spans="1:7" ht="17.149999999999999" x14ac:dyDescent="0.55000000000000004">
@@ -3514,7 +3514,7 @@
         <v>80</v>
       </c>
       <c r="D83" s="8" t="s">
-        <v>389</v>
+        <v>387</v>
       </c>
       <c r="E83" s="9" t="s">
         <v>87</v>
@@ -3590,7 +3590,7 @@
         <v>13</v>
       </c>
       <c r="D88" s="8" t="s">
-        <v>371</v>
+        <v>369</v>
       </c>
       <c r="E88" s="9" t="s">
         <v>275</v>
@@ -3610,7 +3610,7 @@
         <v>80</v>
       </c>
       <c r="D89" s="8" t="s">
-        <v>371</v>
+        <v>369</v>
       </c>
       <c r="E89" s="9" t="s">
         <v>8</v>
@@ -3633,7 +3633,7 @@
         <v>80</v>
       </c>
       <c r="D90" s="8" t="s">
-        <v>391</v>
+        <v>389</v>
       </c>
       <c r="E90" s="9" t="s">
         <v>109</v>
@@ -3656,7 +3656,7 @@
         <v>80</v>
       </c>
       <c r="D91" s="8" t="s">
-        <v>373</v>
+        <v>371</v>
       </c>
       <c r="F91" s="6">
         <v>2</v>
@@ -3676,7 +3676,7 @@
         <v>42</v>
       </c>
       <c r="D92" s="8" t="s">
-        <v>371</v>
+        <v>369</v>
       </c>
       <c r="E92" s="9" t="s">
         <v>271</v>
@@ -3707,7 +3707,7 @@
         <v>13</v>
       </c>
       <c r="D94" s="8" t="s">
-        <v>373</v>
+        <v>371</v>
       </c>
       <c r="F94" s="6">
         <v>2</v>
@@ -3741,7 +3741,7 @@
         <v>95</v>
       </c>
       <c r="D96" s="8" t="s">
-        <v>420</v>
+        <v>418</v>
       </c>
       <c r="E96" s="12" t="s">
         <v>241</v>
@@ -3750,7 +3750,7 @@
         <v>3</v>
       </c>
       <c r="G96" s="14" t="s">
-        <v>422</v>
+        <v>420</v>
       </c>
     </row>
     <row r="97" spans="1:7" ht="17.149999999999999" x14ac:dyDescent="0.55000000000000004">
@@ -3781,7 +3781,7 @@
         <v>80</v>
       </c>
       <c r="D98" s="8" t="s">
-        <v>420</v>
+        <v>418</v>
       </c>
       <c r="E98" s="9" t="s">
         <v>22</v>
@@ -3801,7 +3801,7 @@
         <v>13</v>
       </c>
       <c r="D99" s="8" t="s">
-        <v>371</v>
+        <v>369</v>
       </c>
       <c r="F99" s="6">
         <v>2</v>
@@ -3818,13 +3818,13 @@
         <v>42</v>
       </c>
       <c r="D100" s="8" t="s">
-        <v>418</v>
+        <v>416</v>
       </c>
       <c r="F100" s="6">
         <v>3</v>
       </c>
       <c r="G100" s="14" t="s">
-        <v>419</v>
+        <v>417</v>
       </c>
     </row>
     <row r="101" spans="1:7" ht="17.149999999999999" x14ac:dyDescent="0.55000000000000004">
@@ -3889,13 +3889,13 @@
         <v>95</v>
       </c>
       <c r="D104" s="8" t="s">
+        <v>409</v>
+      </c>
+      <c r="F104" s="6">
+        <v>3</v>
+      </c>
+      <c r="G104" s="14" t="s">
         <v>411</v>
-      </c>
-      <c r="F104" s="6">
-        <v>3</v>
-      </c>
-      <c r="G104" s="14" t="s">
-        <v>413</v>
       </c>
     </row>
     <row r="105" spans="1:7" ht="17.149999999999999" x14ac:dyDescent="0.55000000000000004">
@@ -3909,7 +3909,7 @@
         <v>80</v>
       </c>
       <c r="D105" s="8" t="s">
-        <v>368</v>
+        <v>366</v>
       </c>
       <c r="E105" s="9" t="s">
         <v>93</v>
@@ -3929,13 +3929,16 @@
         <v>80</v>
       </c>
       <c r="D106" s="8" t="s">
-        <v>365</v>
+        <v>421</v>
       </c>
       <c r="E106" s="9" t="s">
         <v>98</v>
       </c>
+      <c r="F106" s="6">
+        <v>2</v>
+      </c>
       <c r="G106" s="14" t="s">
-        <v>367</v>
+        <v>422</v>
       </c>
     </row>
     <row r="107" spans="1:7" ht="17.149999999999999" x14ac:dyDescent="0.55000000000000004">
@@ -3949,7 +3952,7 @@
         <v>13</v>
       </c>
       <c r="D107" s="8" t="s">
-        <v>394</v>
+        <v>392</v>
       </c>
       <c r="F107" s="6">
         <v>3</v>
@@ -3992,7 +3995,7 @@
         <v>80</v>
       </c>
       <c r="D109" s="8" t="s">
-        <v>391</v>
+        <v>389</v>
       </c>
       <c r="E109" s="9" t="s">
         <v>98</v>
@@ -4015,7 +4018,7 @@
         <v>80</v>
       </c>
       <c r="D110" s="8" t="s">
-        <v>409</v>
+        <v>407</v>
       </c>
       <c r="F110" s="6">
         <v>3</v>
@@ -4035,7 +4038,7 @@
         <v>95</v>
       </c>
       <c r="D111" s="8" t="s">
-        <v>391</v>
+        <v>389</v>
       </c>
       <c r="E111" s="9" t="s">
         <v>110</v>
@@ -4078,7 +4081,7 @@
         <v>13</v>
       </c>
       <c r="D113" s="8" t="s">
-        <v>371</v>
+        <v>369</v>
       </c>
       <c r="F113" s="6">
         <v>2</v>
@@ -4095,7 +4098,7 @@
         <v>13</v>
       </c>
       <c r="D114" s="8" t="s">
-        <v>411</v>
+        <v>409</v>
       </c>
       <c r="E114" s="9" t="s">
         <v>128</v>
@@ -4155,7 +4158,7 @@
         <v>6</v>
       </c>
       <c r="D117" s="8" t="s">
-        <v>395</v>
+        <v>393</v>
       </c>
       <c r="E117" s="9" t="s">
         <v>93</v>
@@ -4175,7 +4178,7 @@
         <v>80</v>
       </c>
       <c r="D118" s="8" t="s">
-        <v>388</v>
+        <v>386</v>
       </c>
       <c r="F118" s="6">
         <v>4</v>
@@ -4212,7 +4215,7 @@
         <v>95</v>
       </c>
       <c r="D120" s="8" t="s">
-        <v>388</v>
+        <v>386</v>
       </c>
       <c r="E120" s="9" t="s">
         <v>22</v>
@@ -4221,7 +4224,7 @@
         <v>3</v>
       </c>
       <c r="G120" s="14" t="s">
-        <v>375</v>
+        <v>373</v>
       </c>
     </row>
     <row r="121" spans="1:7" ht="17.149999999999999" x14ac:dyDescent="0.55000000000000004">
@@ -4235,7 +4238,7 @@
         <v>80</v>
       </c>
       <c r="D121" s="8" t="s">
-        <v>414</v>
+        <v>412</v>
       </c>
       <c r="E121" s="9" t="s">
         <v>14</v>
@@ -4244,7 +4247,7 @@
         <v>3</v>
       </c>
       <c r="G121" s="14" t="s">
-        <v>417</v>
+        <v>415</v>
       </c>
     </row>
     <row r="122" spans="1:7" ht="17.149999999999999" x14ac:dyDescent="0.55000000000000004">
@@ -4289,7 +4292,7 @@
         <v>42</v>
       </c>
       <c r="D124" s="8" t="s">
-        <v>394</v>
+        <v>392</v>
       </c>
       <c r="E124" s="9" t="s">
         <v>128</v>
@@ -4309,7 +4312,7 @@
         <v>42</v>
       </c>
       <c r="D125" s="8" t="s">
-        <v>395</v>
+        <v>393</v>
       </c>
       <c r="E125" s="10" t="s">
         <v>185</v>
@@ -4329,13 +4332,13 @@
         <v>13</v>
       </c>
       <c r="D126" s="8" t="s">
+        <v>401</v>
+      </c>
+      <c r="F126" s="6">
+        <v>3</v>
+      </c>
+      <c r="G126" s="14" t="s">
         <v>403</v>
-      </c>
-      <c r="F126" s="6">
-        <v>3</v>
-      </c>
-      <c r="G126" s="14" t="s">
-        <v>405</v>
       </c>
     </row>
     <row r="127" spans="1:7" ht="17.149999999999999" x14ac:dyDescent="0.55000000000000004">
@@ -4349,7 +4352,7 @@
         <v>42</v>
       </c>
       <c r="D127" s="8" t="s">
-        <v>371</v>
+        <v>369</v>
       </c>
       <c r="F127" s="6">
         <v>2</v>
@@ -4366,7 +4369,7 @@
         <v>80</v>
       </c>
       <c r="D128" s="8" t="s">
-        <v>394</v>
+        <v>392</v>
       </c>
       <c r="E128" s="9" t="s">
         <v>131</v>
@@ -4386,7 +4389,7 @@
         <v>95</v>
       </c>
       <c r="D129" s="8" t="s">
-        <v>392</v>
+        <v>390</v>
       </c>
       <c r="E129" s="9" t="s">
         <v>118</v>
@@ -4406,7 +4409,7 @@
         <v>13</v>
       </c>
       <c r="D130" s="8" t="s">
-        <v>374</v>
+        <v>372</v>
       </c>
       <c r="E130" s="9" t="s">
         <v>14</v>
@@ -4417,13 +4420,13 @@
     </row>
     <row r="131" spans="1:7" ht="17.149999999999999" x14ac:dyDescent="0.55000000000000004">
       <c r="A131" s="10" t="s">
-        <v>378</v>
+        <v>376</v>
       </c>
       <c r="C131" s="7" t="s">
         <v>42</v>
       </c>
       <c r="D131" s="8" t="s">
-        <v>379</v>
+        <v>377</v>
       </c>
     </row>
     <row r="132" spans="1:7" ht="17.149999999999999" x14ac:dyDescent="0.55000000000000004">
@@ -4437,7 +4440,7 @@
         <v>13</v>
       </c>
       <c r="D132" s="8" t="s">
-        <v>374</v>
+        <v>372</v>
       </c>
       <c r="F132" s="6">
         <v>2</v>
@@ -4519,7 +4522,7 @@
         <v>80</v>
       </c>
       <c r="D137" s="8" t="s">
-        <v>374</v>
+        <v>372</v>
       </c>
       <c r="E137" s="9" t="s">
         <v>14</v>
@@ -4528,7 +4531,7 @@
         <v>2</v>
       </c>
       <c r="G137" s="14" t="s">
-        <v>377</v>
+        <v>375</v>
       </c>
     </row>
     <row r="138" spans="1:7" ht="17.149999999999999" x14ac:dyDescent="0.55000000000000004">
@@ -4542,7 +4545,7 @@
         <v>42</v>
       </c>
       <c r="D138" s="8" t="s">
-        <v>395</v>
+        <v>393</v>
       </c>
       <c r="E138" s="9" t="s">
         <v>183</v>
@@ -4582,7 +4585,7 @@
         <v>80</v>
       </c>
       <c r="D140" s="8" t="s">
-        <v>369</v>
+        <v>367</v>
       </c>
       <c r="E140" s="9" t="s">
         <v>250</v>
@@ -4605,13 +4608,13 @@
         <v>42</v>
       </c>
       <c r="D141" s="8" t="s">
-        <v>420</v>
+        <v>418</v>
       </c>
       <c r="F141" s="6">
         <v>3</v>
       </c>
       <c r="G141" s="14" t="s">
-        <v>421</v>
+        <v>419</v>
       </c>
     </row>
     <row r="142" spans="1:7" ht="17.149999999999999" x14ac:dyDescent="0.55000000000000004">
@@ -4625,7 +4628,7 @@
         <v>6</v>
       </c>
       <c r="D142" s="8" t="s">
-        <v>371</v>
+        <v>369</v>
       </c>
       <c r="F142" s="6">
         <v>2</v>
@@ -4642,7 +4645,7 @@
         <v>95</v>
       </c>
       <c r="D143" s="8" t="s">
-        <v>393</v>
+        <v>391</v>
       </c>
       <c r="E143" s="9" t="s">
         <v>122</v>
@@ -4662,7 +4665,7 @@
         <v>13</v>
       </c>
       <c r="D144" s="8" t="s">
-        <v>372</v>
+        <v>370</v>
       </c>
       <c r="E144" s="9" t="s">
         <v>22</v>
@@ -4676,7 +4679,7 @@
         <v>13</v>
       </c>
       <c r="D145" s="8" t="s">
-        <v>411</v>
+        <v>409</v>
       </c>
       <c r="E145" s="9" t="s">
         <v>47</v>
@@ -4685,7 +4688,7 @@
         <v>4</v>
       </c>
       <c r="G145" s="14" t="s">
-        <v>412</v>
+        <v>410</v>
       </c>
     </row>
     <row r="146" spans="1:7" ht="17.149999999999999" x14ac:dyDescent="0.55000000000000004">
@@ -4699,7 +4702,7 @@
         <v>13</v>
       </c>
       <c r="D146" s="8" t="s">
-        <v>414</v>
+        <v>412</v>
       </c>
       <c r="E146" s="9" t="s">
         <v>93</v>
@@ -4753,7 +4756,7 @@
         <v>80</v>
       </c>
       <c r="D149" s="8" t="s">
-        <v>369</v>
+        <v>367</v>
       </c>
       <c r="E149" s="9" t="s">
         <v>128</v>
@@ -4762,7 +4765,7 @@
         <v>2</v>
       </c>
       <c r="G149" s="14" t="s">
-        <v>370</v>
+        <v>368</v>
       </c>
     </row>
     <row r="150" spans="1:7" ht="17.149999999999999" x14ac:dyDescent="0.55000000000000004">
@@ -4773,7 +4776,7 @@
         <v>13</v>
       </c>
       <c r="D150" s="8" t="s">
-        <v>403</v>
+        <v>401</v>
       </c>
       <c r="F150" s="6">
         <v>3</v>
@@ -4798,7 +4801,7 @@
         <v>13</v>
       </c>
       <c r="D152" s="8" t="s">
-        <v>406</v>
+        <v>404</v>
       </c>
       <c r="F152" s="6">
         <v>3</v>
@@ -4815,7 +4818,7 @@
         <v>95</v>
       </c>
       <c r="D153" s="8" t="s">
-        <v>410</v>
+        <v>408</v>
       </c>
       <c r="F153" s="6">
         <v>3</v>

</xml_diff>

<commit_message>
2024.12.18 LeetCodeHot100 三刷 栈Done
</commit_message>
<xml_diff>
--- a/2024LeetCode刷题记录.xlsx
+++ b/2024LeetCode刷题记录.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\develop\GithubRepo\LeetCode\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BEE9E607-69DF-44A6-9734-2EBB20B25864}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6EE291AF-D27C-4AAD-808B-8EF47BD7307D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-20916" yWindow="2952" windowWidth="19356" windowHeight="11928" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-19920" yWindow="3384" windowWidth="19356" windowHeight="11832" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="727" uniqueCount="423">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="727" uniqueCount="422">
   <si>
     <t>题目</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -939,10 +939,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>我这猪脑子也懂了</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>215. 数组中的第K个最大元素</t>
   </si>
   <si>
@@ -1343,14 +1339,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>2024.10.30</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>2024.11.01</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>以空间换时间，可以使用的数据结构是栈；哨兵；向左向右扩展；739.题的延申</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -1563,6 +1551,14 @@
   </si>
   <si>
     <t>解法四Hardddd；还是解法三更人性化一点；</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>2024.12.18</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>while、temperatures[st.peek()]下标</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -2021,8 +2017,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G153"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A98" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="G108" sqref="G108"/>
+    <sheetView tabSelected="1" topLeftCell="A99" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="C105" sqref="C105"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="14.15" x14ac:dyDescent="0.35"/>
@@ -2071,7 +2067,7 @@
         <v>80</v>
       </c>
       <c r="D2" s="8" t="s">
-        <v>386</v>
+        <v>383</v>
       </c>
       <c r="F2" s="6">
         <v>3</v>
@@ -2088,13 +2084,13 @@
         <v>42</v>
       </c>
       <c r="D3" s="8" t="s">
-        <v>401</v>
+        <v>398</v>
       </c>
       <c r="F3" s="6">
         <v>3</v>
       </c>
       <c r="G3" s="14" t="s">
-        <v>402</v>
+        <v>399</v>
       </c>
     </row>
     <row r="4" spans="1:7" ht="17.149999999999999" x14ac:dyDescent="0.55000000000000004">
@@ -2105,7 +2101,7 @@
         <v>13</v>
       </c>
       <c r="D4" s="8" t="s">
-        <v>404</v>
+        <v>401</v>
       </c>
       <c r="F4" s="6">
         <v>3</v>
@@ -2116,19 +2112,19 @@
         <v>207</v>
       </c>
       <c r="B5" s="6" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
       <c r="C5" s="7" t="s">
         <v>42</v>
       </c>
       <c r="D5" s="8" t="s">
-        <v>401</v>
+        <v>398</v>
       </c>
       <c r="F5" s="6">
         <v>3</v>
       </c>
       <c r="G5" s="14" t="s">
-        <v>402</v>
+        <v>399</v>
       </c>
     </row>
     <row r="6" spans="1:7" ht="17.149999999999999" x14ac:dyDescent="0.55000000000000004">
@@ -2142,7 +2138,7 @@
         <v>13</v>
       </c>
       <c r="D6" s="8" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="E6" s="9" t="s">
         <v>14</v>
@@ -2162,7 +2158,7 @@
         <v>80</v>
       </c>
       <c r="D7" s="8" t="s">
-        <v>406</v>
+        <v>403</v>
       </c>
       <c r="F7" s="6">
         <v>3</v>
@@ -2170,13 +2166,13 @@
     </row>
     <row r="8" spans="1:7" ht="17.149999999999999" x14ac:dyDescent="0.55000000000000004">
       <c r="A8" s="10" t="s">
-        <v>380</v>
+        <v>377</v>
       </c>
       <c r="C8" s="7" t="s">
         <v>13</v>
       </c>
       <c r="D8" s="8" t="s">
-        <v>377</v>
+        <v>374</v>
       </c>
     </row>
     <row r="9" spans="1:7" ht="17.149999999999999" x14ac:dyDescent="0.55000000000000004">
@@ -2187,7 +2183,7 @@
         <v>13</v>
       </c>
       <c r="D9" s="8" t="s">
-        <v>404</v>
+        <v>401</v>
       </c>
       <c r="F9" s="6">
         <v>3</v>
@@ -2204,7 +2200,7 @@
         <v>42</v>
       </c>
       <c r="D10" s="8" t="s">
-        <v>388</v>
+        <v>385</v>
       </c>
       <c r="E10" s="9" t="s">
         <v>93</v>
@@ -2213,7 +2209,7 @@
         <v>4</v>
       </c>
       <c r="G10" s="14" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
     </row>
     <row r="11" spans="1:7" ht="17.149999999999999" x14ac:dyDescent="0.55000000000000004">
@@ -2224,18 +2220,18 @@
         <v>13</v>
       </c>
       <c r="D11" s="8" t="s">
-        <v>404</v>
+        <v>401</v>
       </c>
       <c r="F11" s="6">
         <v>3</v>
       </c>
       <c r="G11" s="14" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
     </row>
     <row r="12" spans="1:7" ht="17.149999999999999" x14ac:dyDescent="0.55000000000000004">
       <c r="A12" s="10" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="B12" s="6" t="s">
         <v>130</v>
@@ -2244,7 +2240,7 @@
         <v>95</v>
       </c>
       <c r="D12" s="8" t="s">
-        <v>372</v>
+        <v>369</v>
       </c>
       <c r="E12" s="9" t="s">
         <v>14</v>
@@ -2253,7 +2249,7 @@
         <v>2</v>
       </c>
       <c r="G12" s="14" t="s">
-        <v>374</v>
+        <v>371</v>
       </c>
     </row>
     <row r="13" spans="1:7" ht="17.149999999999999" x14ac:dyDescent="0.55000000000000004">
@@ -2278,7 +2274,7 @@
     </row>
     <row r="14" spans="1:7" ht="17.149999999999999" x14ac:dyDescent="0.55000000000000004">
       <c r="A14" s="10" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="B14" s="6" t="s">
         <v>187</v>
@@ -2287,7 +2283,7 @@
         <v>6</v>
       </c>
       <c r="D14" s="8" t="s">
-        <v>371</v>
+        <v>368</v>
       </c>
       <c r="F14" s="6">
         <v>2</v>
@@ -2315,16 +2311,16 @@
     </row>
     <row r="16" spans="1:7" ht="17.149999999999999" x14ac:dyDescent="0.55000000000000004">
       <c r="A16" s="10" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="B16" s="6" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="C16" s="7" t="s">
         <v>42</v>
       </c>
       <c r="D16" s="8" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="E16" s="9" t="s">
         <v>14</v>
@@ -2335,16 +2331,16 @@
     </row>
     <row r="17" spans="1:7" ht="17.149999999999999" x14ac:dyDescent="0.55000000000000004">
       <c r="A17" s="10" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="B17" s="6" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="C17" s="7" t="s">
         <v>13</v>
       </c>
       <c r="D17" s="8" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
       <c r="E17" s="9" t="s">
         <v>14</v>
@@ -2352,13 +2348,13 @@
     </row>
     <row r="18" spans="1:7" ht="17.149999999999999" x14ac:dyDescent="0.55000000000000004">
       <c r="A18" s="10" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
       <c r="C18" s="7" t="s">
         <v>42</v>
       </c>
       <c r="D18" s="8" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
       <c r="E18" s="9" t="s">
         <v>14</v>
@@ -2369,13 +2365,13 @@
         <v>220</v>
       </c>
       <c r="B19" s="6" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
       <c r="C19" s="7" t="s">
         <v>13</v>
       </c>
       <c r="D19" s="8" t="s">
-        <v>408</v>
+        <v>405</v>
       </c>
       <c r="F19" s="6">
         <v>3</v>
@@ -2386,7 +2382,7 @@
     </row>
     <row r="20" spans="1:7" ht="17.149999999999999" x14ac:dyDescent="0.55000000000000004">
       <c r="A20" s="10" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="B20" s="6" t="s">
         <v>79</v>
@@ -2395,7 +2391,7 @@
         <v>80</v>
       </c>
       <c r="D20" s="8" t="s">
-        <v>386</v>
+        <v>383</v>
       </c>
       <c r="F20" s="6">
         <v>3</v>
@@ -2412,7 +2408,7 @@
         <v>95</v>
       </c>
       <c r="D21" s="8" t="s">
-        <v>412</v>
+        <v>409</v>
       </c>
       <c r="E21" s="9" t="s">
         <v>128</v>
@@ -2421,21 +2417,21 @@
         <v>3</v>
       </c>
       <c r="G21" s="14" t="s">
-        <v>414</v>
+        <v>411</v>
       </c>
     </row>
     <row r="22" spans="1:7" ht="17.149999999999999" x14ac:dyDescent="0.55000000000000004">
       <c r="A22" s="10" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="B22" s="6" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="C22" s="7" t="s">
         <v>28</v>
       </c>
       <c r="D22" s="8" t="s">
-        <v>369</v>
+        <v>366</v>
       </c>
       <c r="F22" s="6">
         <v>2</v>
@@ -2452,7 +2448,7 @@
         <v>13</v>
       </c>
       <c r="D23" s="8" t="s">
-        <v>396</v>
+        <v>393</v>
       </c>
       <c r="E23" s="9" t="s">
         <v>87</v>
@@ -2463,7 +2459,7 @@
     </row>
     <row r="24" spans="1:7" ht="17.149999999999999" x14ac:dyDescent="0.55000000000000004">
       <c r="A24" s="10" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="B24" s="6" t="s">
         <v>130</v>
@@ -2472,7 +2468,7 @@
         <v>13</v>
       </c>
       <c r="D24" s="8" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
       <c r="E24" s="9" t="s">
         <v>14</v>
@@ -2486,13 +2482,13 @@
         <v>194</v>
       </c>
       <c r="B25" s="6" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
       <c r="C25" s="7" t="s">
         <v>42</v>
       </c>
       <c r="D25" s="8" t="s">
-        <v>394</v>
+        <v>391</v>
       </c>
       <c r="F25" s="6">
         <v>3</v>
@@ -2506,47 +2502,47 @@
         <v>13</v>
       </c>
       <c r="D26" s="8" t="s">
-        <v>394</v>
+        <v>391</v>
       </c>
       <c r="E26" s="13" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="F26" s="6">
         <v>3</v>
       </c>
       <c r="G26" s="14" t="s">
-        <v>395</v>
+        <v>392</v>
       </c>
     </row>
     <row r="27" spans="1:7" ht="17.149999999999999" x14ac:dyDescent="0.55000000000000004">
       <c r="A27" s="10" t="s">
-        <v>381</v>
+        <v>378</v>
       </c>
       <c r="C27" s="7" t="s">
         <v>42</v>
       </c>
       <c r="D27" s="8" t="s">
-        <v>377</v>
+        <v>374</v>
       </c>
       <c r="E27" s="9" t="s">
-        <v>382</v>
+        <v>379</v>
       </c>
       <c r="G27" s="14" t="s">
-        <v>383</v>
+        <v>380</v>
       </c>
     </row>
     <row r="28" spans="1:7" ht="17.149999999999999" x14ac:dyDescent="0.55000000000000004">
       <c r="A28" s="10" t="s">
+        <v>298</v>
+      </c>
+      <c r="B28" s="6" t="s">
         <v>299</v>
-      </c>
-      <c r="B28" s="6" t="s">
-        <v>300</v>
       </c>
       <c r="C28" s="7" t="s">
         <v>42</v>
       </c>
       <c r="D28" s="8" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="F28" s="6">
         <v>2</v>
@@ -2560,7 +2556,7 @@
         <v>95</v>
       </c>
       <c r="D29" s="8" t="s">
-        <v>400</v>
+        <v>397</v>
       </c>
       <c r="F29" s="6">
         <v>3</v>
@@ -2580,13 +2576,13 @@
         <v>80</v>
       </c>
       <c r="D30" s="8" t="s">
+        <v>393</v>
+      </c>
+      <c r="F30" s="6">
+        <v>3</v>
+      </c>
+      <c r="G30" s="14" t="s">
         <v>396</v>
-      </c>
-      <c r="F30" s="6">
-        <v>3</v>
-      </c>
-      <c r="G30" s="14" t="s">
-        <v>399</v>
       </c>
     </row>
     <row r="31" spans="1:7" ht="17.149999999999999" x14ac:dyDescent="0.55000000000000004">
@@ -2600,7 +2596,7 @@
         <v>13</v>
       </c>
       <c r="D31" s="8" t="s">
-        <v>388</v>
+        <v>385</v>
       </c>
       <c r="E31" s="9" t="s">
         <v>97</v>
@@ -2609,12 +2605,12 @@
         <v>3</v>
       </c>
       <c r="G31" s="14" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
     </row>
     <row r="32" spans="1:7" ht="17.149999999999999" x14ac:dyDescent="0.55000000000000004">
       <c r="A32" s="10" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="B32" s="6" t="s">
         <v>187</v>
@@ -2623,7 +2619,7 @@
         <v>6</v>
       </c>
       <c r="D32" s="8" t="s">
-        <v>371</v>
+        <v>368</v>
       </c>
       <c r="F32" s="6">
         <v>2</v>
@@ -2640,13 +2636,13 @@
         <v>13</v>
       </c>
       <c r="D33" s="8" t="s">
-        <v>421</v>
+        <v>418</v>
       </c>
       <c r="F33" s="6">
         <v>3</v>
       </c>
       <c r="G33" s="14" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
     </row>
     <row r="34" spans="1:7" ht="17.149999999999999" x14ac:dyDescent="0.55000000000000004">
@@ -2660,13 +2656,13 @@
         <v>13</v>
       </c>
       <c r="D34" s="8" t="s">
-        <v>366</v>
+        <v>420</v>
       </c>
       <c r="E34" s="9" t="s">
         <v>103</v>
       </c>
       <c r="F34" s="6">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="35" spans="1:7" ht="17.149999999999999" x14ac:dyDescent="0.55000000000000004">
@@ -2711,41 +2707,41 @@
         <v>6</v>
       </c>
       <c r="D37" s="8" t="s">
-        <v>394</v>
+        <v>391</v>
       </c>
       <c r="E37" s="13" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="F37" s="6">
         <v>3</v>
       </c>
       <c r="G37" s="14" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
     </row>
     <row r="38" spans="1:7" ht="17.149999999999999" x14ac:dyDescent="0.55000000000000004">
       <c r="A38" s="10" t="s">
-        <v>384</v>
+        <v>381</v>
       </c>
       <c r="C38" s="7" t="s">
         <v>42</v>
       </c>
       <c r="D38" s="8" t="s">
-        <v>385</v>
+        <v>382</v>
       </c>
     </row>
     <row r="39" spans="1:7" ht="17.149999999999999" x14ac:dyDescent="0.55000000000000004">
       <c r="A39" s="10" t="s">
+        <v>265</v>
+      </c>
+      <c r="B39" s="6" t="s">
         <v>266</v>
-      </c>
-      <c r="B39" s="6" t="s">
-        <v>267</v>
       </c>
       <c r="C39" s="7" t="s">
         <v>13</v>
       </c>
       <c r="D39" s="8" t="s">
-        <v>369</v>
+        <v>366</v>
       </c>
       <c r="F39" s="6">
         <v>2</v>
@@ -2762,7 +2758,7 @@
         <v>80</v>
       </c>
       <c r="D40" s="8" t="s">
-        <v>409</v>
+        <v>406</v>
       </c>
       <c r="E40" s="9" t="s">
         <v>22</v>
@@ -2779,7 +2775,7 @@
         <v>28</v>
       </c>
       <c r="D41" s="8" t="s">
-        <v>392</v>
+        <v>389</v>
       </c>
       <c r="F41" s="6">
         <v>3</v>
@@ -2793,18 +2789,18 @@
         <v>13</v>
       </c>
       <c r="D42" s="8" t="s">
-        <v>396</v>
+        <v>393</v>
       </c>
       <c r="F42" s="6">
         <v>3</v>
       </c>
       <c r="G42" s="14" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
     </row>
     <row r="43" spans="1:7" ht="17.149999999999999" x14ac:dyDescent="0.55000000000000004">
       <c r="A43" s="10" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="B43" s="6" t="s">
         <v>130</v>
@@ -2813,13 +2809,13 @@
         <v>80</v>
       </c>
       <c r="D43" s="8" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="F43" s="6">
         <v>2</v>
       </c>
       <c r="G43" s="14" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
     </row>
     <row r="44" spans="1:7" ht="17.149999999999999" x14ac:dyDescent="0.55000000000000004">
@@ -2830,13 +2826,13 @@
         <v>13</v>
       </c>
       <c r="D44" s="8" t="s">
-        <v>404</v>
+        <v>401</v>
       </c>
       <c r="F44" s="6">
         <v>3</v>
       </c>
       <c r="G44" s="14" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
     </row>
     <row r="45" spans="1:7" ht="17.149999999999999" x14ac:dyDescent="0.55000000000000004">
@@ -2847,7 +2843,7 @@
         <v>6</v>
       </c>
       <c r="D45" s="8" t="s">
-        <v>396</v>
+        <v>393</v>
       </c>
       <c r="F45" s="6">
         <v>3</v>
@@ -2864,10 +2860,10 @@
         <v>80</v>
       </c>
       <c r="D46" s="8" t="s">
-        <v>366</v>
+        <v>420</v>
       </c>
       <c r="F46" s="6">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="47" spans="1:7" ht="17.149999999999999" x14ac:dyDescent="0.55000000000000004">
@@ -2878,7 +2874,7 @@
         <v>13</v>
       </c>
       <c r="D47" s="8" t="s">
-        <v>408</v>
+        <v>405</v>
       </c>
       <c r="F47" s="6">
         <v>3</v>
@@ -2895,7 +2891,7 @@
         <v>80</v>
       </c>
       <c r="D48" s="8" t="s">
-        <v>394</v>
+        <v>391</v>
       </c>
       <c r="F48" s="6">
         <v>3</v>
@@ -2909,7 +2905,7 @@
         <v>80</v>
       </c>
       <c r="D49" s="8" t="s">
-        <v>409</v>
+        <v>406</v>
       </c>
       <c r="F49" s="6">
         <v>3</v>
@@ -2923,7 +2919,7 @@
         <v>13</v>
       </c>
       <c r="D50" s="8" t="s">
-        <v>409</v>
+        <v>406</v>
       </c>
       <c r="F50" s="6">
         <v>3</v>
@@ -2957,27 +2953,27 @@
         <v>42</v>
       </c>
       <c r="D52" s="8" t="s">
-        <v>396</v>
+        <v>393</v>
       </c>
       <c r="F52" s="6">
         <v>3</v>
       </c>
       <c r="G52" s="14" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
     </row>
     <row r="53" spans="1:7" ht="17.149999999999999" x14ac:dyDescent="0.55000000000000004">
       <c r="A53" s="10" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="B53" s="6" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="C53" s="7" t="s">
         <v>13</v>
       </c>
       <c r="D53" s="8" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="E53" s="9" t="s">
         <v>14</v>
@@ -2985,22 +2981,22 @@
     </row>
     <row r="54" spans="1:7" ht="17.149999999999999" x14ac:dyDescent="0.55000000000000004">
       <c r="A54" s="10" t="s">
+        <v>253</v>
+      </c>
+      <c r="B54" s="6" t="s">
         <v>254</v>
-      </c>
-      <c r="B54" s="6" t="s">
-        <v>255</v>
       </c>
       <c r="C54" s="7" t="s">
         <v>13</v>
       </c>
       <c r="D54" s="8" t="s">
-        <v>369</v>
+        <v>366</v>
       </c>
       <c r="F54" s="6">
         <v>3</v>
       </c>
       <c r="G54" s="14" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
     </row>
     <row r="55" spans="1:7" ht="17.149999999999999" x14ac:dyDescent="0.55000000000000004">
@@ -3051,10 +3047,10 @@
         <v>13</v>
       </c>
       <c r="D57" s="8" t="s">
-        <v>412</v>
+        <v>409</v>
       </c>
       <c r="E57" s="9" t="s">
-        <v>413</v>
+        <v>410</v>
       </c>
       <c r="F57" s="6">
         <v>3</v>
@@ -3068,13 +3064,13 @@
         <v>13</v>
       </c>
       <c r="D58" s="8" t="s">
-        <v>401</v>
+        <v>398</v>
       </c>
       <c r="F58" s="6">
         <v>3</v>
       </c>
       <c r="G58" s="14" t="s">
-        <v>402</v>
+        <v>399</v>
       </c>
     </row>
     <row r="59" spans="1:7" ht="17.149999999999999" x14ac:dyDescent="0.55000000000000004">
@@ -3088,7 +3084,7 @@
         <v>13</v>
       </c>
       <c r="D59" s="8" t="s">
-        <v>400</v>
+        <v>397</v>
       </c>
       <c r="F59" s="6">
         <v>3</v>
@@ -3102,13 +3098,13 @@
         <v>13</v>
       </c>
       <c r="D60" s="8" t="s">
-        <v>404</v>
+        <v>401</v>
       </c>
       <c r="F60" s="6">
         <v>3</v>
       </c>
       <c r="G60" s="14" t="s">
-        <v>405</v>
+        <v>402</v>
       </c>
     </row>
     <row r="61" spans="1:7" ht="17.149999999999999" x14ac:dyDescent="0.55000000000000004">
@@ -3119,7 +3115,7 @@
         <v>95</v>
       </c>
       <c r="D61" s="8" t="s">
-        <v>394</v>
+        <v>391</v>
       </c>
       <c r="F61" s="6">
         <v>3</v>
@@ -3130,13 +3126,13 @@
         <v>219</v>
       </c>
       <c r="B62" s="6" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
       <c r="C62" s="7" t="s">
         <v>80</v>
       </c>
       <c r="D62" s="8" t="s">
-        <v>407</v>
+        <v>404</v>
       </c>
       <c r="E62" s="9" t="s">
         <v>93</v>
@@ -3145,7 +3141,7 @@
         <v>3</v>
       </c>
       <c r="G62" s="14" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
     </row>
     <row r="63" spans="1:7" ht="17.149999999999999" x14ac:dyDescent="0.55000000000000004">
@@ -3153,13 +3149,13 @@
         <v>178</v>
       </c>
       <c r="B63" s="6" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="C63" s="7" t="s">
         <v>6</v>
       </c>
       <c r="D63" s="8" t="s">
-        <v>392</v>
+        <v>389</v>
       </c>
       <c r="F63" s="6">
         <v>3</v>
@@ -3176,7 +3172,7 @@
         <v>95</v>
       </c>
       <c r="D64" s="8" t="s">
-        <v>391</v>
+        <v>388</v>
       </c>
       <c r="E64" s="9" t="s">
         <v>118</v>
@@ -3207,19 +3203,19 @@
     </row>
     <row r="66" spans="1:7" ht="17.149999999999999" x14ac:dyDescent="0.55000000000000004">
       <c r="A66" s="10" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="C66" s="7" t="s">
         <v>95</v>
       </c>
       <c r="D66" s="8" t="s">
-        <v>396</v>
+        <v>393</v>
       </c>
       <c r="F66" s="6">
         <v>3</v>
       </c>
       <c r="G66" s="14" t="s">
-        <v>398</v>
+        <v>395</v>
       </c>
     </row>
     <row r="67" spans="1:7" ht="17.149999999999999" x14ac:dyDescent="0.55000000000000004">
@@ -3233,7 +3229,7 @@
         <v>42</v>
       </c>
       <c r="D67" s="8" t="s">
-        <v>393</v>
+        <v>390</v>
       </c>
       <c r="E67" s="9" t="s">
         <v>93</v>
@@ -3270,19 +3266,19 @@
         <v>199</v>
       </c>
       <c r="B69" s="6" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="C69" s="7" t="s">
         <v>95</v>
       </c>
       <c r="D69" s="8" t="s">
-        <v>396</v>
+        <v>393</v>
       </c>
       <c r="F69" s="6">
         <v>4</v>
       </c>
       <c r="G69" s="14" t="s">
-        <v>397</v>
+        <v>394</v>
       </c>
     </row>
     <row r="70" spans="1:7" ht="17.149999999999999" x14ac:dyDescent="0.55000000000000004">
@@ -3324,13 +3320,13 @@
     </row>
     <row r="72" spans="1:7" ht="17.149999999999999" x14ac:dyDescent="0.55000000000000004">
       <c r="A72" s="10" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="C72" s="7" t="s">
         <v>42</v>
       </c>
       <c r="D72" s="8" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
     </row>
     <row r="73" spans="1:7" ht="17.149999999999999" x14ac:dyDescent="0.55000000000000004">
@@ -3423,7 +3419,7 @@
     </row>
     <row r="78" spans="1:7" ht="17.149999999999999" x14ac:dyDescent="0.55000000000000004">
       <c r="A78" s="10" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="B78" s="6" t="s">
         <v>130</v>
@@ -3432,10 +3428,10 @@
         <v>80</v>
       </c>
       <c r="D78" s="8" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
       <c r="E78" s="13" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
       <c r="F78" s="6">
         <v>2</v>
@@ -3443,16 +3439,16 @@
     </row>
     <row r="79" spans="1:7" ht="17.149999999999999" x14ac:dyDescent="0.55000000000000004">
       <c r="A79" s="10" t="s">
-        <v>379</v>
+        <v>376</v>
       </c>
       <c r="C79" s="7" t="s">
         <v>13</v>
       </c>
       <c r="D79" s="8" t="s">
-        <v>377</v>
+        <v>374</v>
       </c>
       <c r="G79" s="14" t="s">
-        <v>378</v>
+        <v>375</v>
       </c>
     </row>
     <row r="80" spans="1:7" ht="17.149999999999999" x14ac:dyDescent="0.55000000000000004">
@@ -3505,16 +3501,16 @@
     </row>
     <row r="83" spans="1:7" ht="17.149999999999999" x14ac:dyDescent="0.55000000000000004">
       <c r="A83" s="10" t="s">
+        <v>302</v>
+      </c>
+      <c r="B83" s="6" t="s">
         <v>303</v>
-      </c>
-      <c r="B83" s="6" t="s">
-        <v>304</v>
       </c>
       <c r="C83" s="7" t="s">
         <v>80</v>
       </c>
       <c r="D83" s="8" t="s">
-        <v>387</v>
+        <v>384</v>
       </c>
       <c r="E83" s="9" t="s">
         <v>87</v>
@@ -3581,19 +3577,19 @@
     </row>
     <row r="88" spans="1:7" ht="17.149999999999999" x14ac:dyDescent="0.55000000000000004">
       <c r="A88" s="10" t="s">
+        <v>272</v>
+      </c>
+      <c r="B88" s="6" t="s">
         <v>273</v>
-      </c>
-      <c r="B88" s="6" t="s">
-        <v>274</v>
       </c>
       <c r="C88" s="7" t="s">
         <v>13</v>
       </c>
       <c r="D88" s="8" t="s">
-        <v>369</v>
+        <v>366</v>
       </c>
       <c r="E88" s="9" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="F88" s="6">
         <v>2</v>
@@ -3601,16 +3597,16 @@
     </row>
     <row r="89" spans="1:7" ht="17.149999999999999" x14ac:dyDescent="0.55000000000000004">
       <c r="A89" s="10" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="B89" s="6" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="C89" s="7" t="s">
         <v>80</v>
       </c>
       <c r="D89" s="8" t="s">
-        <v>369</v>
+        <v>366</v>
       </c>
       <c r="E89" s="9" t="s">
         <v>8</v>
@@ -3619,7 +3615,7 @@
         <v>2</v>
       </c>
       <c r="G89" s="14" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
     </row>
     <row r="90" spans="1:7" ht="17.149999999999999" x14ac:dyDescent="0.55000000000000004">
@@ -3633,7 +3629,7 @@
         <v>80</v>
       </c>
       <c r="D90" s="8" t="s">
-        <v>389</v>
+        <v>386</v>
       </c>
       <c r="E90" s="9" t="s">
         <v>109</v>
@@ -3642,12 +3638,12 @@
         <v>3</v>
       </c>
       <c r="G90" s="14" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
     </row>
     <row r="91" spans="1:7" ht="17.149999999999999" x14ac:dyDescent="0.55000000000000004">
       <c r="A91" s="10" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="B91" s="6" t="s">
         <v>130</v>
@@ -3656,30 +3652,30 @@
         <v>80</v>
       </c>
       <c r="D91" s="8" t="s">
-        <v>371</v>
+        <v>368</v>
       </c>
       <c r="F91" s="6">
         <v>2</v>
       </c>
       <c r="G91" s="14" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
     </row>
     <row r="92" spans="1:7" ht="17.149999999999999" x14ac:dyDescent="0.55000000000000004">
       <c r="A92" s="10" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="B92" s="6" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="C92" s="7" t="s">
         <v>42</v>
       </c>
       <c r="D92" s="8" t="s">
-        <v>369</v>
+        <v>366</v>
       </c>
       <c r="E92" s="9" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="F92" s="6">
         <v>2</v>
@@ -3687,18 +3683,18 @@
     </row>
     <row r="93" spans="1:7" ht="17.149999999999999" x14ac:dyDescent="0.55000000000000004">
       <c r="A93" s="10" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="C93" s="7" t="s">
         <v>28</v>
       </c>
       <c r="D93" s="8" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
     </row>
     <row r="94" spans="1:7" ht="17.149999999999999" x14ac:dyDescent="0.55000000000000004">
       <c r="A94" s="10" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="B94" s="6" t="s">
         <v>130</v>
@@ -3707,7 +3703,7 @@
         <v>13</v>
       </c>
       <c r="D94" s="8" t="s">
-        <v>371</v>
+        <v>368</v>
       </c>
       <c r="F94" s="6">
         <v>2</v>
@@ -3715,16 +3711,16 @@
     </row>
     <row r="95" spans="1:7" ht="17.149999999999999" x14ac:dyDescent="0.55000000000000004">
       <c r="A95" s="10" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="B95" s="6" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="C95" s="7" t="s">
         <v>13</v>
       </c>
       <c r="D95" s="8" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="F95" s="6">
         <v>2</v>
@@ -3741,7 +3737,7 @@
         <v>95</v>
       </c>
       <c r="D96" s="8" t="s">
-        <v>418</v>
+        <v>415</v>
       </c>
       <c r="E96" s="12" t="s">
         <v>241</v>
@@ -3750,21 +3746,21 @@
         <v>3</v>
       </c>
       <c r="G96" s="14" t="s">
-        <v>420</v>
+        <v>417</v>
       </c>
     </row>
     <row r="97" spans="1:7" ht="17.149999999999999" x14ac:dyDescent="0.55000000000000004">
       <c r="A97" s="10" t="s">
+        <v>341</v>
+      </c>
+      <c r="B97" s="6" t="s">
         <v>342</v>
-      </c>
-      <c r="B97" s="6" t="s">
-        <v>343</v>
       </c>
       <c r="C97" s="7" t="s">
         <v>13</v>
       </c>
       <c r="D97" s="8" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
       <c r="E97" s="9" t="s">
         <v>14</v>
@@ -3781,7 +3777,7 @@
         <v>80</v>
       </c>
       <c r="D98" s="8" t="s">
-        <v>418</v>
+        <v>415</v>
       </c>
       <c r="E98" s="9" t="s">
         <v>22</v>
@@ -3792,16 +3788,16 @@
     </row>
     <row r="99" spans="1:7" ht="17.149999999999999" x14ac:dyDescent="0.55000000000000004">
       <c r="A99" s="10" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="B99" s="6" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="C99" s="7" t="s">
         <v>13</v>
       </c>
       <c r="D99" s="8" t="s">
-        <v>369</v>
+        <v>366</v>
       </c>
       <c r="F99" s="6">
         <v>2</v>
@@ -3818,13 +3814,13 @@
         <v>42</v>
       </c>
       <c r="D100" s="8" t="s">
-        <v>416</v>
+        <v>413</v>
       </c>
       <c r="F100" s="6">
         <v>3</v>
       </c>
       <c r="G100" s="14" t="s">
-        <v>417</v>
+        <v>414</v>
       </c>
     </row>
     <row r="101" spans="1:7" ht="17.149999999999999" x14ac:dyDescent="0.55000000000000004">
@@ -3843,16 +3839,16 @@
     </row>
     <row r="102" spans="1:7" ht="17.149999999999999" x14ac:dyDescent="0.55000000000000004">
       <c r="A102" s="10" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="B102" s="6" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="C102" s="7" t="s">
         <v>13</v>
       </c>
       <c r="D102" s="8" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="E102" s="9" t="s">
         <v>14</v>
@@ -3889,13 +3885,13 @@
         <v>95</v>
       </c>
       <c r="D104" s="8" t="s">
-        <v>409</v>
+        <v>406</v>
       </c>
       <c r="F104" s="6">
         <v>3</v>
       </c>
       <c r="G104" s="14" t="s">
-        <v>411</v>
+        <v>408</v>
       </c>
     </row>
     <row r="105" spans="1:7" ht="17.149999999999999" x14ac:dyDescent="0.55000000000000004">
@@ -3906,16 +3902,16 @@
         <v>248</v>
       </c>
       <c r="C105" s="7" t="s">
-        <v>80</v>
+        <v>95</v>
       </c>
       <c r="D105" s="8" t="s">
-        <v>366</v>
+        <v>420</v>
       </c>
       <c r="E105" s="9" t="s">
         <v>93</v>
       </c>
       <c r="F105" s="6">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="106" spans="1:7" ht="17.149999999999999" x14ac:dyDescent="0.55000000000000004">
@@ -3929,7 +3925,7 @@
         <v>80</v>
       </c>
       <c r="D106" s="8" t="s">
-        <v>421</v>
+        <v>418</v>
       </c>
       <c r="E106" s="9" t="s">
         <v>98</v>
@@ -3938,7 +3934,7 @@
         <v>2</v>
       </c>
       <c r="G106" s="14" t="s">
-        <v>422</v>
+        <v>419</v>
       </c>
     </row>
     <row r="107" spans="1:7" ht="17.149999999999999" x14ac:dyDescent="0.55000000000000004">
@@ -3952,18 +3948,18 @@
         <v>13</v>
       </c>
       <c r="D107" s="8" t="s">
-        <v>392</v>
+        <v>389</v>
       </c>
       <c r="F107" s="6">
         <v>3</v>
       </c>
       <c r="G107" s="14" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
     </row>
     <row r="108" spans="1:7" ht="17.149999999999999" x14ac:dyDescent="0.55000000000000004">
       <c r="A108" s="10" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="B108" s="6" t="s">
         <v>12</v>
@@ -3972,10 +3968,10 @@
         <v>80</v>
       </c>
       <c r="D108" s="8" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="E108" s="9" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="F108" s="6">
         <v>3</v>
@@ -3995,7 +3991,7 @@
         <v>80</v>
       </c>
       <c r="D109" s="8" t="s">
-        <v>389</v>
+        <v>386</v>
       </c>
       <c r="E109" s="9" t="s">
         <v>98</v>
@@ -4012,19 +4008,19 @@
         <v>218</v>
       </c>
       <c r="B110" s="6" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
       <c r="C110" s="7" t="s">
         <v>80</v>
       </c>
       <c r="D110" s="8" t="s">
-        <v>407</v>
+        <v>404</v>
       </c>
       <c r="F110" s="6">
         <v>3</v>
       </c>
       <c r="G110" s="14" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
     </row>
     <row r="111" spans="1:7" ht="17.149999999999999" x14ac:dyDescent="0.55000000000000004">
@@ -4038,7 +4034,7 @@
         <v>95</v>
       </c>
       <c r="D111" s="8" t="s">
-        <v>389</v>
+        <v>386</v>
       </c>
       <c r="E111" s="9" t="s">
         <v>110</v>
@@ -4047,7 +4043,7 @@
         <v>4</v>
       </c>
       <c r="G111" s="14" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
     </row>
     <row r="112" spans="1:7" ht="17.149999999999999" x14ac:dyDescent="0.55000000000000004">
@@ -4072,7 +4068,7 @@
     </row>
     <row r="113" spans="1:7" ht="17.149999999999999" x14ac:dyDescent="0.55000000000000004">
       <c r="A113" s="10" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="B113" s="6" t="s">
         <v>148</v>
@@ -4081,7 +4077,7 @@
         <v>13</v>
       </c>
       <c r="D113" s="8" t="s">
-        <v>369</v>
+        <v>366</v>
       </c>
       <c r="F113" s="6">
         <v>2</v>
@@ -4098,7 +4094,7 @@
         <v>13</v>
       </c>
       <c r="D114" s="8" t="s">
-        <v>409</v>
+        <v>406</v>
       </c>
       <c r="E114" s="9" t="s">
         <v>128</v>
@@ -4132,16 +4128,16 @@
     </row>
     <row r="116" spans="1:7" ht="17.149999999999999" x14ac:dyDescent="0.55000000000000004">
       <c r="A116" s="10" t="s">
+        <v>315</v>
+      </c>
+      <c r="B116" s="6" t="s">
         <v>316</v>
-      </c>
-      <c r="B116" s="6" t="s">
-        <v>317</v>
       </c>
       <c r="C116" s="7" t="s">
         <v>80</v>
       </c>
       <c r="D116" s="8" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="E116" s="9" t="s">
         <v>14</v>
@@ -4158,7 +4154,7 @@
         <v>6</v>
       </c>
       <c r="D117" s="8" t="s">
-        <v>393</v>
+        <v>390</v>
       </c>
       <c r="E117" s="9" t="s">
         <v>93</v>
@@ -4178,27 +4174,27 @@
         <v>80</v>
       </c>
       <c r="D118" s="8" t="s">
-        <v>386</v>
+        <v>383</v>
       </c>
       <c r="F118" s="6">
         <v>4</v>
       </c>
       <c r="G118" s="14" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
     </row>
     <row r="119" spans="1:7" ht="17.149999999999999" x14ac:dyDescent="0.55000000000000004">
       <c r="A119" s="10" t="s">
+        <v>313</v>
+      </c>
+      <c r="B119" s="6" t="s">
         <v>314</v>
-      </c>
-      <c r="B119" s="6" t="s">
-        <v>315</v>
       </c>
       <c r="C119" s="7" t="s">
         <v>80</v>
       </c>
       <c r="D119" s="8" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="E119" s="9" t="s">
         <v>14</v>
@@ -4206,7 +4202,7 @@
     </row>
     <row r="120" spans="1:7" ht="17.149999999999999" x14ac:dyDescent="0.55000000000000004">
       <c r="A120" s="10" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="B120" s="6" t="s">
         <v>130</v>
@@ -4215,7 +4211,7 @@
         <v>95</v>
       </c>
       <c r="D120" s="8" t="s">
-        <v>386</v>
+        <v>383</v>
       </c>
       <c r="E120" s="9" t="s">
         <v>22</v>
@@ -4224,7 +4220,7 @@
         <v>3</v>
       </c>
       <c r="G120" s="14" t="s">
-        <v>373</v>
+        <v>370</v>
       </c>
     </row>
     <row r="121" spans="1:7" ht="17.149999999999999" x14ac:dyDescent="0.55000000000000004">
@@ -4238,7 +4234,7 @@
         <v>80</v>
       </c>
       <c r="D121" s="8" t="s">
-        <v>412</v>
+        <v>409</v>
       </c>
       <c r="E121" s="9" t="s">
         <v>14</v>
@@ -4247,7 +4243,7 @@
         <v>3</v>
       </c>
       <c r="G121" s="14" t="s">
-        <v>415</v>
+        <v>412</v>
       </c>
     </row>
     <row r="122" spans="1:7" ht="17.149999999999999" x14ac:dyDescent="0.55000000000000004">
@@ -4269,16 +4265,16 @@
     </row>
     <row r="123" spans="1:7" ht="17.149999999999999" x14ac:dyDescent="0.55000000000000004">
       <c r="A123" s="10" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="B123" s="6" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="C123" s="7" t="s">
         <v>13</v>
       </c>
       <c r="D123" s="8" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
     </row>
     <row r="124" spans="1:7" ht="17.149999999999999" x14ac:dyDescent="0.55000000000000004">
@@ -4286,13 +4282,13 @@
         <v>127</v>
       </c>
       <c r="B124" s="6" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="C124" s="7" t="s">
         <v>42</v>
       </c>
       <c r="D124" s="8" t="s">
-        <v>392</v>
+        <v>389</v>
       </c>
       <c r="E124" s="9" t="s">
         <v>128</v>
@@ -4306,13 +4302,13 @@
         <v>184</v>
       </c>
       <c r="B125" s="6" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="C125" s="7" t="s">
         <v>42</v>
       </c>
       <c r="D125" s="8" t="s">
-        <v>393</v>
+        <v>390</v>
       </c>
       <c r="E125" s="10" t="s">
         <v>185</v>
@@ -4321,7 +4317,7 @@
         <v>3</v>
       </c>
       <c r="G125" s="14" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
     </row>
     <row r="126" spans="1:7" ht="17.149999999999999" x14ac:dyDescent="0.55000000000000004">
@@ -4332,18 +4328,18 @@
         <v>13</v>
       </c>
       <c r="D126" s="8" t="s">
-        <v>401</v>
+        <v>398</v>
       </c>
       <c r="F126" s="6">
         <v>3</v>
       </c>
       <c r="G126" s="14" t="s">
-        <v>403</v>
+        <v>400</v>
       </c>
     </row>
     <row r="127" spans="1:7" ht="17.149999999999999" x14ac:dyDescent="0.55000000000000004">
       <c r="A127" s="10" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="B127" s="6" t="s">
         <v>148</v>
@@ -4352,7 +4348,7 @@
         <v>42</v>
       </c>
       <c r="D127" s="8" t="s">
-        <v>369</v>
+        <v>366</v>
       </c>
       <c r="F127" s="6">
         <v>2</v>
@@ -4369,7 +4365,7 @@
         <v>80</v>
       </c>
       <c r="D128" s="8" t="s">
-        <v>392</v>
+        <v>389</v>
       </c>
       <c r="E128" s="9" t="s">
         <v>131</v>
@@ -4389,7 +4385,7 @@
         <v>95</v>
       </c>
       <c r="D129" s="8" t="s">
-        <v>390</v>
+        <v>387</v>
       </c>
       <c r="E129" s="9" t="s">
         <v>118</v>
@@ -4400,7 +4396,7 @@
     </row>
     <row r="130" spans="1:7" ht="17.149999999999999" x14ac:dyDescent="0.55000000000000004">
       <c r="A130" s="10" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="B130" s="6" t="s">
         <v>130</v>
@@ -4409,7 +4405,7 @@
         <v>13</v>
       </c>
       <c r="D130" s="8" t="s">
-        <v>372</v>
+        <v>369</v>
       </c>
       <c r="E130" s="9" t="s">
         <v>14</v>
@@ -4420,18 +4416,18 @@
     </row>
     <row r="131" spans="1:7" ht="17.149999999999999" x14ac:dyDescent="0.55000000000000004">
       <c r="A131" s="10" t="s">
-        <v>376</v>
+        <v>373</v>
       </c>
       <c r="C131" s="7" t="s">
         <v>42</v>
       </c>
       <c r="D131" s="8" t="s">
-        <v>377</v>
+        <v>374</v>
       </c>
     </row>
     <row r="132" spans="1:7" ht="17.149999999999999" x14ac:dyDescent="0.55000000000000004">
       <c r="A132" s="10" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="B132" s="6" t="s">
         <v>130</v>
@@ -4440,7 +4436,7 @@
         <v>13</v>
       </c>
       <c r="D132" s="8" t="s">
-        <v>372</v>
+        <v>369</v>
       </c>
       <c r="F132" s="6">
         <v>2</v>
@@ -4468,7 +4464,7 @@
     </row>
     <row r="134" spans="1:7" ht="17.149999999999999" x14ac:dyDescent="0.55000000000000004">
       <c r="A134" s="10" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="B134" s="6" t="s">
         <v>130</v>
@@ -4477,7 +4473,7 @@
         <v>42</v>
       </c>
       <c r="D134" s="8" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
       <c r="F134" s="6">
         <v>2</v>
@@ -4485,13 +4481,13 @@
     </row>
     <row r="135" spans="1:7" ht="17.149999999999999" x14ac:dyDescent="0.55000000000000004">
       <c r="A135" s="10" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="C135" s="7" t="s">
         <v>13</v>
       </c>
       <c r="D135" s="8" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
     </row>
     <row r="136" spans="1:7" ht="17.149999999999999" x14ac:dyDescent="0.55000000000000004">
@@ -4513,7 +4509,7 @@
     </row>
     <row r="137" spans="1:7" ht="17.149999999999999" x14ac:dyDescent="0.55000000000000004">
       <c r="A137" s="10" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="B137" s="6" t="s">
         <v>130</v>
@@ -4522,7 +4518,7 @@
         <v>80</v>
       </c>
       <c r="D137" s="8" t="s">
-        <v>372</v>
+        <v>369</v>
       </c>
       <c r="E137" s="9" t="s">
         <v>14</v>
@@ -4531,7 +4527,7 @@
         <v>2</v>
       </c>
       <c r="G137" s="14" t="s">
-        <v>375</v>
+        <v>372</v>
       </c>
     </row>
     <row r="138" spans="1:7" ht="17.149999999999999" x14ac:dyDescent="0.55000000000000004">
@@ -4539,13 +4535,13 @@
         <v>181</v>
       </c>
       <c r="B138" s="6" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="C138" s="7" t="s">
         <v>42</v>
       </c>
       <c r="D138" s="8" t="s">
-        <v>393</v>
+        <v>390</v>
       </c>
       <c r="E138" s="9" t="s">
         <v>183</v>
@@ -4585,7 +4581,7 @@
         <v>80</v>
       </c>
       <c r="D140" s="8" t="s">
-        <v>367</v>
+        <v>420</v>
       </c>
       <c r="E140" s="9" t="s">
         <v>250</v>
@@ -4594,7 +4590,7 @@
         <v>2</v>
       </c>
       <c r="G140" s="14" t="s">
-        <v>253</v>
+        <v>421</v>
       </c>
     </row>
     <row r="141" spans="1:7" ht="17.149999999999999" x14ac:dyDescent="0.55000000000000004">
@@ -4608,27 +4604,27 @@
         <v>42</v>
       </c>
       <c r="D141" s="8" t="s">
-        <v>418</v>
+        <v>415</v>
       </c>
       <c r="F141" s="6">
         <v>3</v>
       </c>
       <c r="G141" s="14" t="s">
-        <v>419</v>
+        <v>416</v>
       </c>
     </row>
     <row r="142" spans="1:7" ht="17.149999999999999" x14ac:dyDescent="0.55000000000000004">
       <c r="A142" s="10" t="s">
+        <v>267</v>
+      </c>
+      <c r="B142" s="6" t="s">
         <v>268</v>
-      </c>
-      <c r="B142" s="6" t="s">
-        <v>269</v>
       </c>
       <c r="C142" s="7" t="s">
         <v>6</v>
       </c>
       <c r="D142" s="8" t="s">
-        <v>369</v>
+        <v>366</v>
       </c>
       <c r="F142" s="6">
         <v>2</v>
@@ -4645,7 +4641,7 @@
         <v>95</v>
       </c>
       <c r="D143" s="8" t="s">
-        <v>391</v>
+        <v>388</v>
       </c>
       <c r="E143" s="9" t="s">
         <v>122</v>
@@ -4656,7 +4652,7 @@
     </row>
     <row r="144" spans="1:7" ht="17.149999999999999" x14ac:dyDescent="0.55000000000000004">
       <c r="A144" s="10" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="B144" s="6" t="s">
         <v>148</v>
@@ -4665,7 +4661,7 @@
         <v>13</v>
       </c>
       <c r="D144" s="8" t="s">
-        <v>370</v>
+        <v>367</v>
       </c>
       <c r="E144" s="9" t="s">
         <v>22</v>
@@ -4679,7 +4675,7 @@
         <v>13</v>
       </c>
       <c r="D145" s="8" t="s">
-        <v>409</v>
+        <v>406</v>
       </c>
       <c r="E145" s="9" t="s">
         <v>47</v>
@@ -4688,7 +4684,7 @@
         <v>4</v>
       </c>
       <c r="G145" s="14" t="s">
-        <v>410</v>
+        <v>407</v>
       </c>
     </row>
     <row r="146" spans="1:7" ht="17.149999999999999" x14ac:dyDescent="0.55000000000000004">
@@ -4702,7 +4698,7 @@
         <v>13</v>
       </c>
       <c r="D146" s="8" t="s">
-        <v>412</v>
+        <v>409</v>
       </c>
       <c r="E146" s="9" t="s">
         <v>93</v>
@@ -4756,16 +4752,16 @@
         <v>80</v>
       </c>
       <c r="D149" s="8" t="s">
-        <v>367</v>
+        <v>420</v>
       </c>
       <c r="E149" s="9" t="s">
         <v>128</v>
       </c>
       <c r="F149" s="6">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="G149" s="14" t="s">
-        <v>368</v>
+        <v>365</v>
       </c>
     </row>
     <row r="150" spans="1:7" ht="17.149999999999999" x14ac:dyDescent="0.55000000000000004">
@@ -4776,7 +4772,7 @@
         <v>13</v>
       </c>
       <c r="D150" s="8" t="s">
-        <v>401</v>
+        <v>398</v>
       </c>
       <c r="F150" s="6">
         <v>3</v>
@@ -4784,13 +4780,13 @@
     </row>
     <row r="151" spans="1:7" ht="17.149999999999999" x14ac:dyDescent="0.55000000000000004">
       <c r="A151" s="10" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="C151" s="7" t="s">
         <v>42</v>
       </c>
       <c r="D151" s="8" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
     </row>
     <row r="152" spans="1:7" ht="17.149999999999999" x14ac:dyDescent="0.55000000000000004">
@@ -4801,7 +4797,7 @@
         <v>13</v>
       </c>
       <c r="D152" s="8" t="s">
-        <v>404</v>
+        <v>401</v>
       </c>
       <c r="F152" s="6">
         <v>3</v>
@@ -4812,19 +4808,19 @@
         <v>223</v>
       </c>
       <c r="B153" s="6" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
       <c r="C153" s="7" t="s">
         <v>95</v>
       </c>
       <c r="D153" s="8" t="s">
-        <v>408</v>
+        <v>405</v>
       </c>
       <c r="F153" s="6">
         <v>3</v>
       </c>
       <c r="G153" s="14" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
2024.12.19 LeetCodeHot100 三刷 堆Done
</commit_message>
<xml_diff>
--- a/2024LeetCode刷题记录.xlsx
+++ b/2024LeetCode刷题记录.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\develop\GithubRepo\LeetCode\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{428E6B37-C8B8-49F5-BA0B-9F1DF52E067D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F6A63C08-2344-45E9-A172-FF3A4E43DCB7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-19920" yWindow="3384" windowWidth="19356" windowHeight="11832" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-103" yWindow="-103" windowWidth="22149" windowHeight="11829" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="727" uniqueCount="422">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="727" uniqueCount="423">
   <si>
     <t>题目</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -1559,6 +1559,10 @@
   </si>
   <si>
     <t>while、temperatures[st.peek()]下标</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>2024.12.19</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -2017,8 +2021,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G153"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A135" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="C149" sqref="C149"/>
+    <sheetView tabSelected="1" topLeftCell="A81" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="F89" sqref="F89"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="14.15" x14ac:dyDescent="0.35"/>
@@ -2990,13 +2994,10 @@
         <v>13</v>
       </c>
       <c r="D54" s="8" t="s">
-        <v>366</v>
+        <v>422</v>
       </c>
       <c r="F54" s="6">
-        <v>3</v>
-      </c>
-      <c r="G54" s="14" t="s">
-        <v>332</v>
+        <v>4</v>
       </c>
     </row>
     <row r="55" spans="1:7" ht="17.149999999999999" x14ac:dyDescent="0.55000000000000004">
@@ -3015,6 +3016,9 @@
       <c r="E55" s="9" t="s">
         <v>134</v>
       </c>
+      <c r="G55" s="14" t="s">
+        <v>332</v>
+      </c>
     </row>
     <row r="56" spans="1:7" ht="17.149999999999999" x14ac:dyDescent="0.55000000000000004">
       <c r="A56" s="10" t="s">
@@ -3606,13 +3610,13 @@
         <v>80</v>
       </c>
       <c r="D89" s="8" t="s">
-        <v>366</v>
+        <v>422</v>
       </c>
       <c r="E89" s="9" t="s">
         <v>8</v>
       </c>
       <c r="F89" s="6">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="G89" s="14" t="s">
         <v>259</v>
@@ -3794,13 +3798,13 @@
         <v>255</v>
       </c>
       <c r="C99" s="7" t="s">
-        <v>13</v>
+        <v>80</v>
       </c>
       <c r="D99" s="8" t="s">
-        <v>366</v>
+        <v>422</v>
       </c>
       <c r="F99" s="6">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="100" spans="1:7" ht="17.149999999999999" x14ac:dyDescent="0.55000000000000004">

</xml_diff>

<commit_message>
2024.12.20 LeetCodeHot100 三刷 贪心done
</commit_message>
<xml_diff>
--- a/2024LeetCode刷题记录.xlsx
+++ b/2024LeetCode刷题记录.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\develop\GithubRepo\LeetCode\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F6A63C08-2344-45E9-A172-FF3A4E43DCB7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E1E8A4B8-2D52-4B9E-9B8A-DD2EFC67FFD0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-103" yWindow="-103" windowWidth="22149" windowHeight="11829" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="727" uniqueCount="423">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="727" uniqueCount="422">
   <si>
     <t>题目</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -1267,10 +1267,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>2024.09.26</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>ListNode dummy = new ListNode(-1);应付空节点或单节点</t>
   </si>
   <si>
@@ -1347,10 +1343,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>2024.11</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>2024.11.05</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -1563,6 +1555,10 @@
   </si>
   <si>
     <t>2024.12.19</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>2024.12.20</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -2021,8 +2017,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G153"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A81" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="F89" sqref="F89"/>
+    <sheetView tabSelected="1" topLeftCell="A132" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="F144" sqref="F144"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="14.15" x14ac:dyDescent="0.35"/>
@@ -2071,7 +2067,7 @@
         <v>80</v>
       </c>
       <c r="D2" s="8" t="s">
-        <v>383</v>
+        <v>381</v>
       </c>
       <c r="F2" s="6">
         <v>3</v>
@@ -2088,13 +2084,13 @@
         <v>42</v>
       </c>
       <c r="D3" s="8" t="s">
-        <v>398</v>
+        <v>396</v>
       </c>
       <c r="F3" s="6">
         <v>3</v>
       </c>
       <c r="G3" s="14" t="s">
-        <v>399</v>
+        <v>397</v>
       </c>
     </row>
     <row r="4" spans="1:7" ht="17.149999999999999" x14ac:dyDescent="0.55000000000000004">
@@ -2105,7 +2101,7 @@
         <v>13</v>
       </c>
       <c r="D4" s="8" t="s">
-        <v>401</v>
+        <v>399</v>
       </c>
       <c r="F4" s="6">
         <v>3</v>
@@ -2116,19 +2112,19 @@
         <v>207</v>
       </c>
       <c r="B5" s="6" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
       <c r="C5" s="7" t="s">
         <v>42</v>
       </c>
       <c r="D5" s="8" t="s">
-        <v>398</v>
+        <v>396</v>
       </c>
       <c r="F5" s="6">
         <v>3</v>
       </c>
       <c r="G5" s="14" t="s">
-        <v>399</v>
+        <v>397</v>
       </c>
     </row>
     <row r="6" spans="1:7" ht="17.149999999999999" x14ac:dyDescent="0.55000000000000004">
@@ -2162,7 +2158,7 @@
         <v>80</v>
       </c>
       <c r="D7" s="8" t="s">
-        <v>403</v>
+        <v>401</v>
       </c>
       <c r="F7" s="6">
         <v>3</v>
@@ -2170,13 +2166,13 @@
     </row>
     <row r="8" spans="1:7" ht="17.149999999999999" x14ac:dyDescent="0.55000000000000004">
       <c r="A8" s="10" t="s">
-        <v>377</v>
+        <v>375</v>
       </c>
       <c r="C8" s="7" t="s">
         <v>13</v>
       </c>
       <c r="D8" s="8" t="s">
-        <v>374</v>
+        <v>372</v>
       </c>
     </row>
     <row r="9" spans="1:7" ht="17.149999999999999" x14ac:dyDescent="0.55000000000000004">
@@ -2187,7 +2183,7 @@
         <v>13</v>
       </c>
       <c r="D9" s="8" t="s">
-        <v>401</v>
+        <v>399</v>
       </c>
       <c r="F9" s="6">
         <v>3</v>
@@ -2204,7 +2200,7 @@
         <v>42</v>
       </c>
       <c r="D10" s="8" t="s">
-        <v>385</v>
+        <v>383</v>
       </c>
       <c r="E10" s="9" t="s">
         <v>93</v>
@@ -2224,13 +2220,13 @@
         <v>13</v>
       </c>
       <c r="D11" s="8" t="s">
-        <v>401</v>
+        <v>399</v>
       </c>
       <c r="F11" s="6">
         <v>3</v>
       </c>
       <c r="G11" s="14" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
     </row>
     <row r="12" spans="1:7" ht="17.149999999999999" x14ac:dyDescent="0.55000000000000004">
@@ -2244,7 +2240,7 @@
         <v>95</v>
       </c>
       <c r="D12" s="8" t="s">
-        <v>369</v>
+        <v>367</v>
       </c>
       <c r="E12" s="9" t="s">
         <v>14</v>
@@ -2253,7 +2249,7 @@
         <v>2</v>
       </c>
       <c r="G12" s="14" t="s">
-        <v>371</v>
+        <v>369</v>
       </c>
     </row>
     <row r="13" spans="1:7" ht="17.149999999999999" x14ac:dyDescent="0.55000000000000004">
@@ -2287,7 +2283,7 @@
         <v>6</v>
       </c>
       <c r="D14" s="8" t="s">
-        <v>368</v>
+        <v>366</v>
       </c>
       <c r="F14" s="6">
         <v>2</v>
@@ -2324,27 +2320,27 @@
         <v>42</v>
       </c>
       <c r="D16" s="8" t="s">
-        <v>346</v>
+        <v>421</v>
       </c>
       <c r="E16" s="9" t="s">
         <v>14</v>
       </c>
       <c r="F16" s="6">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="17" spans="1:7" ht="17.149999999999999" x14ac:dyDescent="0.55000000000000004">
       <c r="A17" s="10" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="B17" s="6" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
       <c r="C17" s="7" t="s">
         <v>13</v>
       </c>
       <c r="D17" s="8" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="E17" s="9" t="s">
         <v>14</v>
@@ -2352,13 +2348,13 @@
     </row>
     <row r="18" spans="1:7" ht="17.149999999999999" x14ac:dyDescent="0.55000000000000004">
       <c r="A18" s="10" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="C18" s="7" t="s">
         <v>42</v>
       </c>
       <c r="D18" s="8" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
       <c r="E18" s="9" t="s">
         <v>14</v>
@@ -2369,13 +2365,13 @@
         <v>220</v>
       </c>
       <c r="B19" s="6" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
       <c r="C19" s="7" t="s">
         <v>13</v>
       </c>
       <c r="D19" s="8" t="s">
-        <v>405</v>
+        <v>403</v>
       </c>
       <c r="F19" s="6">
         <v>3</v>
@@ -2395,7 +2391,7 @@
         <v>80</v>
       </c>
       <c r="D20" s="8" t="s">
-        <v>383</v>
+        <v>381</v>
       </c>
       <c r="F20" s="6">
         <v>3</v>
@@ -2412,7 +2408,7 @@
         <v>95</v>
       </c>
       <c r="D21" s="8" t="s">
-        <v>409</v>
+        <v>407</v>
       </c>
       <c r="E21" s="9" t="s">
         <v>128</v>
@@ -2421,7 +2417,7 @@
         <v>3</v>
       </c>
       <c r="G21" s="14" t="s">
-        <v>411</v>
+        <v>409</v>
       </c>
     </row>
     <row r="22" spans="1:7" ht="17.149999999999999" x14ac:dyDescent="0.55000000000000004">
@@ -2435,7 +2431,7 @@
         <v>28</v>
       </c>
       <c r="D22" s="8" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
       <c r="F22" s="6">
         <v>2</v>
@@ -2452,7 +2448,7 @@
         <v>13</v>
       </c>
       <c r="D23" s="8" t="s">
-        <v>393</v>
+        <v>391</v>
       </c>
       <c r="E23" s="9" t="s">
         <v>87</v>
@@ -2492,7 +2488,7 @@
         <v>42</v>
       </c>
       <c r="D25" s="8" t="s">
-        <v>391</v>
+        <v>389</v>
       </c>
       <c r="F25" s="6">
         <v>3</v>
@@ -2506,7 +2502,7 @@
         <v>13</v>
       </c>
       <c r="D26" s="8" t="s">
-        <v>391</v>
+        <v>389</v>
       </c>
       <c r="E26" s="13" t="s">
         <v>344</v>
@@ -2515,24 +2511,24 @@
         <v>3</v>
       </c>
       <c r="G26" s="14" t="s">
-        <v>392</v>
+        <v>390</v>
       </c>
     </row>
     <row r="27" spans="1:7" ht="17.149999999999999" x14ac:dyDescent="0.55000000000000004">
       <c r="A27" s="10" t="s">
-        <v>378</v>
+        <v>376</v>
       </c>
       <c r="C27" s="7" t="s">
         <v>42</v>
       </c>
       <c r="D27" s="8" t="s">
-        <v>374</v>
+        <v>372</v>
       </c>
       <c r="E27" s="9" t="s">
-        <v>379</v>
+        <v>377</v>
       </c>
       <c r="G27" s="14" t="s">
-        <v>380</v>
+        <v>378</v>
       </c>
     </row>
     <row r="28" spans="1:7" ht="17.149999999999999" x14ac:dyDescent="0.55000000000000004">
@@ -2560,7 +2556,7 @@
         <v>95</v>
       </c>
       <c r="D29" s="8" t="s">
-        <v>397</v>
+        <v>395</v>
       </c>
       <c r="F29" s="6">
         <v>3</v>
@@ -2580,13 +2576,13 @@
         <v>80</v>
       </c>
       <c r="D30" s="8" t="s">
-        <v>393</v>
+        <v>391</v>
       </c>
       <c r="F30" s="6">
         <v>3</v>
       </c>
       <c r="G30" s="14" t="s">
-        <v>396</v>
+        <v>394</v>
       </c>
     </row>
     <row r="31" spans="1:7" ht="17.149999999999999" x14ac:dyDescent="0.55000000000000004">
@@ -2600,7 +2596,7 @@
         <v>13</v>
       </c>
       <c r="D31" s="8" t="s">
-        <v>385</v>
+        <v>383</v>
       </c>
       <c r="E31" s="9" t="s">
         <v>97</v>
@@ -2623,7 +2619,7 @@
         <v>6</v>
       </c>
       <c r="D32" s="8" t="s">
-        <v>368</v>
+        <v>366</v>
       </c>
       <c r="F32" s="6">
         <v>2</v>
@@ -2640,13 +2636,13 @@
         <v>13</v>
       </c>
       <c r="D33" s="8" t="s">
-        <v>418</v>
+        <v>416</v>
       </c>
       <c r="F33" s="6">
         <v>3</v>
       </c>
       <c r="G33" s="14" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
     </row>
     <row r="34" spans="1:7" ht="17.149999999999999" x14ac:dyDescent="0.55000000000000004">
@@ -2660,7 +2656,7 @@
         <v>13</v>
       </c>
       <c r="D34" s="8" t="s">
-        <v>420</v>
+        <v>418</v>
       </c>
       <c r="E34" s="9" t="s">
         <v>103</v>
@@ -2711,7 +2707,7 @@
         <v>6</v>
       </c>
       <c r="D37" s="8" t="s">
-        <v>391</v>
+        <v>389</v>
       </c>
       <c r="E37" s="13" t="s">
         <v>340</v>
@@ -2725,13 +2721,13 @@
     </row>
     <row r="38" spans="1:7" ht="17.149999999999999" x14ac:dyDescent="0.55000000000000004">
       <c r="A38" s="10" t="s">
-        <v>381</v>
+        <v>379</v>
       </c>
       <c r="C38" s="7" t="s">
         <v>42</v>
       </c>
       <c r="D38" s="8" t="s">
-        <v>382</v>
+        <v>380</v>
       </c>
     </row>
     <row r="39" spans="1:7" ht="17.149999999999999" x14ac:dyDescent="0.55000000000000004">
@@ -2745,7 +2741,7 @@
         <v>13</v>
       </c>
       <c r="D39" s="8" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
       <c r="F39" s="6">
         <v>2</v>
@@ -2762,7 +2758,7 @@
         <v>80</v>
       </c>
       <c r="D40" s="8" t="s">
-        <v>406</v>
+        <v>404</v>
       </c>
       <c r="E40" s="9" t="s">
         <v>22</v>
@@ -2779,7 +2775,7 @@
         <v>28</v>
       </c>
       <c r="D41" s="8" t="s">
-        <v>389</v>
+        <v>387</v>
       </c>
       <c r="F41" s="6">
         <v>3</v>
@@ -2793,13 +2789,13 @@
         <v>13</v>
       </c>
       <c r="D42" s="8" t="s">
-        <v>393</v>
+        <v>391</v>
       </c>
       <c r="F42" s="6">
         <v>3</v>
       </c>
       <c r="G42" s="14" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
     </row>
     <row r="43" spans="1:7" ht="17.149999999999999" x14ac:dyDescent="0.55000000000000004">
@@ -2830,13 +2826,13 @@
         <v>13</v>
       </c>
       <c r="D44" s="8" t="s">
-        <v>401</v>
+        <v>399</v>
       </c>
       <c r="F44" s="6">
         <v>3</v>
       </c>
       <c r="G44" s="14" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
     </row>
     <row r="45" spans="1:7" ht="17.149999999999999" x14ac:dyDescent="0.55000000000000004">
@@ -2847,7 +2843,7 @@
         <v>6</v>
       </c>
       <c r="D45" s="8" t="s">
-        <v>393</v>
+        <v>391</v>
       </c>
       <c r="F45" s="6">
         <v>3</v>
@@ -2864,7 +2860,7 @@
         <v>80</v>
       </c>
       <c r="D46" s="8" t="s">
-        <v>420</v>
+        <v>418</v>
       </c>
       <c r="F46" s="6">
         <v>3</v>
@@ -2878,7 +2874,7 @@
         <v>13</v>
       </c>
       <c r="D47" s="8" t="s">
-        <v>405</v>
+        <v>403</v>
       </c>
       <c r="F47" s="6">
         <v>3</v>
@@ -2895,7 +2891,7 @@
         <v>80</v>
       </c>
       <c r="D48" s="8" t="s">
-        <v>391</v>
+        <v>389</v>
       </c>
       <c r="F48" s="6">
         <v>3</v>
@@ -2909,7 +2905,7 @@
         <v>80</v>
       </c>
       <c r="D49" s="8" t="s">
-        <v>406</v>
+        <v>404</v>
       </c>
       <c r="F49" s="6">
         <v>3</v>
@@ -2923,7 +2919,7 @@
         <v>13</v>
       </c>
       <c r="D50" s="8" t="s">
-        <v>406</v>
+        <v>404</v>
       </c>
       <c r="F50" s="6">
         <v>3</v>
@@ -2957,7 +2953,7 @@
         <v>42</v>
       </c>
       <c r="D52" s="8" t="s">
-        <v>393</v>
+        <v>391</v>
       </c>
       <c r="F52" s="6">
         <v>3</v>
@@ -2994,7 +2990,7 @@
         <v>13</v>
       </c>
       <c r="D54" s="8" t="s">
-        <v>422</v>
+        <v>420</v>
       </c>
       <c r="F54" s="6">
         <v>4</v>
@@ -3051,10 +3047,10 @@
         <v>13</v>
       </c>
       <c r="D57" s="8" t="s">
-        <v>409</v>
+        <v>407</v>
       </c>
       <c r="E57" s="9" t="s">
-        <v>410</v>
+        <v>408</v>
       </c>
       <c r="F57" s="6">
         <v>3</v>
@@ -3068,13 +3064,13 @@
         <v>13</v>
       </c>
       <c r="D58" s="8" t="s">
-        <v>398</v>
+        <v>396</v>
       </c>
       <c r="F58" s="6">
         <v>3</v>
       </c>
       <c r="G58" s="14" t="s">
-        <v>399</v>
+        <v>397</v>
       </c>
     </row>
     <row r="59" spans="1:7" ht="17.149999999999999" x14ac:dyDescent="0.55000000000000004">
@@ -3088,7 +3084,7 @@
         <v>13</v>
       </c>
       <c r="D59" s="8" t="s">
-        <v>397</v>
+        <v>395</v>
       </c>
       <c r="F59" s="6">
         <v>3</v>
@@ -3102,13 +3098,13 @@
         <v>13</v>
       </c>
       <c r="D60" s="8" t="s">
-        <v>401</v>
+        <v>399</v>
       </c>
       <c r="F60" s="6">
         <v>3</v>
       </c>
       <c r="G60" s="14" t="s">
-        <v>402</v>
+        <v>400</v>
       </c>
     </row>
     <row r="61" spans="1:7" ht="17.149999999999999" x14ac:dyDescent="0.55000000000000004">
@@ -3119,7 +3115,7 @@
         <v>95</v>
       </c>
       <c r="D61" s="8" t="s">
-        <v>391</v>
+        <v>389</v>
       </c>
       <c r="F61" s="6">
         <v>3</v>
@@ -3130,13 +3126,13 @@
         <v>219</v>
       </c>
       <c r="B62" s="6" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
       <c r="C62" s="7" t="s">
         <v>80</v>
       </c>
       <c r="D62" s="8" t="s">
-        <v>404</v>
+        <v>402</v>
       </c>
       <c r="E62" s="9" t="s">
         <v>93</v>
@@ -3145,7 +3141,7 @@
         <v>3</v>
       </c>
       <c r="G62" s="14" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
     </row>
     <row r="63" spans="1:7" ht="17.149999999999999" x14ac:dyDescent="0.55000000000000004">
@@ -3159,7 +3155,7 @@
         <v>6</v>
       </c>
       <c r="D63" s="8" t="s">
-        <v>389</v>
+        <v>387</v>
       </c>
       <c r="F63" s="6">
         <v>3</v>
@@ -3176,7 +3172,7 @@
         <v>95</v>
       </c>
       <c r="D64" s="8" t="s">
-        <v>388</v>
+        <v>386</v>
       </c>
       <c r="E64" s="9" t="s">
         <v>118</v>
@@ -3207,19 +3203,19 @@
     </row>
     <row r="66" spans="1:7" ht="17.149999999999999" x14ac:dyDescent="0.55000000000000004">
       <c r="A66" s="10" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="C66" s="7" t="s">
         <v>95</v>
       </c>
       <c r="D66" s="8" t="s">
+        <v>391</v>
+      </c>
+      <c r="F66" s="6">
+        <v>3</v>
+      </c>
+      <c r="G66" s="14" t="s">
         <v>393</v>
-      </c>
-      <c r="F66" s="6">
-        <v>3</v>
-      </c>
-      <c r="G66" s="14" t="s">
-        <v>395</v>
       </c>
     </row>
     <row r="67" spans="1:7" ht="17.149999999999999" x14ac:dyDescent="0.55000000000000004">
@@ -3233,7 +3229,7 @@
         <v>42</v>
       </c>
       <c r="D67" s="8" t="s">
-        <v>390</v>
+        <v>388</v>
       </c>
       <c r="E67" s="9" t="s">
         <v>93</v>
@@ -3276,13 +3272,13 @@
         <v>95</v>
       </c>
       <c r="D69" s="8" t="s">
-        <v>393</v>
+        <v>391</v>
       </c>
       <c r="F69" s="6">
         <v>4</v>
       </c>
       <c r="G69" s="14" t="s">
-        <v>394</v>
+        <v>392</v>
       </c>
     </row>
     <row r="70" spans="1:7" ht="17.149999999999999" x14ac:dyDescent="0.55000000000000004">
@@ -3443,16 +3439,16 @@
     </row>
     <row r="79" spans="1:7" ht="17.149999999999999" x14ac:dyDescent="0.55000000000000004">
       <c r="A79" s="10" t="s">
-        <v>376</v>
+        <v>374</v>
       </c>
       <c r="C79" s="7" t="s">
         <v>13</v>
       </c>
       <c r="D79" s="8" t="s">
-        <v>374</v>
+        <v>372</v>
       </c>
       <c r="G79" s="14" t="s">
-        <v>375</v>
+        <v>373</v>
       </c>
     </row>
     <row r="80" spans="1:7" ht="17.149999999999999" x14ac:dyDescent="0.55000000000000004">
@@ -3514,7 +3510,7 @@
         <v>80</v>
       </c>
       <c r="D83" s="8" t="s">
-        <v>384</v>
+        <v>382</v>
       </c>
       <c r="E83" s="9" t="s">
         <v>87</v>
@@ -3590,7 +3586,7 @@
         <v>13</v>
       </c>
       <c r="D88" s="8" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
       <c r="E88" s="9" t="s">
         <v>274</v>
@@ -3610,7 +3606,7 @@
         <v>80</v>
       </c>
       <c r="D89" s="8" t="s">
-        <v>422</v>
+        <v>420</v>
       </c>
       <c r="E89" s="9" t="s">
         <v>8</v>
@@ -3633,7 +3629,7 @@
         <v>80</v>
       </c>
       <c r="D90" s="8" t="s">
-        <v>386</v>
+        <v>384</v>
       </c>
       <c r="E90" s="9" t="s">
         <v>109</v>
@@ -3656,7 +3652,7 @@
         <v>80</v>
       </c>
       <c r="D91" s="8" t="s">
-        <v>368</v>
+        <v>366</v>
       </c>
       <c r="F91" s="6">
         <v>2</v>
@@ -3676,7 +3672,7 @@
         <v>42</v>
       </c>
       <c r="D92" s="8" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
       <c r="E92" s="9" t="s">
         <v>270</v>
@@ -3707,7 +3703,7 @@
         <v>13</v>
       </c>
       <c r="D94" s="8" t="s">
-        <v>368</v>
+        <v>366</v>
       </c>
       <c r="F94" s="6">
         <v>2</v>
@@ -3741,7 +3737,7 @@
         <v>95</v>
       </c>
       <c r="D96" s="8" t="s">
-        <v>415</v>
+        <v>413</v>
       </c>
       <c r="E96" s="12" t="s">
         <v>241</v>
@@ -3750,7 +3746,7 @@
         <v>3</v>
       </c>
       <c r="G96" s="14" t="s">
-        <v>417</v>
+        <v>415</v>
       </c>
     </row>
     <row r="97" spans="1:7" ht="17.149999999999999" x14ac:dyDescent="0.55000000000000004">
@@ -3781,7 +3777,7 @@
         <v>80</v>
       </c>
       <c r="D98" s="8" t="s">
-        <v>415</v>
+        <v>413</v>
       </c>
       <c r="E98" s="9" t="s">
         <v>22</v>
@@ -3801,7 +3797,7 @@
         <v>80</v>
       </c>
       <c r="D99" s="8" t="s">
-        <v>422</v>
+        <v>420</v>
       </c>
       <c r="F99" s="6">
         <v>3</v>
@@ -3818,13 +3814,13 @@
         <v>42</v>
       </c>
       <c r="D100" s="8" t="s">
-        <v>413</v>
+        <v>411</v>
       </c>
       <c r="F100" s="6">
         <v>3</v>
       </c>
       <c r="G100" s="14" t="s">
-        <v>414</v>
+        <v>412</v>
       </c>
     </row>
     <row r="101" spans="1:7" ht="17.149999999999999" x14ac:dyDescent="0.55000000000000004">
@@ -3889,13 +3885,13 @@
         <v>95</v>
       </c>
       <c r="D104" s="8" t="s">
+        <v>404</v>
+      </c>
+      <c r="F104" s="6">
+        <v>3</v>
+      </c>
+      <c r="G104" s="14" t="s">
         <v>406</v>
-      </c>
-      <c r="F104" s="6">
-        <v>3</v>
-      </c>
-      <c r="G104" s="14" t="s">
-        <v>408</v>
       </c>
     </row>
     <row r="105" spans="1:7" ht="17.149999999999999" x14ac:dyDescent="0.55000000000000004">
@@ -3909,7 +3905,7 @@
         <v>95</v>
       </c>
       <c r="D105" s="8" t="s">
-        <v>420</v>
+        <v>418</v>
       </c>
       <c r="E105" s="9" t="s">
         <v>93</v>
@@ -3929,7 +3925,7 @@
         <v>80</v>
       </c>
       <c r="D106" s="8" t="s">
-        <v>418</v>
+        <v>416</v>
       </c>
       <c r="E106" s="9" t="s">
         <v>98</v>
@@ -3938,7 +3934,7 @@
         <v>2</v>
       </c>
       <c r="G106" s="14" t="s">
-        <v>419</v>
+        <v>417</v>
       </c>
     </row>
     <row r="107" spans="1:7" ht="17.149999999999999" x14ac:dyDescent="0.55000000000000004">
@@ -3952,7 +3948,7 @@
         <v>13</v>
       </c>
       <c r="D107" s="8" t="s">
-        <v>389</v>
+        <v>387</v>
       </c>
       <c r="F107" s="6">
         <v>3</v>
@@ -3995,7 +3991,7 @@
         <v>80</v>
       </c>
       <c r="D109" s="8" t="s">
-        <v>386</v>
+        <v>384</v>
       </c>
       <c r="E109" s="9" t="s">
         <v>98</v>
@@ -4012,19 +4008,19 @@
         <v>218</v>
       </c>
       <c r="B110" s="6" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="C110" s="7" t="s">
         <v>80</v>
       </c>
       <c r="D110" s="8" t="s">
-        <v>404</v>
+        <v>402</v>
       </c>
       <c r="F110" s="6">
         <v>3</v>
       </c>
       <c r="G110" s="14" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
     </row>
     <row r="111" spans="1:7" ht="17.149999999999999" x14ac:dyDescent="0.55000000000000004">
@@ -4038,7 +4034,7 @@
         <v>95</v>
       </c>
       <c r="D111" s="8" t="s">
-        <v>386</v>
+        <v>384</v>
       </c>
       <c r="E111" s="9" t="s">
         <v>110</v>
@@ -4081,10 +4077,10 @@
         <v>13</v>
       </c>
       <c r="D113" s="8" t="s">
-        <v>366</v>
+        <v>421</v>
       </c>
       <c r="F113" s="6">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="114" spans="1:7" ht="17.149999999999999" x14ac:dyDescent="0.55000000000000004">
@@ -4098,7 +4094,7 @@
         <v>13</v>
       </c>
       <c r="D114" s="8" t="s">
-        <v>406</v>
+        <v>404</v>
       </c>
       <c r="E114" s="9" t="s">
         <v>128</v>
@@ -4158,7 +4154,7 @@
         <v>6</v>
       </c>
       <c r="D117" s="8" t="s">
-        <v>390</v>
+        <v>388</v>
       </c>
       <c r="E117" s="9" t="s">
         <v>93</v>
@@ -4178,7 +4174,7 @@
         <v>80</v>
       </c>
       <c r="D118" s="8" t="s">
-        <v>383</v>
+        <v>381</v>
       </c>
       <c r="F118" s="6">
         <v>4</v>
@@ -4215,7 +4211,7 @@
         <v>95</v>
       </c>
       <c r="D120" s="8" t="s">
-        <v>383</v>
+        <v>381</v>
       </c>
       <c r="E120" s="9" t="s">
         <v>22</v>
@@ -4224,7 +4220,7 @@
         <v>3</v>
       </c>
       <c r="G120" s="14" t="s">
-        <v>370</v>
+        <v>368</v>
       </c>
     </row>
     <row r="121" spans="1:7" ht="17.149999999999999" x14ac:dyDescent="0.55000000000000004">
@@ -4238,7 +4234,7 @@
         <v>80</v>
       </c>
       <c r="D121" s="8" t="s">
-        <v>409</v>
+        <v>407</v>
       </c>
       <c r="E121" s="9" t="s">
         <v>14</v>
@@ -4247,7 +4243,7 @@
         <v>3</v>
       </c>
       <c r="G121" s="14" t="s">
-        <v>412</v>
+        <v>410</v>
       </c>
     </row>
     <row r="122" spans="1:7" ht="17.149999999999999" x14ac:dyDescent="0.55000000000000004">
@@ -4292,7 +4288,7 @@
         <v>42</v>
       </c>
       <c r="D124" s="8" t="s">
-        <v>389</v>
+        <v>387</v>
       </c>
       <c r="E124" s="9" t="s">
         <v>128</v>
@@ -4312,7 +4308,7 @@
         <v>42</v>
       </c>
       <c r="D125" s="8" t="s">
-        <v>390</v>
+        <v>388</v>
       </c>
       <c r="E125" s="10" t="s">
         <v>185</v>
@@ -4332,13 +4328,13 @@
         <v>13</v>
       </c>
       <c r="D126" s="8" t="s">
+        <v>396</v>
+      </c>
+      <c r="F126" s="6">
+        <v>3</v>
+      </c>
+      <c r="G126" s="14" t="s">
         <v>398</v>
-      </c>
-      <c r="F126" s="6">
-        <v>3</v>
-      </c>
-      <c r="G126" s="14" t="s">
-        <v>400</v>
       </c>
     </row>
     <row r="127" spans="1:7" ht="17.149999999999999" x14ac:dyDescent="0.55000000000000004">
@@ -4352,10 +4348,10 @@
         <v>42</v>
       </c>
       <c r="D127" s="8" t="s">
-        <v>366</v>
+        <v>421</v>
       </c>
       <c r="F127" s="6">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="128" spans="1:7" ht="17.149999999999999" x14ac:dyDescent="0.55000000000000004">
@@ -4369,7 +4365,7 @@
         <v>80</v>
       </c>
       <c r="D128" s="8" t="s">
-        <v>389</v>
+        <v>387</v>
       </c>
       <c r="E128" s="9" t="s">
         <v>131</v>
@@ -4389,7 +4385,7 @@
         <v>95</v>
       </c>
       <c r="D129" s="8" t="s">
-        <v>387</v>
+        <v>385</v>
       </c>
       <c r="E129" s="9" t="s">
         <v>118</v>
@@ -4409,7 +4405,7 @@
         <v>13</v>
       </c>
       <c r="D130" s="8" t="s">
-        <v>369</v>
+        <v>367</v>
       </c>
       <c r="E130" s="9" t="s">
         <v>14</v>
@@ -4420,13 +4416,13 @@
     </row>
     <row r="131" spans="1:7" ht="17.149999999999999" x14ac:dyDescent="0.55000000000000004">
       <c r="A131" s="10" t="s">
-        <v>373</v>
+        <v>371</v>
       </c>
       <c r="C131" s="7" t="s">
         <v>42</v>
       </c>
       <c r="D131" s="8" t="s">
-        <v>374</v>
+        <v>372</v>
       </c>
     </row>
     <row r="132" spans="1:7" ht="17.149999999999999" x14ac:dyDescent="0.55000000000000004">
@@ -4440,7 +4436,7 @@
         <v>13</v>
       </c>
       <c r="D132" s="8" t="s">
-        <v>369</v>
+        <v>367</v>
       </c>
       <c r="F132" s="6">
         <v>2</v>
@@ -4522,7 +4518,7 @@
         <v>80</v>
       </c>
       <c r="D137" s="8" t="s">
-        <v>369</v>
+        <v>367</v>
       </c>
       <c r="E137" s="9" t="s">
         <v>14</v>
@@ -4531,7 +4527,7 @@
         <v>2</v>
       </c>
       <c r="G137" s="14" t="s">
-        <v>372</v>
+        <v>370</v>
       </c>
     </row>
     <row r="138" spans="1:7" ht="17.149999999999999" x14ac:dyDescent="0.55000000000000004">
@@ -4545,7 +4541,7 @@
         <v>42</v>
       </c>
       <c r="D138" s="8" t="s">
-        <v>390</v>
+        <v>388</v>
       </c>
       <c r="E138" s="9" t="s">
         <v>183</v>
@@ -4585,7 +4581,7 @@
         <v>80</v>
       </c>
       <c r="D140" s="8" t="s">
-        <v>420</v>
+        <v>418</v>
       </c>
       <c r="E140" s="9" t="s">
         <v>250</v>
@@ -4594,7 +4590,7 @@
         <v>2</v>
       </c>
       <c r="G140" s="14" t="s">
-        <v>421</v>
+        <v>419</v>
       </c>
     </row>
     <row r="141" spans="1:7" ht="17.149999999999999" x14ac:dyDescent="0.55000000000000004">
@@ -4608,13 +4604,13 @@
         <v>42</v>
       </c>
       <c r="D141" s="8" t="s">
-        <v>415</v>
+        <v>413</v>
       </c>
       <c r="F141" s="6">
         <v>3</v>
       </c>
       <c r="G141" s="14" t="s">
-        <v>416</v>
+        <v>414</v>
       </c>
     </row>
     <row r="142" spans="1:7" ht="17.149999999999999" x14ac:dyDescent="0.55000000000000004">
@@ -4628,7 +4624,7 @@
         <v>6</v>
       </c>
       <c r="D142" s="8" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
       <c r="F142" s="6">
         <v>2</v>
@@ -4645,7 +4641,7 @@
         <v>95</v>
       </c>
       <c r="D143" s="8" t="s">
-        <v>388</v>
+        <v>386</v>
       </c>
       <c r="E143" s="9" t="s">
         <v>122</v>
@@ -4665,10 +4661,13 @@
         <v>13</v>
       </c>
       <c r="D144" s="8" t="s">
-        <v>367</v>
+        <v>421</v>
       </c>
       <c r="E144" s="9" t="s">
         <v>22</v>
+      </c>
+      <c r="F144" s="6">
+        <v>3</v>
       </c>
     </row>
     <row r="145" spans="1:7" ht="17.149999999999999" x14ac:dyDescent="0.55000000000000004">
@@ -4679,7 +4678,7 @@
         <v>13</v>
       </c>
       <c r="D145" s="8" t="s">
-        <v>406</v>
+        <v>404</v>
       </c>
       <c r="E145" s="9" t="s">
         <v>47</v>
@@ -4688,7 +4687,7 @@
         <v>4</v>
       </c>
       <c r="G145" s="14" t="s">
-        <v>407</v>
+        <v>405</v>
       </c>
     </row>
     <row r="146" spans="1:7" ht="17.149999999999999" x14ac:dyDescent="0.55000000000000004">
@@ -4702,7 +4701,7 @@
         <v>13</v>
       </c>
       <c r="D146" s="8" t="s">
-        <v>409</v>
+        <v>407</v>
       </c>
       <c r="E146" s="9" t="s">
         <v>93</v>
@@ -4756,7 +4755,7 @@
         <v>95</v>
       </c>
       <c r="D149" s="8" t="s">
-        <v>420</v>
+        <v>418</v>
       </c>
       <c r="E149" s="9" t="s">
         <v>128</v>
@@ -4765,7 +4764,7 @@
         <v>3</v>
       </c>
       <c r="G149" s="14" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
     </row>
     <row r="150" spans="1:7" ht="17.149999999999999" x14ac:dyDescent="0.55000000000000004">
@@ -4776,7 +4775,7 @@
         <v>13</v>
       </c>
       <c r="D150" s="8" t="s">
-        <v>398</v>
+        <v>396</v>
       </c>
       <c r="F150" s="6">
         <v>3</v>
@@ -4801,7 +4800,7 @@
         <v>13</v>
       </c>
       <c r="D152" s="8" t="s">
-        <v>401</v>
+        <v>399</v>
       </c>
       <c r="F152" s="6">
         <v>3</v>
@@ -4812,19 +4811,19 @@
         <v>223</v>
       </c>
       <c r="B153" s="6" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
       <c r="C153" s="7" t="s">
         <v>95</v>
       </c>
       <c r="D153" s="8" t="s">
-        <v>405</v>
+        <v>403</v>
       </c>
       <c r="F153" s="6">
         <v>3</v>
       </c>
       <c r="G153" s="14" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
2024.12.21 LeetCodeHot100 四刷 技巧Done
</commit_message>
<xml_diff>
--- a/2024LeetCode刷题记录.xlsx
+++ b/2024LeetCode刷题记录.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\develop\GithubRepo\LeetCode\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E1E8A4B8-2D52-4B9E-9B8A-DD2EFC67FFD0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D9EC2CB5-A5CB-442D-8B6C-2CF75BE520D7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-103" yWindow="-103" windowWidth="22149" windowHeight="11829" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="727" uniqueCount="422">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="729" uniqueCount="423">
   <si>
     <t>题目</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -1339,10 +1339,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>2024.11.02</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>2024.11.05</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -1559,6 +1555,14 @@
   </si>
   <si>
     <t>2024.12.20</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>2024.12.21</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>zero two</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -2017,8 +2021,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G153"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A132" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="F144" sqref="F144"/>
+    <sheetView tabSelected="1" topLeftCell="A74" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="G88" sqref="G88"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="14.15" x14ac:dyDescent="0.35"/>
@@ -2067,7 +2071,7 @@
         <v>80</v>
       </c>
       <c r="D2" s="8" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
       <c r="F2" s="6">
         <v>3</v>
@@ -2084,13 +2088,13 @@
         <v>42</v>
       </c>
       <c r="D3" s="8" t="s">
+        <v>395</v>
+      </c>
+      <c r="F3" s="6">
+        <v>3</v>
+      </c>
+      <c r="G3" s="14" t="s">
         <v>396</v>
-      </c>
-      <c r="F3" s="6">
-        <v>3</v>
-      </c>
-      <c r="G3" s="14" t="s">
-        <v>397</v>
       </c>
     </row>
     <row r="4" spans="1:7" ht="17.149999999999999" x14ac:dyDescent="0.55000000000000004">
@@ -2101,7 +2105,7 @@
         <v>13</v>
       </c>
       <c r="D4" s="8" t="s">
-        <v>399</v>
+        <v>398</v>
       </c>
       <c r="F4" s="6">
         <v>3</v>
@@ -2118,13 +2122,13 @@
         <v>42</v>
       </c>
       <c r="D5" s="8" t="s">
+        <v>395</v>
+      </c>
+      <c r="F5" s="6">
+        <v>3</v>
+      </c>
+      <c r="G5" s="14" t="s">
         <v>396</v>
-      </c>
-      <c r="F5" s="6">
-        <v>3</v>
-      </c>
-      <c r="G5" s="14" t="s">
-        <v>397</v>
       </c>
     </row>
     <row r="6" spans="1:7" ht="17.149999999999999" x14ac:dyDescent="0.55000000000000004">
@@ -2158,7 +2162,7 @@
         <v>80</v>
       </c>
       <c r="D7" s="8" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
       <c r="F7" s="6">
         <v>3</v>
@@ -2166,13 +2170,13 @@
     </row>
     <row r="8" spans="1:7" ht="17.149999999999999" x14ac:dyDescent="0.55000000000000004">
       <c r="A8" s="10" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
       <c r="C8" s="7" t="s">
         <v>13</v>
       </c>
       <c r="D8" s="8" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
     </row>
     <row r="9" spans="1:7" ht="17.149999999999999" x14ac:dyDescent="0.55000000000000004">
@@ -2183,7 +2187,7 @@
         <v>13</v>
       </c>
       <c r="D9" s="8" t="s">
-        <v>399</v>
+        <v>398</v>
       </c>
       <c r="F9" s="6">
         <v>3</v>
@@ -2200,7 +2204,7 @@
         <v>42</v>
       </c>
       <c r="D10" s="8" t="s">
-        <v>383</v>
+        <v>382</v>
       </c>
       <c r="E10" s="9" t="s">
         <v>93</v>
@@ -2220,7 +2224,7 @@
         <v>13</v>
       </c>
       <c r="D11" s="8" t="s">
-        <v>399</v>
+        <v>398</v>
       </c>
       <c r="F11" s="6">
         <v>3</v>
@@ -2240,7 +2244,7 @@
         <v>95</v>
       </c>
       <c r="D12" s="8" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
       <c r="E12" s="9" t="s">
         <v>14</v>
@@ -2249,7 +2253,7 @@
         <v>2</v>
       </c>
       <c r="G12" s="14" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
     </row>
     <row r="13" spans="1:7" ht="17.149999999999999" x14ac:dyDescent="0.55000000000000004">
@@ -2283,7 +2287,7 @@
         <v>6</v>
       </c>
       <c r="D14" s="8" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
       <c r="F14" s="6">
         <v>2</v>
@@ -2320,7 +2324,7 @@
         <v>42</v>
       </c>
       <c r="D16" s="8" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
       <c r="E16" s="9" t="s">
         <v>14</v>
@@ -2371,7 +2375,7 @@
         <v>13</v>
       </c>
       <c r="D19" s="8" t="s">
-        <v>403</v>
+        <v>402</v>
       </c>
       <c r="F19" s="6">
         <v>3</v>
@@ -2391,7 +2395,7 @@
         <v>80</v>
       </c>
       <c r="D20" s="8" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
       <c r="F20" s="6">
         <v>3</v>
@@ -2408,7 +2412,7 @@
         <v>95</v>
       </c>
       <c r="D21" s="8" t="s">
-        <v>407</v>
+        <v>406</v>
       </c>
       <c r="E21" s="9" t="s">
         <v>128</v>
@@ -2417,7 +2421,7 @@
         <v>3</v>
       </c>
       <c r="G21" s="14" t="s">
-        <v>409</v>
+        <v>408</v>
       </c>
     </row>
     <row r="22" spans="1:7" ht="17.149999999999999" x14ac:dyDescent="0.55000000000000004">
@@ -2431,10 +2435,10 @@
         <v>28</v>
       </c>
       <c r="D22" s="8" t="s">
-        <v>365</v>
+        <v>421</v>
       </c>
       <c r="F22" s="6">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="23" spans="1:7" ht="17.149999999999999" x14ac:dyDescent="0.55000000000000004">
@@ -2448,7 +2452,7 @@
         <v>13</v>
       </c>
       <c r="D23" s="8" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
       <c r="E23" s="9" t="s">
         <v>87</v>
@@ -2488,7 +2492,7 @@
         <v>42</v>
       </c>
       <c r="D25" s="8" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
       <c r="F25" s="6">
         <v>3</v>
@@ -2502,7 +2506,7 @@
         <v>13</v>
       </c>
       <c r="D26" s="8" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
       <c r="E26" s="13" t="s">
         <v>344</v>
@@ -2511,24 +2515,24 @@
         <v>3</v>
       </c>
       <c r="G26" s="14" t="s">
-        <v>390</v>
+        <v>389</v>
       </c>
     </row>
     <row r="27" spans="1:7" ht="17.149999999999999" x14ac:dyDescent="0.55000000000000004">
       <c r="A27" s="10" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
       <c r="C27" s="7" t="s">
         <v>42</v>
       </c>
       <c r="D27" s="8" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
       <c r="E27" s="9" t="s">
+        <v>376</v>
+      </c>
+      <c r="G27" s="14" t="s">
         <v>377</v>
-      </c>
-      <c r="G27" s="14" t="s">
-        <v>378</v>
       </c>
     </row>
     <row r="28" spans="1:7" ht="17.149999999999999" x14ac:dyDescent="0.55000000000000004">
@@ -2556,7 +2560,7 @@
         <v>95</v>
       </c>
       <c r="D29" s="8" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
       <c r="F29" s="6">
         <v>3</v>
@@ -2576,13 +2580,13 @@
         <v>80</v>
       </c>
       <c r="D30" s="8" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
       <c r="F30" s="6">
         <v>3</v>
       </c>
       <c r="G30" s="14" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
     </row>
     <row r="31" spans="1:7" ht="17.149999999999999" x14ac:dyDescent="0.55000000000000004">
@@ -2596,7 +2600,7 @@
         <v>13</v>
       </c>
       <c r="D31" s="8" t="s">
-        <v>383</v>
+        <v>382</v>
       </c>
       <c r="E31" s="9" t="s">
         <v>97</v>
@@ -2619,7 +2623,7 @@
         <v>6</v>
       </c>
       <c r="D32" s="8" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
       <c r="F32" s="6">
         <v>2</v>
@@ -2636,7 +2640,7 @@
         <v>13</v>
       </c>
       <c r="D33" s="8" t="s">
-        <v>416</v>
+        <v>415</v>
       </c>
       <c r="F33" s="6">
         <v>3</v>
@@ -2656,7 +2660,7 @@
         <v>13</v>
       </c>
       <c r="D34" s="8" t="s">
-        <v>418</v>
+        <v>417</v>
       </c>
       <c r="E34" s="9" t="s">
         <v>103</v>
@@ -2707,7 +2711,7 @@
         <v>6</v>
       </c>
       <c r="D37" s="8" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
       <c r="E37" s="13" t="s">
         <v>340</v>
@@ -2721,13 +2725,13 @@
     </row>
     <row r="38" spans="1:7" ht="17.149999999999999" x14ac:dyDescent="0.55000000000000004">
       <c r="A38" s="10" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
       <c r="C38" s="7" t="s">
         <v>42</v>
       </c>
       <c r="D38" s="8" t="s">
-        <v>380</v>
+        <v>379</v>
       </c>
     </row>
     <row r="39" spans="1:7" ht="17.149999999999999" x14ac:dyDescent="0.55000000000000004">
@@ -2741,10 +2745,10 @@
         <v>13</v>
       </c>
       <c r="D39" s="8" t="s">
-        <v>365</v>
+        <v>421</v>
       </c>
       <c r="F39" s="6">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="40" spans="1:7" ht="17.149999999999999" x14ac:dyDescent="0.55000000000000004">
@@ -2758,7 +2762,7 @@
         <v>80</v>
       </c>
       <c r="D40" s="8" t="s">
-        <v>404</v>
+        <v>403</v>
       </c>
       <c r="E40" s="9" t="s">
         <v>22</v>
@@ -2775,7 +2779,7 @@
         <v>28</v>
       </c>
       <c r="D41" s="8" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
       <c r="F41" s="6">
         <v>3</v>
@@ -2789,7 +2793,7 @@
         <v>13</v>
       </c>
       <c r="D42" s="8" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
       <c r="F42" s="6">
         <v>3</v>
@@ -2826,7 +2830,7 @@
         <v>13</v>
       </c>
       <c r="D44" s="8" t="s">
-        <v>399</v>
+        <v>398</v>
       </c>
       <c r="F44" s="6">
         <v>3</v>
@@ -2843,7 +2847,7 @@
         <v>6</v>
       </c>
       <c r="D45" s="8" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
       <c r="F45" s="6">
         <v>3</v>
@@ -2860,7 +2864,7 @@
         <v>80</v>
       </c>
       <c r="D46" s="8" t="s">
-        <v>418</v>
+        <v>417</v>
       </c>
       <c r="F46" s="6">
         <v>3</v>
@@ -2874,7 +2878,7 @@
         <v>13</v>
       </c>
       <c r="D47" s="8" t="s">
-        <v>403</v>
+        <v>402</v>
       </c>
       <c r="F47" s="6">
         <v>3</v>
@@ -2891,7 +2895,7 @@
         <v>80</v>
       </c>
       <c r="D48" s="8" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
       <c r="F48" s="6">
         <v>3</v>
@@ -2905,7 +2909,7 @@
         <v>80</v>
       </c>
       <c r="D49" s="8" t="s">
-        <v>404</v>
+        <v>403</v>
       </c>
       <c r="F49" s="6">
         <v>3</v>
@@ -2919,7 +2923,7 @@
         <v>13</v>
       </c>
       <c r="D50" s="8" t="s">
-        <v>404</v>
+        <v>403</v>
       </c>
       <c r="F50" s="6">
         <v>3</v>
@@ -2953,7 +2957,7 @@
         <v>42</v>
       </c>
       <c r="D52" s="8" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
       <c r="F52" s="6">
         <v>3</v>
@@ -2990,7 +2994,7 @@
         <v>13</v>
       </c>
       <c r="D54" s="8" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
       <c r="F54" s="6">
         <v>4</v>
@@ -3047,10 +3051,10 @@
         <v>13</v>
       </c>
       <c r="D57" s="8" t="s">
+        <v>406</v>
+      </c>
+      <c r="E57" s="9" t="s">
         <v>407</v>
-      </c>
-      <c r="E57" s="9" t="s">
-        <v>408</v>
       </c>
       <c r="F57" s="6">
         <v>3</v>
@@ -3064,13 +3068,13 @@
         <v>13</v>
       </c>
       <c r="D58" s="8" t="s">
+        <v>395</v>
+      </c>
+      <c r="F58" s="6">
+        <v>3</v>
+      </c>
+      <c r="G58" s="14" t="s">
         <v>396</v>
-      </c>
-      <c r="F58" s="6">
-        <v>3</v>
-      </c>
-      <c r="G58" s="14" t="s">
-        <v>397</v>
       </c>
     </row>
     <row r="59" spans="1:7" ht="17.149999999999999" x14ac:dyDescent="0.55000000000000004">
@@ -3084,7 +3088,7 @@
         <v>13</v>
       </c>
       <c r="D59" s="8" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
       <c r="F59" s="6">
         <v>3</v>
@@ -3098,13 +3102,13 @@
         <v>13</v>
       </c>
       <c r="D60" s="8" t="s">
+        <v>398</v>
+      </c>
+      <c r="F60" s="6">
+        <v>3</v>
+      </c>
+      <c r="G60" s="14" t="s">
         <v>399</v>
-      </c>
-      <c r="F60" s="6">
-        <v>3</v>
-      </c>
-      <c r="G60" s="14" t="s">
-        <v>400</v>
       </c>
     </row>
     <row r="61" spans="1:7" ht="17.149999999999999" x14ac:dyDescent="0.55000000000000004">
@@ -3115,7 +3119,7 @@
         <v>95</v>
       </c>
       <c r="D61" s="8" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
       <c r="F61" s="6">
         <v>3</v>
@@ -3132,7 +3136,7 @@
         <v>80</v>
       </c>
       <c r="D62" s="8" t="s">
-        <v>402</v>
+        <v>401</v>
       </c>
       <c r="E62" s="9" t="s">
         <v>93</v>
@@ -3155,7 +3159,7 @@
         <v>6</v>
       </c>
       <c r="D63" s="8" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
       <c r="F63" s="6">
         <v>3</v>
@@ -3172,7 +3176,7 @@
         <v>95</v>
       </c>
       <c r="D64" s="8" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
       <c r="E64" s="9" t="s">
         <v>118</v>
@@ -3209,13 +3213,13 @@
         <v>95</v>
       </c>
       <c r="D66" s="8" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
       <c r="F66" s="6">
         <v>3</v>
       </c>
       <c r="G66" s="14" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
     </row>
     <row r="67" spans="1:7" ht="17.149999999999999" x14ac:dyDescent="0.55000000000000004">
@@ -3229,7 +3233,7 @@
         <v>42</v>
       </c>
       <c r="D67" s="8" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
       <c r="E67" s="9" t="s">
         <v>93</v>
@@ -3272,13 +3276,13 @@
         <v>95</v>
       </c>
       <c r="D69" s="8" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
       <c r="F69" s="6">
         <v>4</v>
       </c>
       <c r="G69" s="14" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
     </row>
     <row r="70" spans="1:7" ht="17.149999999999999" x14ac:dyDescent="0.55000000000000004">
@@ -3439,16 +3443,16 @@
     </row>
     <row r="79" spans="1:7" ht="17.149999999999999" x14ac:dyDescent="0.55000000000000004">
       <c r="A79" s="10" t="s">
-        <v>374</v>
+        <v>373</v>
       </c>
       <c r="C79" s="7" t="s">
         <v>13</v>
       </c>
       <c r="D79" s="8" t="s">
+        <v>371</v>
+      </c>
+      <c r="G79" s="14" t="s">
         <v>372</v>
-      </c>
-      <c r="G79" s="14" t="s">
-        <v>373</v>
       </c>
     </row>
     <row r="80" spans="1:7" ht="17.149999999999999" x14ac:dyDescent="0.55000000000000004">
@@ -3510,7 +3514,7 @@
         <v>80</v>
       </c>
       <c r="D83" s="8" t="s">
-        <v>382</v>
+        <v>381</v>
       </c>
       <c r="E83" s="9" t="s">
         <v>87</v>
@@ -3586,13 +3590,16 @@
         <v>13</v>
       </c>
       <c r="D88" s="8" t="s">
-        <v>365</v>
+        <v>421</v>
       </c>
       <c r="E88" s="9" t="s">
         <v>274</v>
       </c>
       <c r="F88" s="6">
-        <v>2</v>
+        <v>3</v>
+      </c>
+      <c r="G88" s="6" t="s">
+        <v>273</v>
       </c>
     </row>
     <row r="89" spans="1:7" ht="17.149999999999999" x14ac:dyDescent="0.55000000000000004">
@@ -3606,7 +3613,7 @@
         <v>80</v>
       </c>
       <c r="D89" s="8" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
       <c r="E89" s="9" t="s">
         <v>8</v>
@@ -3629,7 +3636,7 @@
         <v>80</v>
       </c>
       <c r="D90" s="8" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
       <c r="E90" s="9" t="s">
         <v>109</v>
@@ -3652,7 +3659,7 @@
         <v>80</v>
       </c>
       <c r="D91" s="8" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
       <c r="F91" s="6">
         <v>2</v>
@@ -3672,13 +3679,13 @@
         <v>42</v>
       </c>
       <c r="D92" s="8" t="s">
-        <v>365</v>
+        <v>421</v>
       </c>
       <c r="E92" s="9" t="s">
         <v>270</v>
       </c>
       <c r="F92" s="6">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="93" spans="1:7" ht="17.149999999999999" x14ac:dyDescent="0.55000000000000004">
@@ -3703,7 +3710,7 @@
         <v>13</v>
       </c>
       <c r="D94" s="8" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
       <c r="F94" s="6">
         <v>2</v>
@@ -3737,7 +3744,7 @@
         <v>95</v>
       </c>
       <c r="D96" s="8" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
       <c r="E96" s="12" t="s">
         <v>241</v>
@@ -3746,7 +3753,7 @@
         <v>3</v>
       </c>
       <c r="G96" s="14" t="s">
-        <v>415</v>
+        <v>414</v>
       </c>
     </row>
     <row r="97" spans="1:7" ht="17.149999999999999" x14ac:dyDescent="0.55000000000000004">
@@ -3777,7 +3784,7 @@
         <v>80</v>
       </c>
       <c r="D98" s="8" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
       <c r="E98" s="9" t="s">
         <v>22</v>
@@ -3797,7 +3804,7 @@
         <v>80</v>
       </c>
       <c r="D99" s="8" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
       <c r="F99" s="6">
         <v>3</v>
@@ -3814,13 +3821,13 @@
         <v>42</v>
       </c>
       <c r="D100" s="8" t="s">
+        <v>410</v>
+      </c>
+      <c r="F100" s="6">
+        <v>3</v>
+      </c>
+      <c r="G100" s="14" t="s">
         <v>411</v>
-      </c>
-      <c r="F100" s="6">
-        <v>3</v>
-      </c>
-      <c r="G100" s="14" t="s">
-        <v>412</v>
       </c>
     </row>
     <row r="101" spans="1:7" ht="17.149999999999999" x14ac:dyDescent="0.55000000000000004">
@@ -3885,13 +3892,13 @@
         <v>95</v>
       </c>
       <c r="D104" s="8" t="s">
-        <v>404</v>
+        <v>403</v>
       </c>
       <c r="F104" s="6">
         <v>3</v>
       </c>
       <c r="G104" s="14" t="s">
-        <v>406</v>
+        <v>405</v>
       </c>
     </row>
     <row r="105" spans="1:7" ht="17.149999999999999" x14ac:dyDescent="0.55000000000000004">
@@ -3905,7 +3912,7 @@
         <v>95</v>
       </c>
       <c r="D105" s="8" t="s">
-        <v>418</v>
+        <v>417</v>
       </c>
       <c r="E105" s="9" t="s">
         <v>93</v>
@@ -3925,7 +3932,7 @@
         <v>80</v>
       </c>
       <c r="D106" s="8" t="s">
-        <v>416</v>
+        <v>415</v>
       </c>
       <c r="E106" s="9" t="s">
         <v>98</v>
@@ -3934,7 +3941,7 @@
         <v>2</v>
       </c>
       <c r="G106" s="14" t="s">
-        <v>417</v>
+        <v>416</v>
       </c>
     </row>
     <row r="107" spans="1:7" ht="17.149999999999999" x14ac:dyDescent="0.55000000000000004">
@@ -3948,7 +3955,7 @@
         <v>13</v>
       </c>
       <c r="D107" s="8" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
       <c r="F107" s="6">
         <v>3</v>
@@ -3991,7 +3998,7 @@
         <v>80</v>
       </c>
       <c r="D109" s="8" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
       <c r="E109" s="9" t="s">
         <v>98</v>
@@ -4014,7 +4021,7 @@
         <v>80</v>
       </c>
       <c r="D110" s="8" t="s">
-        <v>402</v>
+        <v>401</v>
       </c>
       <c r="F110" s="6">
         <v>3</v>
@@ -4034,7 +4041,7 @@
         <v>95</v>
       </c>
       <c r="D111" s="8" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
       <c r="E111" s="9" t="s">
         <v>110</v>
@@ -4077,7 +4084,7 @@
         <v>13</v>
       </c>
       <c r="D113" s="8" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
       <c r="F113" s="6">
         <v>3</v>
@@ -4094,7 +4101,7 @@
         <v>13</v>
       </c>
       <c r="D114" s="8" t="s">
-        <v>404</v>
+        <v>403</v>
       </c>
       <c r="E114" s="9" t="s">
         <v>128</v>
@@ -4154,7 +4161,7 @@
         <v>6</v>
       </c>
       <c r="D117" s="8" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
       <c r="E117" s="9" t="s">
         <v>93</v>
@@ -4174,7 +4181,7 @@
         <v>80</v>
       </c>
       <c r="D118" s="8" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
       <c r="F118" s="6">
         <v>4</v>
@@ -4211,7 +4218,7 @@
         <v>95</v>
       </c>
       <c r="D120" s="8" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
       <c r="E120" s="9" t="s">
         <v>22</v>
@@ -4220,7 +4227,7 @@
         <v>3</v>
       </c>
       <c r="G120" s="14" t="s">
-        <v>368</v>
+        <v>367</v>
       </c>
     </row>
     <row r="121" spans="1:7" ht="17.149999999999999" x14ac:dyDescent="0.55000000000000004">
@@ -4234,7 +4241,7 @@
         <v>80</v>
       </c>
       <c r="D121" s="8" t="s">
-        <v>407</v>
+        <v>406</v>
       </c>
       <c r="E121" s="9" t="s">
         <v>14</v>
@@ -4243,7 +4250,7 @@
         <v>3</v>
       </c>
       <c r="G121" s="14" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
     </row>
     <row r="122" spans="1:7" ht="17.149999999999999" x14ac:dyDescent="0.55000000000000004">
@@ -4288,7 +4295,7 @@
         <v>42</v>
       </c>
       <c r="D124" s="8" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
       <c r="E124" s="9" t="s">
         <v>128</v>
@@ -4308,7 +4315,7 @@
         <v>42</v>
       </c>
       <c r="D125" s="8" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
       <c r="E125" s="10" t="s">
         <v>185</v>
@@ -4328,13 +4335,13 @@
         <v>13</v>
       </c>
       <c r="D126" s="8" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
       <c r="F126" s="6">
         <v>3</v>
       </c>
       <c r="G126" s="14" t="s">
-        <v>398</v>
+        <v>397</v>
       </c>
     </row>
     <row r="127" spans="1:7" ht="17.149999999999999" x14ac:dyDescent="0.55000000000000004">
@@ -4348,7 +4355,7 @@
         <v>42</v>
       </c>
       <c r="D127" s="8" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
       <c r="F127" s="6">
         <v>3</v>
@@ -4365,7 +4372,7 @@
         <v>80</v>
       </c>
       <c r="D128" s="8" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
       <c r="E128" s="9" t="s">
         <v>131</v>
@@ -4385,7 +4392,7 @@
         <v>95</v>
       </c>
       <c r="D129" s="8" t="s">
-        <v>385</v>
+        <v>384</v>
       </c>
       <c r="E129" s="9" t="s">
         <v>118</v>
@@ -4405,7 +4412,7 @@
         <v>13</v>
       </c>
       <c r="D130" s="8" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
       <c r="E130" s="9" t="s">
         <v>14</v>
@@ -4416,13 +4423,13 @@
     </row>
     <row r="131" spans="1:7" ht="17.149999999999999" x14ac:dyDescent="0.55000000000000004">
       <c r="A131" s="10" t="s">
-        <v>371</v>
+        <v>370</v>
       </c>
       <c r="C131" s="7" t="s">
         <v>42</v>
       </c>
       <c r="D131" s="8" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
     </row>
     <row r="132" spans="1:7" ht="17.149999999999999" x14ac:dyDescent="0.55000000000000004">
@@ -4436,7 +4443,7 @@
         <v>13</v>
       </c>
       <c r="D132" s="8" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
       <c r="F132" s="6">
         <v>2</v>
@@ -4518,7 +4525,7 @@
         <v>80</v>
       </c>
       <c r="D137" s="8" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
       <c r="E137" s="9" t="s">
         <v>14</v>
@@ -4527,7 +4534,7 @@
         <v>2</v>
       </c>
       <c r="G137" s="14" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
     </row>
     <row r="138" spans="1:7" ht="17.149999999999999" x14ac:dyDescent="0.55000000000000004">
@@ -4541,7 +4548,7 @@
         <v>42</v>
       </c>
       <c r="D138" s="8" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
       <c r="E138" s="9" t="s">
         <v>183</v>
@@ -4581,7 +4588,7 @@
         <v>80</v>
       </c>
       <c r="D140" s="8" t="s">
-        <v>418</v>
+        <v>417</v>
       </c>
       <c r="E140" s="9" t="s">
         <v>250</v>
@@ -4590,7 +4597,7 @@
         <v>2</v>
       </c>
       <c r="G140" s="14" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
     </row>
     <row r="141" spans="1:7" ht="17.149999999999999" x14ac:dyDescent="0.55000000000000004">
@@ -4604,13 +4611,13 @@
         <v>42</v>
       </c>
       <c r="D141" s="8" t="s">
+        <v>412</v>
+      </c>
+      <c r="F141" s="6">
+        <v>3</v>
+      </c>
+      <c r="G141" s="14" t="s">
         <v>413</v>
-      </c>
-      <c r="F141" s="6">
-        <v>3</v>
-      </c>
-      <c r="G141" s="14" t="s">
-        <v>414</v>
       </c>
     </row>
     <row r="142" spans="1:7" ht="17.149999999999999" x14ac:dyDescent="0.55000000000000004">
@@ -4621,13 +4628,16 @@
         <v>268</v>
       </c>
       <c r="C142" s="7" t="s">
-        <v>6</v>
+        <v>13</v>
       </c>
       <c r="D142" s="8" t="s">
-        <v>365</v>
+        <v>421</v>
       </c>
       <c r="F142" s="6">
-        <v>2</v>
+        <v>3</v>
+      </c>
+      <c r="G142" s="14" t="s">
+        <v>422</v>
       </c>
     </row>
     <row r="143" spans="1:7" ht="17.149999999999999" x14ac:dyDescent="0.55000000000000004">
@@ -4641,7 +4651,7 @@
         <v>95</v>
       </c>
       <c r="D143" s="8" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
       <c r="E143" s="9" t="s">
         <v>122</v>
@@ -4661,7 +4671,7 @@
         <v>13</v>
       </c>
       <c r="D144" s="8" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
       <c r="E144" s="9" t="s">
         <v>22</v>
@@ -4678,7 +4688,7 @@
         <v>13</v>
       </c>
       <c r="D145" s="8" t="s">
-        <v>404</v>
+        <v>403</v>
       </c>
       <c r="E145" s="9" t="s">
         <v>47</v>
@@ -4687,7 +4697,7 @@
         <v>4</v>
       </c>
       <c r="G145" s="14" t="s">
-        <v>405</v>
+        <v>404</v>
       </c>
     </row>
     <row r="146" spans="1:7" ht="17.149999999999999" x14ac:dyDescent="0.55000000000000004">
@@ -4701,7 +4711,7 @@
         <v>13</v>
       </c>
       <c r="D146" s="8" t="s">
-        <v>407</v>
+        <v>406</v>
       </c>
       <c r="E146" s="9" t="s">
         <v>93</v>
@@ -4755,7 +4765,7 @@
         <v>95</v>
       </c>
       <c r="D149" s="8" t="s">
-        <v>418</v>
+        <v>417</v>
       </c>
       <c r="E149" s="9" t="s">
         <v>128</v>
@@ -4775,7 +4785,7 @@
         <v>13</v>
       </c>
       <c r="D150" s="8" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
       <c r="F150" s="6">
         <v>3</v>
@@ -4800,7 +4810,7 @@
         <v>13</v>
       </c>
       <c r="D152" s="8" t="s">
-        <v>399</v>
+        <v>398</v>
       </c>
       <c r="F152" s="6">
         <v>3</v>
@@ -4817,7 +4827,7 @@
         <v>95</v>
       </c>
       <c r="D153" s="8" t="s">
-        <v>403</v>
+        <v>402</v>
       </c>
       <c r="F153" s="6">
         <v>3</v>

</xml_diff>

<commit_message>
2024.12.22 LeetCodeHot100 三刷 最后9道 就在今天
</commit_message>
<xml_diff>
--- a/2024LeetCode刷题记录.xlsx
+++ b/2024LeetCode刷题记录.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\develop\GithubRepo\LeetCode\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{92CD09BC-C4E1-4B78-9BB0-ADEB681A2C2E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4BC8F11C-E43D-4B43-B66E-88A5EEDDE176}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-103" yWindow="-103" windowWidth="22149" windowHeight="11829" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-24684" yWindow="5208" windowWidth="16452" windowHeight="8424" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="729" uniqueCount="422">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="730" uniqueCount="422">
   <si>
     <t>题目</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -1185,10 +1185,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>2024.09.20</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>前缀和</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -1201,10 +1197,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>2024.09.23</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>标志位</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -1559,6 +1551,14 @@
   </si>
   <si>
     <t>到底用n+1还是n呢</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>2024.12.22</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>有可能不存在</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -2017,8 +2017,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G153"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="E14" sqref="E14"/>
+    <sheetView tabSelected="1" topLeftCell="A16" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="F24" sqref="F24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="14.15" x14ac:dyDescent="0.35"/>
@@ -2067,7 +2067,7 @@
         <v>80</v>
       </c>
       <c r="D2" s="8" t="s">
-        <v>378</v>
+        <v>376</v>
       </c>
       <c r="F2" s="6">
         <v>3</v>
@@ -2084,13 +2084,13 @@
         <v>42</v>
       </c>
       <c r="D3" s="8" t="s">
-        <v>393</v>
+        <v>391</v>
       </c>
       <c r="F3" s="6">
         <v>3</v>
       </c>
       <c r="G3" s="14" t="s">
-        <v>394</v>
+        <v>392</v>
       </c>
     </row>
     <row r="4" spans="1:7" ht="17.149999999999999" x14ac:dyDescent="0.55000000000000004">
@@ -2101,7 +2101,7 @@
         <v>13</v>
       </c>
       <c r="D4" s="8" t="s">
-        <v>396</v>
+        <v>394</v>
       </c>
       <c r="F4" s="6">
         <v>3</v>
@@ -2112,19 +2112,19 @@
         <v>207</v>
       </c>
       <c r="B5" s="6" t="s">
-        <v>351</v>
+        <v>349</v>
       </c>
       <c r="C5" s="7" t="s">
         <v>42</v>
       </c>
       <c r="D5" s="8" t="s">
-        <v>393</v>
+        <v>391</v>
       </c>
       <c r="F5" s="6">
         <v>3</v>
       </c>
       <c r="G5" s="14" t="s">
-        <v>394</v>
+        <v>392</v>
       </c>
     </row>
     <row r="6" spans="1:7" ht="17.149999999999999" x14ac:dyDescent="0.55000000000000004">
@@ -2158,7 +2158,7 @@
         <v>80</v>
       </c>
       <c r="D7" s="8" t="s">
-        <v>398</v>
+        <v>396</v>
       </c>
       <c r="F7" s="6">
         <v>3</v>
@@ -2166,13 +2166,13 @@
     </row>
     <row r="8" spans="1:7" ht="17.149999999999999" x14ac:dyDescent="0.55000000000000004">
       <c r="A8" s="10" t="s">
-        <v>372</v>
+        <v>370</v>
       </c>
       <c r="C8" s="7" t="s">
         <v>13</v>
       </c>
       <c r="D8" s="8" t="s">
-        <v>369</v>
+        <v>367</v>
       </c>
     </row>
     <row r="9" spans="1:7" ht="17.149999999999999" x14ac:dyDescent="0.55000000000000004">
@@ -2183,7 +2183,7 @@
         <v>13</v>
       </c>
       <c r="D9" s="8" t="s">
-        <v>396</v>
+        <v>394</v>
       </c>
       <c r="F9" s="6">
         <v>3</v>
@@ -2200,7 +2200,7 @@
         <v>42</v>
       </c>
       <c r="D10" s="8" t="s">
-        <v>380</v>
+        <v>378</v>
       </c>
       <c r="E10" s="9" t="s">
         <v>93</v>
@@ -2220,13 +2220,13 @@
         <v>13</v>
       </c>
       <c r="D11" s="8" t="s">
-        <v>396</v>
+        <v>394</v>
       </c>
       <c r="F11" s="6">
         <v>3</v>
       </c>
       <c r="G11" s="14" t="s">
-        <v>353</v>
+        <v>351</v>
       </c>
     </row>
     <row r="12" spans="1:7" ht="17.149999999999999" x14ac:dyDescent="0.55000000000000004">
@@ -2240,7 +2240,7 @@
         <v>95</v>
       </c>
       <c r="D12" s="8" t="s">
-        <v>364</v>
+        <v>362</v>
       </c>
       <c r="E12" s="9" t="s">
         <v>14</v>
@@ -2249,7 +2249,7 @@
         <v>2</v>
       </c>
       <c r="G12" s="14" t="s">
-        <v>366</v>
+        <v>364</v>
       </c>
     </row>
     <row r="13" spans="1:7" ht="17.149999999999999" x14ac:dyDescent="0.55000000000000004">
@@ -2283,7 +2283,7 @@
         <v>6</v>
       </c>
       <c r="D14" s="8" t="s">
-        <v>363</v>
+        <v>361</v>
       </c>
       <c r="F14" s="6">
         <v>2</v>
@@ -2320,7 +2320,7 @@
         <v>42</v>
       </c>
       <c r="D16" s="8" t="s">
-        <v>418</v>
+        <v>416</v>
       </c>
       <c r="E16" s="9" t="s">
         <v>14</v>
@@ -2331,16 +2331,16 @@
     </row>
     <row r="17" spans="1:7" ht="17.149999999999999" x14ac:dyDescent="0.55000000000000004">
       <c r="A17" s="10" t="s">
+        <v>344</v>
+      </c>
+      <c r="B17" s="6" t="s">
         <v>346</v>
-      </c>
-      <c r="B17" s="6" t="s">
-        <v>348</v>
       </c>
       <c r="C17" s="7" t="s">
         <v>13</v>
       </c>
       <c r="D17" s="8" t="s">
-        <v>347</v>
+        <v>345</v>
       </c>
       <c r="E17" s="9" t="s">
         <v>14</v>
@@ -2348,13 +2348,13 @@
     </row>
     <row r="18" spans="1:7" ht="17.149999999999999" x14ac:dyDescent="0.55000000000000004">
       <c r="A18" s="10" t="s">
-        <v>349</v>
+        <v>347</v>
       </c>
       <c r="C18" s="7" t="s">
         <v>42</v>
       </c>
       <c r="D18" s="8" t="s">
-        <v>350</v>
+        <v>348</v>
       </c>
       <c r="E18" s="9" t="s">
         <v>14</v>
@@ -2365,13 +2365,13 @@
         <v>220</v>
       </c>
       <c r="B19" s="6" t="s">
-        <v>358</v>
+        <v>356</v>
       </c>
       <c r="C19" s="7" t="s">
         <v>13</v>
       </c>
       <c r="D19" s="8" t="s">
-        <v>400</v>
+        <v>398</v>
       </c>
       <c r="F19" s="6">
         <v>3</v>
@@ -2391,7 +2391,7 @@
         <v>80</v>
       </c>
       <c r="D20" s="8" t="s">
-        <v>378</v>
+        <v>376</v>
       </c>
       <c r="F20" s="6">
         <v>3</v>
@@ -2408,7 +2408,7 @@
         <v>95</v>
       </c>
       <c r="D21" s="8" t="s">
-        <v>404</v>
+        <v>402</v>
       </c>
       <c r="E21" s="9" t="s">
         <v>128</v>
@@ -2417,7 +2417,7 @@
         <v>3</v>
       </c>
       <c r="G21" s="14" t="s">
-        <v>406</v>
+        <v>404</v>
       </c>
     </row>
     <row r="22" spans="1:7" ht="17.149999999999999" x14ac:dyDescent="0.55000000000000004">
@@ -2431,7 +2431,7 @@
         <v>28</v>
       </c>
       <c r="D22" s="8" t="s">
-        <v>419</v>
+        <v>417</v>
       </c>
       <c r="F22" s="6">
         <v>3</v>
@@ -2448,7 +2448,7 @@
         <v>13</v>
       </c>
       <c r="D23" s="8" t="s">
-        <v>388</v>
+        <v>386</v>
       </c>
       <c r="E23" s="9" t="s">
         <v>87</v>
@@ -2468,13 +2468,13 @@
         <v>13</v>
       </c>
       <c r="D24" s="8" t="s">
-        <v>328</v>
+        <v>420</v>
       </c>
       <c r="E24" s="9" t="s">
         <v>14</v>
       </c>
       <c r="F24" s="6">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="25" spans="1:7" ht="17.149999999999999" x14ac:dyDescent="0.55000000000000004">
@@ -2482,13 +2482,13 @@
         <v>194</v>
       </c>
       <c r="B25" s="6" t="s">
-        <v>341</v>
+        <v>339</v>
       </c>
       <c r="C25" s="7" t="s">
         <v>42</v>
       </c>
       <c r="D25" s="8" t="s">
-        <v>386</v>
+        <v>384</v>
       </c>
       <c r="F25" s="6">
         <v>3</v>
@@ -2502,33 +2502,33 @@
         <v>13</v>
       </c>
       <c r="D26" s="8" t="s">
-        <v>386</v>
+        <v>384</v>
       </c>
       <c r="E26" s="13" t="s">
-        <v>342</v>
+        <v>340</v>
       </c>
       <c r="F26" s="6">
         <v>3</v>
       </c>
       <c r="G26" s="14" t="s">
-        <v>387</v>
+        <v>385</v>
       </c>
     </row>
     <row r="27" spans="1:7" ht="17.149999999999999" x14ac:dyDescent="0.55000000000000004">
       <c r="A27" s="10" t="s">
-        <v>373</v>
+        <v>371</v>
       </c>
       <c r="C27" s="7" t="s">
         <v>42</v>
       </c>
       <c r="D27" s="8" t="s">
-        <v>369</v>
+        <v>367</v>
       </c>
       <c r="E27" s="9" t="s">
-        <v>374</v>
+        <v>372</v>
       </c>
       <c r="G27" s="14" t="s">
-        <v>375</v>
+        <v>373</v>
       </c>
     </row>
     <row r="28" spans="1:7" ht="17.149999999999999" x14ac:dyDescent="0.55000000000000004">
@@ -2556,7 +2556,7 @@
         <v>95</v>
       </c>
       <c r="D29" s="8" t="s">
-        <v>392</v>
+        <v>390</v>
       </c>
       <c r="F29" s="6">
         <v>3</v>
@@ -2576,13 +2576,13 @@
         <v>80</v>
       </c>
       <c r="D30" s="8" t="s">
-        <v>388</v>
+        <v>386</v>
       </c>
       <c r="F30" s="6">
         <v>3</v>
       </c>
       <c r="G30" s="14" t="s">
-        <v>391</v>
+        <v>389</v>
       </c>
     </row>
     <row r="31" spans="1:7" ht="17.149999999999999" x14ac:dyDescent="0.55000000000000004">
@@ -2596,7 +2596,7 @@
         <v>13</v>
       </c>
       <c r="D31" s="8" t="s">
-        <v>380</v>
+        <v>378</v>
       </c>
       <c r="E31" s="9" t="s">
         <v>97</v>
@@ -2619,7 +2619,7 @@
         <v>6</v>
       </c>
       <c r="D32" s="8" t="s">
-        <v>363</v>
+        <v>361</v>
       </c>
       <c r="F32" s="6">
         <v>2</v>
@@ -2636,13 +2636,13 @@
         <v>13</v>
       </c>
       <c r="D33" s="8" t="s">
-        <v>413</v>
+        <v>411</v>
       </c>
       <c r="F33" s="6">
         <v>3</v>
       </c>
       <c r="G33" s="14" t="s">
-        <v>361</v>
+        <v>359</v>
       </c>
     </row>
     <row r="34" spans="1:7" ht="17.149999999999999" x14ac:dyDescent="0.55000000000000004">
@@ -2656,7 +2656,7 @@
         <v>13</v>
       </c>
       <c r="D34" s="8" t="s">
-        <v>415</v>
+        <v>413</v>
       </c>
       <c r="E34" s="9" t="s">
         <v>103</v>
@@ -2707,27 +2707,27 @@
         <v>6</v>
       </c>
       <c r="D37" s="8" t="s">
-        <v>386</v>
+        <v>384</v>
       </c>
       <c r="E37" s="13" t="s">
-        <v>338</v>
+        <v>336</v>
       </c>
       <c r="F37" s="6">
         <v>3</v>
       </c>
       <c r="G37" s="14" t="s">
-        <v>337</v>
+        <v>335</v>
       </c>
     </row>
     <row r="38" spans="1:7" ht="17.149999999999999" x14ac:dyDescent="0.55000000000000004">
       <c r="A38" s="10" t="s">
-        <v>376</v>
+        <v>374</v>
       </c>
       <c r="C38" s="7" t="s">
         <v>42</v>
       </c>
       <c r="D38" s="8" t="s">
-        <v>377</v>
+        <v>375</v>
       </c>
     </row>
     <row r="39" spans="1:7" ht="17.149999999999999" x14ac:dyDescent="0.55000000000000004">
@@ -2741,7 +2741,7 @@
         <v>13</v>
       </c>
       <c r="D39" s="8" t="s">
-        <v>419</v>
+        <v>417</v>
       </c>
       <c r="F39" s="6">
         <v>3</v>
@@ -2758,7 +2758,7 @@
         <v>80</v>
       </c>
       <c r="D40" s="8" t="s">
-        <v>401</v>
+        <v>399</v>
       </c>
       <c r="E40" s="9" t="s">
         <v>22</v>
@@ -2775,7 +2775,7 @@
         <v>28</v>
       </c>
       <c r="D41" s="8" t="s">
-        <v>384</v>
+        <v>382</v>
       </c>
       <c r="F41" s="6">
         <v>3</v>
@@ -2789,13 +2789,13 @@
         <v>13</v>
       </c>
       <c r="D42" s="8" t="s">
-        <v>388</v>
+        <v>386</v>
       </c>
       <c r="F42" s="6">
         <v>3</v>
       </c>
       <c r="G42" s="14" t="s">
-        <v>344</v>
+        <v>342</v>
       </c>
     </row>
     <row r="43" spans="1:7" ht="17.149999999999999" x14ac:dyDescent="0.55000000000000004">
@@ -2809,13 +2809,13 @@
         <v>80</v>
       </c>
       <c r="D43" s="8" t="s">
+        <v>417</v>
+      </c>
+      <c r="F43" s="6">
+        <v>3</v>
+      </c>
+      <c r="G43" s="14" t="s">
         <v>419</v>
-      </c>
-      <c r="F43" s="6">
-        <v>3</v>
-      </c>
-      <c r="G43" s="14" t="s">
-        <v>421</v>
       </c>
     </row>
     <row r="44" spans="1:7" ht="17.149999999999999" x14ac:dyDescent="0.55000000000000004">
@@ -2826,13 +2826,13 @@
         <v>13</v>
       </c>
       <c r="D44" s="8" t="s">
-        <v>396</v>
+        <v>394</v>
       </c>
       <c r="F44" s="6">
         <v>3</v>
       </c>
       <c r="G44" s="14" t="s">
-        <v>352</v>
+        <v>350</v>
       </c>
     </row>
     <row r="45" spans="1:7" ht="17.149999999999999" x14ac:dyDescent="0.55000000000000004">
@@ -2843,7 +2843,7 @@
         <v>6</v>
       </c>
       <c r="D45" s="8" t="s">
-        <v>388</v>
+        <v>386</v>
       </c>
       <c r="F45" s="6">
         <v>3</v>
@@ -2860,7 +2860,7 @@
         <v>80</v>
       </c>
       <c r="D46" s="8" t="s">
-        <v>415</v>
+        <v>413</v>
       </c>
       <c r="F46" s="6">
         <v>3</v>
@@ -2874,7 +2874,7 @@
         <v>13</v>
       </c>
       <c r="D47" s="8" t="s">
-        <v>400</v>
+        <v>398</v>
       </c>
       <c r="F47" s="6">
         <v>3</v>
@@ -2891,7 +2891,7 @@
         <v>80</v>
       </c>
       <c r="D48" s="8" t="s">
-        <v>386</v>
+        <v>384</v>
       </c>
       <c r="F48" s="6">
         <v>3</v>
@@ -2905,7 +2905,7 @@
         <v>80</v>
       </c>
       <c r="D49" s="8" t="s">
-        <v>401</v>
+        <v>399</v>
       </c>
       <c r="F49" s="6">
         <v>3</v>
@@ -2919,7 +2919,7 @@
         <v>13</v>
       </c>
       <c r="D50" s="8" t="s">
-        <v>401</v>
+        <v>399</v>
       </c>
       <c r="F50" s="6">
         <v>3</v>
@@ -2953,27 +2953,27 @@
         <v>42</v>
       </c>
       <c r="D52" s="8" t="s">
-        <v>388</v>
+        <v>386</v>
       </c>
       <c r="F52" s="6">
         <v>3</v>
       </c>
       <c r="G52" s="14" t="s">
-        <v>343</v>
+        <v>341</v>
       </c>
     </row>
     <row r="53" spans="1:7" ht="17.149999999999999" x14ac:dyDescent="0.55000000000000004">
       <c r="A53" s="10" t="s">
+        <v>331</v>
+      </c>
+      <c r="B53" s="6" t="s">
         <v>333</v>
-      </c>
-      <c r="B53" s="6" t="s">
-        <v>335</v>
       </c>
       <c r="C53" s="7" t="s">
         <v>13</v>
       </c>
       <c r="D53" s="8" t="s">
-        <v>334</v>
+        <v>332</v>
       </c>
       <c r="E53" s="9" t="s">
         <v>14</v>
@@ -2990,7 +2990,7 @@
         <v>13</v>
       </c>
       <c r="D54" s="8" t="s">
-        <v>417</v>
+        <v>415</v>
       </c>
       <c r="F54" s="6">
         <v>4</v>
@@ -3013,7 +3013,7 @@
         <v>134</v>
       </c>
       <c r="G55" s="14" t="s">
-        <v>332</v>
+        <v>330</v>
       </c>
     </row>
     <row r="56" spans="1:7" ht="17.149999999999999" x14ac:dyDescent="0.55000000000000004">
@@ -3047,10 +3047,10 @@
         <v>13</v>
       </c>
       <c r="D57" s="8" t="s">
-        <v>404</v>
+        <v>402</v>
       </c>
       <c r="E57" s="9" t="s">
-        <v>405</v>
+        <v>403</v>
       </c>
       <c r="F57" s="6">
         <v>3</v>
@@ -3064,13 +3064,13 @@
         <v>13</v>
       </c>
       <c r="D58" s="8" t="s">
-        <v>393</v>
+        <v>391</v>
       </c>
       <c r="F58" s="6">
         <v>3</v>
       </c>
       <c r="G58" s="14" t="s">
-        <v>394</v>
+        <v>392</v>
       </c>
     </row>
     <row r="59" spans="1:7" ht="17.149999999999999" x14ac:dyDescent="0.55000000000000004">
@@ -3084,7 +3084,7 @@
         <v>13</v>
       </c>
       <c r="D59" s="8" t="s">
-        <v>392</v>
+        <v>390</v>
       </c>
       <c r="F59" s="6">
         <v>3</v>
@@ -3098,13 +3098,13 @@
         <v>13</v>
       </c>
       <c r="D60" s="8" t="s">
-        <v>396</v>
+        <v>394</v>
       </c>
       <c r="F60" s="6">
         <v>3</v>
       </c>
       <c r="G60" s="14" t="s">
-        <v>397</v>
+        <v>395</v>
       </c>
     </row>
     <row r="61" spans="1:7" ht="17.149999999999999" x14ac:dyDescent="0.55000000000000004">
@@ -3115,7 +3115,7 @@
         <v>95</v>
       </c>
       <c r="D61" s="8" t="s">
-        <v>386</v>
+        <v>384</v>
       </c>
       <c r="F61" s="6">
         <v>3</v>
@@ -3126,13 +3126,13 @@
         <v>219</v>
       </c>
       <c r="B62" s="6" t="s">
-        <v>356</v>
+        <v>354</v>
       </c>
       <c r="C62" s="7" t="s">
         <v>80</v>
       </c>
       <c r="D62" s="8" t="s">
-        <v>399</v>
+        <v>397</v>
       </c>
       <c r="E62" s="9" t="s">
         <v>93</v>
@@ -3141,7 +3141,7 @@
         <v>3</v>
       </c>
       <c r="G62" s="14" t="s">
-        <v>357</v>
+        <v>355</v>
       </c>
     </row>
     <row r="63" spans="1:7" ht="17.149999999999999" x14ac:dyDescent="0.55000000000000004">
@@ -3149,13 +3149,13 @@
         <v>178</v>
       </c>
       <c r="B63" s="6" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
       <c r="C63" s="7" t="s">
         <v>6</v>
       </c>
       <c r="D63" s="8" t="s">
-        <v>384</v>
+        <v>382</v>
       </c>
       <c r="F63" s="6">
         <v>3</v>
@@ -3172,7 +3172,7 @@
         <v>95</v>
       </c>
       <c r="D64" s="8" t="s">
-        <v>383</v>
+        <v>381</v>
       </c>
       <c r="E64" s="9" t="s">
         <v>118</v>
@@ -3203,19 +3203,19 @@
     </row>
     <row r="66" spans="1:7" ht="17.149999999999999" x14ac:dyDescent="0.55000000000000004">
       <c r="A66" s="10" t="s">
-        <v>345</v>
+        <v>343</v>
       </c>
       <c r="C66" s="7" t="s">
         <v>95</v>
       </c>
       <c r="D66" s="8" t="s">
+        <v>386</v>
+      </c>
+      <c r="F66" s="6">
+        <v>3</v>
+      </c>
+      <c r="G66" s="14" t="s">
         <v>388</v>
-      </c>
-      <c r="F66" s="6">
-        <v>3</v>
-      </c>
-      <c r="G66" s="14" t="s">
-        <v>390</v>
       </c>
     </row>
     <row r="67" spans="1:7" ht="17.149999999999999" x14ac:dyDescent="0.55000000000000004">
@@ -3229,7 +3229,7 @@
         <v>42</v>
       </c>
       <c r="D67" s="8" t="s">
-        <v>385</v>
+        <v>383</v>
       </c>
       <c r="E67" s="9" t="s">
         <v>93</v>
@@ -3272,13 +3272,13 @@
         <v>95</v>
       </c>
       <c r="D69" s="8" t="s">
-        <v>388</v>
+        <v>386</v>
       </c>
       <c r="F69" s="6">
         <v>4</v>
       </c>
       <c r="G69" s="14" t="s">
-        <v>389</v>
+        <v>387</v>
       </c>
     </row>
     <row r="70" spans="1:7" ht="17.149999999999999" x14ac:dyDescent="0.55000000000000004">
@@ -3428,27 +3428,27 @@
         <v>80</v>
       </c>
       <c r="D78" s="8" t="s">
-        <v>324</v>
+        <v>420</v>
       </c>
       <c r="E78" s="13" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="F78" s="6">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="79" spans="1:7" ht="17.149999999999999" x14ac:dyDescent="0.55000000000000004">
       <c r="A79" s="10" t="s">
-        <v>371</v>
+        <v>369</v>
       </c>
       <c r="C79" s="7" t="s">
         <v>13</v>
       </c>
       <c r="D79" s="8" t="s">
-        <v>369</v>
+        <v>367</v>
       </c>
       <c r="G79" s="14" t="s">
-        <v>370</v>
+        <v>368</v>
       </c>
     </row>
     <row r="80" spans="1:7" ht="17.149999999999999" x14ac:dyDescent="0.55000000000000004">
@@ -3510,7 +3510,7 @@
         <v>80</v>
       </c>
       <c r="D83" s="8" t="s">
-        <v>379</v>
+        <v>377</v>
       </c>
       <c r="E83" s="9" t="s">
         <v>87</v>
@@ -3586,7 +3586,7 @@
         <v>13</v>
       </c>
       <c r="D88" s="8" t="s">
-        <v>419</v>
+        <v>417</v>
       </c>
       <c r="E88" s="9" t="s">
         <v>274</v>
@@ -3609,7 +3609,7 @@
         <v>80</v>
       </c>
       <c r="D89" s="8" t="s">
-        <v>417</v>
+        <v>415</v>
       </c>
       <c r="E89" s="9" t="s">
         <v>8</v>
@@ -3632,7 +3632,7 @@
         <v>80</v>
       </c>
       <c r="D90" s="8" t="s">
-        <v>381</v>
+        <v>379</v>
       </c>
       <c r="E90" s="9" t="s">
         <v>109</v>
@@ -3655,7 +3655,7 @@
         <v>80</v>
       </c>
       <c r="D91" s="8" t="s">
-        <v>363</v>
+        <v>361</v>
       </c>
       <c r="F91" s="6">
         <v>2</v>
@@ -3675,7 +3675,7 @@
         <v>42</v>
       </c>
       <c r="D92" s="8" t="s">
-        <v>419</v>
+        <v>417</v>
       </c>
       <c r="E92" s="9" t="s">
         <v>270</v>
@@ -3706,7 +3706,7 @@
         <v>13</v>
       </c>
       <c r="D94" s="8" t="s">
-        <v>363</v>
+        <v>361</v>
       </c>
       <c r="F94" s="6">
         <v>2</v>
@@ -3723,10 +3723,13 @@
         <v>13</v>
       </c>
       <c r="D95" s="8" t="s">
-        <v>318</v>
+        <v>420</v>
       </c>
       <c r="F95" s="6">
-        <v>2</v>
+        <v>3</v>
+      </c>
+      <c r="G95" s="14" t="s">
+        <v>421</v>
       </c>
     </row>
     <row r="96" spans="1:7" ht="17.149999999999999" x14ac:dyDescent="0.55000000000000004">
@@ -3740,7 +3743,7 @@
         <v>95</v>
       </c>
       <c r="D96" s="8" t="s">
-        <v>410</v>
+        <v>408</v>
       </c>
       <c r="E96" s="12" t="s">
         <v>241</v>
@@ -3749,21 +3752,21 @@
         <v>3</v>
       </c>
       <c r="G96" s="14" t="s">
-        <v>412</v>
+        <v>410</v>
       </c>
     </row>
     <row r="97" spans="1:7" ht="17.149999999999999" x14ac:dyDescent="0.55000000000000004">
       <c r="A97" s="10" t="s">
-        <v>339</v>
+        <v>337</v>
       </c>
       <c r="B97" s="6" t="s">
-        <v>340</v>
+        <v>338</v>
       </c>
       <c r="C97" s="7" t="s">
         <v>13</v>
       </c>
       <c r="D97" s="8" t="s">
-        <v>336</v>
+        <v>334</v>
       </c>
       <c r="E97" s="9" t="s">
         <v>14</v>
@@ -3780,7 +3783,7 @@
         <v>80</v>
       </c>
       <c r="D98" s="8" t="s">
-        <v>410</v>
+        <v>408</v>
       </c>
       <c r="E98" s="9" t="s">
         <v>22</v>
@@ -3800,7 +3803,7 @@
         <v>80</v>
       </c>
       <c r="D99" s="8" t="s">
-        <v>417</v>
+        <v>415</v>
       </c>
       <c r="F99" s="6">
         <v>3</v>
@@ -3817,13 +3820,13 @@
         <v>42</v>
       </c>
       <c r="D100" s="8" t="s">
-        <v>408</v>
+        <v>406</v>
       </c>
       <c r="F100" s="6">
         <v>3</v>
       </c>
       <c r="G100" s="14" t="s">
-        <v>409</v>
+        <v>407</v>
       </c>
     </row>
     <row r="101" spans="1:7" ht="17.149999999999999" x14ac:dyDescent="0.55000000000000004">
@@ -3888,13 +3891,13 @@
         <v>95</v>
       </c>
       <c r="D104" s="8" t="s">
+        <v>399</v>
+      </c>
+      <c r="F104" s="6">
+        <v>3</v>
+      </c>
+      <c r="G104" s="14" t="s">
         <v>401</v>
-      </c>
-      <c r="F104" s="6">
-        <v>3</v>
-      </c>
-      <c r="G104" s="14" t="s">
-        <v>403</v>
       </c>
     </row>
     <row r="105" spans="1:7" ht="17.149999999999999" x14ac:dyDescent="0.55000000000000004">
@@ -3908,7 +3911,7 @@
         <v>95</v>
       </c>
       <c r="D105" s="8" t="s">
-        <v>415</v>
+        <v>413</v>
       </c>
       <c r="E105" s="9" t="s">
         <v>93</v>
@@ -3928,7 +3931,7 @@
         <v>80</v>
       </c>
       <c r="D106" s="8" t="s">
-        <v>413</v>
+        <v>411</v>
       </c>
       <c r="E106" s="9" t="s">
         <v>98</v>
@@ -3937,7 +3940,7 @@
         <v>2</v>
       </c>
       <c r="G106" s="14" t="s">
-        <v>414</v>
+        <v>412</v>
       </c>
     </row>
     <row r="107" spans="1:7" ht="17.149999999999999" x14ac:dyDescent="0.55000000000000004">
@@ -3951,13 +3954,13 @@
         <v>13</v>
       </c>
       <c r="D107" s="8" t="s">
-        <v>384</v>
+        <v>382</v>
       </c>
       <c r="F107" s="6">
         <v>3</v>
       </c>
       <c r="G107" s="14" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
     </row>
     <row r="108" spans="1:7" ht="17.149999999999999" x14ac:dyDescent="0.55000000000000004">
@@ -3994,7 +3997,7 @@
         <v>80</v>
       </c>
       <c r="D109" s="8" t="s">
-        <v>381</v>
+        <v>379</v>
       </c>
       <c r="E109" s="9" t="s">
         <v>98</v>
@@ -4011,19 +4014,19 @@
         <v>218</v>
       </c>
       <c r="B110" s="6" t="s">
-        <v>355</v>
+        <v>353</v>
       </c>
       <c r="C110" s="7" t="s">
         <v>80</v>
       </c>
       <c r="D110" s="8" t="s">
-        <v>399</v>
+        <v>397</v>
       </c>
       <c r="F110" s="6">
         <v>3</v>
       </c>
       <c r="G110" s="14" t="s">
-        <v>354</v>
+        <v>352</v>
       </c>
     </row>
     <row r="111" spans="1:7" ht="17.149999999999999" x14ac:dyDescent="0.55000000000000004">
@@ -4037,7 +4040,7 @@
         <v>95</v>
       </c>
       <c r="D111" s="8" t="s">
-        <v>381</v>
+        <v>379</v>
       </c>
       <c r="E111" s="9" t="s">
         <v>110</v>
@@ -4080,7 +4083,7 @@
         <v>13</v>
       </c>
       <c r="D113" s="8" t="s">
-        <v>418</v>
+        <v>416</v>
       </c>
       <c r="F113" s="6">
         <v>3</v>
@@ -4097,7 +4100,7 @@
         <v>13</v>
       </c>
       <c r="D114" s="8" t="s">
-        <v>401</v>
+        <v>399</v>
       </c>
       <c r="E114" s="9" t="s">
         <v>128</v>
@@ -4157,7 +4160,7 @@
         <v>6</v>
       </c>
       <c r="D117" s="8" t="s">
-        <v>385</v>
+        <v>383</v>
       </c>
       <c r="E117" s="9" t="s">
         <v>93</v>
@@ -4177,7 +4180,7 @@
         <v>80</v>
       </c>
       <c r="D118" s="8" t="s">
-        <v>378</v>
+        <v>376</v>
       </c>
       <c r="F118" s="6">
         <v>4</v>
@@ -4214,7 +4217,7 @@
         <v>95</v>
       </c>
       <c r="D120" s="8" t="s">
-        <v>378</v>
+        <v>376</v>
       </c>
       <c r="E120" s="9" t="s">
         <v>22</v>
@@ -4223,7 +4226,7 @@
         <v>3</v>
       </c>
       <c r="G120" s="14" t="s">
-        <v>365</v>
+        <v>363</v>
       </c>
     </row>
     <row r="121" spans="1:7" ht="17.149999999999999" x14ac:dyDescent="0.55000000000000004">
@@ -4237,7 +4240,7 @@
         <v>80</v>
       </c>
       <c r="D121" s="8" t="s">
-        <v>404</v>
+        <v>402</v>
       </c>
       <c r="E121" s="9" t="s">
         <v>14</v>
@@ -4246,7 +4249,7 @@
         <v>3</v>
       </c>
       <c r="G121" s="14" t="s">
-        <v>407</v>
+        <v>405</v>
       </c>
     </row>
     <row r="122" spans="1:7" ht="17.149999999999999" x14ac:dyDescent="0.55000000000000004">
@@ -4291,7 +4294,7 @@
         <v>42</v>
       </c>
       <c r="D124" s="8" t="s">
-        <v>384</v>
+        <v>382</v>
       </c>
       <c r="E124" s="9" t="s">
         <v>128</v>
@@ -4305,13 +4308,13 @@
         <v>184</v>
       </c>
       <c r="B125" s="6" t="s">
-        <v>331</v>
+        <v>329</v>
       </c>
       <c r="C125" s="7" t="s">
         <v>42</v>
       </c>
       <c r="D125" s="8" t="s">
-        <v>385</v>
+        <v>383</v>
       </c>
       <c r="E125" s="10" t="s">
         <v>185</v>
@@ -4320,7 +4323,7 @@
         <v>3</v>
       </c>
       <c r="G125" s="14" t="s">
-        <v>330</v>
+        <v>328</v>
       </c>
     </row>
     <row r="126" spans="1:7" ht="17.149999999999999" x14ac:dyDescent="0.55000000000000004">
@@ -4331,13 +4334,13 @@
         <v>13</v>
       </c>
       <c r="D126" s="8" t="s">
+        <v>391</v>
+      </c>
+      <c r="F126" s="6">
+        <v>3</v>
+      </c>
+      <c r="G126" s="14" t="s">
         <v>393</v>
-      </c>
-      <c r="F126" s="6">
-        <v>3</v>
-      </c>
-      <c r="G126" s="14" t="s">
-        <v>395</v>
       </c>
     </row>
     <row r="127" spans="1:7" ht="17.149999999999999" x14ac:dyDescent="0.55000000000000004">
@@ -4351,7 +4354,7 @@
         <v>42</v>
       </c>
       <c r="D127" s="8" t="s">
-        <v>418</v>
+        <v>416</v>
       </c>
       <c r="F127" s="6">
         <v>3</v>
@@ -4368,7 +4371,7 @@
         <v>80</v>
       </c>
       <c r="D128" s="8" t="s">
-        <v>384</v>
+        <v>382</v>
       </c>
       <c r="E128" s="9" t="s">
         <v>131</v>
@@ -4388,7 +4391,7 @@
         <v>95</v>
       </c>
       <c r="D129" s="8" t="s">
-        <v>382</v>
+        <v>380</v>
       </c>
       <c r="E129" s="9" t="s">
         <v>118</v>
@@ -4408,7 +4411,7 @@
         <v>13</v>
       </c>
       <c r="D130" s="8" t="s">
-        <v>364</v>
+        <v>362</v>
       </c>
       <c r="E130" s="9" t="s">
         <v>14</v>
@@ -4419,13 +4422,13 @@
     </row>
     <row r="131" spans="1:7" ht="17.149999999999999" x14ac:dyDescent="0.55000000000000004">
       <c r="A131" s="10" t="s">
-        <v>368</v>
+        <v>366</v>
       </c>
       <c r="C131" s="7" t="s">
         <v>42</v>
       </c>
       <c r="D131" s="8" t="s">
-        <v>369</v>
+        <v>367</v>
       </c>
     </row>
     <row r="132" spans="1:7" ht="17.149999999999999" x14ac:dyDescent="0.55000000000000004">
@@ -4439,7 +4442,7 @@
         <v>13</v>
       </c>
       <c r="D132" s="8" t="s">
-        <v>364</v>
+        <v>362</v>
       </c>
       <c r="F132" s="6">
         <v>2</v>
@@ -4476,7 +4479,7 @@
         <v>42</v>
       </c>
       <c r="D134" s="8" t="s">
-        <v>419</v>
+        <v>417</v>
       </c>
       <c r="F134" s="6">
         <v>3</v>
@@ -4521,7 +4524,7 @@
         <v>80</v>
       </c>
       <c r="D137" s="8" t="s">
-        <v>364</v>
+        <v>362</v>
       </c>
       <c r="E137" s="9" t="s">
         <v>14</v>
@@ -4530,7 +4533,7 @@
         <v>2</v>
       </c>
       <c r="G137" s="14" t="s">
-        <v>367</v>
+        <v>365</v>
       </c>
     </row>
     <row r="138" spans="1:7" ht="17.149999999999999" x14ac:dyDescent="0.55000000000000004">
@@ -4538,13 +4541,13 @@
         <v>181</v>
       </c>
       <c r="B138" s="6" t="s">
-        <v>329</v>
+        <v>327</v>
       </c>
       <c r="C138" s="7" t="s">
         <v>42</v>
       </c>
       <c r="D138" s="8" t="s">
-        <v>385</v>
+        <v>383</v>
       </c>
       <c r="E138" s="9" t="s">
         <v>183</v>
@@ -4584,7 +4587,7 @@
         <v>80</v>
       </c>
       <c r="D140" s="8" t="s">
-        <v>415</v>
+        <v>413</v>
       </c>
       <c r="E140" s="9" t="s">
         <v>250</v>
@@ -4593,7 +4596,7 @@
         <v>2</v>
       </c>
       <c r="G140" s="14" t="s">
-        <v>416</v>
+        <v>414</v>
       </c>
     </row>
     <row r="141" spans="1:7" ht="17.149999999999999" x14ac:dyDescent="0.55000000000000004">
@@ -4607,13 +4610,13 @@
         <v>42</v>
       </c>
       <c r="D141" s="8" t="s">
-        <v>410</v>
+        <v>408</v>
       </c>
       <c r="F141" s="6">
         <v>3</v>
       </c>
       <c r="G141" s="14" t="s">
-        <v>411</v>
+        <v>409</v>
       </c>
     </row>
     <row r="142" spans="1:7" ht="17.149999999999999" x14ac:dyDescent="0.55000000000000004">
@@ -4627,13 +4630,13 @@
         <v>13</v>
       </c>
       <c r="D142" s="8" t="s">
-        <v>419</v>
+        <v>417</v>
       </c>
       <c r="F142" s="6">
         <v>3</v>
       </c>
       <c r="G142" s="14" t="s">
-        <v>420</v>
+        <v>418</v>
       </c>
     </row>
     <row r="143" spans="1:7" ht="17.149999999999999" x14ac:dyDescent="0.55000000000000004">
@@ -4647,7 +4650,7 @@
         <v>95</v>
       </c>
       <c r="D143" s="8" t="s">
-        <v>383</v>
+        <v>381</v>
       </c>
       <c r="E143" s="9" t="s">
         <v>122</v>
@@ -4667,7 +4670,7 @@
         <v>13</v>
       </c>
       <c r="D144" s="8" t="s">
-        <v>418</v>
+        <v>416</v>
       </c>
       <c r="E144" s="9" t="s">
         <v>22</v>
@@ -4684,7 +4687,7 @@
         <v>13</v>
       </c>
       <c r="D145" s="8" t="s">
-        <v>401</v>
+        <v>399</v>
       </c>
       <c r="E145" s="9" t="s">
         <v>47</v>
@@ -4693,7 +4696,7 @@
         <v>4</v>
       </c>
       <c r="G145" s="14" t="s">
-        <v>402</v>
+        <v>400</v>
       </c>
     </row>
     <row r="146" spans="1:7" ht="17.149999999999999" x14ac:dyDescent="0.55000000000000004">
@@ -4707,7 +4710,7 @@
         <v>13</v>
       </c>
       <c r="D146" s="8" t="s">
-        <v>404</v>
+        <v>402</v>
       </c>
       <c r="E146" s="9" t="s">
         <v>93</v>
@@ -4761,7 +4764,7 @@
         <v>95</v>
       </c>
       <c r="D149" s="8" t="s">
-        <v>415</v>
+        <v>413</v>
       </c>
       <c r="E149" s="9" t="s">
         <v>128</v>
@@ -4770,7 +4773,7 @@
         <v>3</v>
       </c>
       <c r="G149" s="14" t="s">
-        <v>362</v>
+        <v>360</v>
       </c>
     </row>
     <row r="150" spans="1:7" ht="17.149999999999999" x14ac:dyDescent="0.55000000000000004">
@@ -4781,7 +4784,7 @@
         <v>13</v>
       </c>
       <c r="D150" s="8" t="s">
-        <v>393</v>
+        <v>391</v>
       </c>
       <c r="F150" s="6">
         <v>3</v>
@@ -4806,7 +4809,7 @@
         <v>13</v>
       </c>
       <c r="D152" s="8" t="s">
-        <v>396</v>
+        <v>394</v>
       </c>
       <c r="F152" s="6">
         <v>3</v>
@@ -4817,19 +4820,19 @@
         <v>223</v>
       </c>
       <c r="B153" s="6" t="s">
-        <v>359</v>
+        <v>357</v>
       </c>
       <c r="C153" s="7" t="s">
         <v>95</v>
       </c>
       <c r="D153" s="8" t="s">
-        <v>400</v>
+        <v>398</v>
       </c>
       <c r="F153" s="6">
         <v>3</v>
       </c>
       <c r="G153" s="14" t="s">
-        <v>360</v>
+        <v>358</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
2024.12.22 LeetCodeHot100 三刷 Donegit add .!
</commit_message>
<xml_diff>
--- a/2024LeetCode刷题记录.xlsx
+++ b/2024LeetCode刷题记录.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\develop\GithubRepo\LeetCode\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4BC8F11C-E43D-4B43-B66E-88A5EEDDE176}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{686360DF-1549-4359-86DD-60531F5DA86A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-24684" yWindow="5208" windowWidth="16452" windowHeight="8424" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-103" yWindow="-103" windowWidth="22149" windowHeight="11829" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="730" uniqueCount="422">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="738" uniqueCount="425">
   <si>
     <t>题目</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -87,10 +87,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>注意数组压缩后，背包j是倒序遍历</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>1049.最后一块石头的重量II</t>
   </si>
   <si>
@@ -1123,10 +1119,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>2024.09.04</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>不管移动不移动left，最后都要add right</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -1327,10 +1319,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>2024.11.06</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>Hard</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -1559,6 +1547,31 @@
   </si>
   <si>
     <t>有可能不存在</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>模拟、贪心</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>trick</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>注意数组压缩后，背包j是倒序遍历；int[] dp = new int[target+1];</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>原地的话代码会简洁很多</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>718. 最长重复子数组</t>
+  </si>
+  <si>
+    <t>说明了为什么定义[0,i-1]的原因：方便初始化
+根据dp[i][j]的定义，dp[i][0] 和dp[0][j]其实都是没有意义的！
+滚动数组注意内存循环倒序哦</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -1626,7 +1639,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1667,6 +1680,9 @@
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="fill"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="fill" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1734,10 +1750,10 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{E5AA65A4-B8FD-4A83-87AF-D7798D621280}" name="表1" displayName="表1" ref="A1:G1048574" totalsRowShown="0" headerRowDxfId="8" dataDxfId="7">
-  <autoFilter ref="A1:G1048574" xr:uid="{E5AA65A4-B8FD-4A83-87AF-D7798D621280}"/>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:G153">
-    <sortCondition ref="A1:A1048574"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{E5AA65A4-B8FD-4A83-87AF-D7798D621280}" name="表1" displayName="表1" ref="A1:G1048575" totalsRowShown="0" headerRowDxfId="8" dataDxfId="7">
+  <autoFilter ref="A1:G1048575" xr:uid="{E5AA65A4-B8FD-4A83-87AF-D7798D621280}"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:G154">
+    <sortCondition ref="A1:A1048575"/>
   </sortState>
   <tableColumns count="7">
     <tableColumn id="1" xr3:uid="{F13739C5-C0C0-4506-88D9-2DAD4F8FA2E4}" name="题目" dataDxfId="6"/>
@@ -2015,10 +2031,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G153"/>
+  <dimension ref="A1:G154"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="F24" sqref="F24"/>
+    <sheetView tabSelected="1" topLeftCell="A124" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="G138" sqref="G138"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="14.15" x14ac:dyDescent="0.35"/>
@@ -2050,7 +2066,7 @@
         <v>7</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="G1" s="1" t="s">
         <v>10</v>
@@ -2058,50 +2074,50 @@
     </row>
     <row r="2" spans="1:7" ht="17.149999999999999" x14ac:dyDescent="0.55000000000000004">
       <c r="A2" s="10" t="s">
+        <v>77</v>
+      </c>
+      <c r="B2" s="6" t="s">
         <v>78</v>
       </c>
-      <c r="B2" s="6" t="s">
+      <c r="C2" s="7" t="s">
         <v>79</v>
       </c>
-      <c r="C2" s="7" t="s">
+      <c r="D2" s="8" t="s">
+        <v>373</v>
+      </c>
+      <c r="F2" s="6">
+        <v>3</v>
+      </c>
+      <c r="G2" s="14" t="s">
         <v>80</v>
-      </c>
-      <c r="D2" s="8" t="s">
-        <v>376</v>
-      </c>
-      <c r="F2" s="6">
-        <v>3</v>
-      </c>
-      <c r="G2" s="14" t="s">
-        <v>81</v>
       </c>
     </row>
     <row r="3" spans="1:7" ht="17.149999999999999" x14ac:dyDescent="0.55000000000000004">
       <c r="A3" s="10" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="C3" s="7" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="D3" s="8" t="s">
-        <v>391</v>
+        <v>388</v>
       </c>
       <c r="F3" s="6">
         <v>3</v>
       </c>
       <c r="G3" s="14" t="s">
-        <v>392</v>
+        <v>389</v>
       </c>
     </row>
     <row r="4" spans="1:7" ht="17.149999999999999" x14ac:dyDescent="0.55000000000000004">
       <c r="A4" s="10" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="C4" s="7" t="s">
         <v>13</v>
       </c>
       <c r="D4" s="8" t="s">
-        <v>394</v>
+        <v>391</v>
       </c>
       <c r="F4" s="6">
         <v>3</v>
@@ -2109,27 +2125,27 @@
     </row>
     <row r="5" spans="1:7" ht="17.149999999999999" x14ac:dyDescent="0.55000000000000004">
       <c r="A5" s="10" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="B5" s="6" t="s">
-        <v>349</v>
+        <v>347</v>
       </c>
       <c r="C5" s="7" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="D5" s="8" t="s">
-        <v>391</v>
+        <v>388</v>
       </c>
       <c r="F5" s="6">
         <v>3</v>
       </c>
       <c r="G5" s="14" t="s">
-        <v>392</v>
+        <v>389</v>
       </c>
     </row>
     <row r="6" spans="1:7" ht="17.149999999999999" x14ac:dyDescent="0.55000000000000004">
       <c r="A6" s="4" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B6" s="6" t="s">
         <v>12</v>
@@ -2138,7 +2154,7 @@
         <v>13</v>
       </c>
       <c r="D6" s="8" t="s">
-        <v>311</v>
+        <v>309</v>
       </c>
       <c r="E6" s="9" t="s">
         <v>14</v>
@@ -2147,18 +2163,18 @@
         <v>2</v>
       </c>
       <c r="G6" s="14" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="7" spans="1:7" ht="17.149999999999999" x14ac:dyDescent="0.55000000000000004">
       <c r="A7" s="10" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="C7" s="7" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="D7" s="8" t="s">
-        <v>396</v>
+        <v>393</v>
       </c>
       <c r="F7" s="6">
         <v>3</v>
@@ -2166,24 +2182,24 @@
     </row>
     <row r="8" spans="1:7" ht="17.149999999999999" x14ac:dyDescent="0.55000000000000004">
       <c r="A8" s="10" t="s">
-        <v>370</v>
+        <v>367</v>
       </c>
       <c r="C8" s="7" t="s">
         <v>13</v>
       </c>
       <c r="D8" s="8" t="s">
-        <v>367</v>
+        <v>364</v>
       </c>
     </row>
     <row r="9" spans="1:7" ht="17.149999999999999" x14ac:dyDescent="0.55000000000000004">
       <c r="A9" s="10" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="C9" s="7" t="s">
         <v>13</v>
       </c>
       <c r="D9" s="8" t="s">
-        <v>394</v>
+        <v>391</v>
       </c>
       <c r="F9" s="6">
         <v>3</v>
@@ -2191,99 +2207,99 @@
     </row>
     <row r="10" spans="1:7" ht="17.149999999999999" x14ac:dyDescent="0.55000000000000004">
       <c r="A10" s="10" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="B10" s="6" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="C10" s="7" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="D10" s="8" t="s">
-        <v>378</v>
+        <v>375</v>
       </c>
       <c r="E10" s="9" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="F10" s="6">
         <v>4</v>
       </c>
       <c r="G10" s="14" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
     </row>
     <row r="11" spans="1:7" ht="17.149999999999999" x14ac:dyDescent="0.55000000000000004">
       <c r="A11" s="10" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="C11" s="7" t="s">
         <v>13</v>
       </c>
       <c r="D11" s="8" t="s">
-        <v>394</v>
+        <v>391</v>
       </c>
       <c r="F11" s="6">
         <v>3</v>
       </c>
       <c r="G11" s="14" t="s">
-        <v>351</v>
+        <v>349</v>
       </c>
     </row>
     <row r="12" spans="1:7" ht="17.149999999999999" x14ac:dyDescent="0.55000000000000004">
       <c r="A12" s="10" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="B12" s="6" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="C12" s="7" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="D12" s="8" t="s">
-        <v>362</v>
+        <v>417</v>
       </c>
       <c r="E12" s="9" t="s">
         <v>14</v>
       </c>
       <c r="F12" s="6">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="G12" s="14" t="s">
-        <v>364</v>
+        <v>361</v>
       </c>
     </row>
     <row r="13" spans="1:7" ht="17.149999999999999" x14ac:dyDescent="0.55000000000000004">
       <c r="A13" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="B13" s="6" t="s">
         <v>19</v>
-      </c>
-      <c r="B13" s="6" t="s">
-        <v>20</v>
       </c>
       <c r="C13" s="7" t="s">
         <v>6</v>
       </c>
       <c r="D13" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="E13" s="9" t="s">
         <v>21</v>
       </c>
-      <c r="E13" s="9" t="s">
+      <c r="G13" s="14" t="s">
         <v>22</v>
-      </c>
-      <c r="G13" s="14" t="s">
-        <v>23</v>
       </c>
     </row>
     <row r="14" spans="1:7" ht="17.149999999999999" x14ac:dyDescent="0.55000000000000004">
       <c r="A14" s="10" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="B14" s="6" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="C14" s="7" t="s">
         <v>6</v>
       </c>
       <c r="D14" s="8" t="s">
-        <v>361</v>
+        <v>359</v>
       </c>
       <c r="F14" s="6">
         <v>2</v>
@@ -2311,16 +2327,16 @@
     </row>
     <row r="16" spans="1:7" ht="17.149999999999999" x14ac:dyDescent="0.55000000000000004">
       <c r="A16" s="10" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="B16" s="6" t="s">
-        <v>323</v>
+        <v>321</v>
       </c>
       <c r="C16" s="7" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="D16" s="8" t="s">
-        <v>416</v>
+        <v>413</v>
       </c>
       <c r="E16" s="9" t="s">
         <v>14</v>
@@ -2331,16 +2347,16 @@
     </row>
     <row r="17" spans="1:7" ht="17.149999999999999" x14ac:dyDescent="0.55000000000000004">
       <c r="A17" s="10" t="s">
+        <v>342</v>
+      </c>
+      <c r="B17" s="6" t="s">
         <v>344</v>
-      </c>
-      <c r="B17" s="6" t="s">
-        <v>346</v>
       </c>
       <c r="C17" s="7" t="s">
         <v>13</v>
       </c>
       <c r="D17" s="8" t="s">
-        <v>345</v>
+        <v>343</v>
       </c>
       <c r="E17" s="9" t="s">
         <v>14</v>
@@ -2348,13 +2364,13 @@
     </row>
     <row r="18" spans="1:7" ht="17.149999999999999" x14ac:dyDescent="0.55000000000000004">
       <c r="A18" s="10" t="s">
-        <v>347</v>
+        <v>345</v>
       </c>
       <c r="C18" s="7" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="D18" s="8" t="s">
-        <v>348</v>
+        <v>346</v>
       </c>
       <c r="E18" s="9" t="s">
         <v>14</v>
@@ -2362,36 +2378,36 @@
     </row>
     <row r="19" spans="1:7" ht="17.149999999999999" x14ac:dyDescent="0.55000000000000004">
       <c r="A19" s="10" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="B19" s="6" t="s">
-        <v>356</v>
+        <v>354</v>
       </c>
       <c r="C19" s="7" t="s">
         <v>13</v>
       </c>
       <c r="D19" s="8" t="s">
-        <v>398</v>
+        <v>395</v>
       </c>
       <c r="F19" s="6">
         <v>3</v>
       </c>
       <c r="G19" s="14" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
     </row>
     <row r="20" spans="1:7" ht="17.149999999999999" x14ac:dyDescent="0.55000000000000004">
       <c r="A20" s="10" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="B20" s="6" t="s">
+        <v>78</v>
+      </c>
+      <c r="C20" s="7" t="s">
         <v>79</v>
       </c>
-      <c r="C20" s="7" t="s">
-        <v>80</v>
-      </c>
       <c r="D20" s="8" t="s">
-        <v>376</v>
+        <v>373</v>
       </c>
       <c r="F20" s="6">
         <v>3</v>
@@ -2399,39 +2415,39 @@
     </row>
     <row r="21" spans="1:7" ht="17.149999999999999" x14ac:dyDescent="0.55000000000000004">
       <c r="A21" s="10" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="B21" s="6" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="C21" s="7" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="D21" s="8" t="s">
-        <v>402</v>
+        <v>399</v>
       </c>
       <c r="E21" s="9" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="F21" s="6">
         <v>3</v>
       </c>
       <c r="G21" s="14" t="s">
-        <v>404</v>
+        <v>401</v>
       </c>
     </row>
     <row r="22" spans="1:7" ht="17.149999999999999" x14ac:dyDescent="0.55000000000000004">
       <c r="A22" s="10" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="B22" s="6" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="C22" s="7" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D22" s="8" t="s">
-        <v>417</v>
+        <v>414</v>
       </c>
       <c r="F22" s="6">
         <v>3</v>
@@ -2439,19 +2455,19 @@
     </row>
     <row r="23" spans="1:7" ht="17.149999999999999" x14ac:dyDescent="0.55000000000000004">
       <c r="A23" s="10" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="B23" s="6" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C23" s="7" t="s">
         <v>13</v>
       </c>
       <c r="D23" s="8" t="s">
-        <v>386</v>
+        <v>383</v>
       </c>
       <c r="E23" s="9" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="F23" s="6">
         <v>3</v>
@@ -2459,16 +2475,16 @@
     </row>
     <row r="24" spans="1:7" ht="17.149999999999999" x14ac:dyDescent="0.55000000000000004">
       <c r="A24" s="10" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="B24" s="6" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="C24" s="7" t="s">
         <v>13</v>
       </c>
       <c r="D24" s="8" t="s">
-        <v>420</v>
+        <v>417</v>
       </c>
       <c r="E24" s="9" t="s">
         <v>14</v>
@@ -2479,16 +2495,16 @@
     </row>
     <row r="25" spans="1:7" ht="17.149999999999999" x14ac:dyDescent="0.55000000000000004">
       <c r="A25" s="10" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="B25" s="6" t="s">
-        <v>339</v>
+        <v>337</v>
       </c>
       <c r="C25" s="7" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="D25" s="8" t="s">
-        <v>384</v>
+        <v>381</v>
       </c>
       <c r="F25" s="6">
         <v>3</v>
@@ -2496,53 +2512,53 @@
     </row>
     <row r="26" spans="1:7" ht="17.149999999999999" x14ac:dyDescent="0.55000000000000004">
       <c r="A26" s="10" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="C26" s="7" t="s">
         <v>13</v>
       </c>
       <c r="D26" s="8" t="s">
-        <v>384</v>
+        <v>381</v>
       </c>
       <c r="E26" s="13" t="s">
-        <v>340</v>
+        <v>338</v>
       </c>
       <c r="F26" s="6">
         <v>3</v>
       </c>
       <c r="G26" s="14" t="s">
-        <v>385</v>
+        <v>382</v>
       </c>
     </row>
     <row r="27" spans="1:7" ht="17.149999999999999" x14ac:dyDescent="0.55000000000000004">
       <c r="A27" s="10" t="s">
-        <v>371</v>
+        <v>368</v>
       </c>
       <c r="C27" s="7" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="D27" s="8" t="s">
-        <v>367</v>
+        <v>364</v>
       </c>
       <c r="E27" s="9" t="s">
-        <v>372</v>
+        <v>369</v>
       </c>
       <c r="G27" s="14" t="s">
-        <v>373</v>
+        <v>370</v>
       </c>
     </row>
     <row r="28" spans="1:7" ht="17.149999999999999" x14ac:dyDescent="0.55000000000000004">
       <c r="A28" s="10" t="s">
+        <v>297</v>
+      </c>
+      <c r="B28" s="6" t="s">
         <v>298</v>
       </c>
-      <c r="B28" s="6" t="s">
+      <c r="C28" s="7" t="s">
+        <v>41</v>
+      </c>
+      <c r="D28" s="8" t="s">
         <v>299</v>
-      </c>
-      <c r="C28" s="7" t="s">
-        <v>42</v>
-      </c>
-      <c r="D28" s="8" t="s">
-        <v>300</v>
       </c>
       <c r="F28" s="6">
         <v>2</v>
@@ -2550,116 +2566,119 @@
     </row>
     <row r="29" spans="1:7" ht="17.149999999999999" x14ac:dyDescent="0.55000000000000004">
       <c r="A29" s="10" t="s">
+        <v>203</v>
+      </c>
+      <c r="C29" s="7" t="s">
+        <v>94</v>
+      </c>
+      <c r="D29" s="8" t="s">
+        <v>387</v>
+      </c>
+      <c r="F29" s="6">
+        <v>3</v>
+      </c>
+      <c r="G29" s="14" t="s">
         <v>204</v>
-      </c>
-      <c r="C29" s="7" t="s">
-        <v>95</v>
-      </c>
-      <c r="D29" s="8" t="s">
-        <v>390</v>
-      </c>
-      <c r="F29" s="6">
-        <v>3</v>
-      </c>
-      <c r="G29" s="14" t="s">
-        <v>205</v>
       </c>
     </row>
     <row r="30" spans="1:7" ht="17.149999999999999" x14ac:dyDescent="0.55000000000000004">
       <c r="A30" s="10" t="s">
+        <v>200</v>
+      </c>
+      <c r="B30" s="6" t="s">
         <v>201</v>
       </c>
-      <c r="B30" s="6" t="s">
-        <v>202</v>
-      </c>
       <c r="C30" s="7" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="D30" s="8" t="s">
+        <v>383</v>
+      </c>
+      <c r="F30" s="6">
+        <v>3</v>
+      </c>
+      <c r="G30" s="14" t="s">
         <v>386</v>
-      </c>
-      <c r="F30" s="6">
-        <v>3</v>
-      </c>
-      <c r="G30" s="14" t="s">
-        <v>389</v>
       </c>
     </row>
     <row r="31" spans="1:7" ht="17.149999999999999" x14ac:dyDescent="0.55000000000000004">
       <c r="A31" s="10" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B31" s="6" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="C31" s="7" t="s">
         <v>13</v>
       </c>
       <c r="D31" s="8" t="s">
-        <v>378</v>
+        <v>375</v>
       </c>
       <c r="E31" s="9" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="F31" s="6">
         <v>3</v>
       </c>
       <c r="G31" s="14" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
     </row>
     <row r="32" spans="1:7" ht="17.149999999999999" x14ac:dyDescent="0.55000000000000004">
       <c r="A32" s="10" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="B32" s="6" t="s">
-        <v>187</v>
+        <v>419</v>
       </c>
       <c r="C32" s="7" t="s">
         <v>6</v>
       </c>
       <c r="D32" s="8" t="s">
-        <v>361</v>
+        <v>417</v>
       </c>
       <c r="F32" s="6">
-        <v>2</v>
+        <v>3</v>
+      </c>
+      <c r="G32" s="14" t="s">
+        <v>420</v>
       </c>
     </row>
     <row r="33" spans="1:7" ht="17.149999999999999" x14ac:dyDescent="0.55000000000000004">
       <c r="A33" s="10" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="B33" s="6" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="C33" s="7" t="s">
         <v>13</v>
       </c>
       <c r="D33" s="8" t="s">
-        <v>411</v>
+        <v>408</v>
       </c>
       <c r="F33" s="6">
         <v>3</v>
       </c>
       <c r="G33" s="14" t="s">
-        <v>359</v>
+        <v>357</v>
       </c>
     </row>
     <row r="34" spans="1:7" ht="17.149999999999999" x14ac:dyDescent="0.55000000000000004">
       <c r="A34" s="10" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="B34" s="6" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C34" s="7" t="s">
         <v>13</v>
       </c>
       <c r="D34" s="8" t="s">
-        <v>413</v>
+        <v>410</v>
       </c>
       <c r="E34" s="9" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="F34" s="6">
         <v>3</v>
@@ -2667,81 +2686,81 @@
     </row>
     <row r="35" spans="1:7" ht="17.149999999999999" x14ac:dyDescent="0.55000000000000004">
       <c r="A35" s="10" t="s">
+        <v>103</v>
+      </c>
+      <c r="B35" s="6" t="s">
+        <v>105</v>
+      </c>
+      <c r="C35" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="D35" s="8" t="s">
+        <v>100</v>
+      </c>
+      <c r="E35" s="9" t="s">
         <v>104</v>
-      </c>
-      <c r="B35" s="6" t="s">
-        <v>106</v>
-      </c>
-      <c r="C35" s="7" t="s">
-        <v>28</v>
-      </c>
-      <c r="D35" s="8" t="s">
-        <v>101</v>
-      </c>
-      <c r="E35" s="9" t="s">
-        <v>105</v>
       </c>
     </row>
     <row r="36" spans="1:7" ht="17.149999999999999" x14ac:dyDescent="0.55000000000000004">
       <c r="A36" s="10" t="s">
+        <v>23</v>
+      </c>
+      <c r="B36" s="6" t="s">
         <v>24</v>
       </c>
-      <c r="B36" s="6" t="s">
+      <c r="C36" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="D36" s="8" t="s">
         <v>25</v>
       </c>
-      <c r="C36" s="7" t="s">
-        <v>28</v>
-      </c>
-      <c r="D36" s="8" t="s">
+      <c r="E36" s="9" t="s">
         <v>26</v>
-      </c>
-      <c r="E36" s="9" t="s">
-        <v>27</v>
       </c>
     </row>
     <row r="37" spans="1:7" ht="17.149999999999999" x14ac:dyDescent="0.55000000000000004">
       <c r="A37" s="10" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="C37" s="7" t="s">
         <v>6</v>
       </c>
       <c r="D37" s="8" t="s">
-        <v>384</v>
+        <v>381</v>
       </c>
       <c r="E37" s="13" t="s">
-        <v>336</v>
+        <v>334</v>
       </c>
       <c r="F37" s="6">
         <v>3</v>
       </c>
       <c r="G37" s="14" t="s">
-        <v>335</v>
+        <v>333</v>
       </c>
     </row>
     <row r="38" spans="1:7" ht="17.149999999999999" x14ac:dyDescent="0.55000000000000004">
       <c r="A38" s="10" t="s">
-        <v>374</v>
+        <v>371</v>
       </c>
       <c r="C38" s="7" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="D38" s="8" t="s">
-        <v>375</v>
+        <v>372</v>
       </c>
     </row>
     <row r="39" spans="1:7" ht="17.149999999999999" x14ac:dyDescent="0.55000000000000004">
       <c r="A39" s="10" t="s">
+        <v>264</v>
+      </c>
+      <c r="B39" s="6" t="s">
         <v>265</v>
-      </c>
-      <c r="B39" s="6" t="s">
-        <v>266</v>
       </c>
       <c r="C39" s="7" t="s">
         <v>13</v>
       </c>
       <c r="D39" s="8" t="s">
-        <v>417</v>
+        <v>414</v>
       </c>
       <c r="F39" s="6">
         <v>3</v>
@@ -2749,19 +2768,19 @@
     </row>
     <row r="40" spans="1:7" ht="17.149999999999999" x14ac:dyDescent="0.55000000000000004">
       <c r="A40" s="10" t="s">
+        <v>228</v>
+      </c>
+      <c r="B40" s="6" t="s">
         <v>229</v>
       </c>
-      <c r="B40" s="6" t="s">
-        <v>230</v>
-      </c>
       <c r="C40" s="7" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="D40" s="8" t="s">
-        <v>399</v>
+        <v>396</v>
       </c>
       <c r="E40" s="9" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="F40" s="6">
         <v>3</v>
@@ -2769,13 +2788,13 @@
     </row>
     <row r="41" spans="1:7" ht="17.149999999999999" x14ac:dyDescent="0.55000000000000004">
       <c r="A41" s="4" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="C41" s="7" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D41" s="8" t="s">
-        <v>382</v>
+        <v>379</v>
       </c>
       <c r="F41" s="6">
         <v>3</v>
@@ -2783,67 +2802,67 @@
     </row>
     <row r="42" spans="1:7" ht="17.149999999999999" x14ac:dyDescent="0.55000000000000004">
       <c r="A42" s="10" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="C42" s="7" t="s">
         <v>13</v>
       </c>
       <c r="D42" s="8" t="s">
-        <v>386</v>
+        <v>383</v>
       </c>
       <c r="F42" s="6">
         <v>3</v>
       </c>
       <c r="G42" s="14" t="s">
-        <v>342</v>
+        <v>340</v>
       </c>
     </row>
     <row r="43" spans="1:7" ht="17.149999999999999" x14ac:dyDescent="0.55000000000000004">
       <c r="A43" s="10" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="B43" s="6" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="C43" s="7" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="D43" s="8" t="s">
-        <v>417</v>
+        <v>414</v>
       </c>
       <c r="F43" s="6">
         <v>3</v>
       </c>
       <c r="G43" s="14" t="s">
-        <v>419</v>
+        <v>416</v>
       </c>
     </row>
     <row r="44" spans="1:7" ht="17.149999999999999" x14ac:dyDescent="0.55000000000000004">
       <c r="A44" s="10" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="C44" s="7" t="s">
         <v>13</v>
       </c>
       <c r="D44" s="8" t="s">
-        <v>394</v>
+        <v>391</v>
       </c>
       <c r="F44" s="6">
         <v>3</v>
       </c>
       <c r="G44" s="14" t="s">
-        <v>350</v>
+        <v>348</v>
       </c>
     </row>
     <row r="45" spans="1:7" ht="17.149999999999999" x14ac:dyDescent="0.55000000000000004">
       <c r="A45" s="10" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="C45" s="7" t="s">
         <v>6</v>
       </c>
       <c r="D45" s="8" t="s">
-        <v>386</v>
+        <v>383</v>
       </c>
       <c r="F45" s="6">
         <v>3</v>
@@ -2851,16 +2870,16 @@
     </row>
     <row r="46" spans="1:7" ht="17.149999999999999" x14ac:dyDescent="0.55000000000000004">
       <c r="A46" s="10" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="B46" s="6" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C46" s="7" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="D46" s="8" t="s">
-        <v>413</v>
+        <v>410</v>
       </c>
       <c r="F46" s="6">
         <v>3</v>
@@ -2868,30 +2887,30 @@
     </row>
     <row r="47" spans="1:7" ht="17.149999999999999" x14ac:dyDescent="0.55000000000000004">
       <c r="A47" s="10" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="C47" s="7" t="s">
         <v>13</v>
       </c>
       <c r="D47" s="8" t="s">
-        <v>398</v>
+        <v>395</v>
       </c>
       <c r="F47" s="6">
         <v>3</v>
       </c>
       <c r="G47" s="14" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
     </row>
     <row r="48" spans="1:7" ht="17.149999999999999" x14ac:dyDescent="0.55000000000000004">
       <c r="A48" s="10" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="C48" s="7" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="D48" s="8" t="s">
-        <v>384</v>
+        <v>381</v>
       </c>
       <c r="F48" s="6">
         <v>3</v>
@@ -2899,13 +2918,13 @@
     </row>
     <row r="49" spans="1:7" ht="17.149999999999999" x14ac:dyDescent="0.55000000000000004">
       <c r="A49" s="10" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="C49" s="7" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="D49" s="8" t="s">
-        <v>399</v>
+        <v>396</v>
       </c>
       <c r="F49" s="6">
         <v>3</v>
@@ -2913,13 +2932,13 @@
     </row>
     <row r="50" spans="1:7" ht="17.149999999999999" x14ac:dyDescent="0.55000000000000004">
       <c r="A50" s="10" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="C50" s="7" t="s">
         <v>13</v>
       </c>
       <c r="D50" s="8" t="s">
-        <v>399</v>
+        <v>396</v>
       </c>
       <c r="F50" s="6">
         <v>3</v>
@@ -2927,53 +2946,53 @@
     </row>
     <row r="51" spans="1:7" ht="17.149999999999999" x14ac:dyDescent="0.55000000000000004">
       <c r="A51" s="10" t="s">
+        <v>66</v>
+      </c>
+      <c r="B51" s="6" t="s">
         <v>67</v>
       </c>
-      <c r="B51" s="6" t="s">
+      <c r="C51" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="D51" s="8" t="s">
         <v>68</v>
       </c>
-      <c r="C51" s="7" t="s">
-        <v>28</v>
-      </c>
-      <c r="D51" s="8" t="s">
+      <c r="E51" s="9" t="s">
         <v>69</v>
       </c>
-      <c r="E51" s="9" t="s">
+      <c r="G51" s="14" t="s">
         <v>70</v>
-      </c>
-      <c r="G51" s="14" t="s">
-        <v>71</v>
       </c>
     </row>
     <row r="52" spans="1:7" ht="17.149999999999999" x14ac:dyDescent="0.55000000000000004">
       <c r="A52" s="11" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="C52" s="7" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="D52" s="8" t="s">
-        <v>386</v>
+        <v>383</v>
       </c>
       <c r="F52" s="6">
         <v>3</v>
       </c>
       <c r="G52" s="14" t="s">
-        <v>341</v>
+        <v>339</v>
       </c>
     </row>
     <row r="53" spans="1:7" ht="17.149999999999999" x14ac:dyDescent="0.55000000000000004">
       <c r="A53" s="10" t="s">
+        <v>329</v>
+      </c>
+      <c r="B53" s="6" t="s">
         <v>331</v>
-      </c>
-      <c r="B53" s="6" t="s">
-        <v>333</v>
       </c>
       <c r="C53" s="7" t="s">
         <v>13</v>
       </c>
       <c r="D53" s="8" t="s">
-        <v>332</v>
+        <v>330</v>
       </c>
       <c r="E53" s="9" t="s">
         <v>14</v>
@@ -2981,16 +3000,16 @@
     </row>
     <row r="54" spans="1:7" ht="17.149999999999999" x14ac:dyDescent="0.55000000000000004">
       <c r="A54" s="10" t="s">
+        <v>252</v>
+      </c>
+      <c r="B54" s="6" t="s">
         <v>253</v>
-      </c>
-      <c r="B54" s="6" t="s">
-        <v>254</v>
       </c>
       <c r="C54" s="7" t="s">
         <v>13</v>
       </c>
       <c r="D54" s="8" t="s">
-        <v>415</v>
+        <v>412</v>
       </c>
       <c r="F54" s="6">
         <v>4</v>
@@ -2998,59 +3017,59 @@
     </row>
     <row r="55" spans="1:7" ht="17.149999999999999" x14ac:dyDescent="0.55000000000000004">
       <c r="A55" s="10" t="s">
+        <v>132</v>
+      </c>
+      <c r="B55" s="6" t="s">
+        <v>134</v>
+      </c>
+      <c r="C55" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="D55" s="8" t="s">
+        <v>135</v>
+      </c>
+      <c r="E55" s="9" t="s">
         <v>133</v>
       </c>
-      <c r="B55" s="6" t="s">
-        <v>135</v>
-      </c>
-      <c r="C55" s="7" t="s">
-        <v>28</v>
-      </c>
-      <c r="D55" s="8" t="s">
-        <v>136</v>
-      </c>
-      <c r="E55" s="9" t="s">
-        <v>134</v>
-      </c>
       <c r="G55" s="14" t="s">
-        <v>330</v>
+        <v>328</v>
       </c>
     </row>
     <row r="56" spans="1:7" ht="17.149999999999999" x14ac:dyDescent="0.55000000000000004">
       <c r="A56" s="10" t="s">
+        <v>71</v>
+      </c>
+      <c r="B56" s="6" t="s">
         <v>72</v>
       </c>
-      <c r="B56" s="6" t="s">
+      <c r="C56" s="7" t="s">
+        <v>75</v>
+      </c>
+      <c r="D56" s="8" t="s">
         <v>73</v>
       </c>
-      <c r="C56" s="7" t="s">
+      <c r="E56" s="9" t="s">
+        <v>74</v>
+      </c>
+      <c r="G56" s="14" t="s">
         <v>76</v>
-      </c>
-      <c r="D56" s="8" t="s">
-        <v>74</v>
-      </c>
-      <c r="E56" s="9" t="s">
-        <v>75</v>
-      </c>
-      <c r="G56" s="14" t="s">
-        <v>77</v>
       </c>
     </row>
     <row r="57" spans="1:7" ht="17.149999999999999" x14ac:dyDescent="0.55000000000000004">
       <c r="A57" s="10" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="B57" s="6" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="C57" s="7" t="s">
         <v>13</v>
       </c>
       <c r="D57" s="8" t="s">
-        <v>402</v>
+        <v>399</v>
       </c>
       <c r="E57" s="9" t="s">
-        <v>403</v>
+        <v>400</v>
       </c>
       <c r="F57" s="6">
         <v>3</v>
@@ -3058,33 +3077,33 @@
     </row>
     <row r="58" spans="1:7" ht="17.149999999999999" x14ac:dyDescent="0.55000000000000004">
       <c r="A58" s="10" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="C58" s="7" t="s">
         <v>13</v>
       </c>
       <c r="D58" s="8" t="s">
-        <v>391</v>
+        <v>388</v>
       </c>
       <c r="F58" s="6">
         <v>3</v>
       </c>
       <c r="G58" s="14" t="s">
-        <v>392</v>
+        <v>389</v>
       </c>
     </row>
     <row r="59" spans="1:7" ht="17.149999999999999" x14ac:dyDescent="0.55000000000000004">
       <c r="A59" s="10" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="B59" s="6" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="C59" s="7" t="s">
         <v>13</v>
       </c>
       <c r="D59" s="8" t="s">
-        <v>390</v>
+        <v>387</v>
       </c>
       <c r="F59" s="6">
         <v>3</v>
@@ -3092,30 +3111,30 @@
     </row>
     <row r="60" spans="1:7" ht="17.149999999999999" x14ac:dyDescent="0.55000000000000004">
       <c r="A60" s="10" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="C60" s="7" t="s">
         <v>13</v>
       </c>
       <c r="D60" s="8" t="s">
-        <v>394</v>
+        <v>391</v>
       </c>
       <c r="F60" s="6">
         <v>3</v>
       </c>
       <c r="G60" s="14" t="s">
-        <v>395</v>
+        <v>392</v>
       </c>
     </row>
     <row r="61" spans="1:7" ht="17.149999999999999" x14ac:dyDescent="0.55000000000000004">
       <c r="A61" s="10" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="C61" s="7" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="D61" s="8" t="s">
-        <v>384</v>
+        <v>381</v>
       </c>
       <c r="F61" s="6">
         <v>3</v>
@@ -3123,39 +3142,39 @@
     </row>
     <row r="62" spans="1:7" ht="17.149999999999999" x14ac:dyDescent="0.55000000000000004">
       <c r="A62" s="10" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="B62" s="6" t="s">
-        <v>354</v>
+        <v>352</v>
       </c>
       <c r="C62" s="7" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="D62" s="8" t="s">
-        <v>397</v>
+        <v>394</v>
       </c>
       <c r="E62" s="9" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="F62" s="6">
         <v>3</v>
       </c>
       <c r="G62" s="14" t="s">
-        <v>355</v>
+        <v>353</v>
       </c>
     </row>
     <row r="63" spans="1:7" ht="17.149999999999999" x14ac:dyDescent="0.55000000000000004">
       <c r="A63" s="10" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="B63" s="6" t="s">
-        <v>324</v>
+        <v>322</v>
       </c>
       <c r="C63" s="7" t="s">
         <v>6</v>
       </c>
       <c r="D63" s="8" t="s">
-        <v>382</v>
+        <v>379</v>
       </c>
       <c r="F63" s="6">
         <v>3</v>
@@ -3163,19 +3182,19 @@
     </row>
     <row r="64" spans="1:7" ht="17.149999999999999" x14ac:dyDescent="0.55000000000000004">
       <c r="A64" s="10" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="B64" s="6" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="C64" s="7" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="D64" s="8" t="s">
-        <v>381</v>
+        <v>378</v>
       </c>
       <c r="E64" s="9" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="F64" s="6">
         <v>4</v>
@@ -3183,255 +3202,255 @@
     </row>
     <row r="65" spans="1:7" ht="17.149999999999999" x14ac:dyDescent="0.55000000000000004">
       <c r="A65" s="10" t="s">
+        <v>38</v>
+      </c>
+      <c r="B65" s="6" t="s">
+        <v>40</v>
+      </c>
+      <c r="C65" s="7" t="s">
+        <v>41</v>
+      </c>
+      <c r="D65" s="8" t="s">
+        <v>37</v>
+      </c>
+      <c r="E65" s="9" t="s">
+        <v>21</v>
+      </c>
+      <c r="G65" s="14" t="s">
         <v>39</v>
-      </c>
-      <c r="B65" s="6" t="s">
-        <v>41</v>
-      </c>
-      <c r="C65" s="7" t="s">
-        <v>42</v>
-      </c>
-      <c r="D65" s="8" t="s">
-        <v>38</v>
-      </c>
-      <c r="E65" s="9" t="s">
-        <v>22</v>
-      </c>
-      <c r="G65" s="14" t="s">
-        <v>40</v>
       </c>
     </row>
     <row r="66" spans="1:7" ht="17.149999999999999" x14ac:dyDescent="0.55000000000000004">
       <c r="A66" s="10" t="s">
-        <v>343</v>
+        <v>341</v>
       </c>
       <c r="C66" s="7" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="D66" s="8" t="s">
-        <v>386</v>
+        <v>383</v>
       </c>
       <c r="F66" s="6">
         <v>3</v>
       </c>
       <c r="G66" s="14" t="s">
-        <v>388</v>
+        <v>385</v>
       </c>
     </row>
     <row r="67" spans="1:7" ht="17.149999999999999" x14ac:dyDescent="0.55000000000000004">
       <c r="A67" s="10" t="s">
+        <v>187</v>
+      </c>
+      <c r="B67" s="6" t="s">
+        <v>189</v>
+      </c>
+      <c r="C67" s="7" t="s">
+        <v>41</v>
+      </c>
+      <c r="D67" s="8" t="s">
+        <v>380</v>
+      </c>
+      <c r="E67" s="9" t="s">
+        <v>92</v>
+      </c>
+      <c r="F67" s="6">
+        <v>3</v>
+      </c>
+      <c r="G67" s="14" t="s">
         <v>188</v>
-      </c>
-      <c r="B67" s="6" t="s">
-        <v>190</v>
-      </c>
-      <c r="C67" s="7" t="s">
-        <v>42</v>
-      </c>
-      <c r="D67" s="8" t="s">
-        <v>383</v>
-      </c>
-      <c r="E67" s="9" t="s">
-        <v>93</v>
-      </c>
-      <c r="F67" s="6">
-        <v>3</v>
-      </c>
-      <c r="G67" s="14" t="s">
-        <v>189</v>
       </c>
     </row>
     <row r="68" spans="1:7" ht="17.149999999999999" x14ac:dyDescent="0.55000000000000004">
       <c r="A68" s="10" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B68" s="6" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C68" s="7" t="s">
         <v>6</v>
       </c>
       <c r="D68" s="8" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="E68" s="9" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="G68" s="14" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="69" spans="1:7" ht="17.149999999999999" x14ac:dyDescent="0.55000000000000004">
       <c r="A69" s="10" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="B69" s="6" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="C69" s="7" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="D69" s="8" t="s">
-        <v>386</v>
+        <v>383</v>
       </c>
       <c r="F69" s="6">
         <v>4</v>
       </c>
       <c r="G69" s="14" t="s">
-        <v>387</v>
+        <v>384</v>
       </c>
     </row>
     <row r="70" spans="1:7" ht="17.149999999999999" x14ac:dyDescent="0.55000000000000004">
       <c r="A70" s="10" t="s">
+        <v>61</v>
+      </c>
+      <c r="B70" s="6" t="s">
         <v>62</v>
       </c>
-      <c r="B70" s="6" t="s">
+      <c r="C70" s="7" t="s">
+        <v>41</v>
+      </c>
+      <c r="D70" s="8" t="s">
         <v>63</v>
       </c>
-      <c r="C70" s="7" t="s">
-        <v>42</v>
-      </c>
-      <c r="D70" s="8" t="s">
+      <c r="E70" s="9" t="s">
         <v>64</v>
       </c>
-      <c r="E70" s="9" t="s">
+      <c r="G70" s="14" t="s">
         <v>65</v>
-      </c>
-      <c r="G70" s="14" t="s">
-        <v>66</v>
       </c>
     </row>
     <row r="71" spans="1:7" ht="17.149999999999999" x14ac:dyDescent="0.55000000000000004">
       <c r="A71" s="10" t="s">
+        <v>57</v>
+      </c>
+      <c r="B71" s="6" t="s">
         <v>58</v>
       </c>
-      <c r="B71" s="6" t="s">
+      <c r="C71" s="7" t="s">
+        <v>41</v>
+      </c>
+      <c r="D71" s="8" t="s">
         <v>59</v>
       </c>
-      <c r="C71" s="7" t="s">
-        <v>42</v>
-      </c>
-      <c r="D71" s="8" t="s">
+      <c r="E71" s="9" t="s">
         <v>60</v>
-      </c>
-      <c r="E71" s="9" t="s">
-        <v>61</v>
       </c>
     </row>
     <row r="72" spans="1:7" ht="17.149999999999999" x14ac:dyDescent="0.55000000000000004">
       <c r="A72" s="10" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="C72" s="7" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="D72" s="8" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
     </row>
     <row r="73" spans="1:7" ht="17.149999999999999" x14ac:dyDescent="0.55000000000000004">
       <c r="A73" s="10" t="s">
+        <v>54</v>
+      </c>
+      <c r="B73" s="6" t="s">
+        <v>56</v>
+      </c>
+      <c r="C73" s="7" t="s">
+        <v>41</v>
+      </c>
+      <c r="D73" s="8" t="s">
         <v>55</v>
       </c>
-      <c r="B73" s="6" t="s">
-        <v>57</v>
-      </c>
-      <c r="C73" s="7" t="s">
-        <v>42</v>
-      </c>
-      <c r="D73" s="8" t="s">
-        <v>56</v>
-      </c>
       <c r="E73" s="9" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="74" spans="1:7" ht="17.149999999999999" x14ac:dyDescent="0.55000000000000004">
       <c r="A74" s="10" t="s">
+        <v>114</v>
+      </c>
+      <c r="B74" s="6" t="s">
         <v>115</v>
-      </c>
-      <c r="B74" s="6" t="s">
-        <v>116</v>
       </c>
       <c r="C74" s="7" t="s">
         <v>6</v>
       </c>
       <c r="D74" s="8" t="s">
+        <v>112</v>
+      </c>
+      <c r="E74" s="9" t="s">
         <v>113</v>
-      </c>
-      <c r="E74" s="9" t="s">
-        <v>114</v>
       </c>
     </row>
     <row r="75" spans="1:7" ht="17.149999999999999" x14ac:dyDescent="0.55000000000000004">
       <c r="A75" s="10" t="s">
+        <v>122</v>
+      </c>
+      <c r="B75" s="6" t="s">
         <v>123</v>
       </c>
-      <c r="B75" s="6" t="s">
+      <c r="C75" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="D75" s="8" t="s">
         <v>124</v>
       </c>
-      <c r="C75" s="7" t="s">
-        <v>28</v>
-      </c>
-      <c r="D75" s="8" t="s">
+      <c r="E75" s="9" t="s">
         <v>125</v>
-      </c>
-      <c r="E75" s="9" t="s">
-        <v>126</v>
       </c>
     </row>
     <row r="76" spans="1:7" ht="17.149999999999999" x14ac:dyDescent="0.55000000000000004">
       <c r="A76" s="10" t="s">
+        <v>151</v>
+      </c>
+      <c r="B76" s="6" t="s">
         <v>152</v>
-      </c>
-      <c r="B76" s="6" t="s">
-        <v>153</v>
       </c>
       <c r="C76" s="7" t="s">
         <v>6</v>
       </c>
       <c r="D76" s="8" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="E76" s="9" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="77" spans="1:7" ht="17.149999999999999" x14ac:dyDescent="0.55000000000000004">
       <c r="A77" s="10" t="s">
+        <v>140</v>
+      </c>
+      <c r="B77" s="6" t="s">
         <v>141</v>
-      </c>
-      <c r="B77" s="6" t="s">
-        <v>142</v>
       </c>
       <c r="C77" s="7" t="s">
         <v>6</v>
       </c>
       <c r="D77" s="8" t="s">
+        <v>142</v>
+      </c>
+      <c r="E77" s="9" t="s">
+        <v>144</v>
+      </c>
+      <c r="G77" s="14" t="s">
         <v>143</v>
-      </c>
-      <c r="E77" s="9" t="s">
-        <v>145</v>
-      </c>
-      <c r="G77" s="14" t="s">
-        <v>144</v>
       </c>
     </row>
     <row r="78" spans="1:7" ht="17.149999999999999" x14ac:dyDescent="0.55000000000000004">
       <c r="A78" s="10" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="B78" s="6" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="C78" s="7" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="D78" s="8" t="s">
-        <v>420</v>
+        <v>417</v>
       </c>
       <c r="E78" s="13" t="s">
-        <v>326</v>
+        <v>324</v>
       </c>
       <c r="F78" s="6">
         <v>3</v>
@@ -3439,81 +3458,81 @@
     </row>
     <row r="79" spans="1:7" ht="17.149999999999999" x14ac:dyDescent="0.55000000000000004">
       <c r="A79" s="10" t="s">
-        <v>369</v>
+        <v>366</v>
       </c>
       <c r="C79" s="7" t="s">
         <v>13</v>
       </c>
       <c r="D79" s="8" t="s">
-        <v>367</v>
+        <v>364</v>
       </c>
       <c r="G79" s="14" t="s">
-        <v>368</v>
+        <v>365</v>
       </c>
     </row>
     <row r="80" spans="1:7" ht="17.149999999999999" x14ac:dyDescent="0.55000000000000004">
       <c r="A80" s="10" t="s">
+        <v>42</v>
+      </c>
+      <c r="B80" s="6" t="s">
+        <v>44</v>
+      </c>
+      <c r="C80" s="7" t="s">
+        <v>41</v>
+      </c>
+      <c r="D80" s="8" t="s">
         <v>43</v>
       </c>
-      <c r="B80" s="6" t="s">
+      <c r="E80" s="9" t="s">
+        <v>46</v>
+      </c>
+      <c r="G80" s="14" t="s">
         <v>45</v>
-      </c>
-      <c r="C80" s="7" t="s">
-        <v>42</v>
-      </c>
-      <c r="D80" s="8" t="s">
-        <v>44</v>
-      </c>
-      <c r="E80" s="9" t="s">
-        <v>47</v>
-      </c>
-      <c r="G80" s="14" t="s">
-        <v>46</v>
       </c>
     </row>
     <row r="81" spans="1:7" ht="17.149999999999999" x14ac:dyDescent="0.55000000000000004">
       <c r="A81" s="10" t="s">
+        <v>174</v>
+      </c>
+      <c r="C81" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="D81" s="8" t="s">
         <v>175</v>
-      </c>
-      <c r="C81" s="7" t="s">
-        <v>28</v>
-      </c>
-      <c r="D81" s="8" t="s">
-        <v>176</v>
       </c>
     </row>
     <row r="82" spans="1:7" ht="17.149999999999999" x14ac:dyDescent="0.55000000000000004">
       <c r="A82" s="10" t="s">
+        <v>136</v>
+      </c>
+      <c r="B82" s="6" t="s">
+        <v>138</v>
+      </c>
+      <c r="C82" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="D82" s="8" t="s">
         <v>137</v>
       </c>
-      <c r="B82" s="6" t="s">
+      <c r="E82" s="9" t="s">
         <v>139</v>
-      </c>
-      <c r="C82" s="7" t="s">
-        <v>28</v>
-      </c>
-      <c r="D82" s="8" t="s">
-        <v>138</v>
-      </c>
-      <c r="E82" s="9" t="s">
-        <v>140</v>
       </c>
     </row>
     <row r="83" spans="1:7" ht="17.149999999999999" x14ac:dyDescent="0.55000000000000004">
       <c r="A83" s="10" t="s">
+        <v>301</v>
+      </c>
+      <c r="B83" s="6" t="s">
         <v>302</v>
       </c>
-      <c r="B83" s="6" t="s">
-        <v>303</v>
-      </c>
       <c r="C83" s="7" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="D83" s="8" t="s">
-        <v>377</v>
+        <v>374</v>
       </c>
       <c r="E83" s="9" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="F83" s="6">
         <v>3</v>
@@ -3521,95 +3540,95 @@
     </row>
     <row r="84" spans="1:7" ht="17.149999999999999" x14ac:dyDescent="0.55000000000000004">
       <c r="A84" s="10" t="s">
+        <v>163</v>
+      </c>
+      <c r="C84" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="D84" s="8" t="s">
         <v>164</v>
-      </c>
-      <c r="C84" s="7" t="s">
-        <v>28</v>
-      </c>
-      <c r="D84" s="8" t="s">
-        <v>165</v>
       </c>
     </row>
     <row r="85" spans="1:7" ht="17.149999999999999" x14ac:dyDescent="0.55000000000000004">
       <c r="A85" s="10" t="s">
+        <v>159</v>
+      </c>
+      <c r="B85" s="6" t="s">
+        <v>162</v>
+      </c>
+      <c r="C85" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="D85" s="8" t="s">
         <v>160</v>
       </c>
-      <c r="B85" s="6" t="s">
-        <v>163</v>
-      </c>
-      <c r="C85" s="7" t="s">
-        <v>28</v>
-      </c>
-      <c r="D85" s="8" t="s">
+      <c r="G85" s="14" t="s">
         <v>161</v>
-      </c>
-      <c r="G85" s="14" t="s">
-        <v>162</v>
       </c>
     </row>
     <row r="86" spans="1:7" ht="17.149999999999999" x14ac:dyDescent="0.55000000000000004">
       <c r="A86" s="10" t="s">
+        <v>165</v>
+      </c>
+      <c r="C86" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="D86" s="8" t="s">
         <v>166</v>
-      </c>
-      <c r="C86" s="7" t="s">
-        <v>28</v>
-      </c>
-      <c r="D86" s="8" t="s">
-        <v>167</v>
       </c>
     </row>
     <row r="87" spans="1:7" ht="17.149999999999999" x14ac:dyDescent="0.55000000000000004">
       <c r="A87" s="10" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="B87" s="6" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="C87" s="7" t="s">
         <v>13</v>
       </c>
       <c r="D87" s="8" t="s">
+        <v>156</v>
+      </c>
+      <c r="E87" s="9" t="s">
         <v>157</v>
-      </c>
-      <c r="E87" s="9" t="s">
-        <v>158</v>
       </c>
     </row>
     <row r="88" spans="1:7" ht="17.149999999999999" x14ac:dyDescent="0.55000000000000004">
       <c r="A88" s="10" t="s">
+        <v>271</v>
+      </c>
+      <c r="B88" s="6" t="s">
         <v>272</v>
-      </c>
-      <c r="B88" s="6" t="s">
-        <v>273</v>
       </c>
       <c r="C88" s="7" t="s">
         <v>13</v>
       </c>
       <c r="D88" s="8" t="s">
-        <v>417</v>
+        <v>414</v>
       </c>
       <c r="E88" s="9" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="F88" s="6">
         <v>3</v>
       </c>
       <c r="G88" s="6" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
     </row>
     <row r="89" spans="1:7" ht="17.149999999999999" x14ac:dyDescent="0.55000000000000004">
       <c r="A89" s="10" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="B89" s="6" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="C89" s="7" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="D89" s="8" t="s">
-        <v>415</v>
+        <v>412</v>
       </c>
       <c r="E89" s="9" t="s">
         <v>8</v>
@@ -3618,67 +3637,67 @@
         <v>3</v>
       </c>
       <c r="G89" s="14" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
     </row>
     <row r="90" spans="1:7" ht="17.149999999999999" x14ac:dyDescent="0.55000000000000004">
       <c r="A90" s="10" t="s">
+        <v>107</v>
+      </c>
+      <c r="B90" s="6" t="s">
+        <v>106</v>
+      </c>
+      <c r="C90" s="7" t="s">
+        <v>79</v>
+      </c>
+      <c r="D90" s="8" t="s">
+        <v>376</v>
+      </c>
+      <c r="E90" s="9" t="s">
         <v>108</v>
       </c>
-      <c r="B90" s="6" t="s">
-        <v>107</v>
-      </c>
-      <c r="C90" s="7" t="s">
-        <v>80</v>
-      </c>
-      <c r="D90" s="8" t="s">
-        <v>379</v>
-      </c>
-      <c r="E90" s="9" t="s">
-        <v>109</v>
-      </c>
       <c r="F90" s="6">
         <v>3</v>
       </c>
       <c r="G90" s="14" t="s">
-        <v>308</v>
+        <v>306</v>
       </c>
     </row>
     <row r="91" spans="1:7" ht="17.149999999999999" x14ac:dyDescent="0.55000000000000004">
       <c r="A91" s="10" t="s">
+        <v>280</v>
+      </c>
+      <c r="B91" s="6" t="s">
+        <v>129</v>
+      </c>
+      <c r="C91" s="7" t="s">
+        <v>79</v>
+      </c>
+      <c r="D91" s="8" t="s">
+        <v>417</v>
+      </c>
+      <c r="F91" s="6">
+        <v>3</v>
+      </c>
+      <c r="G91" s="14" t="s">
         <v>281</v>
-      </c>
-      <c r="B91" s="6" t="s">
-        <v>130</v>
-      </c>
-      <c r="C91" s="7" t="s">
-        <v>80</v>
-      </c>
-      <c r="D91" s="8" t="s">
-        <v>361</v>
-      </c>
-      <c r="F91" s="6">
-        <v>2</v>
-      </c>
-      <c r="G91" s="14" t="s">
-        <v>282</v>
       </c>
     </row>
     <row r="92" spans="1:7" ht="17.149999999999999" x14ac:dyDescent="0.55000000000000004">
       <c r="A92" s="10" t="s">
+        <v>268</v>
+      </c>
+      <c r="B92" s="6" t="s">
+        <v>270</v>
+      </c>
+      <c r="C92" s="7" t="s">
+        <v>41</v>
+      </c>
+      <c r="D92" s="8" t="s">
+        <v>414</v>
+      </c>
+      <c r="E92" s="9" t="s">
         <v>269</v>
-      </c>
-      <c r="B92" s="6" t="s">
-        <v>271</v>
-      </c>
-      <c r="C92" s="7" t="s">
-        <v>42</v>
-      </c>
-      <c r="D92" s="8" t="s">
-        <v>417</v>
-      </c>
-      <c r="E92" s="9" t="s">
-        <v>270</v>
       </c>
       <c r="F92" s="6">
         <v>3</v>
@@ -3686,87 +3705,87 @@
     </row>
     <row r="93" spans="1:7" ht="17.149999999999999" x14ac:dyDescent="0.55000000000000004">
       <c r="A93" s="10" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="C93" s="7" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D93" s="8" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
     </row>
     <row r="94" spans="1:7" ht="17.149999999999999" x14ac:dyDescent="0.55000000000000004">
       <c r="A94" s="10" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="B94" s="6" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="C94" s="7" t="s">
         <v>13</v>
       </c>
       <c r="D94" s="8" t="s">
-        <v>361</v>
+        <v>417</v>
       </c>
       <c r="F94" s="6">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="95" spans="1:7" ht="17.149999999999999" x14ac:dyDescent="0.55000000000000004">
       <c r="A95" s="10" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="B95" s="6" t="s">
-        <v>317</v>
+        <v>315</v>
       </c>
       <c r="C95" s="7" t="s">
         <v>13</v>
       </c>
       <c r="D95" s="8" t="s">
-        <v>420</v>
+        <v>417</v>
       </c>
       <c r="F95" s="6">
         <v>3</v>
       </c>
       <c r="G95" s="14" t="s">
-        <v>421</v>
+        <v>418</v>
       </c>
     </row>
     <row r="96" spans="1:7" ht="17.149999999999999" x14ac:dyDescent="0.55000000000000004">
       <c r="A96" s="10" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="B96" s="6" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="C96" s="7" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="D96" s="8" t="s">
-        <v>408</v>
+        <v>405</v>
       </c>
       <c r="E96" s="12" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="F96" s="6">
         <v>3</v>
       </c>
       <c r="G96" s="14" t="s">
-        <v>410</v>
+        <v>407</v>
       </c>
     </row>
     <row r="97" spans="1:7" ht="17.149999999999999" x14ac:dyDescent="0.55000000000000004">
       <c r="A97" s="10" t="s">
-        <v>337</v>
+        <v>335</v>
       </c>
       <c r="B97" s="6" t="s">
-        <v>338</v>
+        <v>336</v>
       </c>
       <c r="C97" s="7" t="s">
         <v>13</v>
       </c>
       <c r="D97" s="8" t="s">
-        <v>334</v>
+        <v>332</v>
       </c>
       <c r="E97" s="9" t="s">
         <v>14</v>
@@ -3774,19 +3793,19 @@
     </row>
     <row r="98" spans="1:7" ht="17.149999999999999" x14ac:dyDescent="0.55000000000000004">
       <c r="A98" s="10" t="s">
+        <v>236</v>
+      </c>
+      <c r="B98" s="6" t="s">
         <v>237</v>
       </c>
-      <c r="B98" s="6" t="s">
-        <v>238</v>
-      </c>
       <c r="C98" s="7" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="D98" s="8" t="s">
-        <v>408</v>
+        <v>405</v>
       </c>
       <c r="E98" s="9" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="F98" s="6">
         <v>3</v>
@@ -3794,16 +3813,16 @@
     </row>
     <row r="99" spans="1:7" ht="17.149999999999999" x14ac:dyDescent="0.55000000000000004">
       <c r="A99" s="10" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="B99" s="6" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="C99" s="7" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="D99" s="8" t="s">
-        <v>415</v>
+        <v>412</v>
       </c>
       <c r="F99" s="6">
         <v>3</v>
@@ -3811,50 +3830,50 @@
     </row>
     <row r="100" spans="1:7" ht="17.149999999999999" x14ac:dyDescent="0.55000000000000004">
       <c r="A100" s="10" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="B100" s="6" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="C100" s="7" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="D100" s="8" t="s">
-        <v>406</v>
+        <v>403</v>
       </c>
       <c r="F100" s="6">
         <v>3</v>
       </c>
       <c r="G100" s="14" t="s">
-        <v>407</v>
+        <v>404</v>
       </c>
     </row>
     <row r="101" spans="1:7" ht="17.149999999999999" x14ac:dyDescent="0.55000000000000004">
       <c r="A101" s="10" t="s">
+        <v>167</v>
+      </c>
+      <c r="B101" s="6" t="s">
+        <v>169</v>
+      </c>
+      <c r="C101" s="7" t="s">
+        <v>41</v>
+      </c>
+      <c r="D101" s="8" t="s">
         <v>168</v>
-      </c>
-      <c r="B101" s="6" t="s">
-        <v>170</v>
-      </c>
-      <c r="C101" s="7" t="s">
-        <v>42</v>
-      </c>
-      <c r="D101" s="8" t="s">
-        <v>169</v>
       </c>
     </row>
     <row r="102" spans="1:7" ht="17.149999999999999" x14ac:dyDescent="0.55000000000000004">
       <c r="A102" s="10" t="s">
+        <v>318</v>
+      </c>
+      <c r="B102" s="6" t="s">
         <v>320</v>
-      </c>
-      <c r="B102" s="6" t="s">
-        <v>322</v>
       </c>
       <c r="C102" s="7" t="s">
         <v>13</v>
       </c>
       <c r="D102" s="8" t="s">
-        <v>321</v>
+        <v>319</v>
       </c>
       <c r="E102" s="9" t="s">
         <v>14</v>
@@ -3862,59 +3881,59 @@
     </row>
     <row r="103" spans="1:7" ht="17.149999999999999" x14ac:dyDescent="0.55000000000000004">
       <c r="A103" s="10" t="s">
+        <v>47</v>
+      </c>
+      <c r="B103" s="6" t="s">
         <v>48</v>
       </c>
-      <c r="B103" s="6" t="s">
+      <c r="C103" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="D103" s="8" t="s">
         <v>49</v>
       </c>
-      <c r="C103" s="7" t="s">
-        <v>28</v>
-      </c>
-      <c r="D103" s="8" t="s">
+      <c r="E103" s="9" t="s">
+        <v>21</v>
+      </c>
+      <c r="G103" s="14" t="s">
         <v>50</v>
-      </c>
-      <c r="E103" s="9" t="s">
-        <v>22</v>
-      </c>
-      <c r="G103" s="14" t="s">
-        <v>51</v>
       </c>
     </row>
     <row r="104" spans="1:7" ht="17.149999999999999" x14ac:dyDescent="0.55000000000000004">
       <c r="A104" s="10" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="B104" s="6" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="C104" s="7" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="D104" s="8" t="s">
-        <v>399</v>
+        <v>396</v>
       </c>
       <c r="F104" s="6">
         <v>3</v>
       </c>
       <c r="G104" s="14" t="s">
-        <v>401</v>
+        <v>398</v>
       </c>
     </row>
     <row r="105" spans="1:7" ht="17.149999999999999" x14ac:dyDescent="0.55000000000000004">
       <c r="A105" s="10" t="s">
+        <v>246</v>
+      </c>
+      <c r="B105" s="6" t="s">
         <v>247</v>
       </c>
-      <c r="B105" s="6" t="s">
-        <v>248</v>
-      </c>
       <c r="C105" s="7" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="D105" s="8" t="s">
-        <v>413</v>
+        <v>410</v>
       </c>
       <c r="E105" s="9" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="F105" s="6">
         <v>3</v>
@@ -3922,168 +3941,168 @@
     </row>
     <row r="106" spans="1:7" ht="17.149999999999999" x14ac:dyDescent="0.55000000000000004">
       <c r="A106" s="10" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="B106" s="6" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="C106" s="7" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="D106" s="8" t="s">
-        <v>411</v>
+        <v>408</v>
       </c>
       <c r="E106" s="9" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="F106" s="6">
         <v>2</v>
       </c>
       <c r="G106" s="14" t="s">
-        <v>412</v>
+        <v>409</v>
       </c>
     </row>
     <row r="107" spans="1:7" ht="17.149999999999999" x14ac:dyDescent="0.55000000000000004">
       <c r="A107" s="10" t="s">
+        <v>178</v>
+      </c>
+      <c r="B107" s="6" t="s">
         <v>179</v>
-      </c>
-      <c r="B107" s="6" t="s">
-        <v>180</v>
       </c>
       <c r="C107" s="7" t="s">
         <v>13</v>
       </c>
       <c r="D107" s="8" t="s">
-        <v>382</v>
+        <v>379</v>
       </c>
       <c r="F107" s="6">
         <v>3</v>
       </c>
       <c r="G107" s="14" t="s">
-        <v>325</v>
+        <v>323</v>
       </c>
     </row>
     <row r="108" spans="1:7" ht="17.149999999999999" x14ac:dyDescent="0.55000000000000004">
       <c r="A108" s="10" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="B108" s="6" t="s">
         <v>12</v>
       </c>
       <c r="C108" s="7" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="D108" s="8" t="s">
+        <v>417</v>
+      </c>
+      <c r="E108" s="9" t="s">
         <v>307</v>
       </c>
-      <c r="E108" s="9" t="s">
-        <v>309</v>
-      </c>
       <c r="F108" s="6">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="G108" s="14" t="s">
-        <v>15</v>
+        <v>421</v>
       </c>
     </row>
     <row r="109" spans="1:7" ht="17.149999999999999" x14ac:dyDescent="0.55000000000000004">
       <c r="A109" s="10" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="B109" s="6" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="C109" s="7" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="D109" s="8" t="s">
-        <v>379</v>
+        <v>376</v>
       </c>
       <c r="E109" s="9" t="s">
+        <v>97</v>
+      </c>
+      <c r="F109" s="6">
+        <v>3</v>
+      </c>
+      <c r="G109" s="14" t="s">
         <v>98</v>
-      </c>
-      <c r="F109" s="6">
-        <v>3</v>
-      </c>
-      <c r="G109" s="14" t="s">
-        <v>99</v>
       </c>
     </row>
     <row r="110" spans="1:7" ht="17.149999999999999" x14ac:dyDescent="0.55000000000000004">
       <c r="A110" s="10" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="B110" s="6" t="s">
-        <v>353</v>
+        <v>351</v>
       </c>
       <c r="C110" s="7" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="D110" s="8" t="s">
-        <v>397</v>
+        <v>394</v>
       </c>
       <c r="F110" s="6">
         <v>3</v>
       </c>
       <c r="G110" s="14" t="s">
-        <v>352</v>
+        <v>350</v>
       </c>
     </row>
     <row r="111" spans="1:7" ht="17.149999999999999" x14ac:dyDescent="0.55000000000000004">
       <c r="A111" s="10" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="B111" s="6" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="C111" s="7" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="D111" s="8" t="s">
-        <v>379</v>
+        <v>376</v>
       </c>
       <c r="E111" s="9" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="F111" s="6">
         <v>4</v>
       </c>
       <c r="G111" s="14" t="s">
-        <v>310</v>
+        <v>308</v>
       </c>
     </row>
     <row r="112" spans="1:7" ht="17.149999999999999" x14ac:dyDescent="0.55000000000000004">
       <c r="A112" s="10" t="s">
+        <v>51</v>
+      </c>
+      <c r="B112" s="6" t="s">
+        <v>48</v>
+      </c>
+      <c r="C112" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="D112" s="8" t="s">
         <v>52</v>
       </c>
-      <c r="B112" s="6" t="s">
-        <v>49</v>
-      </c>
-      <c r="C112" s="7" t="s">
-        <v>28</v>
-      </c>
-      <c r="D112" s="8" t="s">
+      <c r="E112" s="9" t="s">
+        <v>21</v>
+      </c>
+      <c r="G112" s="14" t="s">
         <v>53</v>
-      </c>
-      <c r="E112" s="9" t="s">
-        <v>22</v>
-      </c>
-      <c r="G112" s="14" t="s">
-        <v>54</v>
       </c>
     </row>
     <row r="113" spans="1:7" ht="17.149999999999999" x14ac:dyDescent="0.55000000000000004">
       <c r="A113" s="10" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="B113" s="6" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="C113" s="7" t="s">
         <v>13</v>
       </c>
       <c r="D113" s="8" t="s">
-        <v>416</v>
+        <v>413</v>
       </c>
       <c r="F113" s="6">
         <v>3</v>
@@ -4091,59 +4110,59 @@
     </row>
     <row r="114" spans="1:7" ht="17.149999999999999" x14ac:dyDescent="0.55000000000000004">
       <c r="A114" s="10" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="B114" s="6" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="C114" s="7" t="s">
         <v>13</v>
       </c>
       <c r="D114" s="8" t="s">
-        <v>399</v>
+        <v>396</v>
       </c>
       <c r="E114" s="9" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="F114" s="6">
         <v>3</v>
       </c>
       <c r="G114" s="14" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
     </row>
     <row r="115" spans="1:7" ht="17.149999999999999" x14ac:dyDescent="0.55000000000000004">
       <c r="A115" s="10" t="s">
+        <v>28</v>
+      </c>
+      <c r="B115" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="C115" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="D115" s="8" t="s">
         <v>29</v>
       </c>
-      <c r="B115" s="6" t="s">
-        <v>33</v>
-      </c>
-      <c r="C115" s="7" t="s">
-        <v>28</v>
-      </c>
-      <c r="D115" s="8" t="s">
+      <c r="E115" s="9" t="s">
         <v>30</v>
       </c>
-      <c r="E115" s="9" t="s">
+      <c r="G115" s="14" t="s">
         <v>31</v>
-      </c>
-      <c r="G115" s="14" t="s">
-        <v>32</v>
       </c>
     </row>
     <row r="116" spans="1:7" ht="17.149999999999999" x14ac:dyDescent="0.55000000000000004">
       <c r="A116" s="10" t="s">
-        <v>315</v>
+        <v>313</v>
       </c>
       <c r="B116" s="6" t="s">
-        <v>316</v>
+        <v>314</v>
       </c>
       <c r="C116" s="7" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="D116" s="8" t="s">
-        <v>312</v>
+        <v>310</v>
       </c>
       <c r="E116" s="9" t="s">
         <v>14</v>
@@ -4151,19 +4170,19 @@
     </row>
     <row r="117" spans="1:7" ht="17.149999999999999" x14ac:dyDescent="0.55000000000000004">
       <c r="A117" s="10" t="s">
+        <v>185</v>
+      </c>
+      <c r="B117" s="6" t="s">
         <v>186</v>
-      </c>
-      <c r="B117" s="6" t="s">
-        <v>187</v>
       </c>
       <c r="C117" s="7" t="s">
         <v>6</v>
       </c>
       <c r="D117" s="8" t="s">
-        <v>383</v>
+        <v>380</v>
       </c>
       <c r="E117" s="9" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="F117" s="6">
         <v>2</v>
@@ -4171,36 +4190,36 @@
     </row>
     <row r="118" spans="1:7" ht="17.149999999999999" x14ac:dyDescent="0.55000000000000004">
       <c r="A118" s="10" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B118" s="6" t="s">
+        <v>78</v>
+      </c>
+      <c r="C118" s="7" t="s">
         <v>79</v>
       </c>
-      <c r="C118" s="7" t="s">
-        <v>80</v>
-      </c>
       <c r="D118" s="8" t="s">
-        <v>376</v>
+        <v>373</v>
       </c>
       <c r="F118" s="6">
         <v>4</v>
       </c>
       <c r="G118" s="14" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
     </row>
     <row r="119" spans="1:7" ht="17.149999999999999" x14ac:dyDescent="0.55000000000000004">
       <c r="A119" s="10" t="s">
-        <v>313</v>
+        <v>311</v>
       </c>
       <c r="B119" s="6" t="s">
-        <v>314</v>
+        <v>312</v>
       </c>
       <c r="C119" s="7" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="D119" s="8" t="s">
-        <v>312</v>
+        <v>310</v>
       </c>
       <c r="E119" s="9" t="s">
         <v>14</v>
@@ -4208,39 +4227,39 @@
     </row>
     <row r="120" spans="1:7" ht="17.149999999999999" x14ac:dyDescent="0.55000000000000004">
       <c r="A120" s="10" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="B120" s="6" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="C120" s="7" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="D120" s="8" t="s">
-        <v>376</v>
+        <v>373</v>
       </c>
       <c r="E120" s="9" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="F120" s="6">
         <v>3</v>
       </c>
       <c r="G120" s="14" t="s">
-        <v>363</v>
+        <v>360</v>
       </c>
     </row>
     <row r="121" spans="1:7" ht="17.149999999999999" x14ac:dyDescent="0.55000000000000004">
       <c r="A121" s="10" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="B121" s="6" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="C121" s="7" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="D121" s="8" t="s">
-        <v>402</v>
+        <v>399</v>
       </c>
       <c r="E121" s="9" t="s">
         <v>14</v>
@@ -4249,55 +4268,55 @@
         <v>3</v>
       </c>
       <c r="G121" s="14" t="s">
-        <v>405</v>
+        <v>402</v>
       </c>
     </row>
     <row r="122" spans="1:7" ht="17.149999999999999" x14ac:dyDescent="0.55000000000000004">
       <c r="A122" s="10" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="B122" s="6" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="C122" s="7" t="s">
         <v>6</v>
       </c>
       <c r="D122" s="8" t="s">
+        <v>171</v>
+      </c>
+      <c r="E122" s="9" t="s">
         <v>172</v>
-      </c>
-      <c r="E122" s="9" t="s">
-        <v>173</v>
       </c>
     </row>
     <row r="123" spans="1:7" ht="17.149999999999999" x14ac:dyDescent="0.55000000000000004">
       <c r="A123" s="10" t="s">
-        <v>319</v>
+        <v>317</v>
       </c>
       <c r="B123" s="6" t="s">
-        <v>317</v>
+        <v>315</v>
       </c>
       <c r="C123" s="7" t="s">
         <v>13</v>
       </c>
       <c r="D123" s="8" t="s">
-        <v>318</v>
+        <v>316</v>
       </c>
     </row>
     <row r="124" spans="1:7" ht="17.149999999999999" x14ac:dyDescent="0.55000000000000004">
       <c r="A124" s="10" t="s">
+        <v>126</v>
+      </c>
+      <c r="B124" s="6" t="s">
+        <v>321</v>
+      </c>
+      <c r="C124" s="7" t="s">
+        <v>41</v>
+      </c>
+      <c r="D124" s="8" t="s">
+        <v>379</v>
+      </c>
+      <c r="E124" s="9" t="s">
         <v>127</v>
-      </c>
-      <c r="B124" s="6" t="s">
-        <v>323</v>
-      </c>
-      <c r="C124" s="7" t="s">
-        <v>42</v>
-      </c>
-      <c r="D124" s="8" t="s">
-        <v>382</v>
-      </c>
-      <c r="E124" s="9" t="s">
-        <v>128</v>
       </c>
       <c r="F124" s="6">
         <v>4</v>
@@ -4305,56 +4324,56 @@
     </row>
     <row r="125" spans="1:7" ht="17.149999999999999" x14ac:dyDescent="0.55000000000000004">
       <c r="A125" s="10" t="s">
+        <v>183</v>
+      </c>
+      <c r="B125" s="6" t="s">
+        <v>327</v>
+      </c>
+      <c r="C125" s="7" t="s">
+        <v>41</v>
+      </c>
+      <c r="D125" s="8" t="s">
+        <v>380</v>
+      </c>
+      <c r="E125" s="10" t="s">
         <v>184</v>
       </c>
-      <c r="B125" s="6" t="s">
-        <v>329</v>
-      </c>
-      <c r="C125" s="7" t="s">
-        <v>42</v>
-      </c>
-      <c r="D125" s="8" t="s">
-        <v>383</v>
-      </c>
-      <c r="E125" s="10" t="s">
-        <v>185</v>
-      </c>
       <c r="F125" s="6">
         <v>3</v>
       </c>
       <c r="G125" s="14" t="s">
-        <v>328</v>
+        <v>326</v>
       </c>
     </row>
     <row r="126" spans="1:7" ht="17.149999999999999" x14ac:dyDescent="0.55000000000000004">
       <c r="A126" s="10" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="C126" s="7" t="s">
         <v>13</v>
       </c>
       <c r="D126" s="8" t="s">
-        <v>391</v>
+        <v>388</v>
       </c>
       <c r="F126" s="6">
         <v>3</v>
       </c>
       <c r="G126" s="14" t="s">
-        <v>393</v>
+        <v>390</v>
       </c>
     </row>
     <row r="127" spans="1:7" ht="17.149999999999999" x14ac:dyDescent="0.55000000000000004">
       <c r="A127" s="10" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="B127" s="6" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="C127" s="7" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="D127" s="8" t="s">
-        <v>416</v>
+        <v>413</v>
       </c>
       <c r="F127" s="6">
         <v>3</v>
@@ -4362,19 +4381,19 @@
     </row>
     <row r="128" spans="1:7" ht="17.149999999999999" x14ac:dyDescent="0.55000000000000004">
       <c r="A128" s="10" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="B128" s="6" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="C128" s="7" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="D128" s="8" t="s">
-        <v>382</v>
+        <v>379</v>
       </c>
       <c r="E128" s="9" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="F128" s="6">
         <v>4</v>
@@ -4382,19 +4401,19 @@
     </row>
     <row r="129" spans="1:7" ht="17.149999999999999" x14ac:dyDescent="0.55000000000000004">
       <c r="A129" s="10" t="s">
+        <v>116</v>
+      </c>
+      <c r="B129" s="6" t="s">
+        <v>119</v>
+      </c>
+      <c r="C129" s="7" t="s">
+        <v>94</v>
+      </c>
+      <c r="D129" s="8" t="s">
+        <v>377</v>
+      </c>
+      <c r="E129" s="9" t="s">
         <v>117</v>
-      </c>
-      <c r="B129" s="6" t="s">
-        <v>120</v>
-      </c>
-      <c r="C129" s="7" t="s">
-        <v>95</v>
-      </c>
-      <c r="D129" s="8" t="s">
-        <v>380</v>
-      </c>
-      <c r="E129" s="9" t="s">
-        <v>118</v>
       </c>
       <c r="F129" s="6">
         <v>5</v>
@@ -4402,84 +4421,87 @@
     </row>
     <row r="130" spans="1:7" ht="17.149999999999999" x14ac:dyDescent="0.55000000000000004">
       <c r="A130" s="10" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="B130" s="6" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="C130" s="7" t="s">
         <v>13</v>
       </c>
       <c r="D130" s="8" t="s">
-        <v>362</v>
+        <v>417</v>
       </c>
       <c r="E130" s="9" t="s">
         <v>14</v>
       </c>
       <c r="F130" s="6">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="131" spans="1:7" ht="17.149999999999999" x14ac:dyDescent="0.55000000000000004">
       <c r="A131" s="10" t="s">
-        <v>366</v>
+        <v>363</v>
       </c>
       <c r="C131" s="7" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="D131" s="8" t="s">
-        <v>367</v>
+        <v>364</v>
       </c>
     </row>
     <row r="132" spans="1:7" ht="17.149999999999999" x14ac:dyDescent="0.55000000000000004">
       <c r="A132" s="10" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="B132" s="6" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="C132" s="7" t="s">
         <v>13</v>
       </c>
       <c r="D132" s="8" t="s">
-        <v>362</v>
+        <v>417</v>
       </c>
       <c r="F132" s="6">
-        <v>2</v>
+        <v>3</v>
+      </c>
+      <c r="G132" s="14" t="s">
+        <v>422</v>
       </c>
     </row>
     <row r="133" spans="1:7" ht="17.149999999999999" x14ac:dyDescent="0.55000000000000004">
       <c r="A133" s="10" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="B133" s="6" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="C133" s="7" t="s">
         <v>6</v>
       </c>
       <c r="D133" s="8" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="E133" s="9" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="G133" s="14" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
     </row>
     <row r="134" spans="1:7" ht="17.149999999999999" x14ac:dyDescent="0.55000000000000004">
       <c r="A134" s="10" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="B134" s="6" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="C134" s="7" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="D134" s="8" t="s">
-        <v>417</v>
+        <v>414</v>
       </c>
       <c r="F134" s="6">
         <v>3</v>
@@ -4487,193 +4509,196 @@
     </row>
     <row r="135" spans="1:7" ht="17.149999999999999" x14ac:dyDescent="0.55000000000000004">
       <c r="A135" s="10" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="C135" s="7" t="s">
         <v>13</v>
       </c>
       <c r="D135" s="8" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
     </row>
     <row r="136" spans="1:7" ht="17.149999999999999" x14ac:dyDescent="0.55000000000000004">
       <c r="A136" s="10" t="s">
+        <v>87</v>
+      </c>
+      <c r="B136" s="6" t="s">
         <v>88</v>
       </c>
-      <c r="B136" s="6" t="s">
+      <c r="C136" s="7" t="s">
+        <v>41</v>
+      </c>
+      <c r="D136" s="8" t="s">
+        <v>84</v>
+      </c>
+      <c r="E136" s="9" t="s">
         <v>89</v>
-      </c>
-      <c r="C136" s="7" t="s">
-        <v>42</v>
-      </c>
-      <c r="D136" s="8" t="s">
-        <v>85</v>
-      </c>
-      <c r="E136" s="9" t="s">
-        <v>90</v>
       </c>
     </row>
     <row r="137" spans="1:7" ht="17.149999999999999" x14ac:dyDescent="0.55000000000000004">
       <c r="A137" s="10" t="s">
-        <v>290</v>
+        <v>423</v>
       </c>
       <c r="B137" s="6" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="C137" s="7" t="s">
-        <v>80</v>
+        <v>13</v>
       </c>
       <c r="D137" s="8" t="s">
-        <v>362</v>
+        <v>417</v>
       </c>
       <c r="E137" s="9" t="s">
         <v>14</v>
       </c>
       <c r="F137" s="6">
-        <v>2</v>
-      </c>
-      <c r="G137" s="14" t="s">
-        <v>365</v>
+        <v>1</v>
+      </c>
+      <c r="G137" s="15" t="s">
+        <v>424</v>
       </c>
     </row>
     <row r="138" spans="1:7" ht="17.149999999999999" x14ac:dyDescent="0.55000000000000004">
       <c r="A138" s="10" t="s">
-        <v>181</v>
+        <v>289</v>
       </c>
       <c r="B138" s="6" t="s">
-        <v>327</v>
+        <v>129</v>
       </c>
       <c r="C138" s="7" t="s">
-        <v>42</v>
+        <v>94</v>
       </c>
       <c r="D138" s="8" t="s">
-        <v>383</v>
+        <v>417</v>
       </c>
       <c r="E138" s="9" t="s">
-        <v>183</v>
+        <v>14</v>
       </c>
       <c r="F138" s="6">
         <v>3</v>
       </c>
       <c r="G138" s="14" t="s">
-        <v>182</v>
+        <v>362</v>
       </c>
     </row>
     <row r="139" spans="1:7" ht="17.149999999999999" x14ac:dyDescent="0.55000000000000004">
       <c r="A139" s="10" t="s">
-        <v>111</v>
+        <v>180</v>
       </c>
       <c r="B139" s="6" t="s">
-        <v>112</v>
+        <v>325</v>
       </c>
       <c r="C139" s="7" t="s">
-        <v>6</v>
+        <v>41</v>
       </c>
       <c r="D139" s="8" t="s">
-        <v>113</v>
+        <v>380</v>
       </c>
       <c r="E139" s="9" t="s">
-        <v>114</v>
+        <v>182</v>
+      </c>
+      <c r="F139" s="6">
+        <v>3</v>
+      </c>
+      <c r="G139" s="14" t="s">
+        <v>181</v>
       </c>
     </row>
     <row r="140" spans="1:7" ht="17.149999999999999" x14ac:dyDescent="0.55000000000000004">
       <c r="A140" s="10" t="s">
-        <v>249</v>
+        <v>110</v>
       </c>
       <c r="B140" s="6" t="s">
-        <v>252</v>
+        <v>111</v>
       </c>
       <c r="C140" s="7" t="s">
-        <v>80</v>
+        <v>6</v>
       </c>
       <c r="D140" s="8" t="s">
-        <v>413</v>
+        <v>112</v>
       </c>
       <c r="E140" s="9" t="s">
-        <v>250</v>
-      </c>
-      <c r="F140" s="6">
-        <v>2</v>
-      </c>
-      <c r="G140" s="14" t="s">
-        <v>414</v>
+        <v>113</v>
       </c>
     </row>
     <row r="141" spans="1:7" ht="17.149999999999999" x14ac:dyDescent="0.55000000000000004">
       <c r="A141" s="10" t="s">
-        <v>240</v>
+        <v>248</v>
       </c>
       <c r="B141" s="6" t="s">
-        <v>238</v>
+        <v>251</v>
       </c>
       <c r="C141" s="7" t="s">
-        <v>42</v>
+        <v>79</v>
       </c>
       <c r="D141" s="8" t="s">
-        <v>408</v>
+        <v>410</v>
+      </c>
+      <c r="E141" s="9" t="s">
+        <v>249</v>
       </c>
       <c r="F141" s="6">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="G141" s="14" t="s">
-        <v>409</v>
+        <v>411</v>
       </c>
     </row>
     <row r="142" spans="1:7" ht="17.149999999999999" x14ac:dyDescent="0.55000000000000004">
       <c r="A142" s="10" t="s">
-        <v>267</v>
+        <v>239</v>
       </c>
       <c r="B142" s="6" t="s">
-        <v>268</v>
+        <v>237</v>
       </c>
       <c r="C142" s="7" t="s">
-        <v>13</v>
+        <v>41</v>
       </c>
       <c r="D142" s="8" t="s">
-        <v>417</v>
+        <v>405</v>
       </c>
       <c r="F142" s="6">
         <v>3</v>
       </c>
       <c r="G142" s="14" t="s">
-        <v>418</v>
+        <v>406</v>
       </c>
     </row>
     <row r="143" spans="1:7" ht="17.149999999999999" x14ac:dyDescent="0.55000000000000004">
       <c r="A143" s="10" t="s">
-        <v>119</v>
+        <v>266</v>
       </c>
       <c r="B143" s="6" t="s">
-        <v>107</v>
+        <v>267</v>
       </c>
       <c r="C143" s="7" t="s">
-        <v>95</v>
+        <v>13</v>
       </c>
       <c r="D143" s="8" t="s">
-        <v>381</v>
-      </c>
-      <c r="E143" s="9" t="s">
-        <v>122</v>
+        <v>414</v>
       </c>
       <c r="F143" s="6">
         <v>3</v>
+      </c>
+      <c r="G143" s="14" t="s">
+        <v>415</v>
       </c>
     </row>
     <row r="144" spans="1:7" ht="17.149999999999999" x14ac:dyDescent="0.55000000000000004">
       <c r="A144" s="10" t="s">
-        <v>262</v>
+        <v>118</v>
       </c>
       <c r="B144" s="6" t="s">
-        <v>148</v>
+        <v>106</v>
       </c>
       <c r="C144" s="7" t="s">
-        <v>13</v>
+        <v>94</v>
       </c>
       <c r="D144" s="8" t="s">
-        <v>416</v>
+        <v>378</v>
       </c>
       <c r="E144" s="9" t="s">
-        <v>22</v>
+        <v>121</v>
       </c>
       <c r="F144" s="6">
         <v>3</v>
@@ -4681,158 +4706,178 @@
     </row>
     <row r="145" spans="1:7" ht="17.149999999999999" x14ac:dyDescent="0.55000000000000004">
       <c r="A145" s="10" t="s">
-        <v>228</v>
+        <v>261</v>
+      </c>
+      <c r="B145" s="6" t="s">
+        <v>147</v>
       </c>
       <c r="C145" s="7" t="s">
         <v>13</v>
       </c>
       <c r="D145" s="8" t="s">
-        <v>399</v>
+        <v>413</v>
       </c>
       <c r="E145" s="9" t="s">
-        <v>47</v>
+        <v>21</v>
       </c>
       <c r="F145" s="6">
-        <v>4</v>
-      </c>
-      <c r="G145" s="14" t="s">
-        <v>400</v>
+        <v>3</v>
       </c>
     </row>
     <row r="146" spans="1:7" ht="17.149999999999999" x14ac:dyDescent="0.55000000000000004">
       <c r="A146" s="10" t="s">
-        <v>233</v>
-      </c>
-      <c r="B146" s="6" t="s">
-        <v>230</v>
+        <v>227</v>
       </c>
       <c r="C146" s="7" t="s">
         <v>13</v>
       </c>
       <c r="D146" s="8" t="s">
-        <v>402</v>
+        <v>396</v>
       </c>
       <c r="E146" s="9" t="s">
-        <v>93</v>
+        <v>46</v>
       </c>
       <c r="F146" s="6">
-        <v>3</v>
+        <v>4</v>
+      </c>
+      <c r="G146" s="14" t="s">
+        <v>397</v>
       </c>
     </row>
     <row r="147" spans="1:7" ht="17.149999999999999" x14ac:dyDescent="0.55000000000000004">
       <c r="A147" s="10" t="s">
-        <v>100</v>
+        <v>232</v>
       </c>
       <c r="B147" s="6" t="s">
-        <v>102</v>
+        <v>229</v>
       </c>
       <c r="C147" s="7" t="s">
-        <v>6</v>
+        <v>13</v>
       </c>
       <c r="D147" s="8" t="s">
-        <v>101</v>
+        <v>399</v>
       </c>
       <c r="E147" s="9" t="s">
-        <v>103</v>
+        <v>92</v>
+      </c>
+      <c r="F147" s="6">
+        <v>3</v>
       </c>
     </row>
     <row r="148" spans="1:7" ht="17.149999999999999" x14ac:dyDescent="0.55000000000000004">
       <c r="A148" s="10" t="s">
-        <v>83</v>
+        <v>99</v>
       </c>
       <c r="B148" s="6" t="s">
-        <v>86</v>
+        <v>101</v>
       </c>
       <c r="C148" s="7" t="s">
-        <v>28</v>
+        <v>6</v>
       </c>
       <c r="D148" s="8" t="s">
-        <v>85</v>
+        <v>100</v>
       </c>
       <c r="E148" s="9" t="s">
-        <v>84</v>
+        <v>102</v>
       </c>
     </row>
     <row r="149" spans="1:7" ht="17.149999999999999" x14ac:dyDescent="0.55000000000000004">
       <c r="A149" s="10" t="s">
-        <v>251</v>
+        <v>82</v>
       </c>
       <c r="B149" s="6" t="s">
-        <v>36</v>
+        <v>85</v>
       </c>
       <c r="C149" s="7" t="s">
-        <v>95</v>
+        <v>27</v>
       </c>
       <c r="D149" s="8" t="s">
-        <v>413</v>
+        <v>84</v>
       </c>
       <c r="E149" s="9" t="s">
-        <v>128</v>
-      </c>
-      <c r="F149" s="6">
-        <v>3</v>
-      </c>
-      <c r="G149" s="14" t="s">
-        <v>360</v>
+        <v>83</v>
       </c>
     </row>
     <row r="150" spans="1:7" ht="17.149999999999999" x14ac:dyDescent="0.55000000000000004">
       <c r="A150" s="10" t="s">
-        <v>206</v>
+        <v>250</v>
+      </c>
+      <c r="B150" s="6" t="s">
+        <v>35</v>
       </c>
       <c r="C150" s="7" t="s">
-        <v>13</v>
+        <v>94</v>
       </c>
       <c r="D150" s="8" t="s">
-        <v>391</v>
+        <v>410</v>
+      </c>
+      <c r="E150" s="9" t="s">
+        <v>127</v>
       </c>
       <c r="F150" s="6">
         <v>3</v>
+      </c>
+      <c r="G150" s="14" t="s">
+        <v>358</v>
       </c>
     </row>
     <row r="151" spans="1:7" ht="17.149999999999999" x14ac:dyDescent="0.55000000000000004">
       <c r="A151" s="10" t="s">
-        <v>294</v>
+        <v>205</v>
       </c>
       <c r="C151" s="7" t="s">
-        <v>42</v>
+        <v>13</v>
       </c>
       <c r="D151" s="8" t="s">
-        <v>291</v>
+        <v>388</v>
+      </c>
+      <c r="F151" s="6">
+        <v>3</v>
       </c>
     </row>
     <row r="152" spans="1:7" ht="17.149999999999999" x14ac:dyDescent="0.55000000000000004">
       <c r="A152" s="10" t="s">
-        <v>213</v>
+        <v>293</v>
       </c>
       <c r="C152" s="7" t="s">
-        <v>13</v>
+        <v>41</v>
       </c>
       <c r="D152" s="8" t="s">
-        <v>394</v>
-      </c>
-      <c r="F152" s="6">
-        <v>3</v>
+        <v>290</v>
       </c>
     </row>
     <row r="153" spans="1:7" ht="17.149999999999999" x14ac:dyDescent="0.55000000000000004">
       <c r="A153" s="10" t="s">
-        <v>223</v>
-      </c>
-      <c r="B153" s="6" t="s">
-        <v>357</v>
+        <v>212</v>
       </c>
       <c r="C153" s="7" t="s">
-        <v>95</v>
+        <v>13</v>
       </c>
       <c r="D153" s="8" t="s">
-        <v>398</v>
+        <v>391</v>
       </c>
       <c r="F153" s="6">
         <v>3</v>
       </c>
-      <c r="G153" s="14" t="s">
-        <v>358</v>
+    </row>
+    <row r="154" spans="1:7" ht="17.149999999999999" x14ac:dyDescent="0.55000000000000004">
+      <c r="A154" s="10" t="s">
+        <v>222</v>
+      </c>
+      <c r="B154" s="6" t="s">
+        <v>355</v>
+      </c>
+      <c r="C154" s="7" t="s">
+        <v>94</v>
+      </c>
+      <c r="D154" s="8" t="s">
+        <v>395</v>
+      </c>
+      <c r="F154" s="6">
+        <v>3</v>
+      </c>
+      <c r="G154" s="14" t="s">
+        <v>356</v>
       </c>
     </row>
   </sheetData>
@@ -4856,21 +4901,21 @@
     <hyperlink ref="A2" r:id="rId16" display="https://leetcode.cn/problems/two-sum/" xr:uid="{DCC2FC31-A6D8-4A22-B418-13AC2E7FF237}"/>
     <hyperlink ref="A118" r:id="rId17" display="https://leetcode.cn/problems/group-anagrams/" xr:uid="{8499950A-1DCD-4E4A-9D9A-5A7F78C5486B}"/>
     <hyperlink ref="A20" r:id="rId18" display="https://leetcode.cn/problems/longest-consecutive-sequence/" xr:uid="{AC05C0D0-F6E1-4797-A42E-1235E7280CF6}"/>
-    <hyperlink ref="A148" r:id="rId19" display="https://leetcode.cn/problems/remove-duplicates-from-sorted-list/" xr:uid="{BC1100E9-A72F-40CD-9106-5C6D7E369605}"/>
+    <hyperlink ref="A149" r:id="rId19" display="https://leetcode.cn/problems/remove-duplicates-from-sorted-list/" xr:uid="{BC1100E9-A72F-40CD-9106-5C6D7E369605}"/>
     <hyperlink ref="A83" r:id="rId20" display="https://leetcode.cn/problems/move-zeroes/" xr:uid="{3D57A5B2-C773-46BB-AAC1-384F5B1330AC}"/>
     <hyperlink ref="A136" r:id="rId21" display="https://leetcode.cn/problems/insert-into-a-sorted-circular-linked-list/" xr:uid="{ABF9182A-9A32-45E2-840F-96A729F2801D}"/>
     <hyperlink ref="A10" r:id="rId22" display="https://leetcode.cn/problems/container-with-most-water/" xr:uid="{4ED7D754-A6D7-4998-BB92-60F7FE4E11B9}"/>
     <hyperlink ref="A31" r:id="rId23" display="https://leetcode.cn/problems/3sum/" xr:uid="{0DBAA8D9-3DE9-4828-BFF8-655B84431AA9}"/>
     <hyperlink ref="A109" r:id="rId24" display="https://leetcode.cn/problems/trapping-rain-water/" xr:uid="{9CEE3039-70C6-486C-95F2-1E34859BC2B5}"/>
-    <hyperlink ref="A147" r:id="rId25" display="https://leetcode.cn/problems/remove-duplicates-from-sorted-list-ii/" xr:uid="{95C218B7-1B8A-4890-A292-F56103A4F9BD}"/>
+    <hyperlink ref="A148" r:id="rId25" display="https://leetcode.cn/problems/remove-duplicates-from-sorted-list-ii/" xr:uid="{95C218B7-1B8A-4890-A292-F56103A4F9BD}"/>
     <hyperlink ref="A35" r:id="rId26" display="https://leetcode.cn/problems/binary-tree-upside-down/" xr:uid="{7BE5D44B-F504-4178-853A-BECE3A0D6D9A}"/>
     <hyperlink ref="A90" r:id="rId27" display="https://leetcode.cn/problems/longest-substring-without-repeating-characters/" xr:uid="{3FB010E6-0492-4655-9911-820A190155C4}"/>
     <hyperlink ref="A111" r:id="rId28" display="https://leetcode.cn/problems/find-all-anagrams-in-a-string/" xr:uid="{36A9C6AE-A4CD-4F4E-90F8-8E5D5CB43CAB}"/>
-    <hyperlink ref="A139" r:id="rId29" display="https://leetcode.cn/problems/sentence-similarity/" xr:uid="{771EA040-6E9F-427A-9C87-C5F54FA18B80}"/>
+    <hyperlink ref="A140" r:id="rId29" display="https://leetcode.cn/problems/sentence-similarity/" xr:uid="{771EA040-6E9F-427A-9C87-C5F54FA18B80}"/>
     <hyperlink ref="A74" r:id="rId30" display="https://leetcode.cn/problems/count-of-integers/" xr:uid="{0F898565-2E05-4648-B060-6053E5749B06}"/>
     <hyperlink ref="A129" r:id="rId31" display="https://leetcode.cn/problems/subarray-sum-equals-k/" xr:uid="{2C0B7B2D-05D9-44D3-94B3-5D2FA3D976DF}"/>
     <hyperlink ref="A64" r:id="rId32" display="https://leetcode.cn/problems/sliding-window-maximum/" xr:uid="{0260B44B-AA2D-4584-91E2-1E8B8C0ED199}"/>
-    <hyperlink ref="A143" r:id="rId33" display="https://leetcode.cn/problems/minimum-window-substring/" xr:uid="{185B34CF-C6F2-486E-90A5-D7E59F55DC96}"/>
+    <hyperlink ref="A144" r:id="rId33" display="https://leetcode.cn/problems/minimum-window-substring/" xr:uid="{185B34CF-C6F2-486E-90A5-D7E59F55DC96}"/>
     <hyperlink ref="A75" r:id="rId34" display="https://leetcode.cn/problems/find-maximum-number-of-string-pairs/" xr:uid="{70FF04F5-EBD7-4063-8275-F8933C1B9F4E}"/>
     <hyperlink ref="A124" r:id="rId35" display="https://leetcode.cn/problems/maximum-subarray/" xr:uid="{8CC0531C-8284-4F55-81E2-94DB6B274D9B}"/>
     <hyperlink ref="A128" r:id="rId36" display="https://leetcode.cn/problems/merge-intervals/" xr:uid="{A402C0BD-BF9F-430B-842D-C42671ADDBF0}"/>
@@ -4885,21 +4930,21 @@
     <hyperlink ref="E128" r:id="rId45" xr:uid="{6B77CBE0-0575-4283-A5EA-AACEB5B33C59}"/>
     <hyperlink ref="E124" r:id="rId46" xr:uid="{3229D6F6-BBF7-4C3B-B191-8DEB682A8FD3}"/>
     <hyperlink ref="E75" r:id="rId47" xr:uid="{59B4691E-76E8-4849-BF65-B7D31AC7A96D}"/>
-    <hyperlink ref="E143" r:id="rId48" xr:uid="{4A2B3D38-4B96-4BF0-94E8-EF4F01DADA60}"/>
+    <hyperlink ref="E144" r:id="rId48" xr:uid="{4A2B3D38-4B96-4BF0-94E8-EF4F01DADA60}"/>
     <hyperlink ref="E64" r:id="rId49" xr:uid="{AB333045-700E-4C04-88E4-D32E0F6DB718}"/>
     <hyperlink ref="E129" r:id="rId50" xr:uid="{582C87DD-55DC-4B35-9852-0734F202A602}"/>
     <hyperlink ref="E74" r:id="rId51" xr:uid="{9A949AF4-4EB7-44E4-BACF-B1D5B5248519}"/>
-    <hyperlink ref="E139" r:id="rId52" xr:uid="{70C2F0B7-B280-4BFB-BECF-378146CDDA35}"/>
+    <hyperlink ref="E140" r:id="rId52" xr:uid="{70C2F0B7-B280-4BFB-BECF-378146CDDA35}"/>
     <hyperlink ref="E111" r:id="rId53" xr:uid="{4FDD3B32-5D43-4481-A2CA-C7F81DDF97FA}"/>
     <hyperlink ref="E90" r:id="rId54" xr:uid="{710F1479-585D-4444-83C8-6D53E855AFE0}"/>
     <hyperlink ref="E35" r:id="rId55" xr:uid="{7B7DB3A6-D345-447E-9F9A-467C29F36D49}"/>
-    <hyperlink ref="E147" r:id="rId56" xr:uid="{48A15251-608D-4C90-AD44-6D4945946072}"/>
+    <hyperlink ref="E148" r:id="rId56" xr:uid="{48A15251-608D-4C90-AD44-6D4945946072}"/>
     <hyperlink ref="E109" r:id="rId57" xr:uid="{BD52CDA8-8190-48A9-BD92-085140195F73}"/>
     <hyperlink ref="E31" r:id="rId58" xr:uid="{06E19791-8255-436E-9548-022FA2F67FC7}"/>
     <hyperlink ref="E10" r:id="rId59" xr:uid="{B4600BAD-5CAA-424F-AC24-FBBB647DADA7}"/>
     <hyperlink ref="E136" r:id="rId60" xr:uid="{5A80CC00-AD3B-4F26-9D70-5D113E212D77}"/>
     <hyperlink ref="E83" r:id="rId61" xr:uid="{F62B22C6-0054-4391-8F93-7DCA4A04B6C2}"/>
-    <hyperlink ref="E148" r:id="rId62" xr:uid="{E7AB61B6-DBA5-4869-B79F-21DEA0A21A2A}"/>
+    <hyperlink ref="E149" r:id="rId62" xr:uid="{E7AB61B6-DBA5-4869-B79F-21DEA0A21A2A}"/>
     <hyperlink ref="E56" r:id="rId63" xr:uid="{6C0CBDDC-15AB-41BC-8AD8-3A7678612FFE}"/>
     <hyperlink ref="E51" r:id="rId64" xr:uid="{C082DBA3-BF6F-4354-A2B9-4DFDBCA41E3F}"/>
     <hyperlink ref="E70" r:id="rId65" xr:uid="{4AD655D4-539F-43D1-AF21-FD652B3B7D1A}"/>
@@ -4929,8 +4974,8 @@
     <hyperlink ref="A41" r:id="rId89" xr:uid="{66EB66A9-8D6B-4BF6-A6C3-8A5954733BBF}"/>
     <hyperlink ref="A63" r:id="rId90" display="https://leetcode.cn/problems/product-of-array-except-self/" xr:uid="{A190E6D7-6DC0-41FF-B880-4504E51AD0A8}"/>
     <hyperlink ref="A107" r:id="rId91" display="https://leetcode.cn/problems/first-missing-positive/" xr:uid="{D6CDA410-39D8-4983-9BDC-15727DEDFCB0}"/>
-    <hyperlink ref="A138" r:id="rId92" display="https://leetcode.cn/problems/set-matrix-zeroes/" xr:uid="{C6A1E3B1-09D2-47A0-860B-48FEEBC1056B}"/>
-    <hyperlink ref="E138" r:id="rId93" xr:uid="{078E7176-F40A-4347-A445-D7A9552A387A}"/>
+    <hyperlink ref="A139" r:id="rId92" display="https://leetcode.cn/problems/set-matrix-zeroes/" xr:uid="{C6A1E3B1-09D2-47A0-860B-48FEEBC1056B}"/>
+    <hyperlink ref="E139" r:id="rId93" xr:uid="{078E7176-F40A-4347-A445-D7A9552A387A}"/>
     <hyperlink ref="A125" r:id="rId94" display="https://leetcode.cn/problems/spiral-matrix/" xr:uid="{F8766E35-A34B-4EFF-BDF3-0B4AC5DB8C10}"/>
     <hyperlink ref="E125" r:id="rId95" xr:uid="{2D32183A-312F-4B64-A30F-0AB4B3726872}"/>
     <hyperlink ref="A117" r:id="rId96" display="https://leetcode.cn/problems/rotate-image/" xr:uid="{5CD1B5B0-1C26-42C3-A789-7C54A1599DD5}"/>
@@ -4951,14 +4996,14 @@
     <hyperlink ref="A30" r:id="rId111" display="https://leetcode.cn/problems/sort-list/" xr:uid="{C5653710-89D2-47AD-A92A-5BF876E756D0}"/>
     <hyperlink ref="A59" r:id="rId112" display="https://leetcode.cn/problems/merge-k-sorted-lists/" xr:uid="{24641442-A295-4EC8-88E5-B0C09E4F3CAC}"/>
     <hyperlink ref="A29" r:id="rId113" display="https://leetcode.cn/problems/lru-cache/" xr:uid="{B795428B-A2E2-46EA-A417-AF8114C9EF23}"/>
-    <hyperlink ref="A150" r:id="rId114" display="https://leetcode.cn/problems/binary-tree-inorder-traversal/" xr:uid="{BA958F34-070C-4276-8418-94164694D26B}"/>
+    <hyperlink ref="A151" r:id="rId114" display="https://leetcode.cn/problems/binary-tree-inorder-traversal/" xr:uid="{BA958F34-070C-4276-8418-94164694D26B}"/>
     <hyperlink ref="A5" r:id="rId115" display="https://leetcode.cn/problems/maximum-depth-of-binary-tree/" xr:uid="{E2779ECC-F6F2-4721-B2AF-013E62B4A44D}"/>
     <hyperlink ref="A58" r:id="rId116" display="https://leetcode.cn/problems/invert-binary-tree/" xr:uid="{82BC3859-2166-43DC-BCBF-3CB1A966F7A6}"/>
     <hyperlink ref="A3" r:id="rId117" display="https://leetcode.cn/problems/symmetric-tree/" xr:uid="{B28785EA-ECDF-44CC-8B01-1E8171DD13CE}"/>
     <hyperlink ref="A126" r:id="rId118" display="https://leetcode.cn/problems/diameter-of-binary-tree/" xr:uid="{2359DD9C-2BD5-4AEC-B348-6813975B7912}"/>
     <hyperlink ref="A4" r:id="rId119" display="https://leetcode.cn/problems/binary-tree-level-order-traversal/" xr:uid="{1D68961A-6E60-46DE-B611-D7B5D25133FB}"/>
     <hyperlink ref="A9" r:id="rId120" display="https://leetcode.cn/problems/convert-sorted-array-to-binary-search-tree/" xr:uid="{328BE4BD-3DD5-4615-826F-93546C63D4B0}"/>
-    <hyperlink ref="A152" r:id="rId121" display="https://leetcode.cn/problems/validate-binary-search-tree/" xr:uid="{743EA17A-87FE-4F4B-B0BF-739F3BEC24BD}"/>
+    <hyperlink ref="A153" r:id="rId121" display="https://leetcode.cn/problems/validate-binary-search-tree/" xr:uid="{743EA17A-87FE-4F4B-B0BF-739F3BEC24BD}"/>
     <hyperlink ref="A60" r:id="rId122" display="https://leetcode.cn/problems/kth-smallest-element-in-a-bst/" xr:uid="{E8952E47-A552-42F7-872B-3FB6F8ABE394}"/>
     <hyperlink ref="A44" r:id="rId123" display="https://leetcode.cn/problems/binary-tree-right-side-view/" xr:uid="{742E0E19-C628-4E6A-A389-82FC923F760C}"/>
     <hyperlink ref="A11" r:id="rId124" display="https://leetcode.cn/problems/flatten-binary-tree-to-linked-list/" xr:uid="{11440A7B-C0FC-418F-8923-563E96F7E5C0}"/>
@@ -4968,18 +5013,18 @@
     <hyperlink ref="E62" r:id="rId128" xr:uid="{A9C856D9-9F85-4925-88CC-FF911C4EFD32}"/>
     <hyperlink ref="A19" r:id="rId129" display="https://leetcode.cn/problems/binary-tree-maximum-path-sum/" xr:uid="{3678B77A-8804-4A64-AE6C-41376D22B9BC}"/>
     <hyperlink ref="A47" r:id="rId130" display="https://leetcode.cn/problems/number-of-islands/" xr:uid="{A328C414-4CF6-4425-A56A-201C9BC6AD15}"/>
-    <hyperlink ref="A153" r:id="rId131" display="https://leetcode.cn/problems/rotting-oranges/" xr:uid="{C47F4890-A65B-4EA6-BE20-E06AFE42305B}"/>
+    <hyperlink ref="A154" r:id="rId131" display="https://leetcode.cn/problems/rotting-oranges/" xr:uid="{C47F4890-A65B-4EA6-BE20-E06AFE42305B}"/>
     <hyperlink ref="A49" r:id="rId132" display="https://leetcode.cn/problems/course-schedule/" xr:uid="{E474195F-F1D8-4B40-A072-95AA82E77F7B}"/>
     <hyperlink ref="A50" r:id="rId133" display="https://leetcode.cn/problems/implement-trie-prefix-tree/" xr:uid="{ACDFE2DE-83AA-4BAD-8166-E20BAC48A7C3}"/>
     <hyperlink ref="E114" r:id="rId134" xr:uid="{2E898F41-BA84-45AF-A705-0973EB8DB8EE}"/>
     <hyperlink ref="A114" r:id="rId135" display="https://leetcode.cn/problems/permutations/" xr:uid="{8E4E13D8-2A7F-4DC6-A48B-A54ED93B27C0}"/>
-    <hyperlink ref="A145" r:id="rId136" display="https://leetcode.cn/problems/subsets/" xr:uid="{5C409365-541F-4E98-97A1-A1E29CC4F14F}"/>
-    <hyperlink ref="E145" r:id="rId137" xr:uid="{93490963-1363-4F0C-8181-651E214E0B18}"/>
+    <hyperlink ref="A146" r:id="rId136" display="https://leetcode.cn/problems/subsets/" xr:uid="{5C409365-541F-4E98-97A1-A1E29CC4F14F}"/>
+    <hyperlink ref="E146" r:id="rId137" xr:uid="{93490963-1363-4F0C-8181-651E214E0B18}"/>
     <hyperlink ref="A40" r:id="rId138" display="https://leetcode.cn/problems/letter-combinations-of-a-phone-number/" xr:uid="{A72E7149-0969-4B87-A7FC-139F18FFD8BB}"/>
     <hyperlink ref="E40" r:id="rId139" xr:uid="{31CD6DD9-B828-43FC-B338-7CAE71F2DFDF}"/>
     <hyperlink ref="A104" r:id="rId140" display="https://leetcode.cn/problems/combination-sum/" xr:uid="{EFF7251F-6EB1-4CC3-B4A9-227B600CFFA1}"/>
-    <hyperlink ref="E146" r:id="rId141" xr:uid="{D009558D-60D6-4366-8677-9423BF894976}"/>
-    <hyperlink ref="A146" r:id="rId142" display="https://leetcode.cn/problems/word-search/" xr:uid="{6E176417-751F-4EED-B7EB-3128CCF61581}"/>
+    <hyperlink ref="E147" r:id="rId141" xr:uid="{D009558D-60D6-4366-8677-9423BF894976}"/>
+    <hyperlink ref="A147" r:id="rId142" display="https://leetcode.cn/problems/word-search/" xr:uid="{6E176417-751F-4EED-B7EB-3128CCF61581}"/>
     <hyperlink ref="A57" r:id="rId143" display="https://leetcode.cn/problems/generate-parentheses/" xr:uid="{30406B0C-B20F-496A-A2C4-D948173189C3}"/>
     <hyperlink ref="A21" r:id="rId144" display="https://leetcode.cn/problems/palindrome-partitioning/" xr:uid="{C1C42340-3C82-4BD1-8608-8DFFF96FC75B}"/>
     <hyperlink ref="A121" r:id="rId145" display="https://leetcode.cn/problems/n-queens/" xr:uid="{A0187B26-61AC-4C97-9A36-85A591E506B7}"/>
@@ -4987,7 +5032,7 @@
     <hyperlink ref="E98" r:id="rId147" xr:uid="{DDCFD87D-CD38-43E5-ADAF-24E527C68F8E}"/>
     <hyperlink ref="A98" r:id="rId148" display="https://leetcode.cn/problems/find-first-and-last-position-of-element-in-sorted-array/" xr:uid="{BF08E923-B4D9-4EEF-8E92-E28C605CCE32}"/>
     <hyperlink ref="A100" r:id="rId149" display="https://leetcode.cn/problems/search-insert-position/" xr:uid="{54241F2B-5AB4-4177-BC7C-5360532D265E}"/>
-    <hyperlink ref="A141" r:id="rId150" display="https://leetcode.cn/problems/search-a-2d-matrix/" xr:uid="{B827C295-310F-4C1E-8C97-04E52B4E0D8F}"/>
+    <hyperlink ref="A142" r:id="rId150" display="https://leetcode.cn/problems/search-a-2d-matrix/" xr:uid="{B827C295-310F-4C1E-8C97-04E52B4E0D8F}"/>
     <hyperlink ref="E96" r:id="rId151" xr:uid="{66A0E0DB-2AE8-4C0D-B11E-7E0DDADB9B41}"/>
     <hyperlink ref="A96" r:id="rId152" display="https://leetcode.cn/problems/search-in-rotated-sorted-array/" xr:uid="{B22B927E-2356-4B4E-BF35-F484D36559D4}"/>
     <hyperlink ref="A33" r:id="rId153" display="https://leetcode.cn/problems/find-minimum-in-rotated-sorted-array/" xr:uid="{397D2DAE-9BE0-4951-B83D-824D7FBCE07E}"/>
@@ -4998,10 +5043,10 @@
     <hyperlink ref="A34" r:id="rId158" display="https://leetcode.cn/problems/min-stack/" xr:uid="{BD6D5A5D-9717-4253-A2F5-A43EC62D1A5D}"/>
     <hyperlink ref="A105" r:id="rId159" display="https://leetcode.cn/problems/decode-string/" xr:uid="{0B4CACA8-1935-41CF-967A-CAEFF5AECB53}"/>
     <hyperlink ref="E105" r:id="rId160" xr:uid="{819C9DBC-04AA-4864-81C9-0C3EFC02339D}"/>
-    <hyperlink ref="A140" r:id="rId161" display="https://leetcode.cn/problems/daily-temperatures/" xr:uid="{B26C3125-EB8A-4499-B55F-A0327D4C49FD}"/>
-    <hyperlink ref="E140" r:id="rId162" xr:uid="{71B5751F-3CF1-4DC3-931E-B157AACD6558}"/>
-    <hyperlink ref="A149" r:id="rId163" display="https://leetcode.cn/problems/largest-rectangle-in-histogram/" xr:uid="{43247403-6670-4DAE-A4A7-F82A98DB1B18}"/>
-    <hyperlink ref="E149" r:id="rId164" xr:uid="{B99C6DBE-1E6B-4A91-B8BB-C628FC8F5E39}"/>
+    <hyperlink ref="A141" r:id="rId161" display="https://leetcode.cn/problems/daily-temperatures/" xr:uid="{B26C3125-EB8A-4499-B55F-A0327D4C49FD}"/>
+    <hyperlink ref="E141" r:id="rId162" xr:uid="{71B5751F-3CF1-4DC3-931E-B157AACD6558}"/>
+    <hyperlink ref="A150" r:id="rId163" display="https://leetcode.cn/problems/largest-rectangle-in-histogram/" xr:uid="{43247403-6670-4DAE-A4A7-F82A98DB1B18}"/>
+    <hyperlink ref="E150" r:id="rId164" xr:uid="{B99C6DBE-1E6B-4A91-B8BB-C628FC8F5E39}"/>
     <hyperlink ref="A54" r:id="rId165" display="https://leetcode.cn/problems/kth-largest-element-in-an-array/" xr:uid="{6895E2EE-164A-44EC-87C0-E0780657C4D5}"/>
     <hyperlink ref="E89" r:id="rId166" xr:uid="{9D276BED-6F9B-4561-A6CF-0DEE42145361}"/>
     <hyperlink ref="A89" r:id="rId167" display="https://leetcode.cn/problems/find-median-from-data-stream/" xr:uid="{4DBDEEFB-711A-4C7C-B2FA-E0812141E933}"/>
@@ -5009,11 +5054,11 @@
     <hyperlink ref="A16" r:id="rId169" display="https://leetcode.cn/problems/best-time-to-buy-and-sell-stock/" xr:uid="{725CC9CC-B5C3-4BC9-9C17-C040E5E57AA9}"/>
     <hyperlink ref="A127" r:id="rId170" display="https://leetcode.cn/problems/jump-game/" xr:uid="{073E6AFF-55B0-4CBA-9CBA-8E80417E47AD}"/>
     <hyperlink ref="A113" r:id="rId171" display="https://leetcode.cn/problems/jump-game-ii/" xr:uid="{06A56225-774B-41E5-A4C2-DA953CBB2320}"/>
-    <hyperlink ref="A144" r:id="rId172" display="https://leetcode.cn/problems/partition-labels/" xr:uid="{12848DB0-0318-4BDF-BE64-C3F92DACAB58}"/>
-    <hyperlink ref="E144" r:id="rId173" xr:uid="{47AA8A23-9E0A-418A-8B69-FBEB825EFBA9}"/>
+    <hyperlink ref="A145" r:id="rId172" display="https://leetcode.cn/problems/partition-labels/" xr:uid="{12848DB0-0318-4BDF-BE64-C3F92DACAB58}"/>
+    <hyperlink ref="E145" r:id="rId173" xr:uid="{47AA8A23-9E0A-418A-8B69-FBEB825EFBA9}"/>
     <hyperlink ref="A22" r:id="rId174" display="https://leetcode.cn/problems/single-number/" xr:uid="{9BD4A482-0471-4E20-BFC3-734B1CA35641}"/>
     <hyperlink ref="A39" r:id="rId175" display="https://leetcode.cn/problems/majority-element/" xr:uid="{37CD3B5F-77FD-4FD4-9183-F3C2613312F5}"/>
-    <hyperlink ref="A142" r:id="rId176" display="https://leetcode.cn/problems/sort-colors/" xr:uid="{0933A8C1-E6CB-4D8B-B587-B3AE5E152C60}"/>
+    <hyperlink ref="A143" r:id="rId176" display="https://leetcode.cn/problems/sort-colors/" xr:uid="{0933A8C1-E6CB-4D8B-B587-B3AE5E152C60}"/>
     <hyperlink ref="A92" r:id="rId177" display="https://leetcode.cn/problems/next-permutation/" xr:uid="{00924165-81E0-40E5-9B50-126714BD9EC1}"/>
     <hyperlink ref="E92" r:id="rId178" xr:uid="{FA68184D-DC6E-4B73-905E-7367F174DAB4}"/>
     <hyperlink ref="A88" r:id="rId179" display="https://leetcode.cn/problems/find-the-duplicate-number/" xr:uid="{71AD2502-07F8-491F-B447-E038CFD2DE0A}"/>
@@ -5035,11 +5080,11 @@
     <hyperlink ref="E120" r:id="rId195" xr:uid="{5CB9B51C-4ADC-465D-985F-47361FC2BE8A}"/>
     <hyperlink ref="A12" r:id="rId196" display="https://leetcode.cn/problems/longest-common-subsequence/" xr:uid="{708E0024-B68F-45A5-941B-550E630409AF}"/>
     <hyperlink ref="E12" r:id="rId197" xr:uid="{F6D25B62-12B1-4A86-A3DB-7CC7ACA6C9BC}"/>
-    <hyperlink ref="A137" r:id="rId198" display="https://leetcode.cn/problems/edit-distance/" xr:uid="{F38D478C-0D97-4DB6-852E-47E16D7FF6B2}"/>
-    <hyperlink ref="E137" r:id="rId199" location="%E7%AE%97%E6%B3%95%E5%85%AC%E5%BC%80%E8%AF%BE" xr:uid="{CD3FC349-C931-44B5-AB44-6E548F888619}"/>
+    <hyperlink ref="A138" r:id="rId198" display="https://leetcode.cn/problems/edit-distance/" xr:uid="{F38D478C-0D97-4DB6-852E-47E16D7FF6B2}"/>
+    <hyperlink ref="E138" r:id="rId199" location="%E7%AE%97%E6%B3%95%E5%85%AC%E5%BC%80%E8%AF%BE" xr:uid="{CD3FC349-C931-44B5-AB44-6E548F888619}"/>
     <hyperlink ref="A135" r:id="rId200" display="https://leetcode.cn/problems/binary-search/" xr:uid="{85DCB780-B636-4DA3-8E98-BDD6E2AB99B6}"/>
     <hyperlink ref="A72" r:id="rId201" display="https://leetcode.cn/problems/remove-element/" xr:uid="{74E7E043-E9D5-4F13-8753-25FD9681EED1}"/>
-    <hyperlink ref="A151" r:id="rId202" display="https://leetcode.cn/problems/squares-of-a-sorted-array/" xr:uid="{950D9E34-B826-4CA9-A2F0-6441BEDFF66B}"/>
+    <hyperlink ref="A152" r:id="rId202" display="https://leetcode.cn/problems/squares-of-a-sorted-array/" xr:uid="{950D9E34-B826-4CA9-A2F0-6441BEDFF66B}"/>
     <hyperlink ref="A93" r:id="rId203" display="https://leetcode.cn/problems/make-a-square-with-the-same-color/" xr:uid="{B400DA20-AE2E-4324-AC47-87BA46F421DE}"/>
     <hyperlink ref="A28" r:id="rId204" display="https://leetcode.cn/problems/number-of-students-doing-homework-at-a-given-time/" xr:uid="{AA720C4C-25A2-4B25-89B7-BBECE40C40BB}"/>
     <hyperlink ref="E108" r:id="rId205" location="%E7%AE%97%E6%B3%95%E5%85%AC%E5%BC%80%E8%AF%BE" xr:uid="{B37EB81F-EF1F-4396-86C4-07A4B6B4BD23}"/>
@@ -5072,10 +5117,12 @@
     <hyperlink ref="A38" r:id="rId232" display="https://leetcode.cn/problems/one-edit-distance/" xr:uid="{E5267046-4F48-4788-8D8B-CE1C5168CCE8}"/>
     <hyperlink ref="E57" r:id="rId233" xr:uid="{4149FF56-A218-41F1-9B6F-4A183B8B3BEF}"/>
     <hyperlink ref="E21" r:id="rId234" xr:uid="{0E87DF0C-2792-4918-BDDA-19A654B3DC20}"/>
+    <hyperlink ref="A137" r:id="rId235" display="https://leetcode.cn/problems/maximum-length-of-repeated-subarray/" xr:uid="{F3278CD2-BB0F-4DE2-BA98-C729C413733A}"/>
+    <hyperlink ref="E137" r:id="rId236" location="%E7%AE%97%E6%B3%95%E5%85%AC%E5%BC%80%E8%AF%BE" xr:uid="{6B8A95CC-5586-4C6D-AAA8-86008E5BCE55}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <tableParts count="1">
-    <tablePart r:id="rId235"/>
+    <tablePart r:id="rId237"/>
   </tableParts>
 </worksheet>
 </file>
</xml_diff>